<commit_message>
"Fixing examples and moving employmentStartDate to the correct location"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -13,15 +13,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="229">
   <si>
     <t>Document</t>
   </si>
@@ -1669,56 +1669,6 @@
     <t>New RPN Request</t>
   </si>
   <si>
-    <r>
-      <t>add ‘</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>employment start date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>’ as an optional request field.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>New PRSI exemption option '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>' added</t>
-    </r>
-  </si>
-  <si>
     <t>Submission Request Line Items</t>
   </si>
   <si>
@@ -1763,32 +1713,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 'PRSI Exemption Reason' </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Add ‘</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>employment start date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>’ as an optional request field.</t>
     </r>
   </si>
   <si>
@@ -1945,6 +1869,522 @@
       <t>format</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>New PRSI exemption option '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">' added                                                                                     Payslip requirement removed                                                                                               </t>
+    </r>
+  </si>
+  <si>
+    <t>Example 4.2</t>
+  </si>
+  <si>
+    <t>Example 5.2</t>
+  </si>
+  <si>
+    <t>Example 5.3</t>
+  </si>
+  <si>
+    <t>Example 5.9</t>
+  </si>
+  <si>
+    <t>Example 5.10</t>
+  </si>
+  <si>
+    <t>Example 9.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ppsn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' corrected</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>employeePpsn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineItemIDToDelete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' corrected to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineItemIDsToDelete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>newEmployeeDetails</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> element added</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>taxYear'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>totalRPNCount'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> removed from NewRPNResponse example</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineItemIDToDelete'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> corrected to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lineItemIDsToDelete'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pensionTracingNumber</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' corrected to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pensionTracingNumbers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">incomeTacCalculationBasis' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>corrected to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>incomeTaxCalculationBasis'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pensionTracingNumber' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>corrected format</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uscPaidToDate'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> correct to '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USCDeductedToDate'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">yearlyUSCRateCutOff </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in taxRate property corrected to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yearlyRateCutOff</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Added ‘</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>employment start date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>’ as an optional request field.</t>
+    </r>
+  </si>
+  <si>
+    <t>REST Integration Guide</t>
+  </si>
+  <si>
+    <t>HTTP-Method-Override</t>
+  </si>
+  <si>
+    <t>Example clarified</t>
+  </si>
+  <si>
+    <t>Property description clarified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employeeIDs </t>
+  </si>
+  <si>
+    <r>
+      <t>added ‘</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>employmentStartDate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>’ as an optional request field of newEmployeeDetails property</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Added ‘</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>employment start date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>’ as an optional request field of NewEmployeeDetails property</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -2070,7 +2510,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -2482,53 +2922,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2684,12 +3082,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2709,32 +3101,46 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2782,22 +3188,31 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2808,44 +3223,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2853,68 +3253,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3283,12 +3647,12 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="87"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3313,12 +3677,12 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3361,10 +3725,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="87">
+      <c r="B7" s="91">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3379,8 +3743,8 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="85"/>
-      <c r="B8" s="88"/>
+      <c r="A8" s="89"/>
+      <c r="B8" s="92"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -3393,8 +3757,8 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="85"/>
-      <c r="B9" s="88"/>
+      <c r="A9" s="89"/>
+      <c r="B9" s="92"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3407,8 +3771,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="85"/>
-      <c r="B10" s="88"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="92"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -3421,8 +3785,8 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="85"/>
-      <c r="B11" s="88"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -3435,8 +3799,8 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="89"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="93"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -3449,10 +3813,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="92" t="s">
+      <c r="A13" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="87">
+      <c r="B13" s="91">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -3467,8 +3831,8 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="93"/>
-      <c r="B14" s="89"/>
+      <c r="A14" s="97"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -3517,12 +3881,12 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="83"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="87"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3565,22 +3929,22 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="82"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="83"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="87"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="91">
+      <c r="B21" s="95">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -3595,8 +3959,8 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="95"/>
-      <c r="B22" s="89"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="93"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -3619,18 +3983,18 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="83"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="87"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="91">
+      <c r="B25" s="95">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -3645,8 +4009,8 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="85"/>
-      <c r="B26" s="88"/>
+      <c r="A26" s="89"/>
+      <c r="B26" s="92"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -3659,8 +4023,8 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="85"/>
-      <c r="B27" s="88"/>
+      <c r="A27" s="89"/>
+      <c r="B27" s="92"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -3673,8 +4037,8 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="85"/>
-      <c r="B28" s="88"/>
+      <c r="A28" s="89"/>
+      <c r="B28" s="92"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -3687,8 +4051,8 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="85"/>
-      <c r="B29" s="88"/>
+      <c r="A29" s="89"/>
+      <c r="B29" s="92"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -3701,8 +4065,8 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="85"/>
-      <c r="B30" s="88"/>
+      <c r="A30" s="89"/>
+      <c r="B30" s="92"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -3715,8 +4079,8 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="85"/>
-      <c r="B31" s="88"/>
+      <c r="A31" s="89"/>
+      <c r="B31" s="92"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -3729,8 +4093,8 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="86"/>
-      <c r="B32" s="89"/>
+      <c r="A32" s="90"/>
+      <c r="B32" s="93"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -3855,12 +4219,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="82"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="83"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="87"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -3920,7 +4284,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3930,7 +4294,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4040,10 +4404,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="103" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4054,8 +4418,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="106"/>
-      <c r="B8" s="105"/>
+      <c r="A8" s="102"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -4064,8 +4428,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="106"/>
-      <c r="B9" s="105"/>
+      <c r="A9" s="102"/>
+      <c r="B9" s="103"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -4074,8 +4438,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="106"/>
-      <c r="B10" s="105"/>
+      <c r="A10" s="102"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -4084,8 +4448,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="106"/>
-      <c r="B11" s="105"/>
+      <c r="A11" s="102"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -4094,8 +4458,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="106"/>
-      <c r="B12" s="105"/>
+      <c r="A12" s="102"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -4104,10 +4468,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="103" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4118,8 +4482,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="108"/>
-      <c r="B14" s="105"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -4128,8 +4492,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="108"/>
-      <c r="B15" s="105"/>
+      <c r="A15" s="113"/>
+      <c r="B15" s="103"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -4138,10 +4502,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="109" t="s">
+      <c r="A16" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="100" t="s">
+      <c r="B16" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -4152,8 +4516,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="109"/>
-      <c r="B17" s="100"/>
+      <c r="A17" s="100"/>
+      <c r="B17" s="112"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -4162,8 +4526,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109"/>
-      <c r="B18" s="100"/>
+      <c r="A18" s="100"/>
+      <c r="B18" s="112"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -4172,8 +4536,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109"/>
-      <c r="B19" s="100"/>
+      <c r="A19" s="100"/>
+      <c r="B19" s="112"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -4182,8 +4546,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="109"/>
-      <c r="B20" s="100"/>
+      <c r="A20" s="100"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -4192,29 +4556,29 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="109"/>
-      <c r="B21" s="100"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="112"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="D21" s="67" t="s">
+      <c r="D21" s="65" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="109"/>
-      <c r="B22" s="100"/>
+      <c r="A22" s="100"/>
+      <c r="B22" s="112"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="63" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="109"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="68" t="s">
+      <c r="A23" s="100"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
       <c r="D23" s="54" t="s">
@@ -4222,26 +4586,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="109"/>
-      <c r="B24" s="100"/>
-      <c r="C24" s="109" t="s">
+      <c r="A24" s="100"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="100" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="110" t="s">
+      <c r="D24" s="101" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="109"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="109"/>
-      <c r="D25" s="110"/>
+      <c r="A25" s="100"/>
+      <c r="B25" s="112"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="101"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="106" t="s">
+      <c r="A26" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="105" t="s">
+      <c r="B26" s="103" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -4252,8 +4616,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="106"/>
-      <c r="B27" s="105"/>
+      <c r="A27" s="102"/>
+      <c r="B27" s="103"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -4280,28 +4644,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="107" t="s">
+      <c r="A30" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="105" t="s">
+      <c r="B30" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="109" t="s">
+      <c r="C30" s="100" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="98" t="s">
+      <c r="D30" s="108" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="107"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="109"/>
-      <c r="D31" s="98"/>
+      <c r="A31" s="104"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="100"/>
+      <c r="D31" s="108"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="107"/>
-      <c r="B32" s="105"/>
+      <c r="A32" s="104"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -4310,8 +4674,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="107"/>
-      <c r="B33" s="105"/>
+      <c r="A33" s="104"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -4320,18 +4684,18 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="107"/>
-      <c r="B34" s="105"/>
-      <c r="C34" s="69" t="s">
+      <c r="A34" s="104"/>
+      <c r="B34" s="103"/>
+      <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
-      <c r="D34" s="70" t="s">
+      <c r="D34" s="68" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="107"/>
-      <c r="B35" s="105"/>
+      <c r="A35" s="104"/>
+      <c r="B35" s="103"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -4340,36 +4704,36 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="107"/>
-      <c r="B36" s="105"/>
-      <c r="C36" s="69" t="s">
+      <c r="A36" s="104"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="D36" s="70" t="s">
+      <c r="D36" s="68" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="107"/>
-      <c r="B37" s="105"/>
-      <c r="C37" s="111" t="s">
+      <c r="A37" s="104"/>
+      <c r="B37" s="103"/>
+      <c r="C37" s="105" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="113" t="s">
+      <c r="D37" s="107" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="107"/>
-      <c r="B38" s="105"/>
-      <c r="C38" s="112"/>
-      <c r="D38" s="113"/>
+      <c r="A38" s="104"/>
+      <c r="B38" s="103"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="107"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="106" t="s">
+      <c r="A39" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="105" t="s">
+      <c r="B39" s="103" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -4380,8 +4744,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="106"/>
-      <c r="B40" s="105"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="103"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -4408,10 +4772,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="107" t="s">
+      <c r="A43" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="105" t="s">
+      <c r="B43" s="103" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -4420,8 +4784,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="107"/>
-      <c r="B44" s="105"/>
+      <c r="A44" s="104"/>
+      <c r="B44" s="103"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -4430,20 +4794,20 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="102" t="s">
+      <c r="A45" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="105" t="s">
+      <c r="B45" s="103" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
-      <c r="D45" s="66" t="s">
+      <c r="D45" s="64" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="103"/>
-      <c r="B46" s="105"/>
+      <c r="A46" s="110"/>
+      <c r="B46" s="103"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -4452,8 +4816,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="103"/>
-      <c r="B47" s="105"/>
+      <c r="A47" s="110"/>
+      <c r="B47" s="103"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -4462,8 +4826,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="104"/>
-      <c r="B48" s="105"/>
+      <c r="A48" s="111"/>
+      <c r="B48" s="103"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -4472,10 +4836,10 @@
       </c>
     </row>
     <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="100" t="s">
+      <c r="A49" s="112" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="100" t="s">
+      <c r="B49" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -8579,8 +8943,8 @@
       <c r="XFD49" s="42"/>
     </row>
     <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="100"/>
-      <c r="B50" s="100"/>
+      <c r="A50" s="112"/>
+      <c r="B50" s="112"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -12684,8 +13048,8 @@
       <c r="XFD50" s="42"/>
     </row>
     <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="100"/>
-      <c r="B51" s="100"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="112"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -16789,8 +17153,8 @@
       <c r="XFD51" s="42"/>
     </row>
     <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="100"/>
-      <c r="B52" s="100"/>
+      <c r="A52" s="112"/>
+      <c r="B52" s="112"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -20894,12 +21258,12 @@
       <c r="XFD52" s="42"/>
     </row>
     <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="100"/>
-      <c r="B53" s="100"/>
-      <c r="C53" s="97" t="s">
+      <c r="A53" s="112"/>
+      <c r="B53" s="112"/>
+      <c r="C53" s="115" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="98" t="s">
+      <c r="D53" s="108" t="s">
         <v>144</v>
       </c>
       <c r="H53" s="42"/>
@@ -24999,10 +25363,10 @@
       <c r="XFD53" s="42"/>
     </row>
     <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="100"/>
-      <c r="B54" s="100"/>
-      <c r="C54" s="97"/>
-      <c r="D54" s="98"/>
+      <c r="A54" s="112"/>
+      <c r="B54" s="112"/>
+      <c r="C54" s="115"/>
+      <c r="D54" s="108"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -29120,10 +29484,10 @@
       </c>
     </row>
     <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="99" t="s">
+      <c r="A57" s="116" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="100" t="s">
+      <c r="B57" s="112" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -29134,8 +29498,8 @@
       </c>
     </row>
     <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="99"/>
-      <c r="B58" s="100"/>
+      <c r="A58" s="116"/>
+      <c r="B58" s="112"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -29144,8 +29508,8 @@
       </c>
     </row>
     <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="99"/>
-      <c r="B59" s="100"/>
+      <c r="A59" s="116"/>
+      <c r="B59" s="112"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -29154,8 +29518,8 @@
       </c>
     </row>
     <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="99"/>
-      <c r="B60" s="100"/>
+      <c r="A60" s="116"/>
+      <c r="B60" s="112"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -29164,8 +29528,8 @@
       </c>
     </row>
     <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="99"/>
-      <c r="B61" s="100"/>
+      <c r="A61" s="116"/>
+      <c r="B61" s="112"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -29174,8 +29538,8 @@
       </c>
     </row>
     <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="99"/>
-      <c r="B62" s="100"/>
+      <c r="A62" s="116"/>
+      <c r="B62" s="112"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -29184,8 +29548,8 @@
       </c>
     </row>
     <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="99"/>
-      <c r="B63" s="100"/>
+      <c r="A63" s="116"/>
+      <c r="B63" s="112"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -29194,16 +29558,16 @@
       </c>
     </row>
     <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="99"/>
-      <c r="B64" s="100"/>
+      <c r="A64" s="116"/>
+      <c r="B64" s="112"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="99"/>
-      <c r="B65" s="100"/>
+      <c r="A65" s="116"/>
+      <c r="B65" s="112"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -29212,16 +29576,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="99"/>
-      <c r="B66" s="100"/>
+      <c r="A66" s="116"/>
+      <c r="B66" s="112"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="99"/>
-      <c r="B67" s="100"/>
+      <c r="A67" s="116"/>
+      <c r="B67" s="112"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -29230,8 +29594,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="99"/>
-      <c r="B68" s="100"/>
+      <c r="A68" s="116"/>
+      <c r="B68" s="112"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -29240,8 +29604,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="99"/>
-      <c r="B69" s="100"/>
+      <c r="A69" s="116"/>
+      <c r="B69" s="112"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -29250,8 +29614,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="99"/>
-      <c r="B70" s="100"/>
+      <c r="A70" s="116"/>
+      <c r="B70" s="112"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -29260,8 +29624,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="99"/>
-      <c r="B71" s="100"/>
+      <c r="A71" s="116"/>
+      <c r="B71" s="112"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -29270,8 +29634,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="99"/>
-      <c r="B72" s="100"/>
+      <c r="A72" s="116"/>
+      <c r="B72" s="112"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -29280,16 +29644,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="99"/>
-      <c r="B73" s="100"/>
+      <c r="A73" s="116"/>
+      <c r="B73" s="112"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="99"/>
-      <c r="B74" s="100"/>
+      <c r="A74" s="116"/>
+      <c r="B74" s="112"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -29298,18 +29662,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="99"/>
-      <c r="B75" s="100"/>
-      <c r="C75" s="96"/>
-      <c r="D75" s="101" t="s">
+      <c r="A75" s="116"/>
+      <c r="B75" s="112"/>
+      <c r="C75" s="114"/>
+      <c r="D75" s="117" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="99"/>
-      <c r="B76" s="100"/>
-      <c r="C76" s="96"/>
-      <c r="D76" s="101"/>
+      <c r="A76" s="116"/>
+      <c r="B76" s="112"/>
+      <c r="C76" s="114"/>
+      <c r="D76" s="117"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -29333,8 +29697,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -29343,13 +29707,31 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="B16:B25"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="A39:A40"/>
@@ -29362,24 +29744,6 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="B16:B25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -29388,10 +29752,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29425,182 +29789,182 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="136" t="s">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="71" t="s">
-        <v>198</v>
+      <c r="C4" s="72" t="s">
+        <v>195</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="136"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="119" t="s">
+      <c r="A5" s="102"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="121" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="118" t="s">
-        <v>205</v>
+      <c r="D5" s="120" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="136"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="118"/>
+      <c r="A6" s="102"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="120"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="136"/>
-      <c r="B7" s="105"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="49"/>
+      <c r="A7" s="102"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="136"/>
-      <c r="B8" s="105"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="49"/>
+      <c r="A8" s="102"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="136"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="80"/>
+      <c r="A9" s="102"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="137" t="s">
+    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="113" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="129"/>
-      <c r="D10" s="118" t="s">
+      <c r="C10" s="119"/>
+      <c r="D10" s="120" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="137"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="118"/>
+      <c r="A11" s="113"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="120"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="137"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="129"/>
-      <c r="D12" s="118"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="120"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="138" t="s">
+      <c r="A13" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="112" t="s">
         <v>185</v>
       </c>
       <c r="C13" s="122"/>
-      <c r="D13" s="118" t="s">
-        <v>206</v>
+      <c r="D13" s="120" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="139"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="118"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="120"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="139"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="123"/>
+      <c r="A15" s="100"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="122"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="139"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="123"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="122"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="139"/>
-      <c r="B17" s="100"/>
-      <c r="C17" s="123"/>
+      <c r="A17" s="100"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="122"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="139"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="123"/>
+      <c r="A18" s="100"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="122"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="139"/>
-      <c r="B19" s="100"/>
-      <c r="C19" s="123"/>
+      <c r="A19" s="100"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="122"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="139"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="123"/>
+      <c r="A20" s="100"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="122"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="139"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="123"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="122"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="139"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="123"/>
+      <c r="A22" s="100"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="122"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="140"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="124"/>
+      <c r="A23" s="100"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="122"/>
       <c r="D23" s="58" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="73" t="s">
         <v>187</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C24" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="D24" s="54" t="s">
+      <c r="D24" s="78" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="79" t="s">
+    <row r="25" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="74" t="s">
         <v>185</v>
       </c>
       <c r="C25" s="38"/>
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="73" t="s">
         <v>166</v>
       </c>
     </row>
@@ -29613,80 +29977,92 @@
       <c r="D26" s="39"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="133" t="s">
+      <c r="A27" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="105" t="s">
+      <c r="B27" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="C27" s="73" t="s">
+      <c r="C27" s="79" t="s">
         <v>191</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="134"/>
-      <c r="B28" s="105"/>
-      <c r="C28" s="74" t="s">
+    <row r="28" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="104"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="70" t="s">
         <v>189</v>
       </c>
-      <c r="D28" s="70" t="s">
-        <v>193</v>
+      <c r="D28" s="68" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="134"/>
-      <c r="B29" s="105"/>
-      <c r="C29" s="125" t="s">
+      <c r="A29" s="104"/>
+      <c r="B29" s="103"/>
+      <c r="C29" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="D29" s="126" t="s">
-        <v>204</v>
+      <c r="D29" s="76" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="134"/>
-      <c r="B30" s="105"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="127"/>
+      <c r="A30" s="104"/>
+      <c r="B30" s="103"/>
+      <c r="C30" s="123" t="s">
+        <v>226</v>
+      </c>
+      <c r="D30" s="108" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="134"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="127"/>
+      <c r="A31" s="104"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="108"/>
     </row>
     <row r="32" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="134"/>
-      <c r="B32" s="105"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="127"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="76"/>
     </row>
     <row r="33" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="134"/>
-      <c r="B33" s="105"/>
-      <c r="C33" s="125"/>
-      <c r="D33" s="127"/>
+      <c r="A33" s="75"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="76"/>
     </row>
     <row r="34" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="134"/>
-      <c r="B34" s="105"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="127"/>
+      <c r="A34" s="75"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="76"/>
     </row>
-    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="135"/>
-      <c r="B35" s="105"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="128"/>
+    <row r="35" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="75" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35" s="74" t="s">
+        <v>185</v>
+      </c>
+      <c r="C35" s="79" t="s">
+        <v>223</v>
+      </c>
+      <c r="D35" s="76" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="74" t="s">
         <v>185</v>
       </c>
       <c r="C36" s="38"/>
@@ -29702,24 +30078,24 @@
       <c r="C37" s="39"/>
       <c r="D37" s="44"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="107" t="s">
+    <row r="38" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="105" t="s">
+      <c r="B38" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="C38" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="D38" s="75" t="s">
-        <v>195</v>
+      <c r="C38" s="77" t="s">
+        <v>192</v>
+      </c>
+      <c r="D38" s="82" t="s">
+        <v>193</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="107"/>
-      <c r="B39" s="105"/>
-      <c r="C39" s="72" t="s">
+    <row r="39" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="104"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="69" t="s">
         <v>190</v>
       </c>
       <c r="D39" s="52" t="s">
@@ -29730,81 +30106,81 @@
       <c r="A40" s="102" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="105" t="s">
+      <c r="B40" s="103" t="s">
         <v>185</v>
       </c>
-      <c r="C40" s="114" t="s">
-        <v>197</v>
-      </c>
-      <c r="D40" s="116" t="s">
-        <v>196</v>
+      <c r="C40" s="119" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="100" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="103"/>
-      <c r="B41" s="105"/>
-      <c r="C41" s="115"/>
-      <c r="D41" s="117"/>
+      <c r="A41" s="102"/>
+      <c r="B41" s="103"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="100"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="103"/>
-      <c r="B42" s="105"/>
-      <c r="C42" s="114" t="s">
+      <c r="A42" s="102"/>
+      <c r="B42" s="103"/>
+      <c r="C42" s="119" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="120" t="s">
+      <c r="D42" s="117" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="104"/>
-      <c r="B43" s="105"/>
-      <c r="C43" s="115"/>
-      <c r="D43" s="121"/>
+      <c r="A43" s="102"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="117"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="130" t="s">
+    <row r="44" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="100" t="s">
+      <c r="B44" s="112" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="58"/>
-      <c r="D44" s="47" t="s">
-        <v>202</v>
+      <c r="C44" s="126"/>
+      <c r="D44" s="130" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="131"/>
-      <c r="B45" s="100"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="60" t="s">
-        <v>203</v>
+      <c r="A45" s="116"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="127"/>
+      <c r="D45" s="124" t="s">
+        <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="131"/>
-      <c r="B46" s="100"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="47"/>
+    <row r="46" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="116"/>
+      <c r="B46" s="112"/>
+      <c r="C46" s="127"/>
+      <c r="D46" s="129"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="131"/>
-      <c r="B47" s="100"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="47"/>
+    <row r="47" spans="1:4" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="116"/>
+      <c r="B47" s="112"/>
+      <c r="C47" s="128"/>
+      <c r="D47" s="129"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="131"/>
-      <c r="B48" s="100"/>
-      <c r="C48" s="97"/>
-      <c r="D48" s="98"/>
+    <row r="48" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="116"/>
+      <c r="B48" s="112"/>
+      <c r="C48" s="115"/>
+      <c r="D48" s="129"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="132"/>
-      <c r="B49" s="100"/>
-      <c r="C49" s="97"/>
-      <c r="D49" s="98"/>
+    <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="116"/>
+      <c r="B49" s="112"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="125"/>
     </row>
     <row r="50" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="39" t="s">
@@ -29818,7 +30194,7 @@
       <c r="A51" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="63" t="s">
+      <c r="B51" s="74" t="s">
         <v>185</v>
       </c>
       <c r="C51" s="38"/>
@@ -29827,177 +30203,228 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="99" t="s">
+      <c r="A52" s="112" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="100" t="s">
+      <c r="B52" s="112" t="s">
         <v>185</v>
       </c>
-      <c r="C52" s="58" t="s">
-        <v>200</v>
+      <c r="C52" s="79" t="s">
+        <v>197</v>
       </c>
       <c r="D52" s="47" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="99"/>
-      <c r="B53" s="100"/>
-      <c r="C53" s="58" t="s">
+      <c r="A53" s="112"/>
+      <c r="B53" s="112"/>
+      <c r="C53" s="79" t="s">
         <v>190</v>
       </c>
       <c r="D53" s="47" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="99"/>
-      <c r="B54" s="100"/>
-      <c r="C54" s="58"/>
+    <row r="54" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="112"/>
+      <c r="B54" s="112"/>
+      <c r="C54" s="79" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" s="81" t="s">
+        <v>212</v>
+      </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="99"/>
-      <c r="B55" s="100"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="62"/>
+    <row r="55" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="112"/>
+      <c r="B55" s="112"/>
+      <c r="C55" s="118" t="s">
+        <v>208</v>
+      </c>
+      <c r="D55" s="80" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="99"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="47"/>
+      <c r="A56" s="112"/>
+      <c r="B56" s="112"/>
+      <c r="C56" s="118"/>
+      <c r="D56" s="47" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="99"/>
-      <c r="B57" s="100"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="47"/>
+      <c r="A57" s="112"/>
+      <c r="B57" s="112"/>
+      <c r="C57" s="79" t="s">
+        <v>209</v>
+      </c>
+      <c r="D57" s="46" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="99"/>
-      <c r="B58" s="100"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="47"/>
+      <c r="A58" s="112"/>
+      <c r="B58" s="112"/>
+      <c r="C58" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="D58" s="80" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="99"/>
-      <c r="B59" s="100"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="47"/>
+      <c r="A59" s="112"/>
+      <c r="B59" s="112"/>
+      <c r="C59" s="118" t="s">
+        <v>207</v>
+      </c>
+      <c r="D59" s="46" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="99"/>
-      <c r="B60" s="100"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="47"/>
+      <c r="A60" s="112"/>
+      <c r="B60" s="112"/>
+      <c r="C60" s="118"/>
+      <c r="D60" s="46" t="s">
+        <v>217</v>
+      </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="99"/>
-      <c r="B61" s="100"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="46"/>
+    <row r="61" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="112"/>
+      <c r="B61" s="112"/>
+      <c r="C61" s="118"/>
+      <c r="D61" s="80" t="s">
+        <v>218</v>
+      </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="99"/>
-      <c r="B62" s="100"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="62"/>
+    <row r="62" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="112"/>
+      <c r="B62" s="112"/>
+      <c r="C62" s="119" t="s">
+        <v>206</v>
+      </c>
+      <c r="D62" s="45" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="99"/>
-      <c r="B63" s="100"/>
-      <c r="C63" s="61"/>
-      <c r="D63" s="62"/>
+    <row r="63" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="112"/>
+      <c r="B63" s="112"/>
+      <c r="C63" s="119"/>
+      <c r="D63" s="117" t="s">
+        <v>220</v>
+      </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="99"/>
-      <c r="B64" s="100"/>
-      <c r="C64" s="61"/>
-      <c r="D64" s="47"/>
+    <row r="64" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="112"/>
+      <c r="B64" s="112"/>
+      <c r="C64" s="119"/>
+      <c r="D64" s="117"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="99"/>
-      <c r="B65" s="100"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="47"/>
+    <row r="65" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="112"/>
+      <c r="B65" s="112"/>
+      <c r="C65" s="119"/>
+      <c r="D65" s="117"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="99"/>
-      <c r="B66" s="100"/>
-      <c r="C66" s="58"/>
-      <c r="D66" s="47"/>
+    <row r="66" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="112"/>
+      <c r="B66" s="112"/>
+      <c r="C66" s="119"/>
+      <c r="D66" s="117"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="99"/>
-      <c r="B67" s="100"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="47"/>
+    <row r="67" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="39"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="39"/>
+      <c r="D67" s="44"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="99"/>
-      <c r="B68" s="100"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="49"/>
+      <c r="A68" s="83"/>
+      <c r="B68" s="84"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="99"/>
-      <c r="B69" s="100"/>
-      <c r="C69" s="96"/>
-      <c r="D69" s="47"/>
+      <c r="A69" s="83"/>
+      <c r="B69" s="84"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="99"/>
-      <c r="B70" s="100"/>
-      <c r="C70" s="96"/>
-      <c r="D70" s="101"/>
+      <c r="A70" s="83"/>
+      <c r="B70" s="84"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="99"/>
-      <c r="B71" s="100"/>
-      <c r="D71" s="101"/>
+      <c r="A71" s="83"/>
+      <c r="B71" s="84"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="44"/>
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="35">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C62:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="A52:A66"/>
+    <mergeCell ref="B52:B66"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D45:D49"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="A13:A23"/>
     <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="A27:A35"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="A52:A71"/>
-    <mergeCell ref="B52:B71"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C29:C35"/>
-    <mergeCell ref="D29:D35"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"New Docs and Scenarios"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -13,15 +13,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="234">
   <si>
     <t>Document</t>
   </si>
@@ -2385,12 +2385,28 @@
       <t>’ as an optional request field of NewEmployeeDetails property</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Additional information added in relation to digest algorithms used for ‘Digest’ HTTP header.
+</t>
+  </si>
+  <si>
+    <t>Section 4.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOAP Web Service Integration Guide </t>
+  </si>
+  <si>
+    <t>4.2.2 Timestamp</t>
+  </si>
+  <si>
+    <t>Added "maximum time" line</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2485,6 +2501,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3D3C40"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2926,7 +2949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3118,9 +3141,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3141,6 +3161,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3188,19 +3241,49 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3211,42 +3294,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3256,10 +3303,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3274,11 +3324,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3647,12 +3712,12 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3677,12 +3742,12 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="87"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3725,10 +3790,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="91">
+      <c r="B7" s="101">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3743,8 +3808,8 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
-      <c r="B8" s="92"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -3757,8 +3822,8 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
-      <c r="B9" s="92"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3771,8 +3836,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
-      <c r="B10" s="92"/>
+      <c r="A10" s="99"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -3785,8 +3850,8 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="89"/>
-      <c r="B11" s="92"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -3799,8 +3864,8 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="90"/>
-      <c r="B12" s="93"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -3813,10 +3878,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="91">
+      <c r="B13" s="101">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -3831,8 +3896,8 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="97"/>
-      <c r="B14" s="93"/>
+      <c r="A14" s="107"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -3881,12 +3946,12 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="87"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="97"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -3929,22 +3994,22 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="85" t="s">
+      <c r="A20" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="87"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="97"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="98" t="s">
+      <c r="A21" s="108" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="95">
+      <c r="B21" s="105">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -3959,8 +4024,8 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="99"/>
-      <c r="B22" s="93"/>
+      <c r="A22" s="109"/>
+      <c r="B22" s="103"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -3983,18 +4048,18 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="85" t="s">
+      <c r="A24" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="87"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="97"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="95">
+      <c r="B25" s="105">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4009,8 +4074,8 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="89"/>
-      <c r="B26" s="92"/>
+      <c r="A26" s="99"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4023,8 +4088,8 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="92"/>
+      <c r="A27" s="99"/>
+      <c r="B27" s="102"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4037,8 +4102,8 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="89"/>
-      <c r="B28" s="92"/>
+      <c r="A28" s="99"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4051,8 +4116,8 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="89"/>
-      <c r="B29" s="92"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4065,8 +4130,8 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="89"/>
-      <c r="B30" s="92"/>
+      <c r="A30" s="99"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4079,8 +4144,8 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="89"/>
-      <c r="B31" s="92"/>
+      <c r="A31" s="99"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4093,8 +4158,8 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="90"/>
-      <c r="B32" s="93"/>
+      <c r="A32" s="100"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4219,12 +4284,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="87"/>
+      <c r="B41" s="96"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="97"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -4284,7 +4349,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4294,7 +4359,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4404,10 +4469,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4418,8 +4483,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="102"/>
-      <c r="B8" s="103"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -4428,8 +4493,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="102"/>
-      <c r="B9" s="103"/>
+      <c r="A9" s="120"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -4438,8 +4503,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="102"/>
-      <c r="B10" s="103"/>
+      <c r="A10" s="120"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -4448,8 +4513,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="102"/>
-      <c r="B11" s="103"/>
+      <c r="A11" s="120"/>
+      <c r="B11" s="119"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -4458,8 +4523,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="102"/>
-      <c r="B12" s="103"/>
+      <c r="A12" s="120"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -4468,10 +4533,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4482,8 +4547,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="113"/>
-      <c r="B14" s="103"/>
+      <c r="A14" s="122"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -4492,8 +4557,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="113"/>
-      <c r="B15" s="103"/>
+      <c r="A15" s="122"/>
+      <c r="B15" s="119"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -4502,10 +4567,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="112" t="s">
+      <c r="B16" s="114" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -4516,8 +4581,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
-      <c r="B17" s="112"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="114"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -4526,8 +4591,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
-      <c r="B18" s="112"/>
+      <c r="A18" s="123"/>
+      <c r="B18" s="114"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -4536,8 +4601,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
-      <c r="B19" s="112"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="114"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -4546,8 +4611,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="100"/>
-      <c r="B20" s="112"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="114"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -4556,8 +4621,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
-      <c r="B21" s="112"/>
+      <c r="A21" s="123"/>
+      <c r="B21" s="114"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -4566,8 +4631,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
-      <c r="B22" s="112"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="114"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -4576,8 +4641,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
-      <c r="B23" s="112"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="114"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -4586,26 +4651,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="100"/>
-      <c r="B24" s="112"/>
-      <c r="C24" s="100" t="s">
+      <c r="A24" s="123"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="123" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="101" t="s">
+      <c r="D24" s="124" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="100"/>
-      <c r="B25" s="112"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="101"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="124"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="102" t="s">
+      <c r="A26" s="120" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="103" t="s">
+      <c r="B26" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -4616,8 +4681,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="102"/>
-      <c r="B27" s="103"/>
+      <c r="A27" s="120"/>
+      <c r="B27" s="119"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -4644,28 +4709,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="103" t="s">
+      <c r="B30" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="100" t="s">
+      <c r="C30" s="123" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="108" t="s">
+      <c r="D30" s="112" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="104"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="108"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="119"/>
+      <c r="C31" s="123"/>
+      <c r="D31" s="112"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="104"/>
-      <c r="B32" s="103"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="119"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -4674,8 +4739,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="104"/>
-      <c r="B33" s="103"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="119"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -4684,8 +4749,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="104"/>
-      <c r="B34" s="103"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="119"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -4694,8 +4759,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="104"/>
-      <c r="B35" s="103"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="119"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -4704,8 +4769,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="104"/>
-      <c r="B36" s="103"/>
+      <c r="A36" s="121"/>
+      <c r="B36" s="119"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -4714,26 +4779,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="104"/>
-      <c r="B37" s="103"/>
-      <c r="C37" s="105" t="s">
+      <c r="A37" s="121"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="125" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="107" t="s">
+      <c r="D37" s="127" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="104"/>
-      <c r="B38" s="103"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="107"/>
+      <c r="A38" s="121"/>
+      <c r="B38" s="119"/>
+      <c r="C38" s="126"/>
+      <c r="D38" s="127"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="102" t="s">
+      <c r="A39" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="103" t="s">
+      <c r="B39" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -4744,8 +4809,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="102"/>
-      <c r="B40" s="103"/>
+      <c r="A40" s="120"/>
+      <c r="B40" s="119"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -4772,10 +4837,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="104" t="s">
+      <c r="A43" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="103" t="s">
+      <c r="B43" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -4784,8 +4849,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="104"/>
-      <c r="B44" s="103"/>
+      <c r="A44" s="121"/>
+      <c r="B44" s="119"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -4794,10 +4859,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="109" t="s">
+      <c r="A45" s="116" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="103" t="s">
+      <c r="B45" s="119" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -4806,8 +4871,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="110"/>
-      <c r="B46" s="103"/>
+      <c r="A46" s="117"/>
+      <c r="B46" s="119"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -4816,8 +4881,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="110"/>
-      <c r="B47" s="103"/>
+      <c r="A47" s="117"/>
+      <c r="B47" s="119"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -4826,8 +4891,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="111"/>
-      <c r="B48" s="103"/>
+      <c r="A48" s="118"/>
+      <c r="B48" s="119"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -4836,10 +4901,10 @@
       </c>
     </row>
     <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="112" t="s">
+      <c r="A49" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="114" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -8943,8 +9008,8 @@
       <c r="XFD49" s="42"/>
     </row>
     <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="112"/>
-      <c r="B50" s="112"/>
+      <c r="A50" s="114"/>
+      <c r="B50" s="114"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13048,8 +13113,8 @@
       <c r="XFD50" s="42"/>
     </row>
     <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="112"/>
-      <c r="B51" s="112"/>
+      <c r="A51" s="114"/>
+      <c r="B51" s="114"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17153,8 +17218,8 @@
       <c r="XFD51" s="42"/>
     </row>
     <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="112"/>
-      <c r="B52" s="112"/>
+      <c r="A52" s="114"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21258,12 +21323,12 @@
       <c r="XFD52" s="42"/>
     </row>
     <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="112"/>
-      <c r="B53" s="112"/>
-      <c r="C53" s="115" t="s">
+      <c r="A53" s="114"/>
+      <c r="B53" s="114"/>
+      <c r="C53" s="111" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="108" t="s">
+      <c r="D53" s="112" t="s">
         <v>144</v>
       </c>
       <c r="H53" s="42"/>
@@ -25363,10 +25428,10 @@
       <c r="XFD53" s="42"/>
     </row>
     <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="112"/>
-      <c r="B54" s="112"/>
-      <c r="C54" s="115"/>
-      <c r="D54" s="108"/>
+      <c r="A54" s="114"/>
+      <c r="B54" s="114"/>
+      <c r="C54" s="111"/>
+      <c r="D54" s="112"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -29484,10 +29549,10 @@
       </c>
     </row>
     <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="116" t="s">
+      <c r="A57" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="112" t="s">
+      <c r="B57" s="114" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -29498,8 +29563,8 @@
       </c>
     </row>
     <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="116"/>
-      <c r="B58" s="112"/>
+      <c r="A58" s="113"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -29508,8 +29573,8 @@
       </c>
     </row>
     <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="116"/>
-      <c r="B59" s="112"/>
+      <c r="A59" s="113"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -29518,8 +29583,8 @@
       </c>
     </row>
     <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="116"/>
-      <c r="B60" s="112"/>
+      <c r="A60" s="113"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -29528,8 +29593,8 @@
       </c>
     </row>
     <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="116"/>
-      <c r="B61" s="112"/>
+      <c r="A61" s="113"/>
+      <c r="B61" s="114"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -29538,8 +29603,8 @@
       </c>
     </row>
     <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="116"/>
-      <c r="B62" s="112"/>
+      <c r="A62" s="113"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -29548,8 +29613,8 @@
       </c>
     </row>
     <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="116"/>
-      <c r="B63" s="112"/>
+      <c r="A63" s="113"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -29558,16 +29623,16 @@
       </c>
     </row>
     <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="116"/>
-      <c r="B64" s="112"/>
+      <c r="A64" s="113"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="116"/>
-      <c r="B65" s="112"/>
+      <c r="A65" s="113"/>
+      <c r="B65" s="114"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -29576,16 +29641,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="116"/>
-      <c r="B66" s="112"/>
+      <c r="A66" s="113"/>
+      <c r="B66" s="114"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="116"/>
-      <c r="B67" s="112"/>
+      <c r="A67" s="113"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -29594,8 +29659,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="116"/>
-      <c r="B68" s="112"/>
+      <c r="A68" s="113"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -29604,8 +29669,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="116"/>
-      <c r="B69" s="112"/>
+      <c r="A69" s="113"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -29614,8 +29679,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="116"/>
-      <c r="B70" s="112"/>
+      <c r="A70" s="113"/>
+      <c r="B70" s="114"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -29624,8 +29689,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="116"/>
-      <c r="B71" s="112"/>
+      <c r="A71" s="113"/>
+      <c r="B71" s="114"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -29634,8 +29699,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="116"/>
-      <c r="B72" s="112"/>
+      <c r="A72" s="113"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -29644,16 +29709,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="116"/>
-      <c r="B73" s="112"/>
+      <c r="A73" s="113"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="116"/>
-      <c r="B74" s="112"/>
+      <c r="A74" s="113"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -29662,18 +29727,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="116"/>
-      <c r="B75" s="112"/>
-      <c r="C75" s="114"/>
-      <c r="D75" s="117" t="s">
+      <c r="A75" s="113"/>
+      <c r="B75" s="114"/>
+      <c r="C75" s="110"/>
+      <c r="D75" s="115" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="116"/>
-      <c r="B76" s="112"/>
-      <c r="C76" s="114"/>
-      <c r="D76" s="117"/>
+      <c r="A76" s="113"/>
+      <c r="B76" s="114"/>
+      <c r="C76" s="110"/>
+      <c r="D76" s="115"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -29697,8 +29762,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -29707,19 +29772,25 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="A49:A54"/>
@@ -29732,18 +29803,12 @@
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A25"/>
     <mergeCell ref="B16:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -29752,10 +29817,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:D41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29797,10 +29862,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="119" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -29811,133 +29876,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="102"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="121" t="s">
+      <c r="A5" s="120"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="129" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" s="128" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="120"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="128"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="102"/>
-      <c r="B7" s="103"/>
+      <c r="A7" s="120"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="102"/>
-      <c r="B8" s="103"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="102"/>
-      <c r="B9" s="103"/>
+      <c r="A9" s="120"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="119" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="119"/>
-      <c r="D10" s="120" t="s">
+      <c r="C10" s="131"/>
+      <c r="D10" s="128" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="113"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="120"/>
+      <c r="A11" s="122"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="128"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="113"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="120"/>
+      <c r="A12" s="122"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="128"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="114" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="122"/>
-      <c r="D13" s="120" t="s">
+      <c r="C13" s="130"/>
+      <c r="D13" s="128" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
-      <c r="B14" s="112"/>
-      <c r="C14" s="122"/>
-      <c r="D14" s="120"/>
+      <c r="A14" s="123"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="128"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100"/>
-      <c r="B15" s="112"/>
-      <c r="C15" s="122"/>
+      <c r="A15" s="123"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="130"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="100"/>
-      <c r="B16" s="112"/>
-      <c r="C16" s="122"/>
+      <c r="A16" s="123"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="100"/>
-      <c r="B17" s="112"/>
-      <c r="C17" s="122"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="100"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="122"/>
+      <c r="A18" s="123"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="130"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="100"/>
-      <c r="B19" s="112"/>
-      <c r="C19" s="122"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="100"/>
-      <c r="B20" s="112"/>
-      <c r="C20" s="122"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="100"/>
-      <c r="B21" s="112"/>
-      <c r="C21" s="122"/>
+      <c r="A21" s="123"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="130"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="100"/>
-      <c r="B22" s="112"/>
-      <c r="C22" s="122"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="130"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100"/>
-      <c r="B23" s="112"/>
-      <c r="C23" s="122"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="130"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -29952,423 +30017,435 @@
       <c r="C24" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="D24" s="78" t="s">
+      <c r="D24" s="77" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="48" t="s">
+    <row r="25" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="92" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" s="93" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="94" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" s="67" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="B26" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="73" t="s">
+      <c r="C26" s="38"/>
+      <c r="D26" s="73" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
+    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="104" t="s">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="103" t="s">
+      <c r="B28" s="84" t="s">
         <v>185</v>
       </c>
-      <c r="C27" s="79" t="s">
+      <c r="C28" s="88" t="s">
         <v>191</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D28" s="58" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="104"/>
-      <c r="B28" s="103"/>
-      <c r="C28" s="70" t="s">
+    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="85"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="70" t="s">
         <v>189</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D29" s="68" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="104"/>
-      <c r="B29" s="103"/>
-      <c r="C29" s="79" t="s">
-        <v>190</v>
-      </c>
-      <c r="D29" s="76" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="104"/>
-      <c r="B30" s="103"/>
-      <c r="C30" s="123" t="s">
+      <c r="A30" s="85"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="88" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="86" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="85"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="89" t="s">
         <v>226</v>
       </c>
-      <c r="D30" s="108" t="s">
+      <c r="D31" s="86" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="104"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="118"/>
-      <c r="D31" s="108"/>
+    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="139" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="142" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="91" t="s">
+        <v>230</v>
+      </c>
+      <c r="D32" s="87" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="32" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="76"/>
+    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="140"/>
+      <c r="B33" s="143"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="75"/>
     </row>
-    <row r="33" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="75"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="76"/>
+    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="140"/>
+      <c r="B34" s="143"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="75"/>
     </row>
-    <row r="34" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="75"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="76"/>
+    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="140"/>
+      <c r="B35" s="143"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="75"/>
     </row>
-    <row r="35" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="75" t="s">
-        <v>222</v>
-      </c>
-      <c r="B35" s="74" t="s">
+    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="141"/>
+      <c r="B36" s="144"/>
+      <c r="C36" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" s="75" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="79" t="s">
-        <v>223</v>
-      </c>
-      <c r="D35" s="76" t="s">
-        <v>224</v>
+      <c r="C37" s="38"/>
+      <c r="D37" s="50" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="74" t="s">
+    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="44"/>
+    </row>
+    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="121" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="119" t="s">
         <v>185</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="50" t="s">
-        <v>79</v>
+      <c r="C39" s="76" t="s">
+        <v>192</v>
+      </c>
+      <c r="D39" s="81" t="s">
+        <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="44"/>
-    </row>
-    <row r="38" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="104" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="C38" s="77" t="s">
-        <v>192</v>
-      </c>
-      <c r="D38" s="82" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="104"/>
-      <c r="B39" s="103"/>
-      <c r="C39" s="69" t="s">
+    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="121"/>
+      <c r="B40" s="119"/>
+      <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="D39" s="52" t="s">
+      <c r="D40" s="52" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="102" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="103" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40" s="119" t="s">
-        <v>194</v>
-      </c>
-      <c r="D40" s="100" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="102"/>
-      <c r="B41" s="103"/>
-      <c r="C41" s="119"/>
-      <c r="D41" s="100"/>
+      <c r="A41" s="120" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="119" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="131" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" s="123" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="102"/>
-      <c r="B42" s="103"/>
-      <c r="C42" s="119" t="s">
-        <v>190</v>
-      </c>
-      <c r="D42" s="117" t="s">
-        <v>188</v>
-      </c>
+      <c r="A42" s="120"/>
+      <c r="B42" s="119"/>
+      <c r="C42" s="131"/>
+      <c r="D42" s="123"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="102"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="117"/>
+      <c r="A43" s="120"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="131" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="115" t="s">
+        <v>188</v>
+      </c>
     </row>
-    <row r="44" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="116" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="120"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="131"/>
+      <c r="D44" s="115"/>
+    </row>
+    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="112" t="s">
+      <c r="B45" s="114" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="126"/>
-      <c r="D44" s="130" t="s">
+      <c r="C45" s="135"/>
+      <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="116"/>
-      <c r="B45" s="112"/>
-      <c r="C45" s="127"/>
-      <c r="D45" s="124" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="113"/>
+      <c r="B46" s="114"/>
+      <c r="C46" s="136"/>
+      <c r="D46" s="132" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="116"/>
-      <c r="B46" s="112"/>
-      <c r="C46" s="127"/>
-      <c r="D46" s="129"/>
+    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="113"/>
+      <c r="B47" s="114"/>
+      <c r="C47" s="136"/>
+      <c r="D47" s="133"/>
     </row>
-    <row r="47" spans="1:4" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="116"/>
-      <c r="B47" s="112"/>
-      <c r="C47" s="128"/>
-      <c r="D47" s="129"/>
-    </row>
-    <row r="48" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="116"/>
-      <c r="B48" s="112"/>
-      <c r="C48" s="115"/>
-      <c r="D48" s="129"/>
+    <row r="48" spans="1:4" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="113"/>
+      <c r="B48" s="114"/>
+      <c r="C48" s="137"/>
+      <c r="D48" s="133"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="116"/>
-      <c r="B49" s="112"/>
-      <c r="C49" s="115"/>
-      <c r="D49" s="125"/>
+      <c r="A49" s="113"/>
+      <c r="B49" s="114"/>
+      <c r="C49" s="111"/>
+      <c r="D49" s="133"/>
     </row>
-    <row r="50" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="39" t="s">
+    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="113"/>
+      <c r="B50" s="114"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="134"/>
+    </row>
+    <row r="51" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="44"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="44"/>
     </row>
-    <row r="51" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="48" t="s">
+    <row r="52" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="74" t="s">
+      <c r="B52" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="C51" s="38"/>
-      <c r="D51" s="49" t="s">
+      <c r="C52" s="38"/>
+      <c r="D52" s="49" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="112" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" s="112" t="s">
-        <v>185</v>
-      </c>
-      <c r="C52" s="79" t="s">
-        <v>197</v>
-      </c>
-      <c r="D52" s="47" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="112"/>
-      <c r="B53" s="112"/>
-      <c r="C53" s="79" t="s">
+      <c r="A53" s="114" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="114" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="78" t="s">
+        <v>197</v>
+      </c>
+      <c r="D53" s="47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="114"/>
+      <c r="B54" s="114"/>
+      <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
-      <c r="D53" s="47" t="s">
+      <c r="D54" s="47" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="112"/>
-      <c r="B54" s="112"/>
-      <c r="C54" s="79" t="s">
+    <row r="55" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="114"/>
+      <c r="B55" s="114"/>
+      <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
-      <c r="D54" s="81" t="s">
+      <c r="D55" s="80" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="112"/>
-      <c r="B55" s="112"/>
-      <c r="C55" s="118" t="s">
+    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="114"/>
+      <c r="B56" s="114"/>
+      <c r="C56" s="138" t="s">
         <v>208</v>
       </c>
-      <c r="D55" s="80" t="s">
+      <c r="D56" s="79" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="112"/>
-      <c r="B56" s="112"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="47" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="112"/>
-      <c r="B57" s="112"/>
-      <c r="C57" s="79" t="s">
-        <v>209</v>
-      </c>
-      <c r="D57" s="46" t="s">
-        <v>214</v>
+      <c r="A57" s="114"/>
+      <c r="B57" s="114"/>
+      <c r="C57" s="138"/>
+      <c r="D57" s="47" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="112"/>
-      <c r="B58" s="112"/>
-      <c r="C58" s="79" t="s">
-        <v>210</v>
-      </c>
-      <c r="D58" s="80" t="s">
-        <v>215</v>
+      <c r="A58" s="114"/>
+      <c r="B58" s="114"/>
+      <c r="C58" s="78" t="s">
+        <v>209</v>
+      </c>
+      <c r="D58" s="46" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="112"/>
-      <c r="B59" s="112"/>
-      <c r="C59" s="118" t="s">
-        <v>207</v>
-      </c>
-      <c r="D59" s="46" t="s">
-        <v>216</v>
+      <c r="A59" s="114"/>
+      <c r="B59" s="114"/>
+      <c r="C59" s="78" t="s">
+        <v>210</v>
+      </c>
+      <c r="D59" s="79" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="112"/>
-      <c r="B60" s="112"/>
-      <c r="C60" s="118"/>
+      <c r="A60" s="114"/>
+      <c r="B60" s="114"/>
+      <c r="C60" s="138" t="s">
+        <v>207</v>
+      </c>
       <c r="D60" s="46" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="114"/>
+      <c r="B61" s="114"/>
+      <c r="C61" s="138"/>
+      <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="112"/>
-      <c r="B61" s="112"/>
-      <c r="C61" s="118"/>
-      <c r="D61" s="80" t="s">
+    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="114"/>
+      <c r="B62" s="114"/>
+      <c r="C62" s="138"/>
+      <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="112"/>
-      <c r="B62" s="112"/>
-      <c r="C62" s="119" t="s">
+    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="114"/>
+      <c r="B63" s="114"/>
+      <c r="C63" s="131" t="s">
         <v>206</v>
       </c>
-      <c r="D62" s="45" t="s">
+      <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="112"/>
-      <c r="B63" s="112"/>
-      <c r="C63" s="119"/>
-      <c r="D63" s="117" t="s">
+    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="114"/>
+      <c r="B64" s="114"/>
+      <c r="C64" s="131"/>
+      <c r="D64" s="115" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="112"/>
-      <c r="B64" s="112"/>
-      <c r="C64" s="119"/>
-      <c r="D64" s="117"/>
+    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="114"/>
+      <c r="B65" s="114"/>
+      <c r="C65" s="131"/>
+      <c r="D65" s="115"/>
     </row>
-    <row r="65" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="112"/>
-      <c r="B65" s="112"/>
-      <c r="C65" s="119"/>
-      <c r="D65" s="117"/>
+    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="114"/>
+      <c r="B66" s="114"/>
+      <c r="C66" s="131"/>
+      <c r="D66" s="115"/>
     </row>
-    <row r="66" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="112"/>
-      <c r="B66" s="112"/>
-      <c r="C66" s="119"/>
-      <c r="D66" s="117"/>
+    <row r="67" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="114"/>
+      <c r="B67" s="114"/>
+      <c r="C67" s="131"/>
+      <c r="D67" s="115"/>
     </row>
-    <row r="67" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="39"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="44"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="83"/>
-      <c r="B68" s="84"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="39"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="44"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="83"/>
-      <c r="B69" s="84"/>
+      <c r="A69" s="82"/>
+      <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="83"/>
-      <c r="B70" s="84"/>
+      <c r="A70" s="82"/>
+      <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="83"/>
-      <c r="B71" s="84"/>
+      <c r="A71" s="82"/>
+      <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
+      <c r="A72" s="82"/>
+      <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
@@ -30382,49 +30459,53 @@
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C62:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="A52:A66"/>
-    <mergeCell ref="B52:B66"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D45:D49"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
+  <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="B4:B9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="A13:A23"/>
     <mergeCell ref="B13:B23"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="B53:B67"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"Updating documentation to bring it in line with latest code release"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7656" yWindow="288" windowWidth="15384" windowHeight="10008" activeTab="2"/>
+    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
     <sheet name="v1.0 Milestone 1" sheetId="2" r:id="rId2"/>
     <sheet name="v1.0Milestone 2" sheetId="3" r:id="rId3"/>
+    <sheet name="1.0 Release Candidate 2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="257">
   <si>
     <t>Document</t>
   </si>
@@ -2401,12 +2402,106 @@
   <si>
     <t>Added "maximum time" line</t>
   </si>
+  <si>
+    <t>1.0 Release Candidate 2</t>
+  </si>
+  <si>
+    <t>Enums</t>
+  </si>
+  <si>
+    <t>All Enums capitalised to match REST API</t>
+  </si>
+  <si>
+    <t>REST API</t>
+  </si>
+  <si>
+    <t>Reflects changes to the REST API</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>Additional information added in relation to Content-Type for POST requests.</t>
+  </si>
+  <si>
+    <t>HTTP request example Content-Type value changed from  ‘application/json;charset=UTF-8‘ to application/x-www-form-urlencoded</t>
+  </si>
+  <si>
+    <t>Returns Reconciliation Service Data Items</t>
+  </si>
+  <si>
+    <t>LookupPayrollReturnByPeriodRequest</t>
+  </si>
+  <si>
+    <t>Section added</t>
+  </si>
+  <si>
+    <t>Section 10 added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYE Web Service Examples </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PIT Self Service and ROS Payroll Reporting
+</t>
+  </si>
+  <si>
+    <t>Upload Examples</t>
+  </si>
+  <si>
+    <t>Request Header</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated date pattern on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">employmentStartDate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to be a date and not a datetime</t>
+    </r>
+  </si>
+  <si>
+    <t>New section addded for Returns Reconciliation examples</t>
+  </si>
+  <si>
+    <t>Reflect addition of Returns Reconciliation to schema</t>
+  </si>
+  <si>
+    <t>Updated with Returns Reconciliation</t>
+  </si>
+  <si>
+    <t>Returns Reconciliation Schema</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2508,6 +2603,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3D3C40"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2949,7 +3051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3195,6 +3297,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3344,6 +3473,21 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3685,15 +3829,15 @@
       <selection activeCell="A25" sqref="A25:A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3711,13 +3855,13 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="108"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -3741,19 +3885,19 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="97"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="108"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -3771,7 +3915,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -3789,11 +3933,11 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="98" t="s">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="101">
+      <c r="B7" s="112">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3807,9 +3951,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="99"/>
-      <c r="B8" s="102"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="110"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -3821,9 +3965,9 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
-      <c r="B9" s="102"/>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="110"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3835,9 +3979,9 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="99"/>
-      <c r="B10" s="102"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="110"/>
+      <c r="B10" s="113"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -3849,9 +3993,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="102"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="110"/>
+      <c r="B11" s="113"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -3863,9 +4007,9 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="100"/>
-      <c r="B12" s="103"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="111"/>
+      <c r="B12" s="114"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -3877,11 +4021,11 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="106" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="101">
+      <c r="B13" s="112">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -3895,9 +4039,9 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="107"/>
-      <c r="B14" s="103"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="118"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -3909,7 +4053,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -3927,7 +4071,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -3945,19 +4089,19 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="95" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="96"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="97"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="108"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -3975,7 +4119,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -3993,23 +4137,23 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="95" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="96"/>
-      <c r="C20" s="96"/>
-      <c r="D20" s="97"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="108"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="108" t="s">
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="105">
+      <c r="B21" s="116">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4023,9 +4167,9 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="109"/>
-      <c r="B22" s="103"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="120"/>
+      <c r="B22" s="114"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4033,7 +4177,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4047,19 +4191,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="95" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="96"/>
-      <c r="C24" s="96"/>
-      <c r="D24" s="97"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="108"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="104" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="105">
+      <c r="B25" s="116">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4073,9 +4217,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="99"/>
-      <c r="B26" s="102"/>
+    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="110"/>
+      <c r="B26" s="113"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4087,9 +4231,9 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="99"/>
-      <c r="B27" s="102"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="110"/>
+      <c r="B27" s="113"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4101,9 +4245,9 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="99"/>
-      <c r="B28" s="102"/>
+    <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="110"/>
+      <c r="B28" s="113"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4115,9 +4259,9 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="99"/>
-      <c r="B29" s="102"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="110"/>
+      <c r="B29" s="113"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4129,9 +4273,9 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="99"/>
-      <c r="B30" s="102"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="110"/>
+      <c r="B30" s="113"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4143,9 +4287,9 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="99"/>
-      <c r="B31" s="102"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="110"/>
+      <c r="B31" s="113"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4157,9 +4301,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="100"/>
-      <c r="B32" s="103"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="111"/>
+      <c r="B32" s="114"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4171,7 +4315,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4185,7 +4329,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4199,7 +4343,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4213,7 +4357,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4227,7 +4371,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4241,7 +4385,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4255,7 +4399,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4269,7 +4413,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4283,15 +4427,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="95" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="96"/>
-      <c r="C41" s="96"/>
-      <c r="D41" s="97"/>
+      <c r="B41" s="107"/>
+      <c r="C41" s="107"/>
+      <c r="D41" s="108"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4305,7 +4449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4319,7 +4463,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4333,7 +4477,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4390,19 +4534,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD79"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -4416,7 +4560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -4424,7 +4568,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -4436,7 +4580,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -4448,7 +4592,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -4468,11 +4612,11 @@
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="120" t="s">
+    <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="119" t="s">
+      <c r="B7" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4482,9 +4626,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="120"/>
-      <c r="B8" s="119"/>
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="131"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -4492,9 +4636,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="119"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="131"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -4502,9 +4646,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="119"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="131"/>
+      <c r="B10" s="130"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -4512,9 +4656,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
-      <c r="B11" s="119"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="131"/>
+      <c r="B11" s="130"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -4522,9 +4666,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="120"/>
-      <c r="B12" s="119"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="131"/>
+      <c r="B12" s="130"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -4532,11 +4676,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="122" t="s">
+    <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="133" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="119" t="s">
+      <c r="B13" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4546,9 +4690,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="122"/>
-      <c r="B14" s="119"/>
+    <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="133"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -4556,9 +4700,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="122"/>
-      <c r="B15" s="119"/>
+    <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="133"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -4566,11 +4710,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="123" t="s">
+    <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="114" t="s">
+      <c r="B16" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -4580,9 +4724,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="123"/>
-      <c r="B17" s="114"/>
+    <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="134"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -4590,9 +4734,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="123"/>
-      <c r="B18" s="114"/>
+    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="134"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -4600,9 +4744,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="123"/>
-      <c r="B19" s="114"/>
+    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="134"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -4610,9 +4754,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="123"/>
-      <c r="B20" s="114"/>
+    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="134"/>
+      <c r="B20" s="125"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -4620,9 +4764,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="123"/>
-      <c r="B21" s="114"/>
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="134"/>
+      <c r="B21" s="125"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -4630,9 +4774,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="123"/>
-      <c r="B22" s="114"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="134"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -4640,9 +4784,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123"/>
-      <c r="B23" s="114"/>
+    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="134"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -4650,27 +4794,27 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="123"/>
-      <c r="B24" s="114"/>
-      <c r="C24" s="123" t="s">
+    <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="134"/>
+      <c r="B24" s="125"/>
+      <c r="C24" s="134" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="124" t="s">
+      <c r="D24" s="135" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="123"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="124"/>
+    <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="134"/>
+      <c r="B25" s="125"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="135"/>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="120" t="s">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="131" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="119" t="s">
+      <c r="B26" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -4680,15 +4824,15 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="120"/>
-      <c r="B27" s="119"/>
+    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="131"/>
+      <c r="B27" s="130"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -4700,7 +4844,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -4708,29 +4852,29 @@
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="121" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="132" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="119" t="s">
+      <c r="B30" s="130" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="123" t="s">
+      <c r="C30" s="134" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="112" t="s">
+      <c r="D30" s="123" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="121"/>
-      <c r="B31" s="119"/>
-      <c r="C31" s="123"/>
-      <c r="D31" s="112"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="132"/>
+      <c r="B31" s="130"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="123"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="121"/>
-      <c r="B32" s="119"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="132"/>
+      <c r="B32" s="130"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -4738,9 +4882,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="121"/>
-      <c r="B33" s="119"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="132"/>
+      <c r="B33" s="130"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -4748,9 +4892,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="121"/>
-      <c r="B34" s="119"/>
+    <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="132"/>
+      <c r="B34" s="130"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -4758,9 +4902,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="121"/>
-      <c r="B35" s="119"/>
+    <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="132"/>
+      <c r="B35" s="130"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -4768,9 +4912,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="121"/>
-      <c r="B36" s="119"/>
+    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="132"/>
+      <c r="B36" s="130"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -4778,27 +4922,27 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="121"/>
-      <c r="B37" s="119"/>
-      <c r="C37" s="125" t="s">
+    <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="132"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="136" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="127" t="s">
+      <c r="D37" s="138" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="121"/>
-      <c r="B38" s="119"/>
-      <c r="C38" s="126"/>
-      <c r="D38" s="127"/>
+    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="132"/>
+      <c r="B38" s="130"/>
+      <c r="C38" s="137"/>
+      <c r="D38" s="138"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="120" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="131" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="119" t="s">
+      <c r="B39" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -4808,15 +4952,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="120"/>
-      <c r="B40" s="119"/>
+    <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="131"/>
+      <c r="B40" s="130"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -4828,7 +4972,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
@@ -4836,11 +4980,11 @@
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
     </row>
-    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="121" t="s">
+    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="119" t="s">
+      <c r="B43" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -4848,9 +4992,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="121"/>
-      <c r="B44" s="119"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="132"/>
+      <c r="B44" s="130"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -4858,11 +5002,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="116" t="s">
+    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="119" t="s">
+      <c r="B45" s="130" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -4870,9 +5014,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="117"/>
-      <c r="B46" s="119"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="128"/>
+      <c r="B46" s="130"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -4880,9 +5024,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="117"/>
-      <c r="B47" s="119"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="128"/>
+      <c r="B47" s="130"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -4890,9 +5034,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="118"/>
-      <c r="B48" s="119"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="129"/>
+      <c r="B48" s="130"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -4900,11 +5044,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="114" t="s">
+    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A49" s="125" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="114" t="s">
+      <c r="B49" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9007,9 +9151,9 @@
       <c r="XEZ49" s="42"/>
       <c r="XFD49" s="42"/>
     </row>
-    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="114"/>
-      <c r="B50" s="114"/>
+    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="125"/>
+      <c r="B50" s="125"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13112,9 +13256,9 @@
       <c r="XEZ50" s="42"/>
       <c r="XFD50" s="42"/>
     </row>
-    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="114"/>
-      <c r="B51" s="114"/>
+    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A51" s="125"/>
+      <c r="B51" s="125"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17217,9 +17361,9 @@
       <c r="XEZ51" s="42"/>
       <c r="XFD51" s="42"/>
     </row>
-    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="114"/>
-      <c r="B52" s="114"/>
+    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A52" s="125"/>
+      <c r="B52" s="125"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21322,13 +21466,13 @@
       <c r="XEZ52" s="42"/>
       <c r="XFD52" s="42"/>
     </row>
-    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="114"/>
-      <c r="B53" s="114"/>
-      <c r="C53" s="111" t="s">
+    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A53" s="125"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="122" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="112" t="s">
+      <c r="D53" s="123" t="s">
         <v>144</v>
       </c>
       <c r="H53" s="42"/>
@@ -25427,11 +25571,11 @@
       <c r="XEZ53" s="42"/>
       <c r="XFD53" s="42"/>
     </row>
-    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="114"/>
-      <c r="B54" s="114"/>
-      <c r="C54" s="111"/>
-      <c r="D54" s="112"/>
+    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="125"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="122"/>
+      <c r="D54" s="123"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -29528,7 +29672,7 @@
       <c r="XEZ54" s="42"/>
       <c r="XFD54" s="42"/>
     </row>
-    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
@@ -29536,7 +29680,7 @@
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
     </row>
-    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -29548,11 +29692,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="113" t="s">
+    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A57" s="124" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="114" t="s">
+      <c r="B57" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -29562,9 +29706,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="113"/>
-      <c r="B58" s="114"/>
+    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="124"/>
+      <c r="B58" s="125"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -29572,9 +29716,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="113"/>
-      <c r="B59" s="114"/>
+    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A59" s="124"/>
+      <c r="B59" s="125"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -29582,9 +29726,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="113"/>
-      <c r="B60" s="114"/>
+    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="124"/>
+      <c r="B60" s="125"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -29592,9 +29736,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="113"/>
-      <c r="B61" s="114"/>
+    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A61" s="124"/>
+      <c r="B61" s="125"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -29602,9 +29746,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="113"/>
-      <c r="B62" s="114"/>
+    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A62" s="124"/>
+      <c r="B62" s="125"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -29612,9 +29756,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="113"/>
-      <c r="B63" s="114"/>
+    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A63" s="124"/>
+      <c r="B63" s="125"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -29622,17 +29766,17 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="113"/>
-      <c r="B64" s="114"/>
+    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A64" s="124"/>
+      <c r="B64" s="125"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="113"/>
-      <c r="B65" s="114"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="124"/>
+      <c r="B65" s="125"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -29640,17 +29784,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="113"/>
-      <c r="B66" s="114"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="124"/>
+      <c r="B66" s="125"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="113"/>
-      <c r="B67" s="114"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="124"/>
+      <c r="B67" s="125"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -29658,9 +29802,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="113"/>
-      <c r="B68" s="114"/>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="124"/>
+      <c r="B68" s="125"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -29668,9 +29812,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="113"/>
-      <c r="B69" s="114"/>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="124"/>
+      <c r="B69" s="125"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -29678,9 +29822,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="113"/>
-      <c r="B70" s="114"/>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="124"/>
+      <c r="B70" s="125"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -29688,9 +29832,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="113"/>
-      <c r="B71" s="114"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="124"/>
+      <c r="B71" s="125"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -29698,9 +29842,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="113"/>
-      <c r="B72" s="114"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="124"/>
+      <c r="B72" s="125"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -29708,17 +29852,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="113"/>
-      <c r="B73" s="114"/>
+    <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="124"/>
+      <c r="B73" s="125"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="113"/>
-      <c r="B74" s="114"/>
+    <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="124"/>
+      <c r="B74" s="125"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -29726,21 +29870,21 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="113"/>
-      <c r="B75" s="114"/>
-      <c r="C75" s="110"/>
-      <c r="D75" s="115" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="124"/>
+      <c r="B75" s="125"/>
+      <c r="C75" s="121"/>
+      <c r="D75" s="126" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="113"/>
-      <c r="B76" s="114"/>
-      <c r="C76" s="110"/>
-      <c r="D76" s="115"/>
+    <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="124"/>
+      <c r="B76" s="125"/>
+      <c r="C76" s="121"/>
+      <c r="D76" s="126"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
@@ -29748,13 +29892,13 @@
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -29819,19 +29963,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
-    <col min="3" max="3" width="49.21875" customWidth="1"/>
-    <col min="4" max="4" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -29845,7 +29989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -29861,11 +30005,11 @@
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="120" t="s">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="130" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -29875,134 +30019,134 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="120"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="129" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="131"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="140" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="128" t="s">
+      <c r="D5" s="139" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="119"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="128"/>
+    <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="131"/>
+      <c r="B6" s="130"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="139"/>
     </row>
-    <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="120"/>
-      <c r="B7" s="119"/>
+    <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="131"/>
+      <c r="B7" s="130"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
-    <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="120"/>
-      <c r="B8" s="119"/>
+    <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="131"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
-    <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="119"/>
+    <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="131"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="122" t="s">
+    <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="133" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="119" t="s">
+      <c r="B10" s="130" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="131"/>
-      <c r="D10" s="128" t="s">
+      <c r="C10" s="142"/>
+      <c r="D10" s="139" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="122"/>
-      <c r="B11" s="119"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="128"/>
+    <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="139"/>
     </row>
-    <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="122"/>
-      <c r="B12" s="119"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="128"/>
+    <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="133"/>
+      <c r="B12" s="130"/>
+      <c r="C12" s="142"/>
+      <c r="D12" s="139"/>
     </row>
-    <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="123" t="s">
+    <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="114" t="s">
+      <c r="B13" s="125" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="130"/>
-      <c r="D13" s="128" t="s">
+      <c r="C13" s="141"/>
+      <c r="D13" s="139" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="123"/>
-      <c r="B14" s="114"/>
-      <c r="C14" s="130"/>
-      <c r="D14" s="128"/>
+    <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="134"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="139"/>
     </row>
-    <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="123"/>
-      <c r="B15" s="114"/>
-      <c r="C15" s="130"/>
+    <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="134"/>
+      <c r="B15" s="125"/>
+      <c r="C15" s="141"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="123"/>
-      <c r="B16" s="114"/>
-      <c r="C16" s="130"/>
+      <c r="A16" s="134"/>
+      <c r="B16" s="125"/>
+      <c r="C16" s="141"/>
       <c r="D16" s="49"/>
     </row>
-    <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="123"/>
-      <c r="B17" s="114"/>
-      <c r="C17" s="130"/>
+    <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="134"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="141"/>
       <c r="D17" s="49"/>
     </row>
-    <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="123"/>
-      <c r="B18" s="114"/>
-      <c r="C18" s="130"/>
+    <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="134"/>
+      <c r="B18" s="125"/>
+      <c r="C18" s="141"/>
       <c r="D18" s="49"/>
     </row>
-    <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="123"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="130"/>
+    <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="134"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="141"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="123"/>
-      <c r="B20" s="114"/>
-      <c r="C20" s="130"/>
+    <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="134"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="141"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="123"/>
-      <c r="B21" s="114"/>
-      <c r="C21" s="130"/>
+    <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="134"/>
+      <c r="B21" s="125"/>
+      <c r="C21" s="141"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="123"/>
-      <c r="B22" s="114"/>
-      <c r="C22" s="130"/>
+    <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="134"/>
+      <c r="B22" s="125"/>
+      <c r="C22" s="141"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123"/>
-      <c r="B23" s="114"/>
-      <c r="C23" s="130"/>
+    <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="134"/>
+      <c r="B23" s="125"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30021,7 +30165,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30035,7 +30179,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30055,7 +30199,7 @@
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30079,7 +30223,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30089,7 +30233,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30099,11 +30243,11 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="139" t="s">
+    <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="150" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="142" t="s">
+      <c r="B32" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30113,27 +30257,27 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="140"/>
-      <c r="B33" s="143"/>
+    <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="151"/>
+      <c r="B33" s="154"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="140"/>
-      <c r="B34" s="143"/>
+      <c r="A34" s="151"/>
+      <c r="B34" s="154"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
-    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="140"/>
-      <c r="B35" s="143"/>
+    <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="151"/>
+      <c r="B35" s="154"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
-    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="141"/>
-      <c r="B36" s="144"/>
+    <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="152"/>
+      <c r="B36" s="155"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30161,11 +30305,11 @@
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
     </row>
-    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="121" t="s">
+    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="119" t="s">
+      <c r="B39" s="130" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30175,9 +30319,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="121"/>
-      <c r="B40" s="119"/>
+    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="132"/>
+      <c r="B40" s="130"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30185,87 +30329,87 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="120" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="119" t="s">
+      <c r="B41" s="130" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="131" t="s">
+      <c r="C41" s="142" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="123" t="s">
+      <c r="D41" s="134" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="120"/>
-      <c r="B42" s="119"/>
-      <c r="C42" s="131"/>
-      <c r="D42" s="123"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="131"/>
+      <c r="B42" s="130"/>
+      <c r="C42" s="142"/>
+      <c r="D42" s="134"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="120"/>
-      <c r="B43" s="119"/>
-      <c r="C43" s="131" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="131"/>
+      <c r="B43" s="130"/>
+      <c r="C43" s="142" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="115" t="s">
+      <c r="D43" s="126" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="120"/>
-      <c r="B44" s="119"/>
-      <c r="C44" s="131"/>
-      <c r="D44" s="115"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="131"/>
+      <c r="B44" s="130"/>
+      <c r="C44" s="142"/>
+      <c r="D44" s="126"/>
     </row>
-    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="113" t="s">
+    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="124" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="114" t="s">
+      <c r="B45" s="125" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="135"/>
+      <c r="C45" s="146"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="113"/>
-      <c r="B46" s="114"/>
-      <c r="C46" s="136"/>
-      <c r="D46" s="132" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="124"/>
+      <c r="B46" s="125"/>
+      <c r="C46" s="147"/>
+      <c r="D46" s="143" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="113"/>
-      <c r="B47" s="114"/>
-      <c r="C47" s="136"/>
-      <c r="D47" s="133"/>
+    <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="124"/>
+      <c r="B47" s="125"/>
+      <c r="C47" s="147"/>
+      <c r="D47" s="144"/>
     </row>
-    <row r="48" spans="1:4" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="113"/>
-      <c r="B48" s="114"/>
-      <c r="C48" s="137"/>
-      <c r="D48" s="133"/>
+    <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="124"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="148"/>
+      <c r="D48" s="144"/>
     </row>
-    <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="113"/>
-      <c r="B49" s="114"/>
-      <c r="C49" s="111"/>
-      <c r="D49" s="133"/>
+    <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="124"/>
+      <c r="B49" s="125"/>
+      <c r="C49" s="122"/>
+      <c r="D49" s="144"/>
     </row>
-    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="113"/>
-      <c r="B50" s="114"/>
-      <c r="C50" s="111"/>
-      <c r="D50" s="134"/>
+    <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="124"/>
+      <c r="B50" s="125"/>
+      <c r="C50" s="122"/>
+      <c r="D50" s="145"/>
     </row>
-    <row r="51" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
@@ -30285,11 +30429,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="114" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="114" t="s">
+      <c r="B53" s="125" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30299,9 +30443,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="114"/>
-      <c r="B54" s="114"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="125"/>
+      <c r="B54" s="125"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30309,9 +30453,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="114"/>
-      <c r="B55" s="114"/>
+    <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="125"/>
+      <c r="B55" s="125"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30319,27 +30463,27 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="114"/>
-      <c r="B56" s="114"/>
-      <c r="C56" s="138" t="s">
+    <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="125"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="149" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="114"/>
-      <c r="B57" s="114"/>
-      <c r="C57" s="138"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="125"/>
+      <c r="B57" s="125"/>
+      <c r="C57" s="149"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="114"/>
-      <c r="B58" s="114"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="125"/>
+      <c r="B58" s="125"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30347,9 +30491,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="114"/>
-      <c r="B59" s="114"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="125"/>
+      <c r="B59" s="125"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30357,116 +30501,116 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="114"/>
-      <c r="B60" s="114"/>
-      <c r="C60" s="138" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="125"/>
+      <c r="B60" s="125"/>
+      <c r="C60" s="149" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="114"/>
-      <c r="B61" s="114"/>
-      <c r="C61" s="138"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="125"/>
+      <c r="B61" s="125"/>
+      <c r="C61" s="149"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="114"/>
-      <c r="B62" s="114"/>
-      <c r="C62" s="138"/>
+    <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="125"/>
+      <c r="B62" s="125"/>
+      <c r="C62" s="149"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="114"/>
-      <c r="B63" s="114"/>
-      <c r="C63" s="131" t="s">
+    <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="125"/>
+      <c r="B63" s="125"/>
+      <c r="C63" s="142" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="114"/>
-      <c r="B64" s="114"/>
-      <c r="C64" s="131"/>
-      <c r="D64" s="115" t="s">
+    <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="125"/>
+      <c r="B64" s="125"/>
+      <c r="C64" s="142"/>
+      <c r="D64" s="126" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="114"/>
-      <c r="B65" s="114"/>
-      <c r="C65" s="131"/>
-      <c r="D65" s="115"/>
+    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="125"/>
+      <c r="B65" s="125"/>
+      <c r="C65" s="142"/>
+      <c r="D65" s="126"/>
     </row>
-    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="114"/>
-      <c r="B66" s="114"/>
-      <c r="C66" s="131"/>
-      <c r="D66" s="115"/>
+    <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="125"/>
+      <c r="B66" s="125"/>
+      <c r="C66" s="142"/>
+      <c r="D66" s="126"/>
     </row>
-    <row r="67" spans="1:4" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="114"/>
-      <c r="B67" s="114"/>
-      <c r="C67" s="131"/>
-      <c r="D67" s="115"/>
+    <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="125"/>
+      <c r="B67" s="125"/>
+      <c r="C67" s="142"/>
+      <c r="D67" s="126"/>
     </row>
-    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -30510,4 +30654,270 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="65" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="44"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="156" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="149" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="136" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="157"/>
+      <c r="C4" s="149"/>
+      <c r="D4" s="137"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" s="157"/>
+      <c r="C5" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="98" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="158"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="98" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="159" t="s">
+        <v>237</v>
+      </c>
+      <c r="B8" s="149" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="160"/>
+      <c r="B9" s="149"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="58" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="149" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="149" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="102" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="100" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="149"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="102" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="95" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="98" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="99" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="101" t="s">
+        <v>244</v>
+      </c>
+      <c r="D15" s="98" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="44"/>
+    </row>
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A17" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="99" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="99" t="s">
+        <v>246</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="134" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="149" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="99">
+        <v>10.1</v>
+      </c>
+      <c r="D18" s="58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="134"/>
+      <c r="B19" s="149"/>
+      <c r="C19" s="99">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D19" s="58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="103" t="s">
+        <v>248</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="44"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B21" s="99" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="99" t="s">
+        <v>250</v>
+      </c>
+      <c r="D21" s="104" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B3:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update List of Employees
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LiveDocumentation\paye-employers-documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
+    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -14,15 +19,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="262">
   <si>
     <t>Document</t>
   </si>
@@ -2496,11 +2501,26 @@
   <si>
     <t>Returns Reconciliation Schema</t>
   </si>
+  <si>
+    <t>employmentId</t>
+  </si>
+  <si>
+    <t>added as a simpleType</t>
+  </si>
+  <si>
+    <t>Changed from type 'ros:alpha20' to type 'ns1:employmentID'</t>
+  </si>
+  <si>
+    <t>Employment ID and Director</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description updated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2635,7 +2655,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -3047,11 +3067,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3324,6 +3362,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3370,22 +3411,31 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3396,41 +3446,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3456,23 +3506,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3483,12 +3530,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3531,6 +3588,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3579,7 +3639,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3612,9 +3672,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3647,6 +3724,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3829,15 +3923,15 @@
       <selection activeCell="A25" sqref="A25:A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3855,19 +3949,19 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="108"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="109"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
@@ -3885,19 +3979,19 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="106" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="107"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="108"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="109"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -3915,7 +4009,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -3933,11 +4027,11 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="109" t="s">
+    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="112">
+      <c r="B7" s="113">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3951,9 +4045,9 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="110"/>
-      <c r="B8" s="113"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="111"/>
+      <c r="B8" s="114"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -3965,9 +4059,9 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="110"/>
-      <c r="B9" s="113"/>
+    <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="111"/>
+      <c r="B9" s="114"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3979,9 +4073,9 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="110"/>
-      <c r="B10" s="113"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="111"/>
+      <c r="B10" s="114"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -3993,9 +4087,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="110"/>
-      <c r="B11" s="113"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="111"/>
+      <c r="B11" s="114"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4007,9 +4101,9 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="111"/>
-      <c r="B12" s="114"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="112"/>
+      <c r="B12" s="115"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4021,11 +4115,11 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="117" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="112">
+      <c r="B13" s="113">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4039,9 +4133,9 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="118"/>
-      <c r="B14" s="114"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="119"/>
+      <c r="B14" s="115"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4053,7 +4147,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -4071,7 +4165,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -4089,19 +4183,19 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="106" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="107"/>
-      <c r="C17" s="107"/>
-      <c r="D17" s="108"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="109"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -4119,7 +4213,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4137,23 +4231,23 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="106" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="107"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="108"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="109"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="119" t="s">
+    <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="116">
+      <c r="B21" s="117">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4167,9 +4261,9 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="120"/>
-      <c r="B22" s="114"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="121"/>
+      <c r="B22" s="115"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4177,7 +4271,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4191,19 +4285,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="106" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="107"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="108"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="109"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="115" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="116">
+      <c r="B25" s="117">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4217,9 +4311,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="110"/>
-      <c r="B26" s="113"/>
+    <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="111"/>
+      <c r="B26" s="114"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4231,9 +4325,9 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="110"/>
-      <c r="B27" s="113"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="111"/>
+      <c r="B27" s="114"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4245,9 +4339,9 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="110"/>
-      <c r="B28" s="113"/>
+    <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="111"/>
+      <c r="B28" s="114"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4259,9 +4353,9 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="110"/>
-      <c r="B29" s="113"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="111"/>
+      <c r="B29" s="114"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4273,9 +4367,9 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="110"/>
-      <c r="B30" s="113"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="111"/>
+      <c r="B30" s="114"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4287,9 +4381,9 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="110"/>
-      <c r="B31" s="113"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="111"/>
+      <c r="B31" s="114"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4301,9 +4395,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="111"/>
-      <c r="B32" s="114"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="112"/>
+      <c r="B32" s="115"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4315,7 +4409,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4329,7 +4423,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4343,7 +4437,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4357,7 +4451,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4371,7 +4465,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4385,7 +4479,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4399,7 +4493,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4413,7 +4507,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4427,15 +4521,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="106" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="107" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="107"/>
-      <c r="C41" s="107"/>
-      <c r="D41" s="108"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="108"/>
+      <c r="D41" s="109"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4449,7 +4543,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4463,7 +4557,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4477,7 +4571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4493,7 +4587,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4503,7 +4597,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -4538,15 +4632,15 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -4560,7 +4654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -4568,7 +4662,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -4580,7 +4674,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -4592,7 +4686,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -4612,11 +4706,11 @@
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="131" t="s">
+    <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4626,9 +4720,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="131"/>
-      <c r="B8" s="130"/>
+    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="124"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -4636,9 +4730,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="131"/>
-      <c r="B9" s="130"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="124"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -4646,9 +4740,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="131"/>
-      <c r="B10" s="130"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="124"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -4656,9 +4750,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="131"/>
-      <c r="B11" s="130"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="124"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -4666,9 +4760,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="131"/>
-      <c r="B12" s="130"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="124"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -4676,11 +4770,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="133" t="s">
+    <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="135" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="130" t="s">
+      <c r="B13" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4690,9 +4784,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="133"/>
-      <c r="B14" s="130"/>
+    <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="135"/>
+      <c r="B14" s="125"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -4700,9 +4794,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="133"/>
-      <c r="B15" s="130"/>
+    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="135"/>
+      <c r="B15" s="125"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -4710,11 +4804,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="134" t="s">
+    <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="125" t="s">
+      <c r="B16" s="134" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -4724,9 +4818,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="134"/>
-      <c r="B17" s="125"/>
+    <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="122"/>
+      <c r="B17" s="134"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -4734,9 +4828,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="134"/>
-      <c r="B18" s="125"/>
+    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="122"/>
+      <c r="B18" s="134"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -4744,9 +4838,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="134"/>
-      <c r="B19" s="125"/>
+    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="122"/>
+      <c r="B19" s="134"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -4754,9 +4848,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="134"/>
-      <c r="B20" s="125"/>
+    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="122"/>
+      <c r="B20" s="134"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -4764,9 +4858,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="134"/>
-      <c r="B21" s="125"/>
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="122"/>
+      <c r="B21" s="134"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -4774,9 +4868,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="134"/>
-      <c r="B22" s="125"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="122"/>
+      <c r="B22" s="134"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -4784,9 +4878,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="134"/>
-      <c r="B23" s="125"/>
+    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="122"/>
+      <c r="B23" s="134"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -4794,27 +4888,27 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="134"/>
-      <c r="B24" s="125"/>
-      <c r="C24" s="134" t="s">
+    <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="122"/>
+      <c r="B24" s="134"/>
+      <c r="C24" s="122" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="135" t="s">
+      <c r="D24" s="123" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="134"/>
-      <c r="B25" s="125"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="135"/>
+    <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="122"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="122"/>
+      <c r="D25" s="123"/>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="131" t="s">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="124" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="130" t="s">
+      <c r="B26" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -4824,15 +4918,15 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="131"/>
-      <c r="B27" s="130"/>
+    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="124"/>
+      <c r="B27" s="125"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -4844,7 +4938,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -4852,29 +4946,29 @@
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="132" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="130" t="s">
+      <c r="B30" s="125" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="134" t="s">
+      <c r="C30" s="122" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="123" t="s">
+      <c r="D30" s="130" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="132"/>
-      <c r="B31" s="130"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="123"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="126"/>
+      <c r="B31" s="125"/>
+      <c r="C31" s="122"/>
+      <c r="D31" s="130"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="132"/>
-      <c r="B32" s="130"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="126"/>
+      <c r="B32" s="125"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -4882,9 +4976,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="132"/>
-      <c r="B33" s="130"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="126"/>
+      <c r="B33" s="125"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -4892,9 +4986,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="132"/>
-      <c r="B34" s="130"/>
+    <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="126"/>
+      <c r="B34" s="125"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -4902,9 +4996,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="132"/>
-      <c r="B35" s="130"/>
+    <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="126"/>
+      <c r="B35" s="125"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -4912,9 +5006,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="132"/>
-      <c r="B36" s="130"/>
+    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="126"/>
+      <c r="B36" s="125"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -4922,27 +5016,27 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="132"/>
-      <c r="B37" s="130"/>
-      <c r="C37" s="136" t="s">
+    <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="126"/>
+      <c r="B37" s="125"/>
+      <c r="C37" s="127" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="138" t="s">
+      <c r="D37" s="129" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="132"/>
-      <c r="B38" s="130"/>
-      <c r="C38" s="137"/>
-      <c r="D38" s="138"/>
+    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="126"/>
+      <c r="B38" s="125"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="129"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="131" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="124" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="130" t="s">
+      <c r="B39" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -4952,15 +5046,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="131"/>
-      <c r="B40" s="130"/>
+    <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="124"/>
+      <c r="B40" s="125"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -4972,7 +5066,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
@@ -4980,11 +5074,11 @@
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
     </row>
-    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="132" t="s">
+    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="130" t="s">
+      <c r="B43" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -4992,9 +5086,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="132"/>
-      <c r="B44" s="130"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="126"/>
+      <c r="B44" s="125"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5002,11 +5096,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="127" t="s">
+    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="130" t="s">
+      <c r="B45" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5014,9 +5108,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="128"/>
-      <c r="B46" s="130"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="132"/>
+      <c r="B46" s="125"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5024,9 +5118,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="128"/>
-      <c r="B47" s="130"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="132"/>
+      <c r="B47" s="125"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5034,9 +5128,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="129"/>
-      <c r="B48" s="130"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="133"/>
+      <c r="B48" s="125"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5044,11 +5138,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A49" s="125" t="s">
+    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A49" s="134" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="125" t="s">
+      <c r="B49" s="134" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9151,9 +9245,9 @@
       <c r="XEZ49" s="42"/>
       <c r="XFD49" s="42"/>
     </row>
-    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="125"/>
-      <c r="B50" s="125"/>
+    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="134"/>
+      <c r="B50" s="134"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13256,9 +13350,9 @@
       <c r="XEZ50" s="42"/>
       <c r="XFD50" s="42"/>
     </row>
-    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A51" s="125"/>
-      <c r="B51" s="125"/>
+    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A51" s="134"/>
+      <c r="B51" s="134"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17361,9 +17455,9 @@
       <c r="XEZ51" s="42"/>
       <c r="XFD51" s="42"/>
     </row>
-    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A52" s="125"/>
-      <c r="B52" s="125"/>
+    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A52" s="134"/>
+      <c r="B52" s="134"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21466,13 +21560,13 @@
       <c r="XEZ52" s="42"/>
       <c r="XFD52" s="42"/>
     </row>
-    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A53" s="125"/>
-      <c r="B53" s="125"/>
-      <c r="C53" s="122" t="s">
+    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A53" s="134"/>
+      <c r="B53" s="134"/>
+      <c r="C53" s="137" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="123" t="s">
+      <c r="D53" s="130" t="s">
         <v>144</v>
       </c>
       <c r="H53" s="42"/>
@@ -25571,11 +25665,11 @@
       <c r="XEZ53" s="42"/>
       <c r="XFD53" s="42"/>
     </row>
-    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="125"/>
-      <c r="B54" s="125"/>
-      <c r="C54" s="122"/>
-      <c r="D54" s="123"/>
+    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="134"/>
+      <c r="B54" s="134"/>
+      <c r="C54" s="137"/>
+      <c r="D54" s="130"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -29672,7 +29766,7 @@
       <c r="XEZ54" s="42"/>
       <c r="XFD54" s="42"/>
     </row>
-    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
@@ -29680,7 +29774,7 @@
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
     </row>
-    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -29692,11 +29786,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A57" s="124" t="s">
+    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A57" s="138" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="125" t="s">
+      <c r="B57" s="134" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -29706,9 +29800,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="124"/>
-      <c r="B58" s="125"/>
+    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="138"/>
+      <c r="B58" s="134"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -29716,9 +29810,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A59" s="124"/>
-      <c r="B59" s="125"/>
+    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A59" s="138"/>
+      <c r="B59" s="134"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -29726,9 +29820,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="124"/>
-      <c r="B60" s="125"/>
+    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="138"/>
+      <c r="B60" s="134"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -29736,9 +29830,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A61" s="124"/>
-      <c r="B61" s="125"/>
+    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A61" s="138"/>
+      <c r="B61" s="134"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -29746,9 +29840,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A62" s="124"/>
-      <c r="B62" s="125"/>
+    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A62" s="138"/>
+      <c r="B62" s="134"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -29756,9 +29850,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A63" s="124"/>
-      <c r="B63" s="125"/>
+    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A63" s="138"/>
+      <c r="B63" s="134"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -29766,17 +29860,17 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
-      <c r="A64" s="124"/>
-      <c r="B64" s="125"/>
+    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+      <c r="A64" s="138"/>
+      <c r="B64" s="134"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="124"/>
-      <c r="B65" s="125"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="138"/>
+      <c r="B65" s="134"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -29784,17 +29878,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="124"/>
-      <c r="B66" s="125"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="138"/>
+      <c r="B66" s="134"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="124"/>
-      <c r="B67" s="125"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="138"/>
+      <c r="B67" s="134"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -29802,9 +29896,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="124"/>
-      <c r="B68" s="125"/>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="138"/>
+      <c r="B68" s="134"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -29812,9 +29906,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="124"/>
-      <c r="B69" s="125"/>
+    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="138"/>
+      <c r="B69" s="134"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -29822,9 +29916,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="124"/>
-      <c r="B70" s="125"/>
+    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="138"/>
+      <c r="B70" s="134"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -29832,9 +29926,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="124"/>
-      <c r="B71" s="125"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="138"/>
+      <c r="B71" s="134"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -29842,9 +29936,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="124"/>
-      <c r="B72" s="125"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="138"/>
+      <c r="B72" s="134"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -29852,17 +29946,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="124"/>
-      <c r="B73" s="125"/>
+    <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="138"/>
+      <c r="B73" s="134"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="124"/>
-      <c r="B74" s="125"/>
+    <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="138"/>
+      <c r="B74" s="134"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -29870,21 +29964,21 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="124"/>
-      <c r="B75" s="125"/>
-      <c r="C75" s="121"/>
-      <c r="D75" s="126" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="138"/>
+      <c r="B75" s="134"/>
+      <c r="C75" s="136"/>
+      <c r="D75" s="139" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="124"/>
-      <c r="B76" s="125"/>
-      <c r="C76" s="121"/>
-      <c r="D76" s="126"/>
+    <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="138"/>
+      <c r="B76" s="134"/>
+      <c r="C76" s="136"/>
+      <c r="D76" s="139"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
@@ -29892,13 +29986,13 @@
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -29906,8 +30000,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -29916,13 +30010,31 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="B16:B25"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="A39:A40"/>
@@ -29935,24 +30047,6 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="B16:B25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -29967,15 +30061,15 @@
       <selection activeCell="A53" sqref="A53:A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" customWidth="1"/>
-    <col min="4" max="4" width="80.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="4" max="4" width="80.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -29989,7 +30083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -30005,11 +30099,11 @@
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="131" t="s">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="125" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30019,134 +30113,134 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="131"/>
-      <c r="B5" s="130"/>
-      <c r="C5" s="140" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="124"/>
+      <c r="B5" s="125"/>
+      <c r="C5" s="155" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="139" t="s">
+      <c r="D5" s="154" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="131"/>
-      <c r="B6" s="130"/>
-      <c r="C6" s="140"/>
-      <c r="D6" s="139"/>
+    <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="124"/>
+      <c r="B6" s="125"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="154"/>
     </row>
-    <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="131"/>
-      <c r="B7" s="130"/>
+    <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="124"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
-    <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="131"/>
-      <c r="B8" s="130"/>
+    <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="124"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
-    <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="131"/>
-      <c r="B9" s="130"/>
+    <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="124"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="133" t="s">
+    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="135" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="125" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="142"/>
-      <c r="D10" s="139" t="s">
+      <c r="C10" s="146"/>
+      <c r="D10" s="154" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="133"/>
-      <c r="B11" s="130"/>
-      <c r="C11" s="142"/>
-      <c r="D11" s="139"/>
+    <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="135"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="146"/>
+      <c r="D11" s="154"/>
     </row>
-    <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="133"/>
-      <c r="B12" s="130"/>
-      <c r="C12" s="142"/>
-      <c r="D12" s="139"/>
+    <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="135"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="154"/>
     </row>
-    <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="134" t="s">
+    <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="125" t="s">
+      <c r="B13" s="134" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="141"/>
-      <c r="D13" s="139" t="s">
+      <c r="C13" s="156"/>
+      <c r="D13" s="154" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="134"/>
-      <c r="B14" s="125"/>
-      <c r="C14" s="141"/>
-      <c r="D14" s="139"/>
+    <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="122"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="156"/>
+      <c r="D14" s="154"/>
     </row>
-    <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="134"/>
-      <c r="B15" s="125"/>
-      <c r="C15" s="141"/>
+    <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="122"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="156"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="134"/>
-      <c r="B16" s="125"/>
-      <c r="C16" s="141"/>
+      <c r="A16" s="122"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="156"/>
       <c r="D16" s="49"/>
     </row>
-    <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="134"/>
-      <c r="B17" s="125"/>
-      <c r="C17" s="141"/>
+    <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="122"/>
+      <c r="B17" s="134"/>
+      <c r="C17" s="156"/>
       <c r="D17" s="49"/>
     </row>
-    <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="134"/>
-      <c r="B18" s="125"/>
-      <c r="C18" s="141"/>
+    <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="122"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="156"/>
       <c r="D18" s="49"/>
     </row>
-    <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="134"/>
-      <c r="B19" s="125"/>
-      <c r="C19" s="141"/>
+    <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="122"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="156"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="134"/>
-      <c r="B20" s="125"/>
-      <c r="C20" s="141"/>
+    <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="122"/>
+      <c r="B20" s="134"/>
+      <c r="C20" s="156"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="134"/>
-      <c r="B21" s="125"/>
-      <c r="C21" s="141"/>
+    <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="122"/>
+      <c r="B21" s="134"/>
+      <c r="C21" s="156"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="134"/>
-      <c r="B22" s="125"/>
-      <c r="C22" s="141"/>
+    <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="122"/>
+      <c r="B22" s="134"/>
+      <c r="C22" s="156"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="134"/>
-      <c r="B23" s="125"/>
-      <c r="C23" s="141"/>
+    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="122"/>
+      <c r="B23" s="134"/>
+      <c r="C23" s="156"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30165,7 +30259,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30179,7 +30273,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30199,7 +30293,7 @@
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30223,7 +30317,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30233,7 +30327,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30243,11 +30337,11 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="150" t="s">
+    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="140" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="153" t="s">
+      <c r="B32" s="143" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30257,27 +30351,27 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="151"/>
-      <c r="B33" s="154"/>
+    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="141"/>
+      <c r="B33" s="144"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="151"/>
-      <c r="B34" s="154"/>
+      <c r="A34" s="141"/>
+      <c r="B34" s="144"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
-    <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="151"/>
-      <c r="B35" s="154"/>
+    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="141"/>
+      <c r="B35" s="144"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
-    <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="152"/>
-      <c r="B36" s="155"/>
+    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="142"/>
+      <c r="B36" s="145"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30305,11 +30399,11 @@
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
     </row>
-    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="132" t="s">
+    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="130" t="s">
+      <c r="B39" s="125" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30319,9 +30413,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="132"/>
-      <c r="B40" s="130"/>
+    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="126"/>
+      <c r="B40" s="125"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30329,87 +30423,87 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="131" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="124" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="130" t="s">
+      <c r="B41" s="125" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="142" t="s">
+      <c r="C41" s="146" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="134" t="s">
+      <c r="D41" s="122" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="131"/>
-      <c r="B42" s="130"/>
-      <c r="C42" s="142"/>
-      <c r="D42" s="134"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="124"/>
+      <c r="B42" s="125"/>
+      <c r="C42" s="146"/>
+      <c r="D42" s="122"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="131"/>
-      <c r="B43" s="130"/>
-      <c r="C43" s="142" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="124"/>
+      <c r="B43" s="125"/>
+      <c r="C43" s="146" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="126" t="s">
+      <c r="D43" s="139" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="131"/>
-      <c r="B44" s="130"/>
-      <c r="C44" s="142"/>
-      <c r="D44" s="126"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="124"/>
+      <c r="B44" s="125"/>
+      <c r="C44" s="146"/>
+      <c r="D44" s="139"/>
     </row>
-    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="124" t="s">
+    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="138" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="125" t="s">
+      <c r="B45" s="134" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="146"/>
+      <c r="C45" s="150"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="124"/>
-      <c r="B46" s="125"/>
-      <c r="C46" s="147"/>
-      <c r="D46" s="143" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="138"/>
+      <c r="B46" s="134"/>
+      <c r="C46" s="151"/>
+      <c r="D46" s="147" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="124"/>
-      <c r="B47" s="125"/>
-      <c r="C47" s="147"/>
-      <c r="D47" s="144"/>
+    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="138"/>
+      <c r="B47" s="134"/>
+      <c r="C47" s="151"/>
+      <c r="D47" s="148"/>
     </row>
-    <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="124"/>
-      <c r="B48" s="125"/>
-      <c r="C48" s="148"/>
-      <c r="D48" s="144"/>
+    <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="138"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="152"/>
+      <c r="D48" s="148"/>
     </row>
-    <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="124"/>
-      <c r="B49" s="125"/>
-      <c r="C49" s="122"/>
-      <c r="D49" s="144"/>
+    <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="138"/>
+      <c r="B49" s="134"/>
+      <c r="C49" s="137"/>
+      <c r="D49" s="148"/>
     </row>
-    <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="124"/>
-      <c r="B50" s="125"/>
-      <c r="C50" s="122"/>
-      <c r="D50" s="145"/>
+    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="138"/>
+      <c r="B50" s="134"/>
+      <c r="C50" s="137"/>
+      <c r="D50" s="149"/>
     </row>
-    <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
@@ -30429,11 +30523,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="125" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="134" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="125" t="s">
+      <c r="B53" s="134" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30443,9 +30537,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="125"/>
-      <c r="B54" s="125"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="134"/>
+      <c r="B54" s="134"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30453,9 +30547,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="125"/>
-      <c r="B55" s="125"/>
+    <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="134"/>
+      <c r="B55" s="134"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30463,27 +30557,27 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="125"/>
-      <c r="B56" s="125"/>
-      <c r="C56" s="149" t="s">
+    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="134"/>
+      <c r="B56" s="134"/>
+      <c r="C56" s="153" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="125"/>
-      <c r="B57" s="125"/>
-      <c r="C57" s="149"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="134"/>
+      <c r="B57" s="134"/>
+      <c r="C57" s="153"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="125"/>
-      <c r="B58" s="125"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="134"/>
+      <c r="B58" s="134"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30491,9 +30585,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="125"/>
-      <c r="B59" s="125"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="134"/>
+      <c r="B59" s="134"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30501,135 +30595,129 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="125"/>
-      <c r="B60" s="125"/>
-      <c r="C60" s="149" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="134"/>
+      <c r="B60" s="134"/>
+      <c r="C60" s="153" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="125"/>
-      <c r="B61" s="125"/>
-      <c r="C61" s="149"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="134"/>
+      <c r="B61" s="134"/>
+      <c r="C61" s="153"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="125"/>
-      <c r="B62" s="125"/>
-      <c r="C62" s="149"/>
+    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="134"/>
+      <c r="B62" s="134"/>
+      <c r="C62" s="153"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="125"/>
-      <c r="B63" s="125"/>
-      <c r="C63" s="142" t="s">
+    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="134"/>
+      <c r="B63" s="134"/>
+      <c r="C63" s="146" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="125"/>
-      <c r="B64" s="125"/>
-      <c r="C64" s="142"/>
-      <c r="D64" s="126" t="s">
+    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="134"/>
+      <c r="B64" s="134"/>
+      <c r="C64" s="146"/>
+      <c r="D64" s="139" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="125"/>
-      <c r="B65" s="125"/>
-      <c r="C65" s="142"/>
-      <c r="D65" s="126"/>
+    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="134"/>
+      <c r="B65" s="134"/>
+      <c r="C65" s="146"/>
+      <c r="D65" s="139"/>
     </row>
-    <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="125"/>
-      <c r="B66" s="125"/>
-      <c r="C66" s="142"/>
-      <c r="D66" s="126"/>
+    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="134"/>
+      <c r="B66" s="134"/>
+      <c r="C66" s="146"/>
+      <c r="D66" s="139"/>
     </row>
-    <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="125"/>
-      <c r="B67" s="125"/>
-      <c r="C67" s="142"/>
-      <c r="D67" s="126"/>
+    <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="134"/>
+      <c r="B67" s="134"/>
+      <c r="C67" s="146"/>
+      <c r="D67" s="139"/>
     </row>
-    <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
     </row>
-    <row r="69" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B53:B67"/>
@@ -30643,13 +30731,19 @@
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30658,21 +30752,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30694,33 +30788,33 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="159" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="149" t="s">
+      <c r="C3" s="153" t="s">
         <v>235</v>
       </c>
-      <c r="D3" s="136" t="s">
+      <c r="D3" s="127" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="157"/>
-      <c r="C4" s="149"/>
-      <c r="D4" s="137"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="153"/>
+      <c r="D4" s="128"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="B5" s="157"/>
+      <c r="B5" s="160"/>
       <c r="C5" s="99" t="s">
         <v>22</v>
       </c>
@@ -30728,11 +30822,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="158"/>
+      <c r="B6" s="161"/>
       <c r="C6" s="58"/>
       <c r="D6" s="98" t="s">
         <v>254</v>
@@ -30746,26 +30840,26 @@
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="159" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="157" t="s">
         <v>237</v>
       </c>
-      <c r="B8" s="149" t="s">
+      <c r="B8" s="153" t="s">
         <v>234</v>
       </c>
       <c r="D8" s="58" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="160"/>
-      <c r="B9" s="149"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="158"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="105"/>
       <c r="D9" s="58" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="97" t="s">
         <v>27</v>
       </c>
@@ -30777,11 +30871,11 @@
         <v>238</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="149" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="153" t="s">
         <v>222</v>
       </c>
-      <c r="B11" s="149" t="s">
+      <c r="B11" s="153" t="s">
         <v>234</v>
       </c>
       <c r="C11" s="102" t="s">
@@ -30791,9 +30885,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
-      <c r="B12" s="149"/>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="153"/>
+      <c r="B12" s="153"/>
       <c r="C12" s="102" t="s">
         <v>240</v>
       </c>
@@ -30809,7 +30903,7 @@
       <c r="C13" s="39"/>
       <c r="D13" s="44"/>
     </row>
-    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="95" t="s">
         <v>243</v>
       </c>
@@ -30823,7 +30917,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="96" t="s">
         <v>32</v>
       </c>
@@ -30837,7 +30931,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="39" t="s">
         <v>40</v>
       </c>
@@ -30845,7 +30939,7 @@
       <c r="C16" s="39"/>
       <c r="D16" s="44"/>
     </row>
-    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="58" t="s">
         <v>84</v>
       </c>
@@ -30859,11 +30953,11 @@
         <v>253</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="134" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="122" t="s">
         <v>247</v>
       </c>
-      <c r="B18" s="149" t="s">
+      <c r="B18" s="153" t="s">
         <v>234</v>
       </c>
       <c r="C18" s="99">
@@ -30873,9 +30967,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="134"/>
-      <c r="B19" s="149"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="122"/>
+      <c r="B19" s="153"/>
       <c r="C19" s="99">
         <v>10.199999999999999</v>
       </c>
@@ -30891,7 +30985,7 @@
       <c r="C20" s="39"/>
       <c r="D20" s="44"/>
     </row>
-    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="58" t="s">
         <v>249</v>
       </c>
@@ -30905,8 +30999,71 @@
         <v>251</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="108"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="109"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="162" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="163" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" s="164" t="s">
+        <v>257</v>
+      </c>
+      <c r="D23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="165"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="164" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="167" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="167" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="164" t="s">
+        <v>260</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="167" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="164" t="s">
+        <v>260</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>261</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A8:A9"/>

</xml_diff>

<commit_message>
"PIT Guide, change log, validation rule updates"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMOD_Documentation\paye-employers-documentation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\userdatadubc11\homedir\pbarre02\Desktop_vdi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008" activeTab="3"/>
+    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="290">
   <si>
     <t>Document</t>
   </si>
@@ -2660,6 +2660,27 @@
   <si>
     <t>Sample HTTP Request with full 'Signature' Header</t>
   </si>
+  <si>
+    <t>Date Updated</t>
+  </si>
+  <si>
+    <t>code 3007</t>
+  </si>
+  <si>
+    <t>code 1011</t>
+  </si>
+  <si>
+    <t>Modified</t>
+  </si>
+  <si>
+    <t>PIT Self Service Application Guide</t>
+  </si>
+  <si>
+    <t>Section 7 added (Agent functionality)</t>
+  </si>
+  <si>
+    <t>New section</t>
+  </si>
 </sst>
 </file>
 
@@ -3253,7 +3274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3506,12 +3527,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3521,27 +3538,17 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3564,6 +3571,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3609,20 +3660,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3636,41 +3717,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3696,31 +3759,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3732,34 +3804,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4136,18 +4196,19 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:D45"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4160,24 +4221,28 @@
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="120" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="2"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="131">
+        <v>43056</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
@@ -4190,24 +4255,24 @@
       <c r="D3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="131"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="120" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="131"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -4220,12 +4285,12 @@
       <c r="D5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="131"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -4238,16 +4303,16 @@
       <c r="D6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="131"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="123" t="s">
+    <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="126">
+      <c r="B7" s="138">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4256,86 +4321,86 @@
       <c r="D7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="131"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
-      <c r="B8" s="127"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="136"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="131"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
-      <c r="B9" s="127"/>
+    <row r="9" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="136"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="131"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
-      <c r="B10" s="127"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="136"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="131"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
-      <c r="B11" s="127"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="136"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="131"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="125"/>
-      <c r="B12" s="128"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="137"/>
+      <c r="B12" s="140"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="131"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="131" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="126">
+      <c r="B13" s="138">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4344,26 +4409,26 @@
       <c r="D13" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="131"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="132"/>
-      <c r="B14" s="128"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="144"/>
+      <c r="B14" s="140"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="131"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -4376,12 +4441,12 @@
       <c r="D15" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="131"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -4394,24 +4459,24 @@
       <c r="D16" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="131"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="120" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="121"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="122"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="131"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -4424,12 +4489,12 @@
       <c r="D18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="131"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4442,28 +4507,28 @@
       <c r="D19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="131"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="120" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="121"/>
-      <c r="C20" s="121"/>
-      <c r="D20" s="122"/>
-      <c r="E20" s="2"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="131"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="133" t="s">
+    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="145" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="130">
+      <c r="B21" s="142">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4472,22 +4537,23 @@
       <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="131"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="134"/>
-      <c r="B22" s="128"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="146"/>
+      <c r="B22" s="140"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>39</v>
       </c>
+      <c r="E22" s="131"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4500,20 +4566,22 @@
       <c r="D23" s="36" t="s">
         <v>30</v>
       </c>
+      <c r="E23" s="131"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="120" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="132" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="121"/>
-      <c r="C24" s="121"/>
-      <c r="D24" s="122"/>
+      <c r="B24" s="133"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="131"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="129" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="130">
+      <c r="B25" s="142">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4522,110 +4590,110 @@
       <c r="D25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="131"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="124"/>
-      <c r="B26" s="127"/>
+    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="136"/>
+      <c r="B26" s="139"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="131"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="124"/>
-      <c r="B27" s="127"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="136"/>
+      <c r="B27" s="139"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="131"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="124"/>
-      <c r="B28" s="127"/>
+    <row r="28" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="136"/>
+      <c r="B28" s="139"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="131"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="124"/>
-      <c r="B29" s="127"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="136"/>
+      <c r="B29" s="139"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="131"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="124"/>
-      <c r="B30" s="127"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="136"/>
+      <c r="B30" s="139"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="131"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="124"/>
-      <c r="B31" s="127"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="136"/>
+      <c r="B31" s="139"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="131"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="125"/>
-      <c r="B32" s="128"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="137"/>
+      <c r="B32" s="140"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="131"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4638,8 +4706,9 @@
       <c r="D33" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E33" s="131"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4652,8 +4721,9 @@
       <c r="D34" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E34" s="131"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4666,8 +4736,9 @@
       <c r="D35" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E35" s="131"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4680,8 +4751,9 @@
       <c r="D36" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E36" s="131"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4694,8 +4766,9 @@
       <c r="D37" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E37" s="131"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4708,8 +4781,9 @@
       <c r="D38" s="12" t="s">
         <v>54</v>
       </c>
+      <c r="E38" s="131"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4722,8 +4796,9 @@
       <c r="D39" s="24" t="s">
         <v>55</v>
       </c>
+      <c r="E39" s="131"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4736,16 +4811,18 @@
       <c r="D40" s="26" t="s">
         <v>55</v>
       </c>
+      <c r="E40" s="131"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="120" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="121"/>
-      <c r="C41" s="121"/>
-      <c r="D41" s="122"/>
+      <c r="B41" s="133"/>
+      <c r="C41" s="133"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="131"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4758,8 +4835,9 @@
       <c r="D42" s="9" t="s">
         <v>30</v>
       </c>
+      <c r="E42" s="131"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4772,8 +4850,9 @@
       <c r="D43" s="12" t="s">
         <v>30</v>
       </c>
+      <c r="E43" s="131"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4786,8 +4865,9 @@
       <c r="D44" s="12" t="s">
         <v>30</v>
       </c>
+      <c r="E44" s="131"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4800,10 +4880,11 @@
       <c r="D45" s="16" t="s">
         <v>30</v>
       </c>
+      <c r="E45" s="131"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4813,13 +4894,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="E2:E45"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A41:D41"/>
@@ -4844,19 +4926,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD79"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:A76"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -4869,16 +4952,22 @@
       <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="6" t="s">
+        <v>283</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
+      <c r="E2" s="158">
+        <v>43140</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -4889,8 +4978,9 @@
       <c r="D3" s="53" t="s">
         <v>30</v>
       </c>
+      <c r="E3" s="158"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -4901,8 +4991,9 @@
       <c r="D4" s="53" t="s">
         <v>30</v>
       </c>
+      <c r="E4" s="158"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -4913,20 +5004,22 @@
       <c r="D5" s="53" t="s">
         <v>30</v>
       </c>
+      <c r="E5" s="158"/>
     </row>
-    <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
+      <c r="E6" s="158"/>
     </row>
-    <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="145" t="s">
+    <row r="7" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="144" t="s">
+      <c r="B7" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -4935,62 +5028,68 @@
       <c r="D7" s="41" t="s">
         <v>92</v>
       </c>
+      <c r="E7" s="158"/>
     </row>
-    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="145"/>
-      <c r="B8" s="144"/>
+    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="152"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>91</v>
       </c>
+      <c r="E8" s="158"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="145"/>
-      <c r="B9" s="144"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="152"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>90</v>
       </c>
+      <c r="E9" s="158"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="145"/>
-      <c r="B10" s="144"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="152"/>
+      <c r="B10" s="153"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="46" t="s">
         <v>95</v>
       </c>
+      <c r="E10" s="158"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="145"/>
-      <c r="B11" s="144"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="152"/>
+      <c r="B11" s="153"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
       <c r="D11" s="47" t="s">
         <v>94</v>
       </c>
+      <c r="E11" s="158"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="145"/>
-      <c r="B12" s="144"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="152"/>
+      <c r="B12" s="153"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D12" s="47" t="s">
         <v>97</v>
       </c>
+      <c r="E12" s="158"/>
     </row>
-    <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="147" t="s">
+    <row r="13" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="155" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="144" t="s">
+      <c r="B13" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4999,32 +5098,35 @@
       <c r="D13" s="49" t="s">
         <v>179</v>
       </c>
+      <c r="E13" s="158"/>
     </row>
-    <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="147"/>
-      <c r="B14" s="144"/>
+    <row r="14" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="155"/>
+      <c r="B14" s="153"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
       <c r="D14" s="49" t="s">
         <v>181</v>
       </c>
+      <c r="E14" s="158"/>
     </row>
-    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="147"/>
-      <c r="B15" s="144"/>
+    <row r="15" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="155"/>
+      <c r="B15" s="153"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
       <c r="D15" s="49" t="s">
         <v>183</v>
       </c>
+      <c r="E15" s="158"/>
     </row>
-    <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="148" t="s">
+    <row r="16" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="139" t="s">
+      <c r="B16" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5033,98 +5135,108 @@
       <c r="D16" s="41" t="s">
         <v>184</v>
       </c>
+      <c r="E16" s="158"/>
     </row>
-    <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="148"/>
-      <c r="B17" s="139"/>
+    <row r="17" spans="1:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="150"/>
+      <c r="B17" s="156"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="49" t="s">
         <v>149</v>
       </c>
+      <c r="E17" s="158"/>
     </row>
-    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="148"/>
-      <c r="B18" s="139"/>
+    <row r="18" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="150"/>
+      <c r="B18" s="156"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
       <c r="D18" s="49" t="s">
         <v>150</v>
       </c>
+      <c r="E18" s="158"/>
     </row>
-    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="148"/>
-      <c r="B19" s="139"/>
+    <row r="19" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="150"/>
+      <c r="B19" s="156"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="49" t="s">
         <v>152</v>
       </c>
+      <c r="E19" s="158"/>
     </row>
-    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="148"/>
-      <c r="B20" s="139"/>
+    <row r="20" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="150"/>
+      <c r="B20" s="156"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="49" t="s">
         <v>154</v>
       </c>
+      <c r="E20" s="158"/>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="148"/>
-      <c r="B21" s="139"/>
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="150"/>
+      <c r="B21" s="156"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
       <c r="D21" s="65" t="s">
         <v>156</v>
       </c>
+      <c r="E21" s="158"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="148"/>
-      <c r="B22" s="139"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="150"/>
+      <c r="B22" s="156"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>158</v>
       </c>
+      <c r="E22" s="158"/>
     </row>
-    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="148"/>
-      <c r="B23" s="139"/>
+    <row r="23" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="150"/>
+      <c r="B23" s="156"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>160</v>
       </c>
+      <c r="E23" s="158"/>
     </row>
-    <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="148"/>
-      <c r="B24" s="139"/>
-      <c r="C24" s="148" t="s">
+    <row r="24" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="150"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="150" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="149" t="s">
+      <c r="D24" s="157" t="s">
         <v>162</v>
       </c>
+      <c r="E24" s="158"/>
     </row>
-    <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="148"/>
-      <c r="B25" s="139"/>
-      <c r="C25" s="148"/>
-      <c r="D25" s="149"/>
+    <row r="25" spans="1:5" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="150"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="158"/>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="145" t="s">
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="152" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="144" t="s">
+      <c r="B26" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5133,16 +5245,18 @@
       <c r="D26" s="41" t="s">
         <v>164</v>
       </c>
+      <c r="E26" s="158"/>
     </row>
-    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="145"/>
-      <c r="B27" s="144"/>
+    <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="152"/>
+      <c r="B27" s="153"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
+      <c r="E27" s="158"/>
     </row>
-    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -5153,106 +5267,117 @@
       <c r="D28" s="48" t="s">
         <v>166</v>
       </c>
+      <c r="E28" s="158"/>
     </row>
-    <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
+      <c r="E29" s="158"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="146" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="144" t="s">
+      <c r="B30" s="153" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="148" t="s">
+      <c r="C30" s="150" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="137" t="s">
+      <c r="D30" s="151" t="s">
         <v>177</v>
       </c>
+      <c r="E30" s="158"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="146"/>
-      <c r="B31" s="144"/>
-      <c r="C31" s="148"/>
-      <c r="D31" s="137"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="154"/>
+      <c r="B31" s="153"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="151"/>
+      <c r="E31" s="158"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="146"/>
-      <c r="B32" s="144"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="154"/>
+      <c r="B32" s="153"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
       <c r="D32" s="62" t="s">
         <v>176</v>
       </c>
+      <c r="E32" s="158"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="146"/>
-      <c r="B33" s="144"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="154"/>
+      <c r="B33" s="153"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
       <c r="D33" s="62" t="s">
         <v>175</v>
       </c>
+      <c r="E33" s="158"/>
     </row>
-    <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="146"/>
-      <c r="B34" s="144"/>
+    <row r="34" spans="1:5" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="154"/>
+      <c r="B34" s="153"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
       <c r="D34" s="68" t="s">
         <v>174</v>
       </c>
+      <c r="E34" s="158"/>
     </row>
-    <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="146"/>
-      <c r="B35" s="144"/>
+    <row r="35" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="154"/>
+      <c r="B35" s="153"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
       <c r="D35" s="62" t="s">
         <v>173</v>
       </c>
+      <c r="E35" s="158"/>
     </row>
-    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="146"/>
-      <c r="B36" s="144"/>
+    <row r="36" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="154"/>
+      <c r="B36" s="153"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
       <c r="D36" s="68" t="s">
         <v>172</v>
       </c>
+      <c r="E36" s="158"/>
     </row>
-    <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="146"/>
-      <c r="B37" s="144"/>
-      <c r="C37" s="150" t="s">
+    <row r="37" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="154"/>
+      <c r="B37" s="153"/>
+      <c r="C37" s="147" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="152" t="s">
+      <c r="D37" s="149" t="s">
         <v>171</v>
       </c>
+      <c r="E37" s="158"/>
     </row>
-    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="146"/>
-      <c r="B38" s="144"/>
-      <c r="C38" s="151"/>
-      <c r="D38" s="152"/>
+    <row r="38" spans="1:5" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="154"/>
+      <c r="B38" s="153"/>
+      <c r="C38" s="148"/>
+      <c r="D38" s="149"/>
+      <c r="E38" s="158"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="145" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="144" t="s">
+      <c r="B39" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5261,16 +5386,18 @@
       <c r="D39" s="52" t="s">
         <v>132</v>
       </c>
+      <c r="E39" s="158"/>
     </row>
-    <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="145"/>
-      <c r="B40" s="144"/>
+    <row r="40" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="152"/>
+      <c r="B40" s="153"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
+      <c r="E40" s="158"/>
     </row>
-    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -5281,90 +5408,99 @@
       <c r="D41" s="50" t="s">
         <v>79</v>
       </c>
+      <c r="E41" s="158"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
+      <c r="E42" s="158"/>
     </row>
-    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="146" t="s">
+    <row r="43" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="144" t="s">
+      <c r="B43" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="49" t="s">
         <v>131</v>
       </c>
+      <c r="E43" s="158"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="146"/>
-      <c r="B44" s="144"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="154"/>
+      <c r="B44" s="153"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D44" s="52" t="s">
         <v>132</v>
       </c>
+      <c r="E44" s="158"/>
     </row>
-    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="141" t="s">
+    <row r="45" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="163" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="144" t="s">
+      <c r="B45" s="153" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
       <c r="D45" s="64" t="s">
         <v>103</v>
       </c>
+      <c r="E45" s="158"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="142"/>
-      <c r="B46" s="144"/>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="164"/>
+      <c r="B46" s="153"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
       <c r="D46" s="49" t="s">
         <v>102</v>
       </c>
+      <c r="E46" s="158"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="142"/>
-      <c r="B47" s="144"/>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="164"/>
+      <c r="B47" s="153"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
       <c r="D47" s="49" t="s">
         <v>100</v>
       </c>
+      <c r="E47" s="158"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="143"/>
-      <c r="B48" s="144"/>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="165"/>
+      <c r="B48" s="153"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D48" s="52" t="s">
         <v>132</v>
       </c>
+      <c r="E48" s="158"/>
     </row>
-    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A49" s="139" t="s">
+    <row r="49" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A49" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="139" t="s">
+      <c r="B49" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
       <c r="D49" s="47" t="s">
         <v>104</v>
       </c>
+      <c r="E49" s="158"/>
       <c r="H49" s="42"/>
       <c r="L49" s="42"/>
       <c r="P49" s="42"/>
@@ -9461,15 +9597,16 @@
       <c r="XEZ49" s="42"/>
       <c r="XFD49" s="42"/>
     </row>
-    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="139"/>
-      <c r="B50" s="139"/>
+    <row r="50" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="156"/>
+      <c r="B50" s="156"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
       <c r="D50" s="60" t="s">
         <v>106</v>
       </c>
+      <c r="E50" s="158"/>
       <c r="H50" s="42"/>
       <c r="L50" s="42"/>
       <c r="P50" s="42"/>
@@ -13566,15 +13703,16 @@
       <c r="XEZ50" s="42"/>
       <c r="XFD50" s="42"/>
     </row>
-    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A51" s="139"/>
-      <c r="B51" s="139"/>
+    <row r="51" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A51" s="156"/>
+      <c r="B51" s="156"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
       <c r="D51" s="47" t="s">
         <v>133</v>
       </c>
+      <c r="E51" s="158"/>
       <c r="H51" s="42"/>
       <c r="L51" s="42"/>
       <c r="P51" s="42"/>
@@ -17671,15 +17809,16 @@
       <c r="XEZ51" s="42"/>
       <c r="XFD51" s="42"/>
     </row>
-    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A52" s="139"/>
-      <c r="B52" s="139"/>
+    <row r="52" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A52" s="156"/>
+      <c r="B52" s="156"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
       <c r="D52" s="47" t="s">
         <v>134</v>
       </c>
+      <c r="E52" s="158"/>
       <c r="H52" s="42"/>
       <c r="L52" s="42"/>
       <c r="P52" s="42"/>
@@ -21776,15 +21915,16 @@
       <c r="XEZ52" s="42"/>
       <c r="XFD52" s="42"/>
     </row>
-    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A53" s="139"/>
-      <c r="B53" s="139"/>
-      <c r="C53" s="136" t="s">
+    <row r="53" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A53" s="156"/>
+      <c r="B53" s="156"/>
+      <c r="C53" s="160" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="137" t="s">
+      <c r="D53" s="151" t="s">
         <v>144</v>
       </c>
+      <c r="E53" s="158"/>
       <c r="H53" s="42"/>
       <c r="L53" s="42"/>
       <c r="P53" s="42"/>
@@ -25881,11 +26021,12 @@
       <c r="XEZ53" s="42"/>
       <c r="XFD53" s="42"/>
     </row>
-    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="139"/>
-      <c r="B54" s="139"/>
-      <c r="C54" s="136"/>
-      <c r="D54" s="137"/>
+    <row r="54" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="156"/>
+      <c r="B54" s="156"/>
+      <c r="C54" s="160"/>
+      <c r="D54" s="151"/>
+      <c r="E54" s="158"/>
       <c r="H54" s="42"/>
       <c r="L54" s="42"/>
       <c r="P54" s="42"/>
@@ -29982,15 +30123,16 @@
       <c r="XEZ54" s="42"/>
       <c r="XFD54" s="42"/>
     </row>
-    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
+      <c r="E55" s="158"/>
     </row>
-    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -30001,12 +30143,13 @@
       <c r="D56" s="49" t="s">
         <v>110</v>
       </c>
+      <c r="E56" s="158"/>
     </row>
-    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A57" s="138" t="s">
+    <row r="57" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A57" s="161" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="139" t="s">
+      <c r="B57" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30015,200 +30158,221 @@
       <c r="D57" s="47" t="s">
         <v>111</v>
       </c>
+      <c r="E57" s="158"/>
     </row>
-    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="138"/>
-      <c r="B58" s="139"/>
+    <row r="58" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="161"/>
+      <c r="B58" s="156"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="47" t="s">
         <v>135</v>
       </c>
+      <c r="E58" s="158"/>
     </row>
-    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A59" s="138"/>
-      <c r="B59" s="139"/>
+    <row r="59" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A59" s="161"/>
+      <c r="B59" s="156"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
       <c r="D59" s="47" t="s">
         <v>136</v>
       </c>
+      <c r="E59" s="158"/>
     </row>
-    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="138"/>
-      <c r="B60" s="139"/>
+    <row r="60" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="161"/>
+      <c r="B60" s="156"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
       <c r="D60" s="62" t="s">
         <v>116</v>
       </c>
+      <c r="E60" s="158"/>
     </row>
-    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A61" s="138"/>
-      <c r="B61" s="139"/>
+    <row r="61" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A61" s="161"/>
+      <c r="B61" s="156"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D61" s="47" t="s">
         <v>137</v>
       </c>
+      <c r="E61" s="158"/>
     </row>
-    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A62" s="138"/>
-      <c r="B62" s="139"/>
+    <row r="62" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A62" s="161"/>
+      <c r="B62" s="156"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D62" s="47" t="s">
         <v>138</v>
       </c>
+      <c r="E62" s="158"/>
     </row>
-    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A63" s="138"/>
-      <c r="B63" s="139"/>
+    <row r="63" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A63" s="161"/>
+      <c r="B63" s="156"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
       <c r="D63" s="47" t="s">
         <v>139</v>
       </c>
+      <c r="E63" s="158"/>
     </row>
-    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.3">
-      <c r="A64" s="138"/>
-      <c r="B64" s="139"/>
+    <row r="64" spans="1:1024 1028:2048 2052:3072 3076:4096 4100:5120 5124:6144 6148:7168 7172:8192 8196:9216 9220:10240 10244:11264 11268:12288 12292:13312 13316:14336 14340:15360 15364:16384" x14ac:dyDescent="0.25">
+      <c r="A64" s="161"/>
+      <c r="B64" s="156"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
+      <c r="E64" s="158"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="138"/>
-      <c r="B65" s="139"/>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="161"/>
+      <c r="B65" s="156"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
       <c r="D65" s="47" t="s">
         <v>119</v>
       </c>
+      <c r="E65" s="158"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="138"/>
-      <c r="B66" s="139"/>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="161"/>
+      <c r="B66" s="156"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
+      <c r="E66" s="158"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="138"/>
-      <c r="B67" s="139"/>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="161"/>
+      <c r="B67" s="156"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
       <c r="D67" s="62" t="s">
         <v>140</v>
       </c>
+      <c r="E67" s="158"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="138"/>
-      <c r="B68" s="139"/>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="161"/>
+      <c r="B68" s="156"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
       <c r="D68" s="62" t="s">
         <v>124</v>
       </c>
+      <c r="E68" s="158"/>
     </row>
-    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="138"/>
-      <c r="B69" s="139"/>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="161"/>
+      <c r="B69" s="156"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
       <c r="D69" s="47" t="s">
         <v>141</v>
       </c>
+      <c r="E69" s="158"/>
     </row>
-    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="138"/>
-      <c r="B70" s="139"/>
+    <row r="70" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="161"/>
+      <c r="B70" s="156"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
       <c r="D70" s="47" t="s">
         <v>141</v>
       </c>
+      <c r="E70" s="158"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="138"/>
-      <c r="B71" s="139"/>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="161"/>
+      <c r="B71" s="156"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
       <c r="D71" s="47" t="s">
         <v>142</v>
       </c>
+      <c r="E71" s="158"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="138"/>
-      <c r="B72" s="139"/>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="161"/>
+      <c r="B72" s="156"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
       <c r="D72" s="47" t="s">
         <v>140</v>
       </c>
+      <c r="E72" s="158"/>
     </row>
-    <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="138"/>
-      <c r="B73" s="139"/>
+    <row r="73" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="161"/>
+      <c r="B73" s="156"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
+      <c r="E73" s="158"/>
     </row>
-    <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="138"/>
-      <c r="B74" s="139"/>
+    <row r="74" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="161"/>
+      <c r="B74" s="156"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
       <c r="D74" s="47" t="s">
         <v>143</v>
       </c>
+      <c r="E74" s="158"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="138"/>
-      <c r="B75" s="139"/>
-      <c r="C75" s="135"/>
-      <c r="D75" s="140" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="161"/>
+      <c r="B75" s="156"/>
+      <c r="C75" s="159"/>
+      <c r="D75" s="162" t="s">
         <v>130</v>
       </c>
+      <c r="E75" s="158"/>
     </row>
-    <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="138"/>
-      <c r="B76" s="139"/>
-      <c r="C76" s="135"/>
-      <c r="D76" s="140"/>
+    <row r="76" spans="1:5" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="161"/>
+      <c r="B76" s="156"/>
+      <c r="C76" s="159"/>
+      <c r="D76" s="162"/>
+      <c r="E76" s="158"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
+      <c r="E77" s="158"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -30216,8 +30380,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30226,43 +30390,44 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A30:A38"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
+  <mergeCells count="31">
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E2:E77"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B30:B38"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A25"/>
     <mergeCell ref="B16:B25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30271,21 +30436,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:A67"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" customWidth="1"/>
-    <col min="4" max="4" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30298,28 +30464,35 @@
       <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="6" t="s">
+        <v>283</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
+      <c r="E2" s="131">
+        <v>43179</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
+      <c r="E3" s="131"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="145" t="s">
+    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="152" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30328,140 +30501,160 @@
       <c r="D4" s="49" t="s">
         <v>196</v>
       </c>
+      <c r="E4" s="131"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="145"/>
-      <c r="B5" s="144"/>
-      <c r="C5" s="154" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="152"/>
+      <c r="B5" s="153"/>
+      <c r="C5" s="181" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="153" t="s">
+      <c r="D5" s="180" t="s">
         <v>202</v>
       </c>
+      <c r="E5" s="131"/>
     </row>
-    <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="145"/>
-      <c r="B6" s="144"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="153"/>
+    <row r="6" spans="1:5" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="152"/>
+      <c r="B6" s="153"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="180"/>
+      <c r="E6" s="131"/>
     </row>
-    <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="145"/>
-      <c r="B7" s="144"/>
+    <row r="7" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="152"/>
+      <c r="B7" s="153"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
+      <c r="E7" s="131"/>
     </row>
-    <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="145"/>
-      <c r="B8" s="144"/>
+    <row r="8" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="152"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
+      <c r="E8" s="131"/>
     </row>
-    <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="145"/>
-      <c r="B9" s="144"/>
+    <row r="9" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="152"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
+      <c r="E9" s="131"/>
     </row>
-    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="147" t="s">
+    <row r="10" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="155" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="156"/>
-      <c r="D10" s="153" t="s">
+      <c r="C10" s="172"/>
+      <c r="D10" s="180" t="s">
         <v>186</v>
       </c>
+      <c r="E10" s="131"/>
     </row>
-    <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="147"/>
-      <c r="B11" s="144"/>
-      <c r="C11" s="156"/>
-      <c r="D11" s="153"/>
+    <row r="11" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="155"/>
+      <c r="B11" s="153"/>
+      <c r="C11" s="172"/>
+      <c r="D11" s="180"/>
+      <c r="E11" s="131"/>
     </row>
-    <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="147"/>
-      <c r="B12" s="144"/>
-      <c r="C12" s="156"/>
-      <c r="D12" s="153"/>
+    <row r="12" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="155"/>
+      <c r="B12" s="153"/>
+      <c r="C12" s="172"/>
+      <c r="D12" s="180"/>
+      <c r="E12" s="131"/>
     </row>
-    <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="148" t="s">
+    <row r="13" spans="1:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="153" t="s">
+      <c r="C13" s="182"/>
+      <c r="D13" s="180" t="s">
         <v>203</v>
       </c>
+      <c r="E13" s="131"/>
     </row>
-    <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="148"/>
-      <c r="B14" s="139"/>
-      <c r="C14" s="155"/>
-      <c r="D14" s="153"/>
+    <row r="14" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="150"/>
+      <c r="B14" s="156"/>
+      <c r="C14" s="182"/>
+      <c r="D14" s="180"/>
+      <c r="E14" s="131"/>
     </row>
-    <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="148"/>
-      <c r="B15" s="139"/>
-      <c r="C15" s="155"/>
+    <row r="15" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="150"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="182"/>
       <c r="D15" s="49"/>
+      <c r="E15" s="131"/>
     </row>
-    <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="148"/>
-      <c r="B16" s="139"/>
-      <c r="C16" s="155"/>
+    <row r="16" spans="1:5" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="150"/>
+      <c r="B16" s="156"/>
+      <c r="C16" s="182"/>
       <c r="D16" s="49"/>
+      <c r="E16" s="131"/>
     </row>
-    <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="148"/>
-      <c r="B17" s="139"/>
-      <c r="C17" s="155"/>
+    <row r="17" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="150"/>
+      <c r="B17" s="156"/>
+      <c r="C17" s="182"/>
       <c r="D17" s="49"/>
+      <c r="E17" s="131"/>
     </row>
-    <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="148"/>
-      <c r="B18" s="139"/>
-      <c r="C18" s="155"/>
+    <row r="18" spans="1:5" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="150"/>
+      <c r="B18" s="156"/>
+      <c r="C18" s="182"/>
       <c r="D18" s="49"/>
+      <c r="E18" s="131"/>
     </row>
-    <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="148"/>
-      <c r="B19" s="139"/>
-      <c r="C19" s="155"/>
+    <row r="19" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="150"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="182"/>
       <c r="D19" s="49"/>
+      <c r="E19" s="131"/>
     </row>
-    <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="148"/>
-      <c r="B20" s="139"/>
-      <c r="C20" s="155"/>
+    <row r="20" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="150"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="182"/>
       <c r="D20" s="49"/>
+      <c r="E20" s="131"/>
     </row>
-    <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="148"/>
-      <c r="B21" s="139"/>
-      <c r="C21" s="155"/>
+    <row r="21" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="150"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="182"/>
       <c r="D21" s="49"/>
+      <c r="E21" s="131"/>
     </row>
-    <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="148"/>
-      <c r="B22" s="139"/>
-      <c r="C22" s="155"/>
+    <row r="22" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="150"/>
+      <c r="B22" s="156"/>
+      <c r="C22" s="182"/>
       <c r="D22" s="49"/>
+      <c r="E22" s="131"/>
     </row>
-    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="148"/>
-      <c r="B23" s="139"/>
-      <c r="C23" s="155"/>
+    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="150"/>
+      <c r="B23" s="156"/>
+      <c r="C23" s="182"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
+      <c r="E23" s="131"/>
     </row>
-    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="73" t="s">
         <v>187</v>
       </c>
@@ -30474,8 +30667,9 @@
       <c r="D24" s="77" t="s">
         <v>188</v>
       </c>
+      <c r="E24" s="131"/>
     </row>
-    <row r="25" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30488,8 +30682,9 @@
       <c r="D25" s="67" t="s">
         <v>233</v>
       </c>
+      <c r="E25" s="131"/>
     </row>
-    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30500,16 +30695,18 @@
       <c r="D26" s="73" t="s">
         <v>166</v>
       </c>
+      <c r="E26" s="131"/>
     </row>
-    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
+      <c r="E27" s="131"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30522,8 +30719,9 @@
       <c r="D28" s="58" t="s">
         <v>227</v>
       </c>
+      <c r="E28" s="131"/>
     </row>
-    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="85"/>
       <c r="B29" s="84"/>
       <c r="C29" s="70" t="s">
@@ -30532,8 +30730,9 @@
       <c r="D29" s="68" t="s">
         <v>204</v>
       </c>
+      <c r="E29" s="131"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30542,8 +30741,9 @@
       <c r="D30" s="86" t="s">
         <v>201</v>
       </c>
+      <c r="E30" s="131"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30552,12 +30752,13 @@
       <c r="D31" s="86" t="s">
         <v>225</v>
       </c>
+      <c r="E31" s="131"/>
     </row>
-    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="164" t="s">
+    <row r="32" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="166" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="167" t="s">
+      <c r="B32" s="169" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30566,36 +30767,41 @@
       <c r="D32" s="87" t="s">
         <v>229</v>
       </c>
+      <c r="E32" s="131"/>
     </row>
-    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="165"/>
-      <c r="B33" s="168"/>
+    <row r="33" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="167"/>
+      <c r="B33" s="170"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
+      <c r="E33" s="131"/>
     </row>
-    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="165"/>
-      <c r="B34" s="168"/>
+    <row r="34" spans="1:5" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="167"/>
+      <c r="B34" s="170"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
+      <c r="E34" s="131"/>
     </row>
-    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="165"/>
-      <c r="B35" s="168"/>
+    <row r="35" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="167"/>
+      <c r="B35" s="170"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
+      <c r="E35" s="131"/>
     </row>
-    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="166"/>
-      <c r="B36" s="169"/>
+    <row r="36" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="168"/>
+      <c r="B36" s="171"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
       <c r="D36" s="75" t="s">
         <v>224</v>
       </c>
+      <c r="E36" s="131"/>
     </row>
-    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
         <v>27</v>
       </c>
@@ -30606,20 +30812,22 @@
       <c r="D37" s="50" t="s">
         <v>79</v>
       </c>
+      <c r="E37" s="131"/>
     </row>
-    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
+      <c r="E38" s="131"/>
     </row>
-    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="146" t="s">
+    <row r="39" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="144" t="s">
+      <c r="B39" s="153" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30628,106 +30836,119 @@
       <c r="D39" s="81" t="s">
         <v>193</v>
       </c>
+      <c r="E39" s="131"/>
     </row>
-    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="146"/>
-      <c r="B40" s="144"/>
+    <row r="40" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="154"/>
+      <c r="B40" s="153"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
       <c r="D40" s="52" t="s">
         <v>188</v>
       </c>
+      <c r="E40" s="131"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="145" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="152" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="144" t="s">
+      <c r="B41" s="153" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="156" t="s">
+      <c r="C41" s="172" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="148" t="s">
+      <c r="D41" s="150" t="s">
         <v>228</v>
       </c>
+      <c r="E41" s="131"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="145"/>
-      <c r="B42" s="144"/>
-      <c r="C42" s="156"/>
-      <c r="D42" s="148"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="152"/>
+      <c r="B42" s="153"/>
+      <c r="C42" s="172"/>
+      <c r="D42" s="150"/>
+      <c r="E42" s="131"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="145"/>
-      <c r="B43" s="144"/>
-      <c r="C43" s="156" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="152"/>
+      <c r="B43" s="153"/>
+      <c r="C43" s="172" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="140" t="s">
+      <c r="D43" s="162" t="s">
         <v>188</v>
       </c>
+      <c r="E43" s="131"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="145"/>
-      <c r="B44" s="144"/>
-      <c r="C44" s="156"/>
-      <c r="D44" s="140"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="152"/>
+      <c r="B44" s="153"/>
+      <c r="C44" s="172"/>
+      <c r="D44" s="162"/>
+      <c r="E44" s="131"/>
     </row>
-    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="138" t="s">
+    <row r="45" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="139" t="s">
+      <c r="B45" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="160"/>
+      <c r="C45" s="176"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
+      <c r="E45" s="131"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="138"/>
-      <c r="B46" s="139"/>
-      <c r="C46" s="161"/>
-      <c r="D46" s="157" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="161"/>
+      <c r="B46" s="156"/>
+      <c r="C46" s="177"/>
+      <c r="D46" s="173" t="s">
         <v>200</v>
       </c>
+      <c r="E46" s="131"/>
     </row>
-    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="138"/>
-      <c r="B47" s="139"/>
-      <c r="C47" s="161"/>
-      <c r="D47" s="158"/>
+    <row r="47" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="161"/>
+      <c r="B47" s="156"/>
+      <c r="C47" s="177"/>
+      <c r="D47" s="174"/>
+      <c r="E47" s="131"/>
     </row>
-    <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="138"/>
-      <c r="B48" s="139"/>
-      <c r="C48" s="162"/>
-      <c r="D48" s="158"/>
+    <row r="48" spans="1:5" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="161"/>
+      <c r="B48" s="156"/>
+      <c r="C48" s="178"/>
+      <c r="D48" s="174"/>
+      <c r="E48" s="131"/>
     </row>
-    <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="138"/>
-      <c r="B49" s="139"/>
-      <c r="C49" s="136"/>
-      <c r="D49" s="158"/>
+    <row r="49" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="161"/>
+      <c r="B49" s="156"/>
+      <c r="C49" s="160"/>
+      <c r="D49" s="174"/>
+      <c r="E49" s="131"/>
     </row>
-    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="138"/>
-      <c r="B50" s="139"/>
-      <c r="C50" s="136"/>
-      <c r="D50" s="159"/>
+    <row r="50" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="161"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="160"/>
+      <c r="D50" s="175"/>
+      <c r="E50" s="131"/>
     </row>
-    <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
+      <c r="E51" s="131"/>
     </row>
-    <row r="52" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
         <v>83</v>
       </c>
@@ -30738,12 +30959,13 @@
       <c r="D52" s="49" t="s">
         <v>110</v>
       </c>
+      <c r="E52" s="131"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="139" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="139" t="s">
+      <c r="B53" s="156" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30752,181 +30974,223 @@
       <c r="D53" s="47" t="s">
         <v>198</v>
       </c>
+      <c r="E53" s="131"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="139"/>
-      <c r="B54" s="139"/>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="156"/>
+      <c r="B54" s="156"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
       <c r="D54" s="47" t="s">
         <v>188</v>
       </c>
+      <c r="E54" s="131"/>
     </row>
-    <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="139"/>
-      <c r="B55" s="139"/>
+    <row r="55" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="156"/>
+      <c r="B55" s="156"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
       <c r="D55" s="80" t="s">
         <v>212</v>
       </c>
+      <c r="E55" s="131"/>
     </row>
-    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="139"/>
-      <c r="B56" s="139"/>
-      <c r="C56" s="163" t="s">
+    <row r="56" spans="1:5" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="156"/>
+      <c r="B56" s="156"/>
+      <c r="C56" s="179" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
+      <c r="E56" s="131"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="139"/>
-      <c r="B57" s="139"/>
-      <c r="C57" s="163"/>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="156"/>
+      <c r="B57" s="156"/>
+      <c r="C57" s="179"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
+      <c r="E57" s="131"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="139"/>
-      <c r="B58" s="139"/>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="156"/>
+      <c r="B58" s="156"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
       <c r="D58" s="46" t="s">
         <v>214</v>
       </c>
+      <c r="E58" s="131"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="139"/>
-      <c r="B59" s="139"/>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="156"/>
+      <c r="B59" s="156"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
       <c r="D59" s="79" t="s">
         <v>215</v>
       </c>
+      <c r="E59" s="131"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="139"/>
-      <c r="B60" s="139"/>
-      <c r="C60" s="163" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="156"/>
+      <c r="B60" s="156"/>
+      <c r="C60" s="179" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
+      <c r="E60" s="131"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="139"/>
-      <c r="B61" s="139"/>
-      <c r="C61" s="163"/>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="156"/>
+      <c r="B61" s="156"/>
+      <c r="C61" s="179"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
+      <c r="E61" s="131"/>
     </row>
-    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="139"/>
-      <c r="B62" s="139"/>
-      <c r="C62" s="163"/>
+    <row r="62" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="156"/>
+      <c r="B62" s="156"/>
+      <c r="C62" s="179"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
+      <c r="E62" s="131"/>
     </row>
-    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="139"/>
-      <c r="B63" s="139"/>
-      <c r="C63" s="156" t="s">
+    <row r="63" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="156"/>
+      <c r="B63" s="156"/>
+      <c r="C63" s="172" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
+      <c r="E63" s="131"/>
     </row>
-    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="139"/>
-      <c r="B64" s="139"/>
-      <c r="C64" s="156"/>
-      <c r="D64" s="140" t="s">
+    <row r="64" spans="1:5" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="156"/>
+      <c r="B64" s="156"/>
+      <c r="C64" s="172"/>
+      <c r="D64" s="162" t="s">
         <v>220</v>
       </c>
+      <c r="E64" s="131"/>
     </row>
-    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="139"/>
-      <c r="B65" s="139"/>
-      <c r="C65" s="156"/>
-      <c r="D65" s="140"/>
+    <row r="65" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="156"/>
+      <c r="B65" s="156"/>
+      <c r="C65" s="172"/>
+      <c r="D65" s="162"/>
+      <c r="E65" s="131"/>
     </row>
-    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="139"/>
-      <c r="B66" s="139"/>
-      <c r="C66" s="156"/>
-      <c r="D66" s="140"/>
+    <row r="66" spans="1:5" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="156"/>
+      <c r="B66" s="156"/>
+      <c r="C66" s="172"/>
+      <c r="D66" s="162"/>
+      <c r="E66" s="131"/>
     </row>
-    <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="139"/>
-      <c r="B67" s="139"/>
-      <c r="C67" s="156"/>
-      <c r="D67" s="140"/>
+    <row r="67" spans="1:5" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="156"/>
+      <c r="B67" s="156"/>
+      <c r="C67" s="172"/>
+      <c r="D67" s="162"/>
+      <c r="E67" s="131"/>
     </row>
-    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
+      <c r="E68" s="131"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="E2:E68"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C63:C67"/>
+    <mergeCell ref="A53:A67"/>
+    <mergeCell ref="B53:B67"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C56:C57"/>
     <mergeCell ref="A32:A36"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="A4:A9"/>
@@ -30935,31 +31199,6 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="A13:A23"/>
     <mergeCell ref="B13:B23"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A53:A67"/>
-    <mergeCell ref="B53:B67"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D46:D50"/>
-    <mergeCell ref="C45:C48"/>
-    <mergeCell ref="A45:A50"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30968,21 +31207,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:A40"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30992,129 +31232,164 @@
       <c r="C1" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="116" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="57" t="s">
+        <v>283</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
-      <c r="D2" s="44"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="58"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="148" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="163" t="s">
+      <c r="B3" s="179" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="58"/>
-      <c r="D3" t="s">
+      <c r="D3" s="118" t="s">
         <v>257</v>
       </c>
+      <c r="E3" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="148"/>
-      <c r="B4" s="163"/>
-      <c r="C4" s="104" t="s">
+    <row r="4" spans="1:5" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="150"/>
+      <c r="B4" s="179"/>
+      <c r="C4" s="101" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="119" t="s">
         <v>256</v>
       </c>
+      <c r="E4" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="163"/>
-      <c r="C5" s="104" t="s">
+      <c r="B5" s="179"/>
+      <c r="C5" s="101" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="120" t="s">
         <v>236</v>
       </c>
+      <c r="E5" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="163"/>
-      <c r="C6" s="104" t="s">
+      <c r="B6" s="179"/>
+      <c r="C6" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="107" t="s">
+      <c r="D6" s="120" t="s">
         <v>30</v>
       </c>
+      <c r="E6" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="179" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="190" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="163"/>
+      <c r="B7" s="179"/>
       <c r="C7" s="58"/>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="121" t="s">
         <v>261</v>
       </c>
+      <c r="E7" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="180"/>
-      <c r="B8" s="163"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="191"/>
+      <c r="B8" s="179"/>
       <c r="C8" s="58"/>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="118" t="s">
         <v>276</v>
       </c>
+      <c r="E8" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="163"/>
+      <c r="B9" s="179"/>
       <c r="C9" s="58"/>
-      <c r="D9" s="107" t="s">
+      <c r="D9" s="120" t="s">
         <v>259</v>
       </c>
+      <c r="E9" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="58"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="181" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="187" t="s">
         <v>237</v>
       </c>
-      <c r="B11" s="163" t="s">
+      <c r="B11" s="179" t="s">
         <v>234</v>
       </c>
       <c r="C11" s="58"/>
       <c r="D11" t="s">
         <v>258</v>
       </c>
+      <c r="E11" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="182"/>
-      <c r="B12" s="163"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="188"/>
+      <c r="B12" s="179"/>
       <c r="C12" s="58"/>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="118" t="s">
         <v>252</v>
       </c>
+      <c r="E12" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="183"/>
-      <c r="B13" s="163"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="189"/>
+      <c r="B13" s="179"/>
       <c r="C13" s="58"/>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="118" t="s">
         <v>254</v>
       </c>
+      <c r="E13" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="96" t="s">
         <v>27</v>
       </c>
@@ -31122,358 +31397,491 @@
         <v>234</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="118" t="s">
         <v>238</v>
       </c>
+      <c r="E14" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="163" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="179" t="s">
         <v>222</v>
       </c>
-      <c r="B15" s="163" t="s">
+      <c r="B15" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="170" t="s">
+      <c r="C15" s="198" t="s">
         <v>239</v>
       </c>
-      <c r="D15" s="99" t="s">
+      <c r="D15" s="123" t="s">
         <v>241</v>
       </c>
+      <c r="E15" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="163"/>
-      <c r="B16" s="163"/>
-      <c r="C16" s="171"/>
-      <c r="D16" s="119" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="179"/>
+      <c r="B16" s="179"/>
+      <c r="C16" s="199"/>
+      <c r="D16" s="113" t="s">
         <v>278</v>
       </c>
+      <c r="E16" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="163"/>
-      <c r="B17" s="163"/>
-      <c r="C17" s="101" t="s">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="179"/>
+      <c r="B17" s="179"/>
+      <c r="C17" s="99" t="s">
         <v>240</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="124" t="s">
         <v>242</v>
       </c>
+      <c r="E17" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="116" t="s">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="110" t="s">
         <v>280</v>
       </c>
       <c r="B18" s="58"/>
       <c r="C18" s="61" t="s">
         <v>282</v>
       </c>
-      <c r="D18" s="58" t="s">
+      <c r="D18" s="118" t="s">
         <v>281</v>
       </c>
+      <c r="E18" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
-      <c r="D19" s="44"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="58"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="179" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="190" t="s">
         <v>260</v>
       </c>
-      <c r="B20" s="163" t="s">
+      <c r="B20" s="179" t="s">
         <v>234</v>
       </c>
       <c r="C20" s="58"/>
-      <c r="D20" s="79" t="s">
+      <c r="D20" s="121" t="s">
         <v>261</v>
       </c>
+      <c r="E20" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="180"/>
-      <c r="B21" s="163"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="191"/>
+      <c r="B21" s="179"/>
       <c r="C21" s="58"/>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="118" t="s">
         <v>257</v>
       </c>
+      <c r="E21" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="105" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="102" t="s">
         <v>243</v>
       </c>
       <c r="B22" s="95" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="98" t="s">
+      <c r="C22" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="97" t="s">
+      <c r="D22" s="125" t="s">
         <v>30</v>
       </c>
+      <c r="E22" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="173" t="s">
+    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="192" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="176" t="s">
+      <c r="B23" s="185" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="118" t="s">
         <v>251</v>
       </c>
+      <c r="E23" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="174"/>
-      <c r="B24" s="177"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="193"/>
+      <c r="B24" s="195"/>
       <c r="C24" t="s">
         <v>270</v>
       </c>
-      <c r="D24" s="58" t="s">
+      <c r="D24" s="118" t="s">
         <v>251</v>
       </c>
+      <c r="E24" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="174"/>
-      <c r="B25" s="177"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="193"/>
+      <c r="B25" s="195"/>
       <c r="C25" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="D25" s="58" t="s">
+      <c r="D25" s="118" t="s">
         <v>251</v>
       </c>
+      <c r="E25" s="128">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="174"/>
-      <c r="B26" s="177"/>
-      <c r="C26" s="118" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="193"/>
+      <c r="B26" s="195"/>
+      <c r="C26" s="112" t="s">
         <v>277</v>
       </c>
-      <c r="D26" s="118" t="s">
+      <c r="D26" s="113" t="s">
         <v>102</v>
       </c>
+      <c r="E26" s="130">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="175"/>
-      <c r="B27" s="178"/>
-      <c r="C27" s="100" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="193"/>
+      <c r="B27" s="195"/>
+      <c r="C27" s="58" t="s">
+        <v>284</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="E27" s="127">
+        <v>43279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="193"/>
+      <c r="B28" s="195"/>
+      <c r="C28" s="58" t="s">
+        <v>285</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>286</v>
+      </c>
+      <c r="E28" s="127">
+        <v>43279</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="194"/>
+      <c r="B29" s="186"/>
+      <c r="C29" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="D27" s="112" t="s">
+      <c r="D29" s="125" t="s">
         <v>245</v>
       </c>
+      <c r="E29" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="28" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="39" t="s">
+    <row r="30" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="44"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="117"/>
+      <c r="E30" s="58"/>
     </row>
-    <row r="29" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="115"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="79" t="s">
+    <row r="31" spans="1:5" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="109"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="121" t="s">
         <v>261</v>
       </c>
+      <c r="E31" s="58"/>
     </row>
-    <row r="30" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="148" t="s">
+    <row r="32" spans="1:5" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="163" t="s">
+      <c r="B32" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C30" s="113" t="s">
+      <c r="C32" s="107" t="s">
         <v>246</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D32" s="118" t="s">
         <v>253</v>
       </c>
+      <c r="E32" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="148"/>
-      <c r="B31" s="163"/>
-      <c r="C31" s="113">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="150"/>
+      <c r="B33" s="179"/>
+      <c r="C33" s="107">
         <v>10.1</v>
       </c>
-      <c r="D31" s="58" t="s">
+      <c r="D33" s="118" t="s">
         <v>272</v>
       </c>
+      <c r="E33" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="148"/>
-      <c r="B32" s="163"/>
-      <c r="C32" s="113">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="150"/>
+      <c r="B34" s="179"/>
+      <c r="C34" s="107">
         <v>10.199999999999999</v>
       </c>
-      <c r="D32" s="58" t="s">
+      <c r="D34" s="118" t="s">
         <v>272</v>
       </c>
+      <c r="E34" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="148" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="150" t="s">
         <v>247</v>
       </c>
-      <c r="B33" s="163" t="s">
+      <c r="B35" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C33" s="163"/>
-      <c r="D33" s="172" t="s">
+      <c r="C35" s="179"/>
+      <c r="D35" s="200" t="s">
         <v>261</v>
       </c>
+      <c r="E35" s="196">
+        <v>43270</v>
+      </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="148"/>
-      <c r="B34" s="163"/>
-      <c r="C34" s="163"/>
-      <c r="D34" s="172"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="150"/>
+      <c r="B36" s="179"/>
+      <c r="C36" s="179"/>
+      <c r="D36" s="200"/>
+      <c r="E36" s="197"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="112" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="106" t="s">
         <v>262</v>
       </c>
-      <c r="B35" s="113" t="s">
+      <c r="B37" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="C35" s="113" t="s">
+      <c r="C37" s="107" t="s">
         <v>250</v>
       </c>
-      <c r="D35" s="103" t="s">
+      <c r="D37" s="126" t="s">
         <v>251</v>
       </c>
+      <c r="E37" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="36" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="102" t="s">
+    <row r="38" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="100" t="s">
         <v>248</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="110"/>
-      <c r="D36" s="111"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="115"/>
+      <c r="E38" s="58"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="58" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="B37" s="113" t="s">
+      <c r="B39" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="109" t="s">
+      <c r="C39" s="104" t="s">
         <v>265</v>
       </c>
-      <c r="D37" s="58" t="s">
+      <c r="D39" s="118" t="s">
         <v>267</v>
       </c>
+      <c r="E39" s="127">
+        <v>43244</v>
+      </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="114" t="s">
+    <row r="40" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="58" t="s">
+        <v>287</v>
+      </c>
+      <c r="B40" s="129" t="s">
+        <v>234</v>
+      </c>
+      <c r="C40" s="104" t="s">
+        <v>288</v>
+      </c>
+      <c r="D40" s="118" t="s">
+        <v>289</v>
+      </c>
+      <c r="E40" s="127">
+        <v>43280</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="114"/>
-      <c r="C38" s="114"/>
-      <c r="D38" s="114"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="108"/>
+      <c r="D41" s="114"/>
+      <c r="E41" s="58"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="184" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="176" t="s">
+      <c r="B42" s="185" t="s">
         <v>271</v>
       </c>
-      <c r="C39" s="109" t="s">
+      <c r="C42" s="104" t="s">
         <v>265</v>
       </c>
-      <c r="D39" s="58" t="s">
+      <c r="D42" s="118" t="s">
         <v>267</v>
       </c>
+      <c r="E42" s="127">
+        <v>43259</v>
+      </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="185"/>
-      <c r="B40" s="178"/>
-      <c r="C40" s="109" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="184"/>
+      <c r="B43" s="186"/>
+      <c r="C43" s="104" t="s">
         <v>265</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D43" s="118" t="s">
         <v>266</v>
       </c>
+      <c r="E43" s="127">
+        <v>43259</v>
+      </c>
     </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="108" t="s">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="113" t="s">
+      <c r="B44" s="107" t="s">
         <v>271</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="C44" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D41" s="58" t="s">
+      <c r="D44" s="118" t="s">
         <v>100</v>
       </c>
+      <c r="E44" s="127">
+        <v>43259</v>
+      </c>
     </row>
-    <row r="42" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="108" t="s">
+    <row r="45" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="113" t="s">
+      <c r="B45" s="107" t="s">
         <v>271</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C45" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D42" s="58" t="s">
+      <c r="D45" s="118" t="s">
         <v>263</v>
       </c>
+      <c r="E45" s="127">
+        <v>43259</v>
+      </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="114" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="108" t="s">
         <v>273</v>
       </c>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114"/>
+      <c r="B46" s="108"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="114"/>
+      <c r="E46" s="58"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="58"/>
-      <c r="B44" s="113" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="58"/>
+      <c r="B47" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C47" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="103" t="s">
+      <c r="D47" s="126" t="s">
         <v>274</v>
       </c>
+      <c r="E47" s="127">
+        <v>43265</v>
+      </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="114" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="108" t="s">
         <v>279</v>
       </c>
-      <c r="B45" s="114"/>
-      <c r="C45" s="114"/>
-      <c r="D45" s="114"/>
+      <c r="B48" s="108"/>
+      <c r="C48" s="108"/>
+      <c r="D48" s="114"/>
+      <c r="E48" s="58"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="58"/>
-      <c r="B46" s="117" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="58"/>
+      <c r="B49" s="111" t="s">
         <v>234</v>
       </c>
-      <c r="C46" s="58" t="s">
+      <c r="C49" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="103" t="s">
+      <c r="D49" s="126" t="s">
         <v>274</v>
+      </c>
+      <c r="E49" s="128">
+        <v>43270</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
+  <mergeCells count="21">
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="A11:A13"/>
@@ -31481,17 +31889,11 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="B23:B29"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"New columns in Validation Rule, Error Message Guide and Employment ID Document"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="316">
   <si>
     <t>Document</t>
   </si>
@@ -2732,6 +2732,33 @@
   <si>
     <t>Added Returns Reconciliations endpoints</t>
   </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>Link changed to point to new Error Structure Document</t>
+  </si>
+  <si>
+    <t>Error Structure Guide</t>
+  </si>
+  <si>
+    <t>Employment ID Guide</t>
+  </si>
+  <si>
+    <t>Error Response and Error Response Message</t>
+  </si>
+  <si>
+    <t>code 3012</t>
+  </si>
+  <si>
+    <t>REST HTTP Codes</t>
+  </si>
+  <si>
+    <t>4XX's corrected to 200's</t>
+  </si>
+  <si>
+    <t>code 2040</t>
+  </si>
 </sst>
 </file>
 
@@ -2877,7 +2904,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -3324,28 +3351,17 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -3353,7 +3369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3612,7 +3628,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3620,7 +3635,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3650,9 +3664,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3664,6 +3675,25 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3845,18 +3875,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3874,22 +3892,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4301,12 +4310,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="124"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="130"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4329,12 +4338,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="122" t="s">
+      <c r="A4" s="128" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="124"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="130"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4374,10 +4383,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="128">
+      <c r="B7" s="134">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4391,8 +4400,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="126"/>
-      <c r="B8" s="129"/>
+      <c r="A8" s="132"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4404,8 +4413,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="126"/>
-      <c r="B9" s="129"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4417,8 +4426,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="126"/>
-      <c r="B10" s="129"/>
+      <c r="A10" s="132"/>
+      <c r="B10" s="135"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4430,8 +4439,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="126"/>
-      <c r="B11" s="129"/>
+      <c r="A11" s="132"/>
+      <c r="B11" s="135"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4443,8 +4452,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="127"/>
-      <c r="B12" s="130"/>
+      <c r="A12" s="133"/>
+      <c r="B12" s="136"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4456,10 +4465,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="133" t="s">
+      <c r="A13" s="139" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="128">
+      <c r="B13" s="134">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4473,8 +4482,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="134"/>
-      <c r="B14" s="130"/>
+      <c r="A14" s="140"/>
+      <c r="B14" s="136"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4520,12 +4529,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="122" t="s">
+      <c r="A17" s="128" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="123"/>
-      <c r="C17" s="123"/>
-      <c r="D17" s="124"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="130"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4565,21 +4574,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="122" t="s">
+      <c r="A20" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="123"/>
-      <c r="C20" s="123"/>
-      <c r="D20" s="124"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="130"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="135" t="s">
+      <c r="A21" s="141" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="132">
+      <c r="B21" s="138">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4593,8 +4602,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="136"/>
-      <c r="B22" s="130"/>
+      <c r="A22" s="142"/>
+      <c r="B22" s="136"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4617,18 +4626,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="122" t="s">
+      <c r="A24" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="124"/>
+      <c r="B24" s="129"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="130"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="131" t="s">
+      <c r="A25" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="132">
+      <c r="B25" s="138">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4642,8 +4651,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="126"/>
-      <c r="B26" s="129"/>
+      <c r="A26" s="132"/>
+      <c r="B26" s="135"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4655,8 +4664,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="126"/>
-      <c r="B27" s="129"/>
+      <c r="A27" s="132"/>
+      <c r="B27" s="135"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4668,8 +4677,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="126"/>
-      <c r="B28" s="129"/>
+      <c r="A28" s="132"/>
+      <c r="B28" s="135"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4681,8 +4690,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="126"/>
-      <c r="B29" s="129"/>
+      <c r="A29" s="132"/>
+      <c r="B29" s="135"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4694,8 +4703,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="126"/>
-      <c r="B30" s="129"/>
+      <c r="A30" s="132"/>
+      <c r="B30" s="135"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4707,8 +4716,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="126"/>
-      <c r="B31" s="129"/>
+      <c r="A31" s="132"/>
+      <c r="B31" s="135"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4720,8 +4729,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="127"/>
-      <c r="B32" s="130"/>
+      <c r="A32" s="133"/>
+      <c r="B32" s="136"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4845,12 +4854,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="122" t="s">
+      <c r="A41" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="123"/>
-      <c r="C41" s="123"/>
-      <c r="D41" s="124"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="130"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -5030,10 +5039,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="152" t="s">
+      <c r="A7" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="151" t="s">
+      <c r="B7" s="157" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5044,8 +5053,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="152"/>
-      <c r="B8" s="151"/>
+      <c r="A8" s="158"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5054,8 +5063,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="152"/>
-      <c r="B9" s="151"/>
+      <c r="A9" s="158"/>
+      <c r="B9" s="157"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5064,8 +5073,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="152"/>
-      <c r="B10" s="151"/>
+      <c r="A10" s="158"/>
+      <c r="B10" s="157"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5074,8 +5083,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="152"/>
-      <c r="B11" s="151"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="157"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5084,8 +5093,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="152"/>
-      <c r="B12" s="151"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="157"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5094,10 +5103,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="160" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="151" t="s">
+      <c r="B13" s="157" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5108,8 +5117,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="154"/>
-      <c r="B14" s="151"/>
+      <c r="A14" s="160"/>
+      <c r="B14" s="157"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5118,8 +5127,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="154"/>
-      <c r="B15" s="151"/>
+      <c r="A15" s="160"/>
+      <c r="B15" s="157"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5128,10 +5137,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="137" t="s">
+      <c r="A16" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5142,8 +5151,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="137"/>
-      <c r="B17" s="146"/>
+      <c r="A17" s="143"/>
+      <c r="B17" s="152"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5152,8 +5161,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="137"/>
-      <c r="B18" s="146"/>
+      <c r="A18" s="143"/>
+      <c r="B18" s="152"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5162,8 +5171,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="137"/>
-      <c r="B19" s="146"/>
+      <c r="A19" s="143"/>
+      <c r="B19" s="152"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5172,8 +5181,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="137"/>
-      <c r="B20" s="146"/>
+      <c r="A20" s="143"/>
+      <c r="B20" s="152"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5182,8 +5191,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="137"/>
-      <c r="B21" s="146"/>
+      <c r="A21" s="143"/>
+      <c r="B21" s="152"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5192,8 +5201,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="137"/>
-      <c r="B22" s="146"/>
+      <c r="A22" s="143"/>
+      <c r="B22" s="152"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5202,8 +5211,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="137"/>
-      <c r="B23" s="146"/>
+      <c r="A23" s="143"/>
+      <c r="B23" s="152"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5212,26 +5221,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="137"/>
-      <c r="B24" s="146"/>
-      <c r="C24" s="137" t="s">
+      <c r="A24" s="143"/>
+      <c r="B24" s="152"/>
+      <c r="C24" s="143" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="138" t="s">
+      <c r="D24" s="144" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="137"/>
-      <c r="B25" s="146"/>
-      <c r="C25" s="137"/>
-      <c r="D25" s="138"/>
+      <c r="A25" s="143"/>
+      <c r="B25" s="152"/>
+      <c r="C25" s="143"/>
+      <c r="D25" s="144"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="152" t="s">
+      <c r="A26" s="158" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="151" t="s">
+      <c r="B26" s="157" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5242,8 +5251,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="152"/>
-      <c r="B27" s="151"/>
+      <c r="A27" s="158"/>
+      <c r="B27" s="157"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5270,28 +5279,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="153" t="s">
+      <c r="A30" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="151" t="s">
+      <c r="B30" s="157" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="137" t="s">
+      <c r="C30" s="143" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="141" t="s">
+      <c r="D30" s="147" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="153"/>
-      <c r="B31" s="151"/>
-      <c r="C31" s="137"/>
-      <c r="D31" s="141"/>
+      <c r="A31" s="159"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="143"/>
+      <c r="D31" s="147"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="153"/>
-      <c r="B32" s="151"/>
+      <c r="A32" s="159"/>
+      <c r="B32" s="157"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5300,8 +5309,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="153"/>
-      <c r="B33" s="151"/>
+      <c r="A33" s="159"/>
+      <c r="B33" s="157"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5310,8 +5319,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="153"/>
-      <c r="B34" s="151"/>
+      <c r="A34" s="159"/>
+      <c r="B34" s="157"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5320,8 +5329,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="153"/>
-      <c r="B35" s="151"/>
+      <c r="A35" s="159"/>
+      <c r="B35" s="157"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5330,8 +5339,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="153"/>
-      <c r="B36" s="151"/>
+      <c r="A36" s="159"/>
+      <c r="B36" s="157"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5340,26 +5349,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="153"/>
-      <c r="B37" s="151"/>
-      <c r="C37" s="142" t="s">
+      <c r="A37" s="159"/>
+      <c r="B37" s="157"/>
+      <c r="C37" s="148" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="144" t="s">
+      <c r="D37" s="150" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="153"/>
-      <c r="B38" s="151"/>
-      <c r="C38" s="143"/>
-      <c r="D38" s="144"/>
+      <c r="A38" s="159"/>
+      <c r="B38" s="157"/>
+      <c r="C38" s="149"/>
+      <c r="D38" s="150"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="152" t="s">
+      <c r="A39" s="158" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="151" t="s">
+      <c r="B39" s="157" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5370,8 +5379,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="152"/>
-      <c r="B40" s="151"/>
+      <c r="A40" s="158"/>
+      <c r="B40" s="157"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5398,10 +5407,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="153" t="s">
+      <c r="A43" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="151" t="s">
+      <c r="B43" s="157" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5410,8 +5419,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="153"/>
-      <c r="B44" s="151"/>
+      <c r="A44" s="159"/>
+      <c r="B44" s="157"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5420,10 +5429,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="148" t="s">
+      <c r="A45" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="151" t="s">
+      <c r="B45" s="157" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5432,8 +5441,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="149"/>
-      <c r="B46" s="151"/>
+      <c r="A46" s="155"/>
+      <c r="B46" s="157"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5442,8 +5451,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="149"/>
-      <c r="B47" s="151"/>
+      <c r="A47" s="155"/>
+      <c r="B47" s="157"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5452,8 +5461,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="150"/>
-      <c r="B48" s="151"/>
+      <c r="A48" s="156"/>
+      <c r="B48" s="157"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5462,10 +5471,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="146" t="s">
+      <c r="A49" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="146" t="s">
+      <c r="B49" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9569,8 +9578,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="146"/>
-      <c r="B50" s="146"/>
+      <c r="A50" s="152"/>
+      <c r="B50" s="152"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13674,8 +13683,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="146"/>
-      <c r="B51" s="146"/>
+      <c r="A51" s="152"/>
+      <c r="B51" s="152"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17779,8 +17788,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="146"/>
-      <c r="B52" s="146"/>
+      <c r="A52" s="152"/>
+      <c r="B52" s="152"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21884,12 +21893,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="146"/>
-      <c r="B53" s="146"/>
-      <c r="C53" s="140" t="s">
+      <c r="A53" s="152"/>
+      <c r="B53" s="152"/>
+      <c r="C53" s="146" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="141" t="s">
+      <c r="D53" s="147" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -25989,10 +25998,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="146"/>
-      <c r="B54" s="146"/>
-      <c r="C54" s="140"/>
-      <c r="D54" s="141"/>
+      <c r="A54" s="152"/>
+      <c r="B54" s="152"/>
+      <c r="C54" s="146"/>
+      <c r="D54" s="147"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30110,10 +30119,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="145" t="s">
+      <c r="A57" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="146" t="s">
+      <c r="B57" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30124,8 +30133,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="145"/>
-      <c r="B58" s="146"/>
+      <c r="A58" s="151"/>
+      <c r="B58" s="152"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30134,8 +30143,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="145"/>
-      <c r="B59" s="146"/>
+      <c r="A59" s="151"/>
+      <c r="B59" s="152"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30144,8 +30153,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="145"/>
-      <c r="B60" s="146"/>
+      <c r="A60" s="151"/>
+      <c r="B60" s="152"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30154,8 +30163,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="145"/>
-      <c r="B61" s="146"/>
+      <c r="A61" s="151"/>
+      <c r="B61" s="152"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30164,8 +30173,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="145"/>
-      <c r="B62" s="146"/>
+      <c r="A62" s="151"/>
+      <c r="B62" s="152"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30174,8 +30183,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="145"/>
-      <c r="B63" s="146"/>
+      <c r="A63" s="151"/>
+      <c r="B63" s="152"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30184,16 +30193,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="145"/>
-      <c r="B64" s="146"/>
+      <c r="A64" s="151"/>
+      <c r="B64" s="152"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="145"/>
-      <c r="B65" s="146"/>
+      <c r="A65" s="151"/>
+      <c r="B65" s="152"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30202,16 +30211,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="145"/>
-      <c r="B66" s="146"/>
+      <c r="A66" s="151"/>
+      <c r="B66" s="152"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="145"/>
-      <c r="B67" s="146"/>
+      <c r="A67" s="151"/>
+      <c r="B67" s="152"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30220,8 +30229,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="145"/>
-      <c r="B68" s="146"/>
+      <c r="A68" s="151"/>
+      <c r="B68" s="152"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30230,8 +30239,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="145"/>
-      <c r="B69" s="146"/>
+      <c r="A69" s="151"/>
+      <c r="B69" s="152"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30240,8 +30249,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="145"/>
-      <c r="B70" s="146"/>
+      <c r="A70" s="151"/>
+      <c r="B70" s="152"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30250,8 +30259,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="145"/>
-      <c r="B71" s="146"/>
+      <c r="A71" s="151"/>
+      <c r="B71" s="152"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30260,8 +30269,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="145"/>
-      <c r="B72" s="146"/>
+      <c r="A72" s="151"/>
+      <c r="B72" s="152"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30270,16 +30279,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="145"/>
-      <c r="B73" s="146"/>
+      <c r="A73" s="151"/>
+      <c r="B73" s="152"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="145"/>
-      <c r="B74" s="146"/>
+      <c r="A74" s="151"/>
+      <c r="B74" s="152"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30288,18 +30297,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="145"/>
-      <c r="B75" s="146"/>
-      <c r="C75" s="139"/>
-      <c r="D75" s="147" t="s">
+      <c r="A75" s="151"/>
+      <c r="B75" s="152"/>
+      <c r="C75" s="145"/>
+      <c r="D75" s="153" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="145"/>
-      <c r="B76" s="146"/>
-      <c r="C76" s="139"/>
-      <c r="D76" s="147"/>
+      <c r="A76" s="151"/>
+      <c r="B76" s="152"/>
+      <c r="C76" s="145"/>
+      <c r="D76" s="153"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30423,10 +30432,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="157" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30437,133 +30446,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="152"/>
-      <c r="B5" s="151"/>
-      <c r="C5" s="162" t="s">
+      <c r="A5" s="158"/>
+      <c r="B5" s="157"/>
+      <c r="C5" s="168" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="161" t="s">
+      <c r="D5" s="167" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="152"/>
-      <c r="B6" s="151"/>
-      <c r="C6" s="162"/>
-      <c r="D6" s="161"/>
+      <c r="A6" s="158"/>
+      <c r="B6" s="157"/>
+      <c r="C6" s="168"/>
+      <c r="D6" s="167"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="152"/>
-      <c r="B7" s="151"/>
+      <c r="A7" s="158"/>
+      <c r="B7" s="157"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="152"/>
-      <c r="B8" s="151"/>
+      <c r="A8" s="158"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="152"/>
-      <c r="B9" s="151"/>
+      <c r="A9" s="158"/>
+      <c r="B9" s="157"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="154" t="s">
+      <c r="A10" s="160" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="151" t="s">
+      <c r="B10" s="157" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="164"/>
-      <c r="D10" s="161" t="s">
+      <c r="C10" s="170"/>
+      <c r="D10" s="167" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="154"/>
-      <c r="B11" s="151"/>
-      <c r="C11" s="164"/>
-      <c r="D11" s="161"/>
+      <c r="A11" s="160"/>
+      <c r="B11" s="157"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="167"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="154"/>
-      <c r="B12" s="151"/>
-      <c r="C12" s="164"/>
-      <c r="D12" s="161"/>
+      <c r="A12" s="160"/>
+      <c r="B12" s="157"/>
+      <c r="C12" s="170"/>
+      <c r="D12" s="167"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="137" t="s">
+      <c r="A13" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="146" t="s">
+      <c r="B13" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="163"/>
-      <c r="D13" s="161" t="s">
+      <c r="C13" s="169"/>
+      <c r="D13" s="167" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="137"/>
-      <c r="B14" s="146"/>
-      <c r="C14" s="163"/>
-      <c r="D14" s="161"/>
+      <c r="A14" s="143"/>
+      <c r="B14" s="152"/>
+      <c r="C14" s="169"/>
+      <c r="D14" s="167"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="137"/>
-      <c r="B15" s="146"/>
-      <c r="C15" s="163"/>
+      <c r="A15" s="143"/>
+      <c r="B15" s="152"/>
+      <c r="C15" s="169"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="137"/>
-      <c r="B16" s="146"/>
-      <c r="C16" s="163"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="152"/>
+      <c r="C16" s="169"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="137"/>
-      <c r="B17" s="146"/>
-      <c r="C17" s="163"/>
+      <c r="A17" s="143"/>
+      <c r="B17" s="152"/>
+      <c r="C17" s="169"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="137"/>
-      <c r="B18" s="146"/>
-      <c r="C18" s="163"/>
+      <c r="A18" s="143"/>
+      <c r="B18" s="152"/>
+      <c r="C18" s="169"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="137"/>
-      <c r="B19" s="146"/>
-      <c r="C19" s="163"/>
+      <c r="A19" s="143"/>
+      <c r="B19" s="152"/>
+      <c r="C19" s="169"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="137"/>
-      <c r="B20" s="146"/>
-      <c r="C20" s="163"/>
+      <c r="A20" s="143"/>
+      <c r="B20" s="152"/>
+      <c r="C20" s="169"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="137"/>
-      <c r="B21" s="146"/>
-      <c r="C21" s="163"/>
+      <c r="A21" s="143"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="169"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="137"/>
-      <c r="B22" s="146"/>
-      <c r="C22" s="163"/>
+      <c r="A22" s="143"/>
+      <c r="B22" s="152"/>
+      <c r="C22" s="169"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="137"/>
-      <c r="B23" s="146"/>
-      <c r="C23" s="163"/>
+      <c r="A23" s="143"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="169"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30661,10 +30670,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="155" t="s">
+      <c r="A32" s="161" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="158" t="s">
+      <c r="B32" s="164" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30675,26 +30684,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="156"/>
-      <c r="B33" s="159"/>
+      <c r="A33" s="162"/>
+      <c r="B33" s="165"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="156"/>
-      <c r="B34" s="159"/>
+      <c r="A34" s="162"/>
+      <c r="B34" s="165"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="156"/>
-      <c r="B35" s="159"/>
+      <c r="A35" s="162"/>
+      <c r="B35" s="165"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="157"/>
-      <c r="B36" s="160"/>
+      <c r="A36" s="163"/>
+      <c r="B36" s="166"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30723,10 +30732,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="153" t="s">
+      <c r="A39" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="151" t="s">
+      <c r="B39" s="157" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30737,8 +30746,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="153"/>
-      <c r="B40" s="151"/>
+      <c r="A40" s="159"/>
+      <c r="B40" s="157"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30747,84 +30756,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="152" t="s">
+      <c r="A41" s="158" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="151" t="s">
+      <c r="B41" s="157" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="164" t="s">
+      <c r="C41" s="170" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="137" t="s">
+      <c r="D41" s="143" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="152"/>
-      <c r="B42" s="151"/>
-      <c r="C42" s="164"/>
-      <c r="D42" s="137"/>
+      <c r="A42" s="158"/>
+      <c r="B42" s="157"/>
+      <c r="C42" s="170"/>
+      <c r="D42" s="143"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="152"/>
-      <c r="B43" s="151"/>
-      <c r="C43" s="164" t="s">
+      <c r="A43" s="158"/>
+      <c r="B43" s="157"/>
+      <c r="C43" s="170" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="147" t="s">
+      <c r="D43" s="153" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="152"/>
-      <c r="B44" s="151"/>
-      <c r="C44" s="164"/>
-      <c r="D44" s="147"/>
+      <c r="A44" s="158"/>
+      <c r="B44" s="157"/>
+      <c r="C44" s="170"/>
+      <c r="D44" s="153"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="145" t="s">
+      <c r="A45" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="146" t="s">
+      <c r="B45" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="168"/>
+      <c r="C45" s="174"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="145"/>
-      <c r="B46" s="146"/>
-      <c r="C46" s="169"/>
-      <c r="D46" s="165" t="s">
+      <c r="A46" s="151"/>
+      <c r="B46" s="152"/>
+      <c r="C46" s="175"/>
+      <c r="D46" s="171" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="145"/>
-      <c r="B47" s="146"/>
-      <c r="C47" s="169"/>
-      <c r="D47" s="166"/>
+      <c r="A47" s="151"/>
+      <c r="B47" s="152"/>
+      <c r="C47" s="175"/>
+      <c r="D47" s="172"/>
     </row>
     <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="145"/>
-      <c r="B48" s="146"/>
-      <c r="C48" s="170"/>
-      <c r="D48" s="166"/>
+      <c r="A48" s="151"/>
+      <c r="B48" s="152"/>
+      <c r="C48" s="176"/>
+      <c r="D48" s="172"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="145"/>
-      <c r="B49" s="146"/>
-      <c r="C49" s="140"/>
-      <c r="D49" s="166"/>
+      <c r="A49" s="151"/>
+      <c r="B49" s="152"/>
+      <c r="C49" s="146"/>
+      <c r="D49" s="172"/>
     </row>
     <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="145"/>
-      <c r="B50" s="146"/>
-      <c r="C50" s="140"/>
-      <c r="D50" s="167"/>
+      <c r="A50" s="151"/>
+      <c r="B50" s="152"/>
+      <c r="C50" s="146"/>
+      <c r="D50" s="173"/>
     </row>
     <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30847,10 +30856,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="146" t="s">
+      <c r="A53" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="146" t="s">
+      <c r="B53" s="152" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30861,8 +30870,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="146"/>
-      <c r="B54" s="146"/>
+      <c r="A54" s="152"/>
+      <c r="B54" s="152"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30871,8 +30880,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="146"/>
-      <c r="B55" s="146"/>
+      <c r="A55" s="152"/>
+      <c r="B55" s="152"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30881,9 +30890,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="146"/>
-      <c r="B56" s="146"/>
-      <c r="C56" s="171" t="s">
+      <c r="A56" s="152"/>
+      <c r="B56" s="152"/>
+      <c r="C56" s="177" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30891,16 +30900,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="146"/>
-      <c r="B57" s="146"/>
-      <c r="C57" s="171"/>
+      <c r="A57" s="152"/>
+      <c r="B57" s="152"/>
+      <c r="C57" s="177"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="146"/>
-      <c r="B58" s="146"/>
+      <c r="A58" s="152"/>
+      <c r="B58" s="152"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30909,8 +30918,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="146"/>
-      <c r="B59" s="146"/>
+      <c r="A59" s="152"/>
+      <c r="B59" s="152"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30919,9 +30928,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="146"/>
-      <c r="B60" s="146"/>
-      <c r="C60" s="171" t="s">
+      <c r="A60" s="152"/>
+      <c r="B60" s="152"/>
+      <c r="C60" s="177" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -30929,25 +30938,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="146"/>
-      <c r="B61" s="146"/>
-      <c r="C61" s="171"/>
+      <c r="A61" s="152"/>
+      <c r="B61" s="152"/>
+      <c r="C61" s="177"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="146"/>
-      <c r="B62" s="146"/>
-      <c r="C62" s="171"/>
+      <c r="A62" s="152"/>
+      <c r="B62" s="152"/>
+      <c r="C62" s="177"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="146"/>
-      <c r="B63" s="146"/>
-      <c r="C63" s="164" t="s">
+      <c r="A63" s="152"/>
+      <c r="B63" s="152"/>
+      <c r="C63" s="170" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -30955,30 +30964,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="146"/>
-      <c r="B64" s="146"/>
-      <c r="C64" s="164"/>
-      <c r="D64" s="147" t="s">
+      <c r="A64" s="152"/>
+      <c r="B64" s="152"/>
+      <c r="C64" s="170"/>
+      <c r="D64" s="153" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="146"/>
-      <c r="B65" s="146"/>
-      <c r="C65" s="164"/>
-      <c r="D65" s="147"/>
+      <c r="A65" s="152"/>
+      <c r="B65" s="152"/>
+      <c r="C65" s="170"/>
+      <c r="D65" s="153"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="146"/>
-      <c r="B66" s="146"/>
-      <c r="C66" s="164"/>
-      <c r="D66" s="147"/>
+      <c r="A66" s="152"/>
+      <c r="B66" s="152"/>
+      <c r="C66" s="170"/>
+      <c r="D66" s="153"/>
     </row>
     <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="146"/>
-      <c r="B67" s="146"/>
-      <c r="C67" s="164"/>
-      <c r="D67" s="147"/>
+      <c r="A67" s="152"/>
+      <c r="B67" s="152"/>
+      <c r="C67" s="170"/>
+      <c r="D67" s="153"/>
     </row>
     <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
@@ -31075,10 +31084,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31096,7 +31105,7 @@
       <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="112" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="57" t="s">
@@ -31108,28 +31117,28 @@
         <v>24</v>
       </c>
       <c r="B2" s="39"/>
-      <c r="C2" s="102"/>
+      <c r="C2" s="101"/>
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="177" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="101"/>
+      <c r="C3" s="100"/>
       <c r="D3" s="58" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="137"/>
-      <c r="B4" s="171"/>
-      <c r="C4" s="115" t="s">
+      <c r="A4" s="143"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="113" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="117" t="s">
         <v>256</v>
       </c>
     </row>
@@ -31137,11 +31146,11 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="171"/>
-      <c r="C5" s="115" t="s">
+      <c r="B5" s="177"/>
+      <c r="C5" s="113" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="113" t="s">
+      <c r="D5" s="111" t="s">
         <v>236</v>
       </c>
     </row>
@@ -31149,28 +31158,28 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="171"/>
-      <c r="C6" s="115" t="s">
+      <c r="B6" s="177"/>
+      <c r="C6" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="113" t="s">
+      <c r="D6" s="111" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="180" t="s">
+      <c r="A7" s="186" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="171"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="177"/>
+      <c r="C7" s="100"/>
       <c r="D7" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="181"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="101"/>
+      <c r="A8" s="187"/>
+      <c r="B8" s="177"/>
+      <c r="C8" s="100"/>
       <c r="D8" s="58" t="s">
         <v>276</v>
       </c>
@@ -31179,8 +31188,8 @@
       <c r="A9" t="s">
         <v>290</v>
       </c>
-      <c r="B9" s="171"/>
-      <c r="C9" s="101" t="s">
+      <c r="B9" s="177"/>
+      <c r="C9" s="100" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="58"/>
@@ -31189,9 +31198,9 @@
       <c r="A10" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="171"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="113" t="s">
+      <c r="B10" s="177"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="111" t="s">
         <v>259</v>
       </c>
     </row>
@@ -31200,40 +31209,40 @@
         <v>28</v>
       </c>
       <c r="B11" s="39"/>
-      <c r="C11" s="102"/>
+      <c r="C11" s="101"/>
       <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="188" t="s">
+      <c r="A12" s="190" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="175" t="s">
+      <c r="B12" s="181" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="101"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="58" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="189"/>
-      <c r="B13" s="176"/>
-      <c r="C13" s="101"/>
+      <c r="A13" s="191"/>
+      <c r="B13" s="182"/>
+      <c r="C13" s="100"/>
       <c r="D13" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="189"/>
-      <c r="B14" s="176"/>
-      <c r="C14" s="101"/>
+      <c r="A14" s="191"/>
+      <c r="B14" s="182"/>
+      <c r="C14" s="100"/>
       <c r="D14" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="190"/>
-      <c r="B15" s="177"/>
+      <c r="A15" s="192"/>
+      <c r="B15" s="183"/>
       <c r="C15" s="58" t="s">
         <v>300</v>
       </c>
@@ -31242,53 +31251,53 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="198" t="s">
+      <c r="A16" s="197" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="171" t="s">
+      <c r="B16" s="177" t="s">
         <v>234</v>
       </c>
       <c r="C16" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="D16" s="109" t="s">
+      <c r="D16" s="107" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="199"/>
-      <c r="B17" s="171"/>
+      <c r="A17" s="198"/>
+      <c r="B17" s="177"/>
       <c r="C17" s="58"/>
       <c r="D17" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="137" t="s">
+      <c r="A18" s="177" t="s">
         <v>222</v>
       </c>
-      <c r="B18" s="171" t="s">
+      <c r="B18" s="177" t="s">
         <v>234</v>
       </c>
-      <c r="C18" s="192" t="s">
+      <c r="C18" s="194" t="s">
         <v>239</v>
       </c>
-      <c r="D18" s="121" t="s">
+      <c r="D18" s="118" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="137"/>
-      <c r="B19" s="171"/>
-      <c r="C19" s="193"/>
-      <c r="D19" s="109" t="s">
+      <c r="A19" s="177"/>
+      <c r="B19" s="177"/>
+      <c r="C19" s="194"/>
+      <c r="D19" s="107" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="137"/>
-      <c r="B20" s="171"/>
-      <c r="C20" s="196" t="s">
+      <c r="A20" s="177"/>
+      <c r="B20" s="177"/>
+      <c r="C20" s="194" t="s">
         <v>240</v>
       </c>
       <c r="D20" s="58" t="s">
@@ -31296,472 +31305,560 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="137"/>
-      <c r="B21" s="171"/>
-      <c r="C21" s="197"/>
+      <c r="A21" s="177"/>
+      <c r="B21" s="177"/>
+      <c r="C21" s="194"/>
       <c r="D21" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="177"/>
+      <c r="B22" s="177"/>
+      <c r="C22" s="120" t="s">
+        <v>307</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="152" t="s">
         <v>296</v>
       </c>
-      <c r="B22" s="171" t="s">
+      <c r="B23" s="177" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="C23" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D23" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="146"/>
-      <c r="B23" s="171"/>
-      <c r="C23" s="61" t="s">
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="152"/>
+      <c r="B24" s="177"/>
+      <c r="C24" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D24" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39" t="s">
+    <row r="25" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="102"/>
-      <c r="D24" s="44"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="180" t="s">
-        <v>260</v>
-      </c>
-      <c r="B25" s="171" t="s">
-        <v>234</v>
-      </c>
+      <c r="B25" s="39"/>
       <c r="C25" s="101"/>
-      <c r="D25" s="79" t="s">
-        <v>261</v>
-      </c>
+      <c r="D25" s="44"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="181"/>
-      <c r="B26" s="171"/>
-      <c r="C26" s="101"/>
-      <c r="D26" s="58" t="s">
-        <v>257</v>
+      <c r="A26" s="186" t="s">
+        <v>260</v>
+      </c>
+      <c r="B26" s="177" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="100"/>
+      <c r="D26" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="96" t="s">
+      <c r="A27" s="187"/>
+      <c r="B27" s="177"/>
+      <c r="C27" s="100"/>
+      <c r="D27" s="58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B28" s="104" t="s">
         <v>234</v>
       </c>
-      <c r="C27" s="115" t="s">
+      <c r="C28" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="113" t="s">
+      <c r="D28" s="111" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="182" t="s">
+    <row r="29" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="185" t="s">
+      <c r="B29" s="177" t="s">
         <v>234</v>
       </c>
-      <c r="C28" s="101" t="s">
+      <c r="C29" s="122" t="s">
         <v>268</v>
-      </c>
-      <c r="D28" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="183"/>
-      <c r="B29" s="186"/>
-      <c r="C29" t="s">
-        <v>270</v>
       </c>
       <c r="D29" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="183"/>
-      <c r="B30" s="186"/>
-      <c r="C30" s="101" t="s">
-        <v>269</v>
+      <c r="A30" s="152"/>
+      <c r="B30" s="177"/>
+      <c r="C30" s="122" t="s">
+        <v>270</v>
       </c>
       <c r="D30" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="183"/>
-      <c r="B31" s="186"/>
-      <c r="C31" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D31" s="109" t="s">
-        <v>102</v>
+      <c r="A31" s="152"/>
+      <c r="B31" s="177"/>
+      <c r="C31" s="122" t="s">
+        <v>269</v>
+      </c>
+      <c r="D31" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="183"/>
-      <c r="B32" s="186"/>
-      <c r="C32" s="101" t="s">
-        <v>282</v>
-      </c>
-      <c r="D32" s="58" t="s">
-        <v>251</v>
+      <c r="A32" s="152"/>
+      <c r="B32" s="177"/>
+      <c r="C32" s="123" t="s">
+        <v>277</v>
+      </c>
+      <c r="D32" s="107" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="183"/>
-      <c r="B33" s="186"/>
-      <c r="C33" s="101" t="s">
-        <v>283</v>
+      <c r="A33" s="152"/>
+      <c r="B33" s="177"/>
+      <c r="C33" s="122" t="s">
+        <v>282</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="183"/>
-      <c r="B34" s="186"/>
-      <c r="C34" s="104" t="s">
-        <v>288</v>
-      </c>
-      <c r="D34" s="109" t="s">
-        <v>251</v>
+      <c r="A34" s="152"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="122" t="s">
+        <v>283</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="183"/>
-      <c r="B35" s="186"/>
-      <c r="C35" s="104" t="s">
-        <v>302</v>
-      </c>
-      <c r="D35" s="109" t="s">
+      <c r="A35" s="152"/>
+      <c r="B35" s="177"/>
+      <c r="C35" s="123" t="s">
+        <v>288</v>
+      </c>
+      <c r="D35" s="107" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="183"/>
-      <c r="B36" s="186"/>
-      <c r="C36" s="104" t="s">
+      <c r="A36" s="152"/>
+      <c r="B36" s="177"/>
+      <c r="C36" s="123" t="s">
+        <v>302</v>
+      </c>
+      <c r="D36" s="107" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="152"/>
+      <c r="B37" s="177"/>
+      <c r="C37" s="123" t="s">
         <v>289</v>
       </c>
-      <c r="D36" s="109" t="s">
+      <c r="D37" s="107" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="184"/>
-      <c r="B37" s="187"/>
-      <c r="C37" s="116" t="s">
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="152"/>
+      <c r="B38" s="177"/>
+      <c r="C38" s="124" t="s">
         <v>244</v>
       </c>
-      <c r="D37" s="113" t="s">
+      <c r="D38" s="119" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="102"/>
-      <c r="D38" s="44"/>
+    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="152"/>
+      <c r="B39" s="177"/>
+      <c r="C39" s="125" t="s">
+        <v>311</v>
+      </c>
+      <c r="D39" s="107" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="39" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="99"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="101"/>
-      <c r="D39" s="79" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="171" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" s="171" t="s">
-        <v>234</v>
-      </c>
-      <c r="C40" s="115" t="s">
-        <v>246</v>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="152"/>
+      <c r="B40" s="177"/>
+      <c r="C40" s="122" t="s">
+        <v>312</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>253</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="171"/>
-      <c r="B41" s="171"/>
-      <c r="C41" s="115">
-        <v>10.1</v>
-      </c>
-      <c r="D41" s="58" t="s">
-        <v>272</v>
+      <c r="A41" s="152"/>
+      <c r="B41" s="177"/>
+      <c r="C41" s="123" t="s">
+        <v>313</v>
+      </c>
+      <c r="D41" s="107" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="171"/>
-      <c r="B42" s="171"/>
-      <c r="C42" s="115">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D42" s="58" t="s">
-        <v>272</v>
+      <c r="A42" s="152"/>
+      <c r="B42" s="177"/>
+      <c r="C42" s="123" t="s">
+        <v>315</v>
+      </c>
+      <c r="D42" s="107" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="171"/>
-      <c r="B43" s="171"/>
-      <c r="C43" s="117" t="s">
-        <v>293</v>
-      </c>
-      <c r="D43" s="111" t="s">
-        <v>294</v>
+      <c r="A43" s="152"/>
+      <c r="B43" s="177"/>
+      <c r="C43" s="126" t="s">
+        <v>268</v>
+      </c>
+      <c r="D43" s="127" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="137" t="s">
-        <v>247</v>
-      </c>
-      <c r="B44" s="171" t="s">
+      <c r="A44" s="58" t="s">
+        <v>309</v>
+      </c>
+      <c r="B44" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="194"/>
-      <c r="D44" s="191" t="s">
-        <v>261</v>
+      <c r="C44" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="107" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="137"/>
-      <c r="B45" s="171"/>
-      <c r="C45" s="195"/>
-      <c r="D45" s="191"/>
+      <c r="A45" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="B45" s="121" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="107" t="s">
+        <v>274</v>
+      </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="107" t="s">
-        <v>262</v>
-      </c>
-      <c r="B46" s="108" t="s">
+    <row r="46" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="39"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="44"/>
+    </row>
+    <row r="47" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="99"/>
+      <c r="B47" s="67"/>
+      <c r="C47" s="100"/>
+      <c r="D47" s="79" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="177" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="177" t="s">
         <v>234</v>
       </c>
-      <c r="C46" s="115" t="s">
-        <v>250</v>
-      </c>
-      <c r="D46" s="109" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="105"/>
-      <c r="D47" s="98"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="B48" s="108" t="s">
-        <v>234</v>
-      </c>
-      <c r="C48" s="118" t="s">
-        <v>265</v>
+      <c r="C48" s="113" t="s">
+        <v>246</v>
       </c>
       <c r="D48" s="58" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="172" t="s">
-        <v>285</v>
-      </c>
-      <c r="B49" s="175" t="s">
-        <v>234</v>
-      </c>
-      <c r="C49" s="119" t="s">
-        <v>295</v>
+      <c r="A49" s="177"/>
+      <c r="B49" s="177"/>
+      <c r="C49" s="113">
+        <v>10.1</v>
       </c>
       <c r="D49" s="58" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="173"/>
-      <c r="B50" s="176"/>
-      <c r="C50" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="D50" s="109" t="s">
-        <v>306</v>
+      <c r="A50" s="177"/>
+      <c r="B50" s="177"/>
+      <c r="C50" s="113">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D50" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="174"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="177"/>
       <c r="B51" s="177"/>
-      <c r="C51" s="118" t="s">
-        <v>286</v>
-      </c>
-      <c r="D51" s="58" t="s">
-        <v>287</v>
+      <c r="C51" s="114" t="s">
+        <v>293</v>
+      </c>
+      <c r="D51" s="109" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="98"/>
-      <c r="C52" s="112"/>
-      <c r="D52" s="98"/>
+      <c r="A52" s="143" t="s">
+        <v>247</v>
+      </c>
+      <c r="B52" s="177" t="s">
+        <v>234</v>
+      </c>
+      <c r="C52" s="195"/>
+      <c r="D52" s="193" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="178" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="185" t="s">
-        <v>271</v>
-      </c>
-      <c r="C53" s="118" t="s">
-        <v>265</v>
-      </c>
-      <c r="D53" s="58" t="s">
-        <v>267</v>
-      </c>
+      <c r="A53" s="143"/>
+      <c r="B53" s="177"/>
+      <c r="C53" s="196"/>
+      <c r="D53" s="193"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="179"/>
-      <c r="B54" s="187"/>
-      <c r="C54" s="118" t="s">
+      <c r="A54" s="105" t="s">
+        <v>262</v>
+      </c>
+      <c r="B54" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="113" t="s">
+        <v>250</v>
+      </c>
+      <c r="D54" s="107" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B55" s="39"/>
+      <c r="C55" s="103"/>
+      <c r="D55" s="98"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B56" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C56" s="115" t="s">
         <v>265</v>
       </c>
-      <c r="D54" s="58" t="s">
-        <v>266</v>
+      <c r="D56" s="58" t="s">
+        <v>267</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="97" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="108" t="s">
-        <v>271</v>
-      </c>
-      <c r="C55" s="103" t="s">
-        <v>264</v>
-      </c>
-      <c r="D55" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B56" s="110" t="s">
-        <v>271</v>
-      </c>
-      <c r="C56" s="101"/>
-      <c r="D56" s="61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="97" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="108" t="s">
-        <v>271</v>
-      </c>
-      <c r="C57" s="103" t="s">
-        <v>264</v>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="178" t="s">
+        <v>285</v>
+      </c>
+      <c r="B57" s="181" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="116" t="s">
+        <v>295</v>
       </c>
       <c r="D57" s="58" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B58" s="98"/>
-      <c r="C58" s="112"/>
-      <c r="D58" s="98"/>
+      <c r="A58" s="179"/>
+      <c r="B58" s="182"/>
+      <c r="C58" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D58" s="107" t="s">
+        <v>306</v>
+      </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="58"/>
-      <c r="B59" s="108" t="s">
-        <v>234</v>
-      </c>
-      <c r="C59" s="101" t="s">
-        <v>30</v>
-      </c>
-      <c r="D59" s="109" t="s">
-        <v>274</v>
+    <row r="59" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="180"/>
+      <c r="B59" s="183"/>
+      <c r="C59" s="115" t="s">
+        <v>286</v>
+      </c>
+      <c r="D59" s="58" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="98" t="s">
-        <v>279</v>
+        <v>56</v>
       </c>
       <c r="B60" s="98"/>
-      <c r="C60" s="112"/>
+      <c r="C60" s="110"/>
       <c r="D60" s="98"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="58"/>
-      <c r="B61" s="108" t="s">
+      <c r="A61" s="184" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="188" t="s">
+        <v>271</v>
+      </c>
+      <c r="C61" s="115" t="s">
+        <v>265</v>
+      </c>
+      <c r="D61" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="185"/>
+      <c r="B62" s="189"/>
+      <c r="C62" s="115" t="s">
+        <v>265</v>
+      </c>
+      <c r="D62" s="58" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="97" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C63" s="102" t="s">
+        <v>264</v>
+      </c>
+      <c r="D63" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="B64" s="108" t="s">
+        <v>271</v>
+      </c>
+      <c r="C64" s="100"/>
+      <c r="D64" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C65" s="102" t="s">
+        <v>264</v>
+      </c>
+      <c r="D65" s="58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B66" s="98"/>
+      <c r="C66" s="110"/>
+      <c r="D66" s="98"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="58"/>
+      <c r="B67" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C61" s="101" t="s">
+      <c r="C67" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="D61" s="109" t="s">
+      <c r="D67" s="107" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B68" s="98"/>
+      <c r="C68" s="110"/>
+      <c r="D68" s="98"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="58"/>
+      <c r="B69" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C69" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" s="107" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C52:C53"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A52:A53"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B10"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A28:A37"/>
-    <mergeCell ref="B28:B37"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B61:B62"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A29:A43"/>
+    <mergeCell ref="B29:B43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
"ROS Payroll Application Guide"
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="341">
   <si>
     <t>Document</t>
   </si>
@@ -2759,12 +2759,129 @@
   <si>
     <t>code 2040</t>
   </si>
+  <si>
+    <t>Endpoints corrected from ‘paye/employers’ to ‘paye-employers’</t>
+  </si>
+  <si>
+    <t>Sample request-target corrected from ‘softwareused’ to ‘softwareUsed’</t>
+  </si>
+  <si>
+    <t>codes 1014, 1002</t>
+  </si>
+  <si>
+    <t>code 3013</t>
+  </si>
+  <si>
+    <t>path changed to N/A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cert does not have appropriate permissions.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' changed to '</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Agent does not have appropriate permissions.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">'
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Validation Ref 142</t>
+  </si>
+  <si>
+    <t>Updated to 'Warning:  No PPSN or employment ID provided.'</t>
+  </si>
+  <si>
+    <t>Validation Ref 51</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Headers included</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> description updated</t>
+  </si>
+  <si>
+    <t>addressLine</t>
+  </si>
+  <si>
+    <t>Look Up Payroll by Return Period</t>
+  </si>
+  <si>
+    <t>Request body removed</t>
+  </si>
+  <si>
+    <t>Returns Reconciliations WSDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema location </t>
+  </si>
+  <si>
+    <t>corrected to 'returns_reconciliation/returns_reconciliation-schema.xsd'</t>
+  </si>
+  <si>
+    <t>RPN: Data Items</t>
+  </si>
+  <si>
+    <t>positive numbers only'</t>
+  </si>
+  <si>
+    <t>updated to match schema ' [ -999999999 .. 999999999.99 ]'</t>
+  </si>
+  <si>
+    <t>updated to match the schema</t>
+  </si>
+  <si>
+    <t>Eircode validation rules</t>
+  </si>
+  <si>
+    <t>code 2051</t>
+  </si>
+  <si>
+    <t>code 3008</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2877,6 +2994,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2904,7 +3036,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -3316,60 +3448,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3628,49 +3711,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3684,16 +3726,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3844,68 +3894,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4310,12 +4306,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="130"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="115"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4338,12 +4334,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="129"/>
-      <c r="C4" s="129"/>
-      <c r="D4" s="130"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="115"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4383,10 +4379,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="131" t="s">
+      <c r="A7" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="134">
+      <c r="B7" s="119">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4400,8 +4396,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="132"/>
-      <c r="B8" s="135"/>
+      <c r="A8" s="117"/>
+      <c r="B8" s="120"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4413,8 +4409,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="132"/>
-      <c r="B9" s="135"/>
+      <c r="A9" s="117"/>
+      <c r="B9" s="120"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4426,8 +4422,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="132"/>
-      <c r="B10" s="135"/>
+      <c r="A10" s="117"/>
+      <c r="B10" s="120"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4439,8 +4435,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="132"/>
-      <c r="B11" s="135"/>
+      <c r="A11" s="117"/>
+      <c r="B11" s="120"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4452,8 +4448,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="133"/>
-      <c r="B12" s="136"/>
+      <c r="A12" s="118"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4465,10 +4461,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="139" t="s">
+      <c r="A13" s="124" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="134">
+      <c r="B13" s="119">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4482,8 +4478,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="140"/>
-      <c r="B14" s="136"/>
+      <c r="A14" s="125"/>
+      <c r="B14" s="121"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4529,12 +4525,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="128" t="s">
+      <c r="A17" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="129"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="130"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="115"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4574,21 +4570,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="128" t="s">
+      <c r="A20" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="129"/>
-      <c r="C20" s="129"/>
-      <c r="D20" s="130"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="114"/>
+      <c r="D20" s="115"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="141" t="s">
+      <c r="A21" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="138">
+      <c r="B21" s="123">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4602,8 +4598,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="142"/>
-      <c r="B22" s="136"/>
+      <c r="A22" s="127"/>
+      <c r="B22" s="121"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4626,18 +4622,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="128" t="s">
+      <c r="A24" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="129"/>
-      <c r="C24" s="129"/>
-      <c r="D24" s="130"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="115"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="137" t="s">
+      <c r="A25" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="138">
+      <c r="B25" s="123">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4651,8 +4647,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="132"/>
-      <c r="B26" s="135"/>
+      <c r="A26" s="117"/>
+      <c r="B26" s="120"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4664,8 +4660,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="132"/>
-      <c r="B27" s="135"/>
+      <c r="A27" s="117"/>
+      <c r="B27" s="120"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4677,8 +4673,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="132"/>
-      <c r="B28" s="135"/>
+      <c r="A28" s="117"/>
+      <c r="B28" s="120"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4690,8 +4686,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="132"/>
-      <c r="B29" s="135"/>
+      <c r="A29" s="117"/>
+      <c r="B29" s="120"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4703,8 +4699,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="132"/>
-      <c r="B30" s="135"/>
+      <c r="A30" s="117"/>
+      <c r="B30" s="120"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4716,8 +4712,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="132"/>
-      <c r="B31" s="135"/>
+      <c r="A31" s="117"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4729,8 +4725,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="133"/>
-      <c r="B32" s="136"/>
+      <c r="A32" s="118"/>
+      <c r="B32" s="121"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4854,12 +4850,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="128" t="s">
+      <c r="A41" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="129"/>
-      <c r="C41" s="129"/>
-      <c r="D41" s="130"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="115"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
@@ -5039,10 +5035,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="158" t="s">
+      <c r="A7" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5053,8 +5049,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="158"/>
-      <c r="B8" s="157"/>
+      <c r="A8" s="143"/>
+      <c r="B8" s="142"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5063,8 +5059,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="158"/>
-      <c r="B9" s="157"/>
+      <c r="A9" s="143"/>
+      <c r="B9" s="142"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5073,8 +5069,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="158"/>
-      <c r="B10" s="157"/>
+      <c r="A10" s="143"/>
+      <c r="B10" s="142"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5083,8 +5079,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="158"/>
-      <c r="B11" s="157"/>
+      <c r="A11" s="143"/>
+      <c r="B11" s="142"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5093,8 +5089,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="158"/>
-      <c r="B12" s="157"/>
+      <c r="A12" s="143"/>
+      <c r="B12" s="142"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5103,10 +5099,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="160" t="s">
+      <c r="A13" s="145" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5117,8 +5113,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="160"/>
-      <c r="B14" s="157"/>
+      <c r="A14" s="145"/>
+      <c r="B14" s="142"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5127,8 +5123,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="160"/>
-      <c r="B15" s="157"/>
+      <c r="A15" s="145"/>
+      <c r="B15" s="142"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5137,10 +5133,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="143" t="s">
+      <c r="A16" s="128" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="152" t="s">
+      <c r="B16" s="137" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5151,8 +5147,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="143"/>
-      <c r="B17" s="152"/>
+      <c r="A17" s="128"/>
+      <c r="B17" s="137"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5161,8 +5157,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="143"/>
-      <c r="B18" s="152"/>
+      <c r="A18" s="128"/>
+      <c r="B18" s="137"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5171,8 +5167,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="143"/>
-      <c r="B19" s="152"/>
+      <c r="A19" s="128"/>
+      <c r="B19" s="137"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5181,8 +5177,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="143"/>
-      <c r="B20" s="152"/>
+      <c r="A20" s="128"/>
+      <c r="B20" s="137"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5191,8 +5187,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="143"/>
-      <c r="B21" s="152"/>
+      <c r="A21" s="128"/>
+      <c r="B21" s="137"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5201,8 +5197,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="143"/>
-      <c r="B22" s="152"/>
+      <c r="A22" s="128"/>
+      <c r="B22" s="137"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5211,8 +5207,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="143"/>
-      <c r="B23" s="152"/>
+      <c r="A23" s="128"/>
+      <c r="B23" s="137"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5221,26 +5217,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="143"/>
-      <c r="B24" s="152"/>
-      <c r="C24" s="143" t="s">
+      <c r="A24" s="128"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="128" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="144" t="s">
+      <c r="D24" s="129" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="143"/>
-      <c r="B25" s="152"/>
-      <c r="C25" s="143"/>
-      <c r="D25" s="144"/>
+      <c r="A25" s="128"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="129"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="158" t="s">
+      <c r="A26" s="143" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="157" t="s">
+      <c r="B26" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5251,8 +5247,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="158"/>
-      <c r="B27" s="157"/>
+      <c r="A27" s="143"/>
+      <c r="B27" s="142"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5279,28 +5275,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="159" t="s">
+      <c r="A30" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="157" t="s">
+      <c r="B30" s="142" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="143" t="s">
+      <c r="C30" s="128" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="147" t="s">
+      <c r="D30" s="132" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="159"/>
-      <c r="B31" s="157"/>
-      <c r="C31" s="143"/>
-      <c r="D31" s="147"/>
+      <c r="A31" s="144"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="128"/>
+      <c r="D31" s="132"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="159"/>
-      <c r="B32" s="157"/>
+      <c r="A32" s="144"/>
+      <c r="B32" s="142"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5309,8 +5305,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="159"/>
-      <c r="B33" s="157"/>
+      <c r="A33" s="144"/>
+      <c r="B33" s="142"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5319,8 +5315,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="159"/>
-      <c r="B34" s="157"/>
+      <c r="A34" s="144"/>
+      <c r="B34" s="142"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5329,8 +5325,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="159"/>
-      <c r="B35" s="157"/>
+      <c r="A35" s="144"/>
+      <c r="B35" s="142"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5339,8 +5335,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="159"/>
-      <c r="B36" s="157"/>
+      <c r="A36" s="144"/>
+      <c r="B36" s="142"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5349,26 +5345,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="159"/>
-      <c r="B37" s="157"/>
-      <c r="C37" s="148" t="s">
+      <c r="A37" s="144"/>
+      <c r="B37" s="142"/>
+      <c r="C37" s="133" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="150" t="s">
+      <c r="D37" s="135" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="159"/>
-      <c r="B38" s="157"/>
-      <c r="C38" s="149"/>
-      <c r="D38" s="150"/>
+      <c r="A38" s="144"/>
+      <c r="B38" s="142"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="135"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="158" t="s">
+      <c r="A39" s="143" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="157" t="s">
+      <c r="B39" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5379,8 +5375,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="158"/>
-      <c r="B40" s="157"/>
+      <c r="A40" s="143"/>
+      <c r="B40" s="142"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5407,10 +5403,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="159" t="s">
+      <c r="A43" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="157" t="s">
+      <c r="B43" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5419,8 +5415,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="159"/>
-      <c r="B44" s="157"/>
+      <c r="A44" s="144"/>
+      <c r="B44" s="142"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5429,10 +5425,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="154" t="s">
+      <c r="A45" s="139" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="157" t="s">
+      <c r="B45" s="142" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5441,8 +5437,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="155"/>
-      <c r="B46" s="157"/>
+      <c r="A46" s="140"/>
+      <c r="B46" s="142"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5451,8 +5447,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="155"/>
-      <c r="B47" s="157"/>
+      <c r="A47" s="140"/>
+      <c r="B47" s="142"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5461,8 +5457,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="156"/>
-      <c r="B48" s="157"/>
+      <c r="A48" s="141"/>
+      <c r="B48" s="142"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5471,10 +5467,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="152" t="s">
+      <c r="A49" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="152" t="s">
+      <c r="B49" s="137" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9578,8 +9574,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="152"/>
-      <c r="B50" s="152"/>
+      <c r="A50" s="137"/>
+      <c r="B50" s="137"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13683,8 +13679,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="152"/>
-      <c r="B51" s="152"/>
+      <c r="A51" s="137"/>
+      <c r="B51" s="137"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17788,8 +17784,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="152"/>
-      <c r="B52" s="152"/>
+      <c r="A52" s="137"/>
+      <c r="B52" s="137"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21893,12 +21889,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="152"/>
-      <c r="B53" s="152"/>
-      <c r="C53" s="146" t="s">
+      <c r="A53" s="137"/>
+      <c r="B53" s="137"/>
+      <c r="C53" s="131" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="147" t="s">
+      <c r="D53" s="132" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -25998,10 +25994,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="152"/>
-      <c r="B54" s="152"/>
-      <c r="C54" s="146"/>
-      <c r="D54" s="147"/>
+      <c r="A54" s="137"/>
+      <c r="B54" s="137"/>
+      <c r="C54" s="131"/>
+      <c r="D54" s="132"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30119,10 +30115,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="151" t="s">
+      <c r="A57" s="136" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="152" t="s">
+      <c r="B57" s="137" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30133,8 +30129,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="151"/>
-      <c r="B58" s="152"/>
+      <c r="A58" s="136"/>
+      <c r="B58" s="137"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30143,8 +30139,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="151"/>
-      <c r="B59" s="152"/>
+      <c r="A59" s="136"/>
+      <c r="B59" s="137"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30153,8 +30149,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="151"/>
-      <c r="B60" s="152"/>
+      <c r="A60" s="136"/>
+      <c r="B60" s="137"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30163,8 +30159,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="151"/>
-      <c r="B61" s="152"/>
+      <c r="A61" s="136"/>
+      <c r="B61" s="137"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30173,8 +30169,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="151"/>
-      <c r="B62" s="152"/>
+      <c r="A62" s="136"/>
+      <c r="B62" s="137"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30183,8 +30179,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="151"/>
-      <c r="B63" s="152"/>
+      <c r="A63" s="136"/>
+      <c r="B63" s="137"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30193,16 +30189,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="151"/>
-      <c r="B64" s="152"/>
+      <c r="A64" s="136"/>
+      <c r="B64" s="137"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="151"/>
-      <c r="B65" s="152"/>
+      <c r="A65" s="136"/>
+      <c r="B65" s="137"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30211,16 +30207,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="151"/>
-      <c r="B66" s="152"/>
+      <c r="A66" s="136"/>
+      <c r="B66" s="137"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="151"/>
-      <c r="B67" s="152"/>
+      <c r="A67" s="136"/>
+      <c r="B67" s="137"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30229,8 +30225,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="151"/>
-      <c r="B68" s="152"/>
+      <c r="A68" s="136"/>
+      <c r="B68" s="137"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30239,8 +30235,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="151"/>
-      <c r="B69" s="152"/>
+      <c r="A69" s="136"/>
+      <c r="B69" s="137"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30249,8 +30245,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="151"/>
-      <c r="B70" s="152"/>
+      <c r="A70" s="136"/>
+      <c r="B70" s="137"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30259,8 +30255,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="151"/>
-      <c r="B71" s="152"/>
+      <c r="A71" s="136"/>
+      <c r="B71" s="137"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30269,8 +30265,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="151"/>
-      <c r="B72" s="152"/>
+      <c r="A72" s="136"/>
+      <c r="B72" s="137"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30279,16 +30275,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="151"/>
-      <c r="B73" s="152"/>
+      <c r="A73" s="136"/>
+      <c r="B73" s="137"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="151"/>
-      <c r="B74" s="152"/>
+      <c r="A74" s="136"/>
+      <c r="B74" s="137"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30297,18 +30293,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="151"/>
-      <c r="B75" s="152"/>
-      <c r="C75" s="145"/>
-      <c r="D75" s="153" t="s">
+      <c r="A75" s="136"/>
+      <c r="B75" s="137"/>
+      <c r="C75" s="130"/>
+      <c r="D75" s="138" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="151"/>
-      <c r="B76" s="152"/>
-      <c r="C76" s="145"/>
-      <c r="D76" s="153"/>
+      <c r="A76" s="136"/>
+      <c r="B76" s="137"/>
+      <c r="C76" s="130"/>
+      <c r="D76" s="138"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
@@ -30432,10 +30428,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="158" t="s">
+      <c r="A4" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="142" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30446,133 +30442,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="158"/>
-      <c r="B5" s="157"/>
-      <c r="C5" s="168" t="s">
+      <c r="A5" s="143"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="153" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="167" t="s">
+      <c r="D5" s="152" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="158"/>
-      <c r="B6" s="157"/>
-      <c r="C6" s="168"/>
-      <c r="D6" s="167"/>
+      <c r="A6" s="143"/>
+      <c r="B6" s="142"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="152"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="158"/>
-      <c r="B7" s="157"/>
+      <c r="A7" s="143"/>
+      <c r="B7" s="142"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="158"/>
-      <c r="B8" s="157"/>
+      <c r="A8" s="143"/>
+      <c r="B8" s="142"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="158"/>
-      <c r="B9" s="157"/>
+      <c r="A9" s="143"/>
+      <c r="B9" s="142"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="160" t="s">
+      <c r="A10" s="145" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="142" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="170"/>
-      <c r="D10" s="167" t="s">
+      <c r="C10" s="155"/>
+      <c r="D10" s="152" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="160"/>
-      <c r="B11" s="157"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="167"/>
+      <c r="A11" s="145"/>
+      <c r="B11" s="142"/>
+      <c r="C11" s="155"/>
+      <c r="D11" s="152"/>
     </row>
     <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="160"/>
-      <c r="B12" s="157"/>
-      <c r="C12" s="170"/>
-      <c r="D12" s="167"/>
+      <c r="A12" s="145"/>
+      <c r="B12" s="142"/>
+      <c r="C12" s="155"/>
+      <c r="D12" s="152"/>
     </row>
     <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="143" t="s">
+      <c r="A13" s="128" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="152" t="s">
+      <c r="B13" s="137" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="169"/>
-      <c r="D13" s="167" t="s">
+      <c r="C13" s="154"/>
+      <c r="D13" s="152" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="143"/>
-      <c r="B14" s="152"/>
-      <c r="C14" s="169"/>
-      <c r="D14" s="167"/>
+      <c r="A14" s="128"/>
+      <c r="B14" s="137"/>
+      <c r="C14" s="154"/>
+      <c r="D14" s="152"/>
     </row>
     <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="143"/>
-      <c r="B15" s="152"/>
-      <c r="C15" s="169"/>
+      <c r="A15" s="128"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="154"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="143"/>
-      <c r="B16" s="152"/>
-      <c r="C16" s="169"/>
+      <c r="A16" s="128"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="154"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="143"/>
-      <c r="B17" s="152"/>
-      <c r="C17" s="169"/>
+      <c r="A17" s="128"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="154"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="143"/>
-      <c r="B18" s="152"/>
-      <c r="C18" s="169"/>
+      <c r="A18" s="128"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="154"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="143"/>
-      <c r="B19" s="152"/>
-      <c r="C19" s="169"/>
+      <c r="A19" s="128"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="154"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="143"/>
-      <c r="B20" s="152"/>
-      <c r="C20" s="169"/>
+      <c r="A20" s="128"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="154"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="143"/>
-      <c r="B21" s="152"/>
-      <c r="C21" s="169"/>
+      <c r="A21" s="128"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="154"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="143"/>
-      <c r="B22" s="152"/>
-      <c r="C22" s="169"/>
+      <c r="A22" s="128"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="154"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="143"/>
-      <c r="B23" s="152"/>
-      <c r="C23" s="169"/>
+      <c r="A23" s="128"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="154"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30670,10 +30666,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="161" t="s">
+      <c r="A32" s="146" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="149" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30684,26 +30680,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="162"/>
-      <c r="B33" s="165"/>
+      <c r="A33" s="147"/>
+      <c r="B33" s="150"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="162"/>
-      <c r="B34" s="165"/>
+      <c r="A34" s="147"/>
+      <c r="B34" s="150"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="162"/>
-      <c r="B35" s="165"/>
+      <c r="A35" s="147"/>
+      <c r="B35" s="150"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="163"/>
-      <c r="B36" s="166"/>
+      <c r="A36" s="148"/>
+      <c r="B36" s="151"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30732,10 +30728,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="159" t="s">
+      <c r="A39" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="157" t="s">
+      <c r="B39" s="142" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30746,8 +30742,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="159"/>
-      <c r="B40" s="157"/>
+      <c r="A40" s="144"/>
+      <c r="B40" s="142"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30756,84 +30752,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="158" t="s">
+      <c r="A41" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="157" t="s">
+      <c r="B41" s="142" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="170" t="s">
+      <c r="C41" s="155" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="143" t="s">
+      <c r="D41" s="128" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="158"/>
-      <c r="B42" s="157"/>
-      <c r="C42" s="170"/>
-      <c r="D42" s="143"/>
+      <c r="A42" s="143"/>
+      <c r="B42" s="142"/>
+      <c r="C42" s="155"/>
+      <c r="D42" s="128"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="158"/>
-      <c r="B43" s="157"/>
-      <c r="C43" s="170" t="s">
+      <c r="A43" s="143"/>
+      <c r="B43" s="142"/>
+      <c r="C43" s="155" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="153" t="s">
+      <c r="D43" s="138" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="158"/>
-      <c r="B44" s="157"/>
-      <c r="C44" s="170"/>
-      <c r="D44" s="153"/>
+      <c r="A44" s="143"/>
+      <c r="B44" s="142"/>
+      <c r="C44" s="155"/>
+      <c r="D44" s="138"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="151" t="s">
+      <c r="A45" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="152" t="s">
+      <c r="B45" s="137" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="174"/>
+      <c r="C45" s="159"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="151"/>
-      <c r="B46" s="152"/>
-      <c r="C46" s="175"/>
-      <c r="D46" s="171" t="s">
+      <c r="A46" s="136"/>
+      <c r="B46" s="137"/>
+      <c r="C46" s="160"/>
+      <c r="D46" s="156" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="151"/>
-      <c r="B47" s="152"/>
-      <c r="C47" s="175"/>
-      <c r="D47" s="172"/>
+      <c r="A47" s="136"/>
+      <c r="B47" s="137"/>
+      <c r="C47" s="160"/>
+      <c r="D47" s="157"/>
     </row>
     <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="151"/>
-      <c r="B48" s="152"/>
-      <c r="C48" s="176"/>
-      <c r="D48" s="172"/>
+      <c r="A48" s="136"/>
+      <c r="B48" s="137"/>
+      <c r="C48" s="161"/>
+      <c r="D48" s="157"/>
     </row>
     <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="151"/>
-      <c r="B49" s="152"/>
-      <c r="C49" s="146"/>
-      <c r="D49" s="172"/>
+      <c r="A49" s="136"/>
+      <c r="B49" s="137"/>
+      <c r="C49" s="131"/>
+      <c r="D49" s="157"/>
     </row>
     <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="151"/>
-      <c r="B50" s="152"/>
-      <c r="C50" s="146"/>
-      <c r="D50" s="173"/>
+      <c r="A50" s="136"/>
+      <c r="B50" s="137"/>
+      <c r="C50" s="131"/>
+      <c r="D50" s="158"/>
     </row>
     <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
@@ -30856,10 +30852,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="152" t="s">
+      <c r="A53" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="152" t="s">
+      <c r="B53" s="137" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30870,8 +30866,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="152"/>
-      <c r="B54" s="152"/>
+      <c r="A54" s="137"/>
+      <c r="B54" s="137"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30880,8 +30876,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="152"/>
-      <c r="B55" s="152"/>
+      <c r="A55" s="137"/>
+      <c r="B55" s="137"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30890,9 +30886,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="152"/>
-      <c r="B56" s="152"/>
-      <c r="C56" s="177" t="s">
+      <c r="A56" s="137"/>
+      <c r="B56" s="137"/>
+      <c r="C56" s="162" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30900,16 +30896,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="152"/>
-      <c r="B57" s="152"/>
-      <c r="C57" s="177"/>
+      <c r="A57" s="137"/>
+      <c r="B57" s="137"/>
+      <c r="C57" s="162"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="152"/>
-      <c r="B58" s="152"/>
+      <c r="A58" s="137"/>
+      <c r="B58" s="137"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30918,8 +30914,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="152"/>
-      <c r="B59" s="152"/>
+      <c r="A59" s="137"/>
+      <c r="B59" s="137"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30928,9 +30924,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="152"/>
-      <c r="B60" s="152"/>
-      <c r="C60" s="177" t="s">
+      <c r="A60" s="137"/>
+      <c r="B60" s="137"/>
+      <c r="C60" s="162" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -30938,25 +30934,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="152"/>
-      <c r="B61" s="152"/>
-      <c r="C61" s="177"/>
+      <c r="A61" s="137"/>
+      <c r="B61" s="137"/>
+      <c r="C61" s="162"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="152"/>
-      <c r="B62" s="152"/>
-      <c r="C62" s="177"/>
+      <c r="A62" s="137"/>
+      <c r="B62" s="137"/>
+      <c r="C62" s="162"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="152"/>
-      <c r="B63" s="152"/>
-      <c r="C63" s="170" t="s">
+      <c r="A63" s="137"/>
+      <c r="B63" s="137"/>
+      <c r="C63" s="155" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -30964,30 +30960,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="152"/>
-      <c r="B64" s="152"/>
-      <c r="C64" s="170"/>
-      <c r="D64" s="153" t="s">
+      <c r="A64" s="137"/>
+      <c r="B64" s="137"/>
+      <c r="C64" s="155"/>
+      <c r="D64" s="138" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="152"/>
-      <c r="B65" s="152"/>
-      <c r="C65" s="170"/>
-      <c r="D65" s="153"/>
+      <c r="A65" s="137"/>
+      <c r="B65" s="137"/>
+      <c r="C65" s="155"/>
+      <c r="D65" s="138"/>
     </row>
     <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="152"/>
-      <c r="B66" s="152"/>
-      <c r="C66" s="170"/>
-      <c r="D66" s="153"/>
+      <c r="A66" s="137"/>
+      <c r="B66" s="137"/>
+      <c r="C66" s="155"/>
+      <c r="D66" s="138"/>
     </row>
     <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="152"/>
-      <c r="B67" s="152"/>
-      <c r="C67" s="170"/>
-      <c r="D67" s="153"/>
+      <c r="A67" s="137"/>
+      <c r="B67" s="137"/>
+      <c r="C67" s="155"/>
+      <c r="D67" s="138"/>
     </row>
     <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39"/>
@@ -31084,10 +31080,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31105,7 +31101,7 @@
       <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="55" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="57" t="s">
@@ -31117,28 +31113,28 @@
         <v>24</v>
       </c>
       <c r="B2" s="39"/>
-      <c r="C2" s="101"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="143" t="s">
+      <c r="A3" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="162" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="100"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="58" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="143"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="113" t="s">
+      <c r="A4" s="128"/>
+      <c r="B4" s="162"/>
+      <c r="C4" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="D4" s="117" t="s">
+      <c r="D4" s="102" t="s">
         <v>256</v>
       </c>
     </row>
@@ -31146,11 +31142,11 @@
       <c r="A5" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="113" t="s">
+      <c r="B5" s="162"/>
+      <c r="C5" s="106" t="s">
         <v>235</v>
       </c>
-      <c r="D5" s="111" t="s">
+      <c r="D5" s="104" t="s">
         <v>236</v>
       </c>
     </row>
@@ -31158,707 +31154,881 @@
       <c r="A6" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="177"/>
-      <c r="C6" s="113" t="s">
+      <c r="B6" s="162"/>
+      <c r="C6" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D6" s="104" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="186" t="s">
+      <c r="A7" s="162" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="177"/>
-      <c r="C7" s="100"/>
+      <c r="B7" s="162"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="187"/>
-      <c r="B8" s="177"/>
-      <c r="C8" s="100"/>
+      <c r="A8" s="162"/>
+      <c r="B8" s="162"/>
+      <c r="C8" s="58"/>
       <c r="D8" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>290</v>
-      </c>
-      <c r="B9" s="177"/>
-      <c r="C9" s="100" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="58"/>
+      <c r="A9" s="162"/>
+      <c r="B9" s="162"/>
+      <c r="C9" s="110" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="58" t="s">
+        <v>290</v>
+      </c>
+      <c r="B10" s="162"/>
+      <c r="C10" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="58"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="177"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="111" t="s">
+      <c r="B11" s="162"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="104" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="190" t="s">
-        <v>237</v>
-      </c>
-      <c r="B12" s="181" t="s">
-        <v>234</v>
-      </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="58" t="s">
-        <v>258</v>
+      <c r="A12" s="100" t="s">
+        <v>331</v>
+      </c>
+      <c r="B12" s="162"/>
+      <c r="C12" s="58" t="s">
+        <v>332</v>
+      </c>
+      <c r="D12" s="100" t="s">
+        <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="191"/>
-      <c r="B13" s="182"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="58" t="s">
-        <v>252</v>
-      </c>
+    <row r="13" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="191"/>
-      <c r="B14" s="182"/>
-      <c r="C14" s="100"/>
+      <c r="A14" s="163" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="162" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="58"/>
       <c r="D14" s="58" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="192"/>
-      <c r="B15" s="183"/>
-      <c r="C15" s="58" t="s">
-        <v>300</v>
-      </c>
+      <c r="A15" s="163"/>
+      <c r="B15" s="162"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="58" t="s">
-        <v>301</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="197" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="177" t="s">
-        <v>234</v>
-      </c>
-      <c r="C16" s="58" t="s">
-        <v>303</v>
-      </c>
-      <c r="D16" s="107" t="s">
-        <v>304</v>
+      <c r="A16" s="163"/>
+      <c r="B16" s="162"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="198"/>
-      <c r="B17" s="177"/>
-      <c r="C17" s="58"/>
+      <c r="A17" s="163"/>
+      <c r="B17" s="162"/>
+      <c r="C17" s="58" t="s">
+        <v>300</v>
+      </c>
       <c r="D17" s="58" t="s">
-        <v>238</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="177" t="s">
-        <v>222</v>
-      </c>
-      <c r="B18" s="177" t="s">
-        <v>234</v>
-      </c>
-      <c r="C18" s="194" t="s">
-        <v>239</v>
-      </c>
-      <c r="D18" s="118" t="s">
-        <v>241</v>
+      <c r="A18" s="163"/>
+      <c r="B18" s="162"/>
+      <c r="C18" s="58" t="s">
+        <v>328</v>
+      </c>
+      <c r="D18" s="100" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="177"/>
-      <c r="B19" s="177"/>
-      <c r="C19" s="194"/>
-      <c r="D19" s="107" t="s">
-        <v>278</v>
+      <c r="A19" s="144" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="162" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="100" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="177"/>
-      <c r="B20" s="177"/>
-      <c r="C20" s="194" t="s">
-        <v>240</v>
-      </c>
+      <c r="A20" s="144"/>
+      <c r="B20" s="162"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="58" t="s">
-        <v>299</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="177"/>
-      <c r="B21" s="177"/>
-      <c r="C21" s="194"/>
-      <c r="D21" s="61" t="s">
-        <v>242</v>
+      <c r="A21" s="144"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="108" t="s">
+        <v>329</v>
+      </c>
+      <c r="D21" s="100" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="177"/>
-      <c r="B22" s="177"/>
-      <c r="C22" s="120" t="s">
-        <v>307</v>
-      </c>
-      <c r="D22" s="58" t="s">
-        <v>308</v>
+      <c r="A22" s="128" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" s="162" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="165" t="s">
+        <v>239</v>
+      </c>
+      <c r="D22" s="103" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="152" t="s">
-        <v>296</v>
-      </c>
-      <c r="B23" s="177" t="s">
-        <v>234</v>
-      </c>
-      <c r="C23" s="58" t="s">
-        <v>297</v>
-      </c>
-      <c r="D23" s="58" t="s">
-        <v>298</v>
+      <c r="A23" s="128"/>
+      <c r="B23" s="162"/>
+      <c r="C23" s="165"/>
+      <c r="D23" s="100" t="s">
+        <v>278</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="152"/>
-      <c r="B24" s="177"/>
-      <c r="C24" s="61" t="s">
-        <v>281</v>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="128"/>
+      <c r="B24" s="162"/>
+      <c r="C24" s="165" t="s">
+        <v>240</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="44"/>
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="128"/>
+      <c r="B25" s="162"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="61" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="186" t="s">
-        <v>260</v>
-      </c>
-      <c r="B26" s="177" t="s">
-        <v>234</v>
-      </c>
-      <c r="C26" s="100"/>
-      <c r="D26" s="79" t="s">
-        <v>261</v>
+      <c r="A26" s="128"/>
+      <c r="B26" s="162"/>
+      <c r="C26" s="105" t="s">
+        <v>307</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="187"/>
-      <c r="B27" s="177"/>
-      <c r="C27" s="100"/>
+      <c r="A27" s="128"/>
+      <c r="B27" s="162"/>
+      <c r="C27" s="105">
+        <v>2.1</v>
+      </c>
       <c r="D27" s="58" t="s">
-        <v>257</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="B28" s="104" t="s">
+      <c r="A28" s="128"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="105" t="s">
+        <v>239</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="137" t="s">
+        <v>296</v>
+      </c>
+      <c r="B29" s="162" t="s">
         <v>234</v>
       </c>
-      <c r="C28" s="113" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="111" t="s">
-        <v>30</v>
+      <c r="C29" s="58" t="s">
+        <v>297</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>298</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="152" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="177" t="s">
-        <v>234</v>
-      </c>
-      <c r="C29" s="122" t="s">
-        <v>268</v>
-      </c>
-      <c r="D29" s="58" t="s">
-        <v>251</v>
+    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="137"/>
+      <c r="B30" s="162"/>
+      <c r="C30" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>280</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="152"/>
-      <c r="B30" s="177"/>
-      <c r="C30" s="122" t="s">
-        <v>270</v>
-      </c>
-      <c r="D30" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="152"/>
-      <c r="B31" s="177"/>
-      <c r="C31" s="122" t="s">
-        <v>269</v>
-      </c>
-      <c r="D31" s="58" t="s">
-        <v>251</v>
-      </c>
+    <row r="31" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="44"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="152"/>
-      <c r="B32" s="177"/>
-      <c r="C32" s="123" t="s">
-        <v>277</v>
-      </c>
-      <c r="D32" s="107" t="s">
-        <v>102</v>
+      <c r="A32" s="128" t="s">
+        <v>260</v>
+      </c>
+      <c r="B32" s="162" t="s">
+        <v>234</v>
+      </c>
+      <c r="C32" s="58"/>
+      <c r="D32" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="152"/>
-      <c r="B33" s="177"/>
-      <c r="C33" s="122" t="s">
-        <v>282</v>
-      </c>
+      <c r="A33" s="128"/>
+      <c r="B33" s="162"/>
+      <c r="C33" s="58"/>
       <c r="D33" s="58" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="152"/>
-      <c r="B34" s="177"/>
-      <c r="C34" s="122" t="s">
-        <v>283</v>
-      </c>
-      <c r="D34" s="58" t="s">
-        <v>284</v>
+      <c r="A34" s="58" t="s">
+        <v>334</v>
+      </c>
+      <c r="B34" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="C34" s="79" t="s">
+        <v>335</v>
+      </c>
+      <c r="D34" s="100" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="152"/>
-      <c r="B35" s="177"/>
-      <c r="C35" s="123" t="s">
-        <v>288</v>
-      </c>
-      <c r="D35" s="107" t="s">
-        <v>251</v>
+      <c r="A35" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35" s="105" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" s="106" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="104" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="152"/>
-      <c r="B36" s="177"/>
-      <c r="C36" s="123" t="s">
-        <v>302</v>
-      </c>
-      <c r="D36" s="107" t="s">
+    <row r="36" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="137" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="162" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="58" t="s">
+        <v>268</v>
+      </c>
+      <c r="D36" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="152"/>
-      <c r="B37" s="177"/>
-      <c r="C37" s="123" t="s">
-        <v>289</v>
-      </c>
-      <c r="D37" s="107" t="s">
+      <c r="A37" s="137"/>
+      <c r="B37" s="162"/>
+      <c r="C37" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="D37" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="137"/>
+      <c r="B38" s="162"/>
+      <c r="C38" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="137"/>
+      <c r="B39" s="162"/>
+      <c r="C39" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D39" s="100" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="152"/>
-      <c r="B38" s="177"/>
-      <c r="C38" s="124" t="s">
-        <v>244</v>
-      </c>
-      <c r="D38" s="119" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="152"/>
-      <c r="B39" s="177"/>
-      <c r="C39" s="125" t="s">
-        <v>311</v>
-      </c>
-      <c r="D39" s="107" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="152"/>
-      <c r="B40" s="177"/>
-      <c r="C40" s="122" t="s">
-        <v>312</v>
+      <c r="A40" s="137"/>
+      <c r="B40" s="162"/>
+      <c r="C40" s="58" t="s">
+        <v>282</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>100</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="152"/>
-      <c r="B41" s="177"/>
-      <c r="C41" s="123" t="s">
-        <v>313</v>
-      </c>
-      <c r="D41" s="107" t="s">
-        <v>314</v>
+      <c r="A41" s="137"/>
+      <c r="B41" s="162"/>
+      <c r="C41" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="152"/>
-      <c r="B42" s="177"/>
-      <c r="C42" s="123" t="s">
-        <v>315</v>
-      </c>
-      <c r="D42" s="107" t="s">
-        <v>102</v>
+      <c r="A42" s="137"/>
+      <c r="B42" s="162"/>
+      <c r="C42" s="100" t="s">
+        <v>288</v>
+      </c>
+      <c r="D42" s="100" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="152"/>
-      <c r="B43" s="177"/>
-      <c r="C43" s="126" t="s">
-        <v>268</v>
-      </c>
-      <c r="D43" s="127" t="s">
-        <v>102</v>
+      <c r="A43" s="137"/>
+      <c r="B43" s="162"/>
+      <c r="C43" s="100" t="s">
+        <v>302</v>
+      </c>
+      <c r="D43" s="100" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B44" s="121" t="s">
-        <v>234</v>
-      </c>
-      <c r="C44" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="107" t="s">
-        <v>274</v>
+      <c r="A44" s="137"/>
+      <c r="B44" s="162"/>
+      <c r="C44" s="100" t="s">
+        <v>289</v>
+      </c>
+      <c r="D44" s="100" t="s">
+        <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="58" t="s">
-        <v>310</v>
-      </c>
-      <c r="B45" s="121" t="s">
-        <v>234</v>
-      </c>
-      <c r="C45" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="107" t="s">
-        <v>274</v>
+    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="137"/>
+      <c r="B45" s="162"/>
+      <c r="C45" s="107" t="s">
+        <v>244</v>
+      </c>
+      <c r="D45" s="104" t="s">
+        <v>245</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="101"/>
-      <c r="D46" s="44"/>
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="137"/>
+      <c r="B46" s="162"/>
+      <c r="C46" s="108" t="s">
+        <v>311</v>
+      </c>
+      <c r="D46" s="100" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="47" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="99"/>
-      <c r="B47" s="67"/>
-      <c r="C47" s="100"/>
-      <c r="D47" s="79" t="s">
-        <v>261</v>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="137"/>
+      <c r="B47" s="162"/>
+      <c r="C47" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D47" s="58" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="177" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" s="177" t="s">
-        <v>234</v>
-      </c>
-      <c r="C48" s="113" t="s">
-        <v>246</v>
-      </c>
-      <c r="D48" s="58" t="s">
-        <v>253</v>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="137"/>
+      <c r="B48" s="162"/>
+      <c r="C48" s="100" t="s">
+        <v>313</v>
+      </c>
+      <c r="D48" s="100" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="177"/>
-      <c r="B49" s="177"/>
-      <c r="C49" s="113">
-        <v>10.1</v>
-      </c>
-      <c r="D49" s="58" t="s">
-        <v>272</v>
+      <c r="A49" s="137"/>
+      <c r="B49" s="162"/>
+      <c r="C49" s="100" t="s">
+        <v>315</v>
+      </c>
+      <c r="D49" s="100" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="177"/>
-      <c r="B50" s="177"/>
-      <c r="C50" s="113">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D50" s="58" t="s">
-        <v>272</v>
+      <c r="A50" s="137"/>
+      <c r="B50" s="162"/>
+      <c r="C50" s="100" t="s">
+        <v>268</v>
+      </c>
+      <c r="D50" s="100" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="177"/>
-      <c r="B51" s="177"/>
-      <c r="C51" s="114" t="s">
-        <v>293</v>
-      </c>
-      <c r="D51" s="109" t="s">
-        <v>294</v>
+      <c r="A51" s="137"/>
+      <c r="B51" s="162"/>
+      <c r="C51" s="58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D51" s="58" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="143" t="s">
-        <v>247</v>
-      </c>
-      <c r="B52" s="177" t="s">
-        <v>234</v>
-      </c>
-      <c r="C52" s="195"/>
-      <c r="D52" s="193" t="s">
-        <v>261</v>
+      <c r="A52" s="137"/>
+      <c r="B52" s="162"/>
+      <c r="C52" s="100" t="s">
+        <v>283</v>
+      </c>
+      <c r="D52" s="100" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="143"/>
-      <c r="B53" s="177"/>
-      <c r="C53" s="196"/>
-      <c r="D53" s="193"/>
+      <c r="A53" s="137"/>
+      <c r="B53" s="162"/>
+      <c r="C53" s="100" t="s">
+        <v>319</v>
+      </c>
+      <c r="D53" s="100" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="105" t="s">
-        <v>262</v>
-      </c>
-      <c r="B54" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C54" s="113" t="s">
-        <v>250</v>
-      </c>
-      <c r="D54" s="107" t="s">
+    <row r="54" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="137"/>
+      <c r="B54" s="162"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="109" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="137"/>
+      <c r="B55" s="162"/>
+      <c r="C55" s="100" t="s">
+        <v>322</v>
+      </c>
+      <c r="D55" s="100" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="103"/>
-      <c r="D55" s="98"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="B56" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C56" s="115" t="s">
-        <v>265</v>
-      </c>
-      <c r="D56" s="58" t="s">
-        <v>267</v>
+      <c r="A56" s="137"/>
+      <c r="B56" s="162"/>
+      <c r="C56" s="100" t="s">
+        <v>268</v>
+      </c>
+      <c r="D56" s="100" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="178" t="s">
-        <v>285</v>
-      </c>
-      <c r="B57" s="181" t="s">
-        <v>234</v>
-      </c>
-      <c r="C57" s="116" t="s">
-        <v>295</v>
-      </c>
-      <c r="D57" s="58" t="s">
+      <c r="A57" s="137"/>
+      <c r="B57" s="162"/>
+      <c r="C57" s="100" t="s">
+        <v>339</v>
+      </c>
+      <c r="D57" s="100" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="179"/>
-      <c r="B58" s="182"/>
-      <c r="C58" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="D58" s="107" t="s">
-        <v>306</v>
+      <c r="A58" s="137"/>
+      <c r="B58" s="162"/>
+      <c r="C58" s="100" t="s">
+        <v>340</v>
+      </c>
+      <c r="D58" s="100" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="180"/>
-      <c r="B59" s="183"/>
-      <c r="C59" s="115" t="s">
-        <v>286</v>
-      </c>
-      <c r="D59" s="58" t="s">
-        <v>287</v>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="137"/>
+      <c r="B59" s="162"/>
+      <c r="C59" s="100" t="s">
+        <v>324</v>
+      </c>
+      <c r="D59" s="100" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="98"/>
-      <c r="C60" s="110"/>
-      <c r="D60" s="98"/>
+      <c r="A60" s="58"/>
+      <c r="B60" s="58"/>
+      <c r="C60" s="100" t="s">
+        <v>338</v>
+      </c>
+      <c r="D60" s="100" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="184" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="188" t="s">
-        <v>271</v>
-      </c>
-      <c r="C61" s="115" t="s">
-        <v>265</v>
-      </c>
-      <c r="D61" s="58" t="s">
-        <v>267</v>
+      <c r="A61" s="58" t="s">
+        <v>309</v>
+      </c>
+      <c r="B61" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C61" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" s="100" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="185"/>
-      <c r="B62" s="189"/>
-      <c r="C62" s="115" t="s">
-        <v>265</v>
-      </c>
-      <c r="D62" s="58" t="s">
-        <v>266</v>
+      <c r="A62" s="58" t="s">
+        <v>310</v>
+      </c>
+      <c r="B62" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C62" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="100" t="s">
+        <v>274</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="97" t="s">
-        <v>59</v>
-      </c>
-      <c r="B63" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C63" s="102" t="s">
-        <v>264</v>
-      </c>
-      <c r="D63" s="58" t="s">
-        <v>100</v>
-      </c>
+    <row r="63" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="44"/>
     </row>
-    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B64" s="108" t="s">
-        <v>271</v>
-      </c>
-      <c r="C64" s="100"/>
-      <c r="D64" s="61" t="s">
-        <v>292</v>
+    <row r="64" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="99"/>
+      <c r="B64" s="67"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="97" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C65" s="102" t="s">
-        <v>264</v>
+    <row r="65" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="162" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="162" t="s">
+        <v>234</v>
+      </c>
+      <c r="C65" s="106" t="s">
+        <v>246</v>
       </c>
       <c r="D65" s="58" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B66" s="98"/>
-      <c r="C66" s="110"/>
-      <c r="D66" s="98"/>
+      <c r="A66" s="162"/>
+      <c r="B66" s="162"/>
+      <c r="C66" s="106">
+        <v>10.1</v>
+      </c>
+      <c r="D66" s="58" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="58"/>
-      <c r="B67" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C67" s="100" t="s">
-        <v>30</v>
-      </c>
-      <c r="D67" s="107" t="s">
-        <v>274</v>
+      <c r="A67" s="162"/>
+      <c r="B67" s="162"/>
+      <c r="C67" s="106">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D67" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="98" t="s">
-        <v>279</v>
-      </c>
-      <c r="B68" s="98"/>
-      <c r="C68" s="110"/>
-      <c r="D68" s="98"/>
+      <c r="A68" s="162"/>
+      <c r="B68" s="162"/>
+      <c r="C68" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="D68" s="101" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="58"/>
-      <c r="B69" s="106" t="s">
+      <c r="A69" s="128" t="s">
+        <v>247</v>
+      </c>
+      <c r="B69" s="162" t="s">
         <v>234</v>
       </c>
-      <c r="C69" s="100" t="s">
+      <c r="C69" s="162"/>
+      <c r="D69" s="164" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="128"/>
+      <c r="B70" s="162"/>
+      <c r="C70" s="162"/>
+      <c r="D70" s="164"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="104" t="s">
+        <v>262</v>
+      </c>
+      <c r="B71" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" s="106" t="s">
+        <v>250</v>
+      </c>
+      <c r="D71" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B72" s="39"/>
+      <c r="C72" s="98"/>
+      <c r="D72" s="98"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B73" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="112" t="s">
+        <v>265</v>
+      </c>
+      <c r="D73" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="128" t="s">
+        <v>285</v>
+      </c>
+      <c r="B74" s="162" t="s">
+        <v>234</v>
+      </c>
+      <c r="C74" s="101" t="s">
+        <v>295</v>
+      </c>
+      <c r="D74" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="128"/>
+      <c r="B75" s="162"/>
+      <c r="C75" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D75" s="100" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="128"/>
+      <c r="B76" s="162"/>
+      <c r="C76" s="112" t="s">
+        <v>286</v>
+      </c>
+      <c r="D76" s="58" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B77" s="98"/>
+      <c r="C77" s="98"/>
+      <c r="D77" s="98"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="145" t="s">
+        <v>58</v>
+      </c>
+      <c r="B78" s="162" t="s">
+        <v>271</v>
+      </c>
+      <c r="C78" s="112" t="s">
+        <v>265</v>
+      </c>
+      <c r="D78" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="145"/>
+      <c r="B79" s="162"/>
+      <c r="C79" s="112" t="s">
+        <v>265</v>
+      </c>
+      <c r="D79" s="58" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="97" t="s">
+        <v>59</v>
+      </c>
+      <c r="B80" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C80" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D80" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="B81" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C81" s="58"/>
+      <c r="D81" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B82" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C82" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D82" s="58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B83" s="98"/>
+      <c r="C83" s="98"/>
+      <c r="D83" s="98"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="58"/>
+      <c r="B84" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="107" t="s">
+      <c r="D84" s="100" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B85" s="98"/>
+      <c r="C85" s="98"/>
+      <c r="D85" s="98"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="58"/>
+      <c r="B86" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C86" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86" s="100" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A36:A59"/>
+    <mergeCell ref="B36:B59"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A69:A70"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A29:A43"/>
-    <mergeCell ref="B29:B43"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B3:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated date format and added SOAP workshop slides
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PMOD_Documentation\paye-employers-documentation\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owalsh01\IdeaProjects\paye-employers-documentation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7656" yWindow="288" windowWidth="15396" windowHeight="10008" activeTab="3"/>
+    <workbookView xWindow="7650" yWindow="285" windowWidth="15390" windowHeight="10005" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="353">
   <si>
     <t>Document</t>
   </si>
@@ -2908,6 +2908,12 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>SOAP Request Authentication</t>
+  </si>
+  <si>
+    <t>Accepted Date specification updated</t>
   </si>
 </sst>
 </file>
@@ -3491,7 +3497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3793,6 +3799,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3838,38 +3850,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3892,6 +3874,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3911,45 +3953,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3972,6 +3975,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4350,15 +4362,15 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="48.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4375,18 +4387,18 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="117" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="119"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="121"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
@@ -4403,18 +4415,18 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="117" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="119"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="121"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>33</v>
       </c>
@@ -4431,7 +4443,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>34</v>
       </c>
@@ -4448,11 +4460,11 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="120" t="s">
+    <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="123">
+      <c r="B7" s="125">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4465,9 +4477,9 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="121"/>
-      <c r="B8" s="124"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="123"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4478,9 +4490,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="121"/>
-      <c r="B9" s="124"/>
+    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="123"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4491,9 +4503,9 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="121"/>
-      <c r="B10" s="124"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="123"/>
+      <c r="B10" s="126"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4504,9 +4516,9 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="121"/>
-      <c r="B11" s="124"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="123"/>
+      <c r="B11" s="126"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4517,9 +4529,9 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="122"/>
-      <c r="B12" s="125"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="124"/>
+      <c r="B12" s="127"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4530,11 +4542,11 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="128" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="123">
+      <c r="B13" s="125">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4547,9 +4559,9 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="129"/>
-      <c r="B14" s="125"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="131"/>
+      <c r="B14" s="127"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4560,7 +4572,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>44</v>
       </c>
@@ -4577,7 +4589,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>45</v>
       </c>
@@ -4594,18 +4606,18 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="117" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="119"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="121"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
@@ -4622,7 +4634,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
@@ -4639,22 +4651,22 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="117" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="118"/>
-      <c r="C20" s="118"/>
-      <c r="D20" s="119"/>
+      <c r="B20" s="120"/>
+      <c r="C20" s="120"/>
+      <c r="D20" s="121"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="130" t="s">
+    <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="127">
+      <c r="B21" s="129">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4667,9 +4679,9 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="131"/>
-      <c r="B22" s="125"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="133"/>
+      <c r="B22" s="127"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4677,7 +4689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>32</v>
       </c>
@@ -4691,19 +4703,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="117" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="118"/>
-      <c r="C24" s="118"/>
-      <c r="D24" s="119"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="121"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="126" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="127">
+      <c r="B25" s="129">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4716,9 +4728,9 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="121"/>
-      <c r="B26" s="124"/>
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="123"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4729,9 +4741,9 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="121"/>
-      <c r="B27" s="124"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="123"/>
+      <c r="B27" s="126"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4742,9 +4754,9 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="121"/>
-      <c r="B28" s="124"/>
+    <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="123"/>
+      <c r="B28" s="126"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4755,9 +4767,9 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="121"/>
-      <c r="B29" s="124"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="123"/>
+      <c r="B29" s="126"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4768,9 +4780,9 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="121"/>
-      <c r="B30" s="124"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="123"/>
+      <c r="B30" s="126"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4781,9 +4793,9 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="121"/>
-      <c r="B31" s="124"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="123"/>
+      <c r="B31" s="126"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4794,9 +4806,9 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="122"/>
-      <c r="B32" s="125"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="124"/>
+      <c r="B32" s="127"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4807,7 +4819,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -4821,7 +4833,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>49</v>
       </c>
@@ -4835,7 +4847,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>50</v>
       </c>
@@ -4849,7 +4861,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4863,7 +4875,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4877,7 +4889,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>53</v>
       </c>
@@ -4891,7 +4903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>46</v>
       </c>
@@ -4905,7 +4917,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -4919,15 +4931,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="117" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="118"/>
-      <c r="C41" s="118"/>
-      <c r="D41" s="119"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="121"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>57</v>
       </c>
@@ -4941,7 +4953,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>58</v>
       </c>
@@ -4955,7 +4967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>59</v>
       </c>
@@ -4969,7 +4981,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>60</v>
       </c>
@@ -4985,7 +4997,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4995,7 +5007,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5030,15 +5042,15 @@
       <selection activeCell="A30" sqref="A30:A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" style="42" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -5052,7 +5064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -5060,7 +5072,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>81</v>
       </c>
@@ -5072,7 +5084,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>82</v>
       </c>
@@ -5084,7 +5096,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>78</v>
       </c>
@@ -5096,7 +5108,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>24</v>
       </c>
@@ -5104,11 +5116,11 @@
       <c r="C6" s="39"/>
       <c r="D6" s="44"/>
     </row>
-    <row r="7" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="132" t="s">
+    <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="133" t="s">
+      <c r="B7" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5118,9 +5130,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="132"/>
-      <c r="B8" s="133"/>
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="149"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5128,9 +5140,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="132"/>
-      <c r="B9" s="133"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="149"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5138,9 +5150,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="132"/>
-      <c r="B10" s="133"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="149"/>
+      <c r="B10" s="148"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5148,9 +5160,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="132"/>
-      <c r="B11" s="133"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="149"/>
+      <c r="B11" s="148"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5158,9 +5170,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="132"/>
-      <c r="B12" s="133"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="149"/>
+      <c r="B12" s="148"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5168,11 +5180,11 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="135" t="s">
+    <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="151" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="133" t="s">
+      <c r="B13" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5182,9 +5194,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="135"/>
-      <c r="B14" s="133"/>
+    <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="151"/>
+      <c r="B14" s="148"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5192,9 +5204,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="135"/>
-      <c r="B15" s="133"/>
+    <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="151"/>
+      <c r="B15" s="148"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5202,11 +5214,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="136" t="s">
+    <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="137" t="s">
+      <c r="B16" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5216,9 +5228,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="136"/>
-      <c r="B17" s="137"/>
+    <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="134"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5226,9 +5238,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="136"/>
-      <c r="B18" s="137"/>
+    <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="134"/>
+      <c r="B18" s="143"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5236,9 +5248,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="136"/>
-      <c r="B19" s="137"/>
+    <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="134"/>
+      <c r="B19" s="143"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5246,9 +5258,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="136"/>
-      <c r="B20" s="137"/>
+    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="134"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5256,9 +5268,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="136"/>
-      <c r="B21" s="137"/>
+    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="134"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5266,9 +5278,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="136"/>
-      <c r="B22" s="137"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="134"/>
+      <c r="B22" s="143"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5276,9 +5288,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="136"/>
-      <c r="B23" s="137"/>
+    <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="134"/>
+      <c r="B23" s="143"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5286,27 +5298,27 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="136"/>
-      <c r="B24" s="137"/>
-      <c r="C24" s="136" t="s">
+    <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="134"/>
+      <c r="B24" s="143"/>
+      <c r="C24" s="134" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="143" t="s">
+      <c r="D24" s="135" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="136"/>
-      <c r="B25" s="137"/>
-      <c r="C25" s="136"/>
-      <c r="D25" s="143"/>
+    <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="134"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="135"/>
     </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="132" t="s">
+    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="149" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="133" t="s">
+      <c r="B26" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5316,15 +5328,15 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="132"/>
-      <c r="B27" s="133"/>
+    <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="149"/>
+      <c r="B27" s="148"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>165</v>
       </c>
@@ -5336,7 +5348,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
@@ -5344,29 +5356,29 @@
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="134" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="150" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="133" t="s">
+      <c r="B30" s="148" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="136" t="s">
+      <c r="C30" s="134" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="146" t="s">
+      <c r="D30" s="138" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="134"/>
-      <c r="B31" s="133"/>
-      <c r="C31" s="136"/>
-      <c r="D31" s="146"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="150"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="138"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="134"/>
-      <c r="B32" s="133"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="150"/>
+      <c r="B32" s="148"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5374,9 +5386,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="134"/>
-      <c r="B33" s="133"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="150"/>
+      <c r="B33" s="148"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5384,9 +5396,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="134"/>
-      <c r="B34" s="133"/>
+    <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="150"/>
+      <c r="B34" s="148"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5394,9 +5406,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="134"/>
-      <c r="B35" s="133"/>
+    <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="150"/>
+      <c r="B35" s="148"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5404,9 +5416,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="134"/>
-      <c r="B36" s="133"/>
+    <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="150"/>
+      <c r="B36" s="148"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5414,27 +5426,27 @@
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="134"/>
-      <c r="B37" s="133"/>
-      <c r="C37" s="147" t="s">
+    <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="150"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="139" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="149" t="s">
+      <c r="D37" s="141" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="134"/>
-      <c r="B38" s="133"/>
-      <c r="C38" s="148"/>
-      <c r="D38" s="149"/>
+    <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="150"/>
+      <c r="B38" s="148"/>
+      <c r="C38" s="140"/>
+      <c r="D38" s="141"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="132" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="149" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="133" t="s">
+      <c r="B39" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5444,15 +5456,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="132"/>
-      <c r="B40" s="133"/>
+    <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="149"/>
+      <c r="B40" s="148"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>27</v>
       </c>
@@ -5464,7 +5476,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>29</v>
       </c>
@@ -5472,11 +5484,11 @@
       <c r="C42" s="39"/>
       <c r="D42" s="44"/>
     </row>
-    <row r="43" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="134" t="s">
+    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="150" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5484,9 +5496,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="134"/>
-      <c r="B44" s="133"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="150"/>
+      <c r="B44" s="148"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5494,11 +5506,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="140" t="s">
+    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="133" t="s">
+      <c r="B45" s="148" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5506,9 +5518,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="141"/>
-      <c r="B46" s="133"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="146"/>
+      <c r="B46" s="148"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5516,9 +5528,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="141"/>
-      <c r="B47" s="133"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="146"/>
+      <c r="B47" s="148"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5526,9 +5538,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="142"/>
-      <c r="B48" s="133"/>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="147"/>
+      <c r="B48" s="148"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5536,11 +5548,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A49" s="137" t="s">
+    <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A49" s="143" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="137" t="s">
+      <c r="B49" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9643,9 +9655,9 @@
       <c r="XEY49" s="42"/>
       <c r="XFC49" s="42"/>
     </row>
-    <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="137"/>
-      <c r="B50" s="137"/>
+    <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="143"/>
+      <c r="B50" s="143"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13748,9 +13760,9 @@
       <c r="XEY50" s="42"/>
       <c r="XFC50" s="42"/>
     </row>
-    <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A51" s="137"/>
-      <c r="B51" s="137"/>
+    <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A51" s="143"/>
+      <c r="B51" s="143"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17853,9 +17865,9 @@
       <c r="XEY51" s="42"/>
       <c r="XFC51" s="42"/>
     </row>
-    <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A52" s="137"/>
-      <c r="B52" s="137"/>
+    <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A52" s="143"/>
+      <c r="B52" s="143"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21958,13 +21970,13 @@
       <c r="XEY52" s="42"/>
       <c r="XFC52" s="42"/>
     </row>
-    <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A53" s="137"/>
-      <c r="B53" s="137"/>
-      <c r="C53" s="145" t="s">
+    <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A53" s="143"/>
+      <c r="B53" s="143"/>
+      <c r="C53" s="137" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="146" t="s">
+      <c r="D53" s="138" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26063,11 +26075,11 @@
       <c r="XEY53" s="42"/>
       <c r="XFC53" s="42"/>
     </row>
-    <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="137"/>
-      <c r="B54" s="137"/>
-      <c r="C54" s="145"/>
-      <c r="D54" s="146"/>
+    <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="143"/>
+      <c r="B54" s="143"/>
+      <c r="C54" s="137"/>
+      <c r="D54" s="138"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30164,7 +30176,7 @@
       <c r="XEY54" s="42"/>
       <c r="XFC54" s="42"/>
     </row>
-    <row r="55" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
       <c r="A55" s="39" t="s">
         <v>40</v>
       </c>
@@ -30172,7 +30184,7 @@
       <c r="C55" s="39"/>
       <c r="D55" s="44"/>
     </row>
-    <row r="56" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
@@ -30184,11 +30196,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A57" s="138" t="s">
+    <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A57" s="142" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="137" t="s">
+      <c r="B57" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30198,9 +30210,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="138"/>
-      <c r="B58" s="137"/>
+    <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="142"/>
+      <c r="B58" s="143"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30208,9 +30220,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A59" s="138"/>
-      <c r="B59" s="137"/>
+    <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A59" s="142"/>
+      <c r="B59" s="143"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30218,9 +30230,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="138"/>
-      <c r="B60" s="137"/>
+    <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="142"/>
+      <c r="B60" s="143"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30228,9 +30240,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A61" s="138"/>
-      <c r="B61" s="137"/>
+    <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A61" s="142"/>
+      <c r="B61" s="143"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30238,9 +30250,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A62" s="138"/>
-      <c r="B62" s="137"/>
+    <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A62" s="142"/>
+      <c r="B62" s="143"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30248,9 +30260,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A63" s="138"/>
-      <c r="B63" s="137"/>
+    <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A63" s="142"/>
+      <c r="B63" s="143"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30258,17 +30270,17 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.3">
-      <c r="A64" s="138"/>
-      <c r="B64" s="137"/>
+    <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
+      <c r="A64" s="142"/>
+      <c r="B64" s="143"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="138"/>
-      <c r="B65" s="137"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="142"/>
+      <c r="B65" s="143"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30276,17 +30288,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="138"/>
-      <c r="B66" s="137"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="142"/>
+      <c r="B66" s="143"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="138"/>
-      <c r="B67" s="137"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="142"/>
+      <c r="B67" s="143"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30294,9 +30306,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="138"/>
-      <c r="B68" s="137"/>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="142"/>
+      <c r="B68" s="143"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30304,9 +30316,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="138"/>
-      <c r="B69" s="137"/>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="142"/>
+      <c r="B69" s="143"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30314,9 +30326,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="138"/>
-      <c r="B70" s="137"/>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="142"/>
+      <c r="B70" s="143"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30324,9 +30336,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="138"/>
-      <c r="B71" s="137"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="142"/>
+      <c r="B71" s="143"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30334,9 +30346,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="138"/>
-      <c r="B72" s="137"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="142"/>
+      <c r="B72" s="143"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30344,17 +30356,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="138"/>
-      <c r="B73" s="137"/>
+    <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="142"/>
+      <c r="B73" s="143"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="138"/>
-      <c r="B74" s="137"/>
+    <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="142"/>
+      <c r="B74" s="143"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30362,21 +30374,21 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="138"/>
-      <c r="B75" s="137"/>
-      <c r="C75" s="144"/>
-      <c r="D75" s="139" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="142"/>
+      <c r="B75" s="143"/>
+      <c r="C75" s="136"/>
+      <c r="D75" s="144" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="138"/>
-      <c r="B76" s="137"/>
-      <c r="C76" s="144"/>
-      <c r="D76" s="139"/>
+    <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="142"/>
+      <c r="B76" s="143"/>
+      <c r="C76" s="136"/>
+      <c r="D76" s="144"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
         <v>56</v>
       </c>
@@ -30384,13 +30396,13 @@
       <c r="C77" s="39"/>
       <c r="D77" s="44"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="48"/>
       <c r="B78" s="40"/>
       <c r="C78" s="38"/>
       <c r="D78" s="50"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="48"/>
       <c r="B79" s="40"/>
       <c r="C79" s="38"/>
@@ -30398,8 +30410,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30408,29 +30420,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30445,6 +30441,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30459,15 +30471,15 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" customWidth="1"/>
-    <col min="4" max="4" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -30481,7 +30493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>77</v>
       </c>
@@ -30489,7 +30501,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>24</v>
       </c>
@@ -30497,11 +30509,11 @@
       <c r="C3" s="39"/>
       <c r="D3" s="44"/>
     </row>
-    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="132" t="s">
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="148" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30511,9 +30523,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="132"/>
-      <c r="B5" s="133"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="149"/>
+      <c r="B5" s="148"/>
       <c r="C5" s="159" t="s">
         <v>190</v>
       </c>
@@ -30521,59 +30533,59 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="132"/>
-      <c r="B6" s="133"/>
+    <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="149"/>
+      <c r="B6" s="148"/>
       <c r="C6" s="159"/>
       <c r="D6" s="158"/>
     </row>
-    <row r="7" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="132"/>
-      <c r="B7" s="133"/>
+    <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="149"/>
+      <c r="B7" s="148"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
-    <row r="8" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="132"/>
-      <c r="B8" s="133"/>
+    <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="149"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
-    <row r="9" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="132"/>
-      <c r="B9" s="133"/>
+    <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="149"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
-    <row r="10" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="135" t="s">
+    <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="151" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="148" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="157"/>
+      <c r="C10" s="161"/>
       <c r="D10" s="158" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="135"/>
-      <c r="B11" s="133"/>
-      <c r="C11" s="157"/>
+    <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="151"/>
+      <c r="B11" s="148"/>
+      <c r="C11" s="161"/>
       <c r="D11" s="158"/>
     </row>
-    <row r="12" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="135"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="157"/>
+    <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="151"/>
+      <c r="B12" s="148"/>
+      <c r="C12" s="161"/>
       <c r="D12" s="158"/>
     </row>
-    <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="136" t="s">
+    <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="134" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="137" t="s">
+      <c r="B13" s="143" t="s">
         <v>185</v>
       </c>
       <c r="C13" s="160"/>
@@ -30581,69 +30593,69 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="136"/>
-      <c r="B14" s="137"/>
+    <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="134"/>
+      <c r="B14" s="143"/>
       <c r="C14" s="160"/>
       <c r="D14" s="158"/>
     </row>
-    <row r="15" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="136"/>
-      <c r="B15" s="137"/>
+    <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="134"/>
+      <c r="B15" s="143"/>
       <c r="C15" s="160"/>
       <c r="D15" s="49"/>
     </row>
-    <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="136"/>
-      <c r="B16" s="137"/>
+    <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="134"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="160"/>
       <c r="D16" s="49"/>
     </row>
-    <row r="17" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="136"/>
-      <c r="B17" s="137"/>
+    <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="134"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="160"/>
       <c r="D17" s="49"/>
     </row>
-    <row r="18" spans="1:4" ht="41.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="136"/>
-      <c r="B18" s="137"/>
+    <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="134"/>
+      <c r="B18" s="143"/>
       <c r="C18" s="160"/>
       <c r="D18" s="49"/>
     </row>
-    <row r="19" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="136"/>
-      <c r="B19" s="137"/>
+    <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="134"/>
+      <c r="B19" s="143"/>
       <c r="C19" s="160"/>
       <c r="D19" s="49"/>
     </row>
-    <row r="20" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="136"/>
-      <c r="B20" s="137"/>
+    <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="134"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="160"/>
       <c r="D20" s="49"/>
     </row>
-    <row r="21" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="136"/>
-      <c r="B21" s="137"/>
+    <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="134"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="160"/>
       <c r="D21" s="49"/>
     </row>
-    <row r="22" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="136"/>
-      <c r="B22" s="137"/>
+    <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="134"/>
+      <c r="B22" s="143"/>
       <c r="C22" s="160"/>
       <c r="D22" s="49"/>
     </row>
-    <row r="23" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="136"/>
-      <c r="B23" s="137"/>
+    <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="134"/>
+      <c r="B23" s="143"/>
       <c r="C23" s="160"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="73" t="s">
         <v>187</v>
       </c>
@@ -30657,7 +30669,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="92" t="s">
         <v>231</v>
       </c>
@@ -30671,7 +30683,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>165</v>
       </c>
@@ -30683,7 +30695,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39" t="s">
         <v>28</v>
       </c>
@@ -30691,7 +30703,7 @@
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
     </row>
-    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="85" t="s">
         <v>26</v>
       </c>
@@ -30705,7 +30717,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="85"/>
       <c r="B29" s="84"/>
       <c r="C29" s="70" t="s">
@@ -30715,7 +30727,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="85"/>
       <c r="B30" s="84"/>
       <c r="C30" s="88" t="s">
@@ -30725,7 +30737,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="85"/>
       <c r="B31" s="84"/>
       <c r="C31" s="89" t="s">
@@ -30735,11 +30747,11 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="161" t="s">
+    <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="152" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="164" t="s">
+      <c r="B32" s="155" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30749,27 +30761,27 @@
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="162"/>
-      <c r="B33" s="165"/>
+    <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="153"/>
+      <c r="B33" s="156"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
-    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="162"/>
-      <c r="B34" s="165"/>
+    <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="153"/>
+      <c r="B34" s="156"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
-    <row r="35" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="162"/>
-      <c r="B35" s="165"/>
+    <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="153"/>
+      <c r="B35" s="156"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
-    <row r="36" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="163"/>
-      <c r="B36" s="166"/>
+    <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="154"/>
+      <c r="B36" s="157"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30777,7 +30789,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
         <v>27</v>
       </c>
@@ -30789,7 +30801,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
         <v>29</v>
       </c>
@@ -30797,11 +30809,11 @@
       <c r="C38" s="39"/>
       <c r="D38" s="44"/>
     </row>
-    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="134" t="s">
+    <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="150" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="133" t="s">
+      <c r="B39" s="148" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30811,9 +30823,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="134"/>
-      <c r="B40" s="133"/>
+    <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="150"/>
+      <c r="B40" s="148"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30821,87 +30833,87 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="132" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="149" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="133" t="s">
+      <c r="B41" s="148" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="157" t="s">
+      <c r="C41" s="161" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="136" t="s">
+      <c r="D41" s="134" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="132"/>
-      <c r="B42" s="133"/>
-      <c r="C42" s="157"/>
-      <c r="D42" s="136"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="149"/>
+      <c r="B42" s="148"/>
+      <c r="C42" s="161"/>
+      <c r="D42" s="134"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="132"/>
-      <c r="B43" s="133"/>
-      <c r="C43" s="157" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="149"/>
+      <c r="B43" s="148"/>
+      <c r="C43" s="161" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="139" t="s">
+      <c r="D43" s="144" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="132"/>
-      <c r="B44" s="133"/>
-      <c r="C44" s="157"/>
-      <c r="D44" s="139"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="149"/>
+      <c r="B44" s="148"/>
+      <c r="C44" s="161"/>
+      <c r="D44" s="144"/>
     </row>
-    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="138" t="s">
+    <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="137" t="s">
+      <c r="B45" s="143" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="153"/>
+      <c r="C45" s="165"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="138"/>
-      <c r="B46" s="137"/>
-      <c r="C46" s="154"/>
-      <c r="D46" s="150" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="142"/>
+      <c r="B46" s="143"/>
+      <c r="C46" s="166"/>
+      <c r="D46" s="162" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="138"/>
-      <c r="B47" s="137"/>
-      <c r="C47" s="154"/>
-      <c r="D47" s="151"/>
+    <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="142"/>
+      <c r="B47" s="143"/>
+      <c r="C47" s="166"/>
+      <c r="D47" s="163"/>
     </row>
-    <row r="48" spans="1:4" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="138"/>
-      <c r="B48" s="137"/>
-      <c r="C48" s="155"/>
-      <c r="D48" s="151"/>
+    <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="142"/>
+      <c r="B48" s="143"/>
+      <c r="C48" s="167"/>
+      <c r="D48" s="163"/>
     </row>
-    <row r="49" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="138"/>
-      <c r="B49" s="137"/>
-      <c r="C49" s="145"/>
-      <c r="D49" s="151"/>
+    <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="142"/>
+      <c r="B49" s="143"/>
+      <c r="C49" s="137"/>
+      <c r="D49" s="163"/>
     </row>
-    <row r="50" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="138"/>
-      <c r="B50" s="137"/>
-      <c r="C50" s="145"/>
-      <c r="D50" s="152"/>
+    <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="142"/>
+      <c r="B50" s="143"/>
+      <c r="C50" s="137"/>
+      <c r="D50" s="164"/>
     </row>
-    <row r="51" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
         <v>40</v>
       </c>
@@ -30909,7 +30921,7 @@
       <c r="C51" s="39"/>
       <c r="D51" s="44"/>
     </row>
-    <row r="52" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A52" s="48" t="s">
         <v>83</v>
       </c>
@@ -30921,11 +30933,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="137" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="143" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="137" t="s">
+      <c r="B53" s="143" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30935,9 +30947,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="137"/>
-      <c r="B54" s="137"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="143"/>
+      <c r="B54" s="143"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30945,9 +30957,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="137"/>
-      <c r="B55" s="137"/>
+    <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="143"/>
+      <c r="B55" s="143"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30955,27 +30967,27 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="137"/>
-      <c r="B56" s="137"/>
-      <c r="C56" s="156" t="s">
+    <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="143"/>
+      <c r="B56" s="143"/>
+      <c r="C56" s="168" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="137"/>
-      <c r="B57" s="137"/>
-      <c r="C57" s="156"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="143"/>
+      <c r="B57" s="143"/>
+      <c r="C57" s="168"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="137"/>
-      <c r="B58" s="137"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="143"/>
+      <c r="B58" s="143"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30983,9 +30995,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="137"/>
-      <c r="B59" s="137"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="143"/>
+      <c r="B59" s="143"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -30993,139 +31005,122 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="137"/>
-      <c r="B60" s="137"/>
-      <c r="C60" s="156" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="143"/>
+      <c r="B60" s="143"/>
+      <c r="C60" s="168" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="137"/>
-      <c r="B61" s="137"/>
-      <c r="C61" s="156"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="143"/>
+      <c r="B61" s="143"/>
+      <c r="C61" s="168"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="137"/>
-      <c r="B62" s="137"/>
-      <c r="C62" s="156"/>
+    <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="143"/>
+      <c r="B62" s="143"/>
+      <c r="C62" s="168"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="137"/>
-      <c r="B63" s="137"/>
-      <c r="C63" s="157" t="s">
+    <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="143"/>
+      <c r="B63" s="143"/>
+      <c r="C63" s="161" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="137"/>
-      <c r="B64" s="137"/>
-      <c r="C64" s="157"/>
-      <c r="D64" s="139" t="s">
+    <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="143"/>
+      <c r="B64" s="143"/>
+      <c r="C64" s="161"/>
+      <c r="D64" s="144" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="137"/>
-      <c r="B65" s="137"/>
-      <c r="C65" s="157"/>
-      <c r="D65" s="139"/>
+    <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="143"/>
+      <c r="B65" s="143"/>
+      <c r="C65" s="161"/>
+      <c r="D65" s="144"/>
     </row>
-    <row r="66" spans="1:4" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="137"/>
-      <c r="B66" s="137"/>
-      <c r="C66" s="157"/>
-      <c r="D66" s="139"/>
+    <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="143"/>
+      <c r="B66" s="143"/>
+      <c r="C66" s="161"/>
+      <c r="D66" s="144"/>
     </row>
-    <row r="67" spans="1:4" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="137"/>
-      <c r="B67" s="137"/>
-      <c r="C67" s="157"/>
-      <c r="D67" s="139"/>
+    <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="143"/>
+      <c r="B67" s="143"/>
+      <c r="C67" s="161"/>
+      <c r="D67" s="144"/>
     </row>
-    <row r="68" spans="1:4" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
       <c r="D68" s="44"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="82"/>
       <c r="B69" s="83"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="82"/>
       <c r="B70" s="83"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="82"/>
       <c r="B71" s="83"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="82"/>
       <c r="B72" s="83"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31142,6 +31137,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31150,21 +31162,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:B66"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -31178,7 +31190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>341</v>
       </c>
@@ -31186,11 +31198,11 @@
       <c r="C2" s="39"/>
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="170" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="169" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="170" t="s">
+      <c r="B3" s="169" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="114" t="s">
@@ -31200,9 +31212,9 @@
         <v>344</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="170"/>
-      <c r="B4" s="170"/>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="169"/>
+      <c r="B4" s="169"/>
       <c r="C4" s="114" t="s">
         <v>347</v>
       </c>
@@ -31210,7 +31222,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
         <v>24</v>
       </c>
@@ -31218,11 +31230,11 @@
       <c r="C5" s="39"/>
       <c r="D5" s="44"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="136" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="173" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="58"/>
@@ -31230,9 +31242,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="136"/>
-      <c r="B7" s="156"/>
+    <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="134"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="106" t="s">
         <v>235</v>
       </c>
@@ -31240,11 +31252,11 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="156"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="106" t="s">
         <v>235</v>
       </c>
@@ -31252,11 +31264,11 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="156"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="106" t="s">
         <v>22</v>
       </c>
@@ -31264,27 +31276,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="156" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="168" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="156"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="58"/>
       <c r="D10" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="156"/>
-      <c r="B11" s="156"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="168"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="58"/>
       <c r="D11" s="58" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="156"/>
-      <c r="B12" s="156"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="168"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="110" t="s">
         <v>325</v>
       </c>
@@ -31292,795 +31304,789 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="156"/>
-      <c r="C13" s="58" t="s">
+      <c r="B13" s="174"/>
+      <c r="C13" s="118" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="58"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="156"/>
+      <c r="B14" s="174"/>
       <c r="C14" s="58"/>
       <c r="D14" s="104" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="100" t="s">
         <v>331</v>
       </c>
-      <c r="B15" s="156"/>
-      <c r="C15" s="58" t="s">
+      <c r="B15" s="174"/>
+      <c r="C15" s="118" t="s">
         <v>332</v>
       </c>
       <c r="D15" s="100" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="100" t="s">
+        <v>351</v>
+      </c>
+      <c r="B16" s="175"/>
+      <c r="C16" s="118" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="100"/>
+    </row>
+    <row r="17" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="169" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="176" t="s">
         <v>237</v>
       </c>
-      <c r="B17" s="156" t="s">
+      <c r="B18" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="169"/>
-      <c r="B18" s="156"/>
       <c r="C18" s="58"/>
       <c r="D18" s="58" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="169"/>
-      <c r="B19" s="156"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="176"/>
+      <c r="B19" s="168"/>
       <c r="C19" s="58"/>
       <c r="D19" s="58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="176"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="169"/>
-      <c r="B20" s="156"/>
-      <c r="C20" s="58" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="176"/>
+      <c r="B21" s="168"/>
+      <c r="C21" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D21" s="58" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="169"/>
-      <c r="B21" s="156"/>
-      <c r="C21" s="58" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="176"/>
+      <c r="B22" s="168"/>
+      <c r="C22" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="D21" s="100" t="s">
+      <c r="D22" s="100" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="134" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="150" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="156" t="s">
+      <c r="B23" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="C23" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="D22" s="100" t="s">
+      <c r="D23" s="100" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="134"/>
-      <c r="B23" s="156"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="150"/>
+      <c r="B24" s="168"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="134"/>
-      <c r="B24" s="156"/>
-      <c r="C24" s="108" t="s">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="150"/>
+      <c r="B25" s="168"/>
+      <c r="C25" s="108" t="s">
         <v>329</v>
       </c>
-      <c r="D24" s="100" t="s">
+      <c r="D25" s="100" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="156" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="168" t="s">
         <v>222</v>
       </c>
-      <c r="B25" s="156" t="s">
+      <c r="B26" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="C25" s="167" t="s">
+      <c r="C26" s="177" t="s">
         <v>239</v>
       </c>
-      <c r="D25" s="103" t="s">
+      <c r="D26" s="103" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="156"/>
-      <c r="B26" s="156"/>
-      <c r="C26" s="167"/>
-      <c r="D26" s="100" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="168"/>
+      <c r="B27" s="168"/>
+      <c r="C27" s="177"/>
+      <c r="D27" s="100" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="156"/>
-      <c r="B27" s="156"/>
-      <c r="C27" s="167" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="168"/>
+      <c r="B28" s="168"/>
+      <c r="C28" s="177" t="s">
         <v>240</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D28" s="58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="156"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="167"/>
-      <c r="D28" s="61" t="s">
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="168"/>
+      <c r="B29" s="168"/>
+      <c r="C29" s="177"/>
+      <c r="D29" s="61" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="156"/>
-      <c r="B29" s="156"/>
-      <c r="C29" s="105" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="168"/>
+      <c r="B30" s="168"/>
+      <c r="C30" s="105" t="s">
         <v>307</v>
       </c>
-      <c r="D29" s="58" t="s">
+      <c r="D30" s="58" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="156"/>
-      <c r="B30" s="156"/>
-      <c r="C30" s="105">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="168"/>
+      <c r="B31" s="168"/>
+      <c r="C31" s="105">
         <v>2.1</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D31" s="58" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="156"/>
-      <c r="B31" s="156"/>
-      <c r="C31" s="105" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="168"/>
+      <c r="B32" s="168"/>
+      <c r="C32" s="105" t="s">
         <v>239</v>
       </c>
-      <c r="D31" s="58" t="s">
+      <c r="D32" s="58" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="156"/>
-      <c r="B32" s="156"/>
-      <c r="C32" s="115" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="168"/>
+      <c r="B33" s="168"/>
+      <c r="C33" s="117" t="s">
         <v>239</v>
       </c>
-      <c r="D32" s="116" t="s">
+      <c r="D33" s="116" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="137" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="168"/>
+      <c r="B34" s="168"/>
+      <c r="C34" s="115" t="s">
+        <v>239</v>
+      </c>
+      <c r="D34" s="100" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="143" t="s">
         <v>296</v>
       </c>
-      <c r="B33" s="156" t="s">
+      <c r="B35" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="C33" s="58" t="s">
+      <c r="C35" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D33" s="58" t="s">
+      <c r="D35" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="137"/>
-      <c r="B34" s="156"/>
-      <c r="C34" s="61" t="s">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="143"/>
+      <c r="B36" s="168"/>
+      <c r="C36" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D34" s="58" t="s">
+      <c r="D36" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="137"/>
-      <c r="B35" s="156"/>
-      <c r="C35" s="58" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="143"/>
+      <c r="B37" s="168"/>
+      <c r="C37" s="58" t="s">
         <v>350</v>
       </c>
-      <c r="D35" s="58" t="s">
+      <c r="D37" s="58" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="39" t="s">
+    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="44"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="44"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="136" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="134" t="s">
         <v>260</v>
       </c>
-      <c r="B37" s="156" t="s">
+      <c r="B39" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="C37" s="58"/>
-      <c r="D37" s="79" t="s">
+      <c r="C39" s="58"/>
+      <c r="D39" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="136"/>
-      <c r="B38" s="156"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="134"/>
+      <c r="B40" s="168"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="58" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="58" t="s">
         <v>334</v>
       </c>
-      <c r="B39" s="105" t="s">
+      <c r="B41" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="79" t="s">
+      <c r="C41" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D39" s="100" t="s">
+      <c r="D41" s="100" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="96" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B40" s="105" t="s">
+      <c r="B42" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="C40" s="106" t="s">
+      <c r="C42" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="104" t="s">
+      <c r="D42" s="104" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="171" t="s">
+    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="170" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="174" t="s">
+      <c r="B43" s="173" t="s">
         <v>234</v>
       </c>
-      <c r="C41" s="58" t="s">
+      <c r="C43" s="58" t="s">
         <v>268</v>
-      </c>
-      <c r="D41" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="172"/>
-      <c r="B42" s="175"/>
-      <c r="C42" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="D42" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="172"/>
-      <c r="B43" s="175"/>
-      <c r="C43" s="58" t="s">
-        <v>269</v>
       </c>
       <c r="D43" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="172"/>
-      <c r="B44" s="175"/>
-      <c r="C44" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D44" s="100" t="s">
-        <v>102</v>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="171"/>
+      <c r="B44" s="174"/>
+      <c r="C44" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="D44" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="172"/>
-      <c r="B45" s="175"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="171"/>
+      <c r="B45" s="174"/>
       <c r="C45" s="58" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D45" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="172"/>
-      <c r="B46" s="175"/>
-      <c r="C46" s="58" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="171"/>
+      <c r="B46" s="174"/>
+      <c r="C46" s="100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D46" s="100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="171"/>
+      <c r="B47" s="174"/>
+      <c r="C47" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="D47" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="171"/>
+      <c r="B48" s="174"/>
+      <c r="C48" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="D46" s="58" t="s">
+      <c r="D48" s="58" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="172"/>
-      <c r="B47" s="175"/>
-      <c r="C47" s="100" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="171"/>
+      <c r="B49" s="174"/>
+      <c r="C49" s="100" t="s">
         <v>288</v>
       </c>
-      <c r="D47" s="100" t="s">
+      <c r="D49" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="172"/>
-      <c r="B48" s="175"/>
-      <c r="C48" s="100" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="171"/>
+      <c r="B50" s="174"/>
+      <c r="C50" s="100" t="s">
         <v>302</v>
       </c>
-      <c r="D48" s="100" t="s">
+      <c r="D50" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="172"/>
-      <c r="B49" s="175"/>
-      <c r="C49" s="100" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="171"/>
+      <c r="B51" s="174"/>
+      <c r="C51" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="D49" s="100" t="s">
+      <c r="D51" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="172"/>
-      <c r="B50" s="175"/>
-      <c r="C50" s="107" t="s">
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="171"/>
+      <c r="B52" s="174"/>
+      <c r="C52" s="107" t="s">
         <v>244</v>
       </c>
-      <c r="D50" s="104" t="s">
+      <c r="D52" s="104" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="172"/>
-      <c r="B51" s="175"/>
-      <c r="C51" s="108" t="s">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="171"/>
+      <c r="B53" s="174"/>
+      <c r="C53" s="108" t="s">
         <v>311</v>
       </c>
-      <c r="D51" s="100" t="s">
+      <c r="D53" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="172"/>
-      <c r="B52" s="175"/>
-      <c r="C52" s="58" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="171"/>
+      <c r="B54" s="174"/>
+      <c r="C54" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="D52" s="58" t="s">
+      <c r="D54" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="172"/>
-      <c r="B53" s="175"/>
-      <c r="C53" s="100" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="171"/>
+      <c r="B55" s="174"/>
+      <c r="C55" s="100" t="s">
         <v>313</v>
       </c>
-      <c r="D53" s="100" t="s">
+      <c r="D55" s="100" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="172"/>
-      <c r="B54" s="175"/>
-      <c r="C54" s="100" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="171"/>
+      <c r="B56" s="174"/>
+      <c r="C56" s="100" t="s">
         <v>315</v>
       </c>
-      <c r="D54" s="100" t="s">
+      <c r="D56" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="172"/>
-      <c r="B55" s="175"/>
-      <c r="C55" s="100" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="171"/>
+      <c r="B57" s="174"/>
+      <c r="C57" s="100" t="s">
         <v>268</v>
       </c>
-      <c r="D55" s="100" t="s">
+      <c r="D57" s="100" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="172"/>
-      <c r="B56" s="175"/>
-      <c r="C56" s="58" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="171"/>
+      <c r="B58" s="174"/>
+      <c r="C58" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="D56" s="58" t="s">
+      <c r="D58" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="172"/>
-      <c r="B57" s="175"/>
-      <c r="C57" s="100" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="171"/>
+      <c r="B59" s="174"/>
+      <c r="C59" s="100" t="s">
         <v>283</v>
       </c>
-      <c r="D57" s="100" t="s">
+      <c r="D59" s="100" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="172"/>
-      <c r="B58" s="175"/>
-      <c r="C58" s="100" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="171"/>
+      <c r="B60" s="174"/>
+      <c r="C60" s="100" t="s">
         <v>319</v>
-      </c>
-      <c r="D58" s="100" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A59" s="172"/>
-      <c r="B59" s="175"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="109" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="172"/>
-      <c r="B60" s="175"/>
-      <c r="C60" s="100" t="s">
-        <v>322</v>
       </c>
       <c r="D60" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="172"/>
-      <c r="B61" s="175"/>
-      <c r="C61" s="100" t="s">
-        <v>268</v>
-      </c>
-      <c r="D61" s="100" t="s">
-        <v>251</v>
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="171"/>
+      <c r="B61" s="174"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="109" t="s">
+        <v>321</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="172"/>
-      <c r="B62" s="175"/>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="171"/>
+      <c r="B62" s="174"/>
       <c r="C62" s="100" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="D62" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="172"/>
-      <c r="B63" s="175"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="171"/>
+      <c r="B63" s="174"/>
       <c r="C63" s="100" t="s">
-        <v>340</v>
+        <v>268</v>
       </c>
       <c r="D63" s="100" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="172"/>
-      <c r="B64" s="175"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="171"/>
+      <c r="B64" s="174"/>
       <c r="C64" s="100" t="s">
+        <v>339</v>
+      </c>
+      <c r="D64" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="171"/>
+      <c r="B65" s="174"/>
+      <c r="C65" s="100" t="s">
+        <v>340</v>
+      </c>
+      <c r="D65" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="171"/>
+      <c r="B66" s="174"/>
+      <c r="C66" s="100" t="s">
         <v>324</v>
       </c>
-      <c r="D64" s="100" t="s">
+      <c r="D66" s="100" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="172"/>
-      <c r="B65" s="175"/>
-      <c r="C65" s="116" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="171"/>
+      <c r="B67" s="174"/>
+      <c r="C67" s="116" t="s">
         <v>345</v>
       </c>
-      <c r="D65" s="116" t="s">
+      <c r="D67" s="116" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="173"/>
-      <c r="B66" s="176"/>
-      <c r="C66" s="100" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="172"/>
+      <c r="B68" s="175"/>
+      <c r="C68" s="100" t="s">
         <v>338</v>
       </c>
-      <c r="D66" s="100" t="s">
+      <c r="D68" s="100" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="58" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="58" t="s">
         <v>309</v>
       </c>
-      <c r="B67" s="106" t="s">
+      <c r="B69" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C67" s="58" t="s">
+      <c r="C69" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D67" s="100" t="s">
+      <c r="D69" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="58" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="B68" s="106" t="s">
+      <c r="B70" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C68" s="58" t="s">
+      <c r="C70" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D68" s="100" t="s">
+      <c r="D70" s="100" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="39" t="s">
+    <row r="71" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B69" s="39"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="44"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="44"/>
     </row>
-    <row r="70" spans="1:4" ht="31.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="99"/>
-      <c r="B70" s="67"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="79" t="s">
+    <row r="72" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="99"/>
+      <c r="B72" s="67"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="156" t="s">
+    <row r="73" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="168" t="s">
         <v>84</v>
       </c>
-      <c r="B71" s="156" t="s">
+      <c r="B73" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="C71" s="106" t="s">
+      <c r="C73" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="D71" s="58" t="s">
+      <c r="D73" s="58" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="156"/>
-      <c r="B72" s="156"/>
-      <c r="C72" s="106">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="168"/>
+      <c r="B74" s="168"/>
+      <c r="C74" s="106">
         <v>10.1</v>
       </c>
-      <c r="D72" s="58" t="s">
+      <c r="D74" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="156"/>
-      <c r="B73" s="156"/>
-      <c r="C73" s="106">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="168"/>
+      <c r="B75" s="168"/>
+      <c r="C75" s="106">
         <v>10.199999999999999</v>
       </c>
-      <c r="D73" s="58" t="s">
+      <c r="D75" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="156"/>
-      <c r="B74" s="156"/>
-      <c r="C74" s="111" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="168"/>
+      <c r="B76" s="168"/>
+      <c r="C76" s="111" t="s">
         <v>293</v>
       </c>
-      <c r="D74" s="101" t="s">
+      <c r="D76" s="101" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="136" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="134" t="s">
         <v>247</v>
       </c>
-      <c r="B75" s="156" t="s">
+      <c r="B77" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="C75" s="156"/>
-      <c r="D75" s="168" t="s">
+      <c r="C77" s="168"/>
+      <c r="D77" s="178" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="136"/>
-      <c r="B76" s="156"/>
-      <c r="C76" s="156"/>
-      <c r="D76" s="168"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="134"/>
+      <c r="B78" s="168"/>
+      <c r="C78" s="168"/>
+      <c r="D78" s="178"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="104" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="104" t="s">
         <v>262</v>
-      </c>
-      <c r="B77" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C77" s="106" t="s">
-        <v>250</v>
-      </c>
-      <c r="D77" s="100" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B78" s="39"/>
-      <c r="C78" s="98"/>
-      <c r="D78" s="98"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="58" t="s">
-        <v>249</v>
       </c>
       <c r="B79" s="106" t="s">
         <v>234</v>
       </c>
-      <c r="C79" s="112" t="s">
+      <c r="C79" s="106" t="s">
+        <v>250</v>
+      </c>
+      <c r="D79" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B80" s="39"/>
+      <c r="C80" s="98"/>
+      <c r="D80" s="98"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B81" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C81" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D79" s="58" t="s">
+      <c r="D81" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="136" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="134" t="s">
         <v>285</v>
       </c>
-      <c r="B80" s="156" t="s">
+      <c r="B82" s="168" t="s">
         <v>234</v>
       </c>
-      <c r="C80" s="101" t="s">
+      <c r="C82" s="101" t="s">
         <v>295</v>
       </c>
-      <c r="D80" s="58" t="s">
+      <c r="D82" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="136"/>
-      <c r="B81" s="156"/>
-      <c r="C81" s="58" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="134"/>
+      <c r="B83" s="168"/>
+      <c r="C83" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D81" s="100" t="s">
+      <c r="D83" s="100" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="136"/>
-      <c r="B82" s="156"/>
-      <c r="C82" s="112" t="s">
+    <row r="84" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="134"/>
+      <c r="B84" s="168"/>
+      <c r="C84" s="112" t="s">
         <v>286</v>
       </c>
-      <c r="D82" s="58" t="s">
+      <c r="D84" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="98" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="B83" s="98"/>
-      <c r="C83" s="98"/>
-      <c r="D83" s="98"/>
+      <c r="B85" s="98"/>
+      <c r="C85" s="98"/>
+      <c r="D85" s="98"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="135" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="151" t="s">
         <v>58</v>
       </c>
-      <c r="B84" s="156" t="s">
+      <c r="B86" s="168" t="s">
         <v>271</v>
       </c>
-      <c r="C84" s="112" t="s">
+      <c r="C86" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D84" s="58" t="s">
+      <c r="D86" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="135"/>
-      <c r="B85" s="156"/>
-      <c r="C85" s="112" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="151"/>
+      <c r="B87" s="168"/>
+      <c r="C87" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="D85" s="58" t="s">
+      <c r="D87" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="97" t="s">
+    <row r="88" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="97" t="s">
         <v>59</v>
-      </c>
-      <c r="B86" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C86" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D86" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A87" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B87" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C87" s="58"/>
-      <c r="D87" s="61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A88" s="97" t="s">
-        <v>60</v>
       </c>
       <c r="B88" s="106" t="s">
         <v>271</v>
@@ -32089,38 +32095,44 @@
         <v>264</v>
       </c>
       <c r="D88" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="B89" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C89" s="58"/>
+      <c r="D89" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B90" s="106" t="s">
+        <v>271</v>
+      </c>
+      <c r="C90" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D90" s="58" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="98" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="98" t="s">
         <v>273</v>
-      </c>
-      <c r="B89" s="98"/>
-      <c r="C89" s="98"/>
-      <c r="D89" s="98"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="58"/>
-      <c r="B90" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C90" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D90" s="100" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="98" t="s">
-        <v>279</v>
       </c>
       <c r="B91" s="98"/>
       <c r="C91" s="98"/>
       <c r="D91" s="98"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="58"/>
       <c r="B92" s="106" t="s">
         <v>234</v>
@@ -32132,37 +32144,57 @@
         <v>274</v>
       </c>
     </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B93" s="98"/>
+      <c r="C93" s="98"/>
+      <c r="D93" s="98"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="58"/>
+      <c r="B94" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="C94" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D94" s="100" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A26:A34"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A41:A66"/>
-    <mergeCell ref="B41:B66"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A43:A68"/>
+    <mergeCell ref="B43:B68"/>
+    <mergeCell ref="B6:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor fixes and addition of handshake endpoint
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,17 +20,17 @@
   <definedNames>
     <definedName name="_Toc520203303" localSheetId="3">'1.0 Release Candidate 2'!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="369">
   <si>
     <t>Document</t>
   </si>
@@ -2914,6 +2914,54 @@
   </si>
   <si>
     <t>Accepted Date specification updated</t>
+  </si>
+  <si>
+    <t>code 4002</t>
+  </si>
+  <si>
+    <t>Added to Payroll Submission</t>
+  </si>
+  <si>
+    <t>Corrected to Async</t>
+  </si>
+  <si>
+    <t>code 4002, 4003, 4004, 1010</t>
+  </si>
+  <si>
+    <t>code 3015</t>
+  </si>
+  <si>
+    <t>code 2012, 2013</t>
+  </si>
+  <si>
+    <t>Payroll Submission</t>
+  </si>
+  <si>
+    <t>line item ID specified to be within same payroll run</t>
+  </si>
+  <si>
+    <t>newRPN request</t>
+  </si>
+  <si>
+    <t>removed typo from schema location namespace in example</t>
+  </si>
+  <si>
+    <t>removed typo from PRSIExempt tag in example</t>
+  </si>
+  <si>
+    <t>code 2021</t>
+  </si>
+  <si>
+    <t>Updated Description</t>
+  </si>
+  <si>
+    <t>code 1111</t>
+  </si>
+  <si>
+    <t>RPN Return</t>
+  </si>
+  <si>
+    <t>Removed Required field. Updated Description</t>
   </si>
 </sst>
 </file>
@@ -3081,7 +3129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -3493,11 +3541,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3753,9 +3819,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3805,6 +3868,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3850,8 +3938,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3874,66 +3992,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3955,16 +4013,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3976,14 +4061,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4388,12 +4515,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="121"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="129"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4416,12 +4543,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="121"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="129"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4461,10 +4588,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="125">
+      <c r="B7" s="133">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4478,8 +4605,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="126"/>
+      <c r="A8" s="131"/>
+      <c r="B8" s="134"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4491,8 +4618,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="123"/>
-      <c r="B9" s="126"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="134"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4504,8 +4631,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="123"/>
-      <c r="B10" s="126"/>
+      <c r="A10" s="131"/>
+      <c r="B10" s="134"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4517,8 +4644,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="123"/>
-      <c r="B11" s="126"/>
+      <c r="A11" s="131"/>
+      <c r="B11" s="134"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4530,8 +4657,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="124"/>
-      <c r="B12" s="127"/>
+      <c r="A12" s="132"/>
+      <c r="B12" s="135"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4543,10 +4670,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="130" t="s">
+      <c r="A13" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="125">
+      <c r="B13" s="133">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4560,8 +4687,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="131"/>
-      <c r="B14" s="127"/>
+      <c r="A14" s="139"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4607,12 +4734,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="119" t="s">
+      <c r="A17" s="127" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="121"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="129"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4652,21 +4779,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="119" t="s">
+      <c r="A20" s="127" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="120"/>
-      <c r="C20" s="120"/>
-      <c r="D20" s="121"/>
+      <c r="B20" s="128"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="129"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="132" t="s">
+      <c r="A21" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="129">
+      <c r="B21" s="137">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4680,8 +4807,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="133"/>
-      <c r="B22" s="127"/>
+      <c r="A22" s="141"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4704,18 +4831,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="119" t="s">
+      <c r="A24" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="120"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="121"/>
+      <c r="B24" s="128"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="129"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="128" t="s">
+      <c r="A25" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="129">
+      <c r="B25" s="137">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4729,8 +4856,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="123"/>
-      <c r="B26" s="126"/>
+      <c r="A26" s="131"/>
+      <c r="B26" s="134"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4742,8 +4869,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="123"/>
-      <c r="B27" s="126"/>
+      <c r="A27" s="131"/>
+      <c r="B27" s="134"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4755,8 +4882,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="123"/>
-      <c r="B28" s="126"/>
+      <c r="A28" s="131"/>
+      <c r="B28" s="134"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4768,8 +4895,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="123"/>
-      <c r="B29" s="126"/>
+      <c r="A29" s="131"/>
+      <c r="B29" s="134"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4781,8 +4908,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="123"/>
-      <c r="B30" s="126"/>
+      <c r="A30" s="131"/>
+      <c r="B30" s="134"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4794,8 +4921,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="123"/>
-      <c r="B31" s="126"/>
+      <c r="A31" s="131"/>
+      <c r="B31" s="134"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4807,8 +4934,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="124"/>
-      <c r="B32" s="127"/>
+      <c r="A32" s="132"/>
+      <c r="B32" s="135"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -4932,12 +5059,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="119" t="s">
+      <c r="A41" s="127" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="120"/>
-      <c r="C41" s="120"/>
-      <c r="D41" s="121"/>
+      <c r="B41" s="128"/>
+      <c r="C41" s="128"/>
+      <c r="D41" s="129"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -4997,7 +5124,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5007,7 +5134,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5117,10 +5244,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="149" t="s">
+      <c r="A7" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="148" t="s">
+      <c r="B7" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5131,8 +5258,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="149"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="143"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5141,8 +5268,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="149"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="142"/>
+      <c r="B9" s="143"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5151,8 +5278,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="149"/>
-      <c r="B10" s="148"/>
+      <c r="A10" s="142"/>
+      <c r="B10" s="143"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5161,8 +5288,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="149"/>
-      <c r="B11" s="148"/>
+      <c r="A11" s="142"/>
+      <c r="B11" s="143"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5171,8 +5298,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
-      <c r="B12" s="148"/>
+      <c r="A12" s="142"/>
+      <c r="B12" s="143"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5181,10 +5308,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="145" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5195,8 +5322,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="151"/>
-      <c r="B14" s="148"/>
+      <c r="A14" s="145"/>
+      <c r="B14" s="143"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5205,8 +5332,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="151"/>
-      <c r="B15" s="148"/>
+      <c r="A15" s="145"/>
+      <c r="B15" s="143"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5215,10 +5342,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="134" t="s">
+      <c r="A16" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="143" t="s">
+      <c r="B16" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5229,8 +5356,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="134"/>
-      <c r="B17" s="143"/>
+      <c r="A17" s="146"/>
+      <c r="B17" s="147"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5239,8 +5366,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="134"/>
-      <c r="B18" s="143"/>
+      <c r="A18" s="146"/>
+      <c r="B18" s="147"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5249,8 +5376,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="134"/>
-      <c r="B19" s="143"/>
+      <c r="A19" s="146"/>
+      <c r="B19" s="147"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5259,8 +5386,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="134"/>
-      <c r="B20" s="143"/>
+      <c r="A20" s="146"/>
+      <c r="B20" s="147"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5269,8 +5396,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="134"/>
-      <c r="B21" s="143"/>
+      <c r="A21" s="146"/>
+      <c r="B21" s="147"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5279,8 +5406,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="134"/>
-      <c r="B22" s="143"/>
+      <c r="A22" s="146"/>
+      <c r="B22" s="147"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5289,8 +5416,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="134"/>
-      <c r="B23" s="143"/>
+      <c r="A23" s="146"/>
+      <c r="B23" s="147"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5299,26 +5426,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="134"/>
-      <c r="B24" s="143"/>
-      <c r="C24" s="134" t="s">
+      <c r="A24" s="146"/>
+      <c r="B24" s="147"/>
+      <c r="C24" s="146" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="135" t="s">
+      <c r="D24" s="153" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="134"/>
-      <c r="B25" s="143"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="135"/>
+      <c r="A25" s="146"/>
+      <c r="B25" s="147"/>
+      <c r="C25" s="146"/>
+      <c r="D25" s="153"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="149" t="s">
+      <c r="A26" s="142" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="148" t="s">
+      <c r="B26" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5329,8 +5456,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="149"/>
-      <c r="B27" s="148"/>
+      <c r="A27" s="142"/>
+      <c r="B27" s="143"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5357,28 +5484,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="150" t="s">
+      <c r="A30" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="143" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="134" t="s">
+      <c r="C30" s="146" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="138" t="s">
+      <c r="D30" s="156" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="150"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="134"/>
-      <c r="D31" s="138"/>
+      <c r="A31" s="144"/>
+      <c r="B31" s="143"/>
+      <c r="C31" s="146"/>
+      <c r="D31" s="156"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="150"/>
-      <c r="B32" s="148"/>
+      <c r="A32" s="144"/>
+      <c r="B32" s="143"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5387,8 +5514,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="150"/>
-      <c r="B33" s="148"/>
+      <c r="A33" s="144"/>
+      <c r="B33" s="143"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5397,8 +5524,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="150"/>
-      <c r="B34" s="148"/>
+      <c r="A34" s="144"/>
+      <c r="B34" s="143"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5407,8 +5534,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="150"/>
-      <c r="B35" s="148"/>
+      <c r="A35" s="144"/>
+      <c r="B35" s="143"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5417,8 +5544,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="150"/>
-      <c r="B36" s="148"/>
+      <c r="A36" s="144"/>
+      <c r="B36" s="143"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5427,26 +5554,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="150"/>
-      <c r="B37" s="148"/>
-      <c r="C37" s="139" t="s">
+      <c r="A37" s="144"/>
+      <c r="B37" s="143"/>
+      <c r="C37" s="157" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="141" t="s">
+      <c r="D37" s="159" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="150"/>
-      <c r="B38" s="148"/>
-      <c r="C38" s="140"/>
-      <c r="D38" s="141"/>
+      <c r="A38" s="144"/>
+      <c r="B38" s="143"/>
+      <c r="C38" s="158"/>
+      <c r="D38" s="159"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="149" t="s">
+      <c r="A39" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5457,8 +5584,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="149"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="142"/>
+      <c r="B40" s="143"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5485,10 +5612,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="150" t="s">
+      <c r="A43" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="148" t="s">
+      <c r="B43" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5497,8 +5624,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="150"/>
-      <c r="B44" s="148"/>
+      <c r="A44" s="144"/>
+      <c r="B44" s="143"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5507,10 +5634,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="145" t="s">
+      <c r="A45" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="148" t="s">
+      <c r="B45" s="143" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5519,8 +5646,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="146"/>
-      <c r="B46" s="148"/>
+      <c r="A46" s="151"/>
+      <c r="B46" s="143"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5529,8 +5656,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="146"/>
-      <c r="B47" s="148"/>
+      <c r="A47" s="151"/>
+      <c r="B47" s="143"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5539,8 +5666,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="147"/>
-      <c r="B48" s="148"/>
+      <c r="A48" s="152"/>
+      <c r="B48" s="143"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5549,10 +5676,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="143" t="s">
+      <c r="A49" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="143" t="s">
+      <c r="B49" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9656,8 +9783,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="143"/>
-      <c r="B50" s="143"/>
+      <c r="A50" s="147"/>
+      <c r="B50" s="147"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13761,8 +13888,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="143"/>
-      <c r="B51" s="143"/>
+      <c r="A51" s="147"/>
+      <c r="B51" s="147"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -17866,8 +17993,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="143"/>
-      <c r="B52" s="143"/>
+      <c r="A52" s="147"/>
+      <c r="B52" s="147"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -21971,12 +22098,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="143"/>
-      <c r="B53" s="143"/>
-      <c r="C53" s="137" t="s">
+      <c r="A53" s="147"/>
+      <c r="B53" s="147"/>
+      <c r="C53" s="155" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="138" t="s">
+      <c r="D53" s="156" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26076,10 +26203,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="143"/>
-      <c r="B54" s="143"/>
-      <c r="C54" s="137"/>
-      <c r="D54" s="138"/>
+      <c r="A54" s="147"/>
+      <c r="B54" s="147"/>
+      <c r="C54" s="155"/>
+      <c r="D54" s="156"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30197,10 +30324,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="142" t="s">
+      <c r="A57" s="148" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="143" t="s">
+      <c r="B57" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30211,8 +30338,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="142"/>
-      <c r="B58" s="143"/>
+      <c r="A58" s="148"/>
+      <c r="B58" s="147"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30221,8 +30348,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="142"/>
-      <c r="B59" s="143"/>
+      <c r="A59" s="148"/>
+      <c r="B59" s="147"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30231,8 +30358,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="142"/>
-      <c r="B60" s="143"/>
+      <c r="A60" s="148"/>
+      <c r="B60" s="147"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30241,8 +30368,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="142"/>
-      <c r="B61" s="143"/>
+      <c r="A61" s="148"/>
+      <c r="B61" s="147"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30251,8 +30378,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="142"/>
-      <c r="B62" s="143"/>
+      <c r="A62" s="148"/>
+      <c r="B62" s="147"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30261,8 +30388,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="142"/>
-      <c r="B63" s="143"/>
+      <c r="A63" s="148"/>
+      <c r="B63" s="147"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30271,16 +30398,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="142"/>
-      <c r="B64" s="143"/>
+      <c r="A64" s="148"/>
+      <c r="B64" s="147"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="142"/>
-      <c r="B65" s="143"/>
+      <c r="A65" s="148"/>
+      <c r="B65" s="147"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30289,16 +30416,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="142"/>
-      <c r="B66" s="143"/>
+      <c r="A66" s="148"/>
+      <c r="B66" s="147"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="142"/>
-      <c r="B67" s="143"/>
+      <c r="A67" s="148"/>
+      <c r="B67" s="147"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30307,8 +30434,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="142"/>
-      <c r="B68" s="143"/>
+      <c r="A68" s="148"/>
+      <c r="B68" s="147"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30317,8 +30444,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="142"/>
-      <c r="B69" s="143"/>
+      <c r="A69" s="148"/>
+      <c r="B69" s="147"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30327,8 +30454,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="142"/>
-      <c r="B70" s="143"/>
+      <c r="A70" s="148"/>
+      <c r="B70" s="147"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30337,8 +30464,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="142"/>
-      <c r="B71" s="143"/>
+      <c r="A71" s="148"/>
+      <c r="B71" s="147"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30347,8 +30474,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="142"/>
-      <c r="B72" s="143"/>
+      <c r="A72" s="148"/>
+      <c r="B72" s="147"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30357,16 +30484,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="142"/>
-      <c r="B73" s="143"/>
+      <c r="A73" s="148"/>
+      <c r="B73" s="147"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="142"/>
-      <c r="B74" s="143"/>
+      <c r="A74" s="148"/>
+      <c r="B74" s="147"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30375,18 +30502,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="142"/>
-      <c r="B75" s="143"/>
-      <c r="C75" s="136"/>
-      <c r="D75" s="144" t="s">
+      <c r="A75" s="148"/>
+      <c r="B75" s="147"/>
+      <c r="C75" s="154"/>
+      <c r="D75" s="149" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="142"/>
-      <c r="B76" s="143"/>
-      <c r="C76" s="136"/>
-      <c r="D76" s="144"/>
+      <c r="A76" s="148"/>
+      <c r="B76" s="147"/>
+      <c r="C76" s="154"/>
+      <c r="D76" s="149"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30410,8 +30537,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30420,13 +30547,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30441,22 +30584,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30510,10 +30637,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="148" t="s">
+      <c r="B4" s="143" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30524,133 +30651,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="149"/>
-      <c r="B5" s="148"/>
-      <c r="C5" s="159" t="s">
+      <c r="A5" s="142"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="169" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="158" t="s">
+      <c r="D5" s="168" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="149"/>
-      <c r="B6" s="148"/>
-      <c r="C6" s="159"/>
-      <c r="D6" s="158"/>
+      <c r="A6" s="142"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="168"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="149"/>
-      <c r="B7" s="148"/>
+      <c r="A7" s="142"/>
+      <c r="B7" s="143"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="149"/>
-      <c r="B8" s="148"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="143"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="149"/>
-      <c r="B9" s="148"/>
+      <c r="A9" s="142"/>
+      <c r="B9" s="143"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="151" t="s">
+      <c r="A10" s="145" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="143" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="161"/>
-      <c r="D10" s="158" t="s">
+      <c r="C10" s="167"/>
+      <c r="D10" s="168" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="151"/>
-      <c r="B11" s="148"/>
-      <c r="C11" s="161"/>
-      <c r="D11" s="158"/>
+      <c r="A11" s="145"/>
+      <c r="B11" s="143"/>
+      <c r="C11" s="167"/>
+      <c r="D11" s="168"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="151"/>
-      <c r="B12" s="148"/>
-      <c r="C12" s="161"/>
-      <c r="D12" s="158"/>
+      <c r="A12" s="145"/>
+      <c r="B12" s="143"/>
+      <c r="C12" s="167"/>
+      <c r="D12" s="168"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="134" t="s">
+      <c r="A13" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="143" t="s">
+      <c r="B13" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="160"/>
-      <c r="D13" s="158" t="s">
+      <c r="C13" s="170"/>
+      <c r="D13" s="168" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="134"/>
-      <c r="B14" s="143"/>
-      <c r="C14" s="160"/>
-      <c r="D14" s="158"/>
+      <c r="A14" s="146"/>
+      <c r="B14" s="147"/>
+      <c r="C14" s="170"/>
+      <c r="D14" s="168"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="134"/>
-      <c r="B15" s="143"/>
-      <c r="C15" s="160"/>
+      <c r="A15" s="146"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="170"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="134"/>
-      <c r="B16" s="143"/>
-      <c r="C16" s="160"/>
+      <c r="A16" s="146"/>
+      <c r="B16" s="147"/>
+      <c r="C16" s="170"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="134"/>
-      <c r="B17" s="143"/>
-      <c r="C17" s="160"/>
+      <c r="A17" s="146"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="170"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="134"/>
-      <c r="B18" s="143"/>
-      <c r="C18" s="160"/>
+      <c r="A18" s="146"/>
+      <c r="B18" s="147"/>
+      <c r="C18" s="170"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="134"/>
-      <c r="B19" s="143"/>
-      <c r="C19" s="160"/>
+      <c r="A19" s="146"/>
+      <c r="B19" s="147"/>
+      <c r="C19" s="170"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="134"/>
-      <c r="B20" s="143"/>
-      <c r="C20" s="160"/>
+      <c r="A20" s="146"/>
+      <c r="B20" s="147"/>
+      <c r="C20" s="170"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="134"/>
-      <c r="B21" s="143"/>
-      <c r="C21" s="160"/>
+      <c r="A21" s="146"/>
+      <c r="B21" s="147"/>
+      <c r="C21" s="170"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="134"/>
-      <c r="B22" s="143"/>
-      <c r="C22" s="160"/>
+      <c r="A22" s="146"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="170"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="134"/>
-      <c r="B23" s="143"/>
-      <c r="C23" s="160"/>
+      <c r="A23" s="146"/>
+      <c r="B23" s="147"/>
+      <c r="C23" s="170"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30748,10 +30875,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="152" t="s">
+      <c r="A32" s="171" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="155" t="s">
+      <c r="B32" s="174" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30762,26 +30889,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="153"/>
-      <c r="B33" s="156"/>
+      <c r="A33" s="172"/>
+      <c r="B33" s="175"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="153"/>
-      <c r="B34" s="156"/>
+      <c r="A34" s="172"/>
+      <c r="B34" s="175"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="153"/>
-      <c r="B35" s="156"/>
+      <c r="A35" s="172"/>
+      <c r="B35" s="175"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="154"/>
-      <c r="B36" s="157"/>
+      <c r="A36" s="173"/>
+      <c r="B36" s="176"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30810,10 +30937,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="150" t="s">
+      <c r="A39" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="143" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30824,8 +30951,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="150"/>
-      <c r="B40" s="148"/>
+      <c r="A40" s="144"/>
+      <c r="B40" s="143"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30834,84 +30961,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="149" t="s">
+      <c r="A41" s="142" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="148" t="s">
+      <c r="B41" s="143" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="161" t="s">
+      <c r="C41" s="167" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="134" t="s">
+      <c r="D41" s="146" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="149"/>
-      <c r="B42" s="148"/>
-      <c r="C42" s="161"/>
-      <c r="D42" s="134"/>
+      <c r="A42" s="142"/>
+      <c r="B42" s="143"/>
+      <c r="C42" s="167"/>
+      <c r="D42" s="146"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="149"/>
-      <c r="B43" s="148"/>
-      <c r="C43" s="161" t="s">
+      <c r="A43" s="142"/>
+      <c r="B43" s="143"/>
+      <c r="C43" s="167" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="144" t="s">
+      <c r="D43" s="149" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="149"/>
-      <c r="B44" s="148"/>
-      <c r="C44" s="161"/>
-      <c r="D44" s="144"/>
+      <c r="A44" s="142"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="167"/>
+      <c r="D44" s="149"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="142" t="s">
+      <c r="A45" s="148" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="143" t="s">
+      <c r="B45" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="165"/>
+      <c r="C45" s="163"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="142"/>
-      <c r="B46" s="143"/>
-      <c r="C46" s="166"/>
-      <c r="D46" s="162" t="s">
+      <c r="A46" s="148"/>
+      <c r="B46" s="147"/>
+      <c r="C46" s="164"/>
+      <c r="D46" s="160" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="142"/>
-      <c r="B47" s="143"/>
-      <c r="C47" s="166"/>
-      <c r="D47" s="163"/>
+      <c r="A47" s="148"/>
+      <c r="B47" s="147"/>
+      <c r="C47" s="164"/>
+      <c r="D47" s="161"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="142"/>
-      <c r="B48" s="143"/>
-      <c r="C48" s="167"/>
-      <c r="D48" s="163"/>
+      <c r="A48" s="148"/>
+      <c r="B48" s="147"/>
+      <c r="C48" s="165"/>
+      <c r="D48" s="161"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="142"/>
-      <c r="B49" s="143"/>
-      <c r="C49" s="137"/>
-      <c r="D49" s="163"/>
+      <c r="A49" s="148"/>
+      <c r="B49" s="147"/>
+      <c r="C49" s="155"/>
+      <c r="D49" s="161"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="142"/>
-      <c r="B50" s="143"/>
-      <c r="C50" s="137"/>
-      <c r="D50" s="164"/>
+      <c r="A50" s="148"/>
+      <c r="B50" s="147"/>
+      <c r="C50" s="155"/>
+      <c r="D50" s="162"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -30934,10 +31061,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="143" t="s">
+      <c r="A53" s="147" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="143" t="s">
+      <c r="B53" s="147" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -30948,8 +31075,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="143"/>
-      <c r="B54" s="143"/>
+      <c r="A54" s="147"/>
+      <c r="B54" s="147"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -30958,8 +31085,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="143"/>
-      <c r="B55" s="143"/>
+      <c r="A55" s="147"/>
+      <c r="B55" s="147"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -30968,9 +31095,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="143"/>
-      <c r="B56" s="143"/>
-      <c r="C56" s="168" t="s">
+      <c r="A56" s="147"/>
+      <c r="B56" s="147"/>
+      <c r="C56" s="166" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -30978,16 +31105,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="143"/>
-      <c r="B57" s="143"/>
-      <c r="C57" s="168"/>
+      <c r="A57" s="147"/>
+      <c r="B57" s="147"/>
+      <c r="C57" s="166"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="143"/>
-      <c r="B58" s="143"/>
+      <c r="A58" s="147"/>
+      <c r="B58" s="147"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -30996,8 +31123,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="143"/>
-      <c r="B59" s="143"/>
+      <c r="A59" s="147"/>
+      <c r="B59" s="147"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31006,9 +31133,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="143"/>
-      <c r="B60" s="143"/>
-      <c r="C60" s="168" t="s">
+      <c r="A60" s="147"/>
+      <c r="B60" s="147"/>
+      <c r="C60" s="166" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31016,25 +31143,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="143"/>
-      <c r="B61" s="143"/>
-      <c r="C61" s="168"/>
+      <c r="A61" s="147"/>
+      <c r="B61" s="147"/>
+      <c r="C61" s="166"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="143"/>
-      <c r="B62" s="143"/>
-      <c r="C62" s="168"/>
+      <c r="A62" s="147"/>
+      <c r="B62" s="147"/>
+      <c r="C62" s="166"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="143"/>
-      <c r="B63" s="143"/>
-      <c r="C63" s="161" t="s">
+      <c r="A63" s="147"/>
+      <c r="B63" s="147"/>
+      <c r="C63" s="167" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31042,30 +31169,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="143"/>
-      <c r="B64" s="143"/>
-      <c r="C64" s="161"/>
-      <c r="D64" s="144" t="s">
+      <c r="A64" s="147"/>
+      <c r="B64" s="147"/>
+      <c r="C64" s="167"/>
+      <c r="D64" s="149" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="143"/>
-      <c r="B65" s="143"/>
-      <c r="C65" s="161"/>
-      <c r="D65" s="144"/>
+      <c r="A65" s="147"/>
+      <c r="B65" s="147"/>
+      <c r="C65" s="167"/>
+      <c r="D65" s="149"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="143"/>
-      <c r="B66" s="143"/>
-      <c r="C66" s="161"/>
-      <c r="D66" s="144"/>
+      <c r="A66" s="147"/>
+      <c r="B66" s="147"/>
+      <c r="C66" s="167"/>
+      <c r="D66" s="149"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="143"/>
-      <c r="B67" s="143"/>
-      <c r="C67" s="161"/>
-      <c r="D67" s="144"/>
+      <c r="A67" s="147"/>
+      <c r="B67" s="147"/>
+      <c r="C67" s="167"/>
+      <c r="D67" s="149"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31121,6 +31248,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31137,23 +31281,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31162,10 +31289,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31199,23 +31326,23 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="169" t="s">
+      <c r="A3" s="185" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="113" t="s">
         <v>343</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="112" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="169"/>
-      <c r="B4" s="169"/>
-      <c r="C4" s="114" t="s">
+      <c r="A4" s="185"/>
+      <c r="B4" s="179"/>
+      <c r="C4" s="113" t="s">
         <v>347</v>
       </c>
       <c r="D4" s="58" t="s">
@@ -31231,10 +31358,10 @@
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="134" t="s">
+      <c r="A6" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="173" t="s">
+      <c r="B6" s="166" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="58"/>
@@ -31243,61 +31370,67 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="134"/>
-      <c r="B7" s="174"/>
-      <c r="C7" s="106" t="s">
+      <c r="A7" s="146"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="105" t="s">
         <v>235</v>
       </c>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="101" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="174"/>
-      <c r="C8" s="106" t="s">
+      <c r="B8" s="122" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="105" t="s">
         <v>235</v>
       </c>
-      <c r="D8" s="104" t="s">
+      <c r="D8" s="103" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="96" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="174"/>
-      <c r="C9" s="106" t="s">
+      <c r="B9" s="122" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="104" t="s">
+      <c r="D9" s="103" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="168" t="s">
+      <c r="A10" s="146" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="166" t="s">
+        <v>234</v>
+      </c>
       <c r="C10" s="58"/>
       <c r="D10" s="79" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="168"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="146"/>
+      <c r="B11" s="166"/>
       <c r="C11" s="58"/>
       <c r="D11" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="168"/>
-      <c r="B12" s="174"/>
-      <c r="C12" s="110" t="s">
+      <c r="A12" s="146"/>
+      <c r="B12" s="166"/>
+      <c r="C12" s="109" t="s">
         <v>325</v>
       </c>
       <c r="D12" s="58" t="s">
@@ -31305,896 +31438,1027 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="96" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="174"/>
-      <c r="C13" s="118" t="s">
+      <c r="B13" s="122" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" s="117" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="58"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="186" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="174"/>
+      <c r="B14" s="180" t="s">
+        <v>234</v>
+      </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="121" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="100" t="s">
-        <v>331</v>
-      </c>
-      <c r="B15" s="174"/>
-      <c r="C15" s="118" t="s">
-        <v>332</v>
-      </c>
-      <c r="D15" s="100" t="s">
-        <v>333</v>
+      <c r="A15" s="187"/>
+      <c r="B15" s="181"/>
+      <c r="C15" s="120" t="s">
+        <v>361</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="100" t="s">
-        <v>351</v>
-      </c>
-      <c r="B16" s="175"/>
-      <c r="C16" s="118" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="100"/>
+      <c r="A16" s="187"/>
+      <c r="B16" s="181"/>
+      <c r="C16" s="120" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>363</v>
+      </c>
     </row>
-    <row r="17" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="187"/>
+      <c r="B17" s="181"/>
+      <c r="C17" s="126" t="s">
+        <v>367</v>
+      </c>
+      <c r="D17" s="99" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="176" t="s">
-        <v>237</v>
-      </c>
-      <c r="B18" s="168" t="s">
-        <v>234</v>
-      </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58" t="s">
-        <v>258</v>
+      <c r="A18" s="188"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="120" t="s">
+        <v>359</v>
+      </c>
+      <c r="D18" s="99" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="176"/>
-      <c r="B19" s="168"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58" t="s">
-        <v>252</v>
+      <c r="A19" s="189" t="s">
+        <v>331</v>
+      </c>
+      <c r="B19" s="122" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="117" t="s">
+        <v>332</v>
+      </c>
+      <c r="D19" s="99" t="s">
+        <v>333</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="176"/>
-      <c r="B20" s="168"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58" t="s">
-        <v>254</v>
-      </c>
+    <row r="20" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="189" t="s">
+        <v>351</v>
+      </c>
+      <c r="B20" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="117" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="99"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="176"/>
-      <c r="B21" s="168"/>
-      <c r="C21" s="58" t="s">
-        <v>300</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>301</v>
-      </c>
+      <c r="A21" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="176"/>
-      <c r="B22" s="168"/>
-      <c r="C22" s="58" t="s">
-        <v>328</v>
-      </c>
-      <c r="D22" s="100" t="s">
-        <v>327</v>
+      <c r="A22" s="190" t="s">
+        <v>237</v>
+      </c>
+      <c r="B22" s="180" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="150" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="168" t="s">
-        <v>234</v>
-      </c>
-      <c r="C23" s="58" t="s">
-        <v>303</v>
-      </c>
-      <c r="D23" s="100" t="s">
-        <v>304</v>
+      <c r="A23" s="191"/>
+      <c r="B23" s="181"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="150"/>
-      <c r="B24" s="168"/>
+      <c r="A24" s="191"/>
+      <c r="B24" s="181"/>
       <c r="C24" s="58"/>
       <c r="D24" s="58" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="150"/>
-      <c r="B25" s="168"/>
-      <c r="C25" s="108" t="s">
-        <v>329</v>
-      </c>
-      <c r="D25" s="100" t="s">
-        <v>330</v>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="191"/>
+      <c r="B25" s="181"/>
+      <c r="C25" s="58" t="s">
+        <v>300</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="168" t="s">
-        <v>222</v>
-      </c>
-      <c r="B26" s="168" t="s">
-        <v>234</v>
-      </c>
-      <c r="C26" s="177" t="s">
-        <v>239</v>
-      </c>
-      <c r="D26" s="103" t="s">
-        <v>241</v>
+      <c r="A26" s="192"/>
+      <c r="B26" s="182"/>
+      <c r="C26" s="58" t="s">
+        <v>328</v>
+      </c>
+      <c r="D26" s="99" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="168"/>
-      <c r="B27" s="168"/>
-      <c r="C27" s="177"/>
-      <c r="D27" s="100" t="s">
-        <v>278</v>
+      <c r="A27" s="150" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="180" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D27" s="99" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="168"/>
-      <c r="B28" s="168"/>
-      <c r="C28" s="177" t="s">
-        <v>240</v>
-      </c>
+      <c r="A28" s="151"/>
+      <c r="B28" s="181"/>
+      <c r="C28" s="58"/>
       <c r="D28" s="58" t="s">
-        <v>299</v>
+        <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="168"/>
-      <c r="B29" s="168"/>
-      <c r="C29" s="177"/>
-      <c r="D29" s="61" t="s">
-        <v>242</v>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="151"/>
+      <c r="B29" s="181"/>
+      <c r="C29" s="107" t="s">
+        <v>329</v>
+      </c>
+      <c r="D29" s="99" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="168"/>
-      <c r="B30" s="168"/>
-      <c r="C30" s="105" t="s">
-        <v>307</v>
-      </c>
-      <c r="D30" s="58" t="s">
-        <v>308</v>
+      <c r="A30" s="151"/>
+      <c r="B30" s="181"/>
+      <c r="C30" s="107" t="s">
+        <v>359</v>
+      </c>
+      <c r="D30" s="99" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="168"/>
-      <c r="B31" s="168"/>
-      <c r="C31" s="105">
-        <v>2.1</v>
-      </c>
-      <c r="D31" s="58" t="s">
-        <v>316</v>
+      <c r="A31" s="152"/>
+      <c r="B31" s="182"/>
+      <c r="C31" s="107" t="s">
+        <v>367</v>
+      </c>
+      <c r="D31" s="99" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="168"/>
-      <c r="B32" s="168"/>
-      <c r="C32" s="105" t="s">
+      <c r="A32" s="157" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="180" t="s">
+        <v>234</v>
+      </c>
+      <c r="C32" s="183" t="s">
         <v>239</v>
       </c>
-      <c r="D32" s="58" t="s">
-        <v>317</v>
+      <c r="D32" s="102" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="168"/>
-      <c r="B33" s="168"/>
-      <c r="C33" s="117" t="s">
-        <v>239</v>
-      </c>
-      <c r="D33" s="116" t="s">
-        <v>346</v>
+      <c r="A33" s="193"/>
+      <c r="B33" s="181"/>
+      <c r="C33" s="184"/>
+      <c r="D33" s="99" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="168"/>
-      <c r="B34" s="168"/>
-      <c r="C34" s="115" t="s">
-        <v>239</v>
-      </c>
-      <c r="D34" s="100" t="s">
-        <v>352</v>
+      <c r="A34" s="193"/>
+      <c r="B34" s="181"/>
+      <c r="C34" s="177" t="s">
+        <v>240</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>299</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="143" t="s">
-        <v>296</v>
-      </c>
-      <c r="B35" s="168" t="s">
-        <v>234</v>
-      </c>
-      <c r="C35" s="58" t="s">
-        <v>297</v>
-      </c>
-      <c r="D35" s="58" t="s">
-        <v>298</v>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="193"/>
+      <c r="B35" s="181"/>
+      <c r="C35" s="177"/>
+      <c r="D35" s="61" t="s">
+        <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="143"/>
-      <c r="B36" s="168"/>
-      <c r="C36" s="61" t="s">
-        <v>281</v>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="193"/>
+      <c r="B36" s="181"/>
+      <c r="C36" s="104" t="s">
+        <v>307</v>
       </c>
       <c r="D36" s="58" t="s">
-        <v>280</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="143"/>
-      <c r="B37" s="168"/>
-      <c r="C37" s="58" t="s">
-        <v>350</v>
+      <c r="A37" s="193"/>
+      <c r="B37" s="181"/>
+      <c r="C37" s="104">
+        <v>2.1</v>
       </c>
       <c r="D37" s="58" t="s">
-        <v>349</v>
+        <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="44"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="193"/>
+      <c r="B38" s="181"/>
+      <c r="C38" s="104" t="s">
+        <v>239</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="134" t="s">
-        <v>260</v>
-      </c>
-      <c r="B39" s="168" t="s">
+      <c r="A39" s="193"/>
+      <c r="B39" s="181"/>
+      <c r="C39" s="116" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" s="115" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="158"/>
+      <c r="B40" s="182"/>
+      <c r="C40" s="114" t="s">
+        <v>239</v>
+      </c>
+      <c r="D40" s="99" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="194" t="s">
+        <v>296</v>
+      </c>
+      <c r="B41" s="180" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="79" t="s">
-        <v>261</v>
+      <c r="C41" s="58" t="s">
+        <v>297</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="134"/>
-      <c r="B40" s="168"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58" t="s">
-        <v>257</v>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="195"/>
+      <c r="B42" s="181"/>
+      <c r="C42" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>280</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="58" t="s">
-        <v>334</v>
-      </c>
-      <c r="B41" s="105" t="s">
-        <v>234</v>
-      </c>
-      <c r="C41" s="79" t="s">
-        <v>335</v>
-      </c>
-      <c r="D41" s="100" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="B42" s="105" t="s">
-        <v>234</v>
-      </c>
-      <c r="C42" s="106" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="104" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="170" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="173" t="s">
-        <v>234</v>
-      </c>
+    <row r="43" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="196"/>
+      <c r="B43" s="182"/>
       <c r="C43" s="58" t="s">
-        <v>268</v>
+        <v>350</v>
       </c>
       <c r="D43" s="58" t="s">
-        <v>251</v>
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="171"/>
-      <c r="B44" s="174"/>
-      <c r="C44" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="D44" s="58" t="s">
-        <v>251</v>
-      </c>
+      <c r="A44" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="44"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="171"/>
-      <c r="B45" s="174"/>
-      <c r="C45" s="58" t="s">
-        <v>269</v>
-      </c>
-      <c r="D45" s="58" t="s">
-        <v>251</v>
+      <c r="A45" s="157" t="s">
+        <v>260</v>
+      </c>
+      <c r="B45" s="180" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="58"/>
+      <c r="D45" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="171"/>
-      <c r="B46" s="174"/>
-      <c r="C46" s="100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D46" s="100" t="s">
-        <v>102</v>
+      <c r="A46" s="158"/>
+      <c r="B46" s="182"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="171"/>
-      <c r="B47" s="174"/>
-      <c r="C47" s="58" t="s">
-        <v>282</v>
-      </c>
-      <c r="D47" s="58" t="s">
-        <v>251</v>
+      <c r="A47" s="96" t="s">
+        <v>334</v>
+      </c>
+      <c r="B47" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C47" s="79" t="s">
+        <v>335</v>
+      </c>
+      <c r="D47" s="99" t="s">
+        <v>336</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="171"/>
-      <c r="B48" s="174"/>
-      <c r="C48" s="58" t="s">
-        <v>283</v>
-      </c>
-      <c r="D48" s="58" t="s">
-        <v>284</v>
+    <row r="48" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="B48" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C48" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="103" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="171"/>
-      <c r="B49" s="174"/>
-      <c r="C49" s="100" t="s">
-        <v>288</v>
-      </c>
-      <c r="D49" s="100" t="s">
+    <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="194" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="180" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="58" t="s">
+        <v>268</v>
+      </c>
+      <c r="D49" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="171"/>
-      <c r="B50" s="174"/>
-      <c r="C50" s="100" t="s">
-        <v>302</v>
-      </c>
-      <c r="D50" s="100" t="s">
+      <c r="A50" s="195"/>
+      <c r="B50" s="181"/>
+      <c r="C50" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="D50" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="171"/>
-      <c r="B51" s="174"/>
-      <c r="C51" s="100" t="s">
-        <v>289</v>
-      </c>
-      <c r="D51" s="100" t="s">
+      <c r="A51" s="195"/>
+      <c r="B51" s="181"/>
+      <c r="C51" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D51" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="195"/>
+      <c r="B52" s="181"/>
+      <c r="C52" s="99" t="s">
+        <v>277</v>
+      </c>
+      <c r="D52" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="171"/>
-      <c r="B52" s="174"/>
-      <c r="C52" s="107" t="s">
-        <v>244</v>
-      </c>
-      <c r="D52" s="104" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="171"/>
-      <c r="B53" s="174"/>
-      <c r="C53" s="108" t="s">
-        <v>311</v>
-      </c>
-      <c r="D53" s="100" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="195"/>
+      <c r="B53" s="181"/>
+      <c r="C53" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="D53" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="171"/>
-      <c r="B54" s="174"/>
+      <c r="A54" s="195"/>
+      <c r="B54" s="181"/>
       <c r="C54" s="58" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="D54" s="58" t="s">
-        <v>100</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="171"/>
-      <c r="B55" s="174"/>
-      <c r="C55" s="100" t="s">
-        <v>313</v>
-      </c>
-      <c r="D55" s="100" t="s">
-        <v>314</v>
+      <c r="A55" s="195"/>
+      <c r="B55" s="181"/>
+      <c r="C55" s="99" t="s">
+        <v>288</v>
+      </c>
+      <c r="D55" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="171"/>
-      <c r="B56" s="174"/>
-      <c r="C56" s="100" t="s">
-        <v>315</v>
-      </c>
-      <c r="D56" s="100" t="s">
-        <v>102</v>
+      <c r="A56" s="195"/>
+      <c r="B56" s="181"/>
+      <c r="C56" s="99" t="s">
+        <v>302</v>
+      </c>
+      <c r="D56" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="171"/>
-      <c r="B57" s="174"/>
-      <c r="C57" s="100" t="s">
-        <v>268</v>
-      </c>
-      <c r="D57" s="100" t="s">
+      <c r="A57" s="195"/>
+      <c r="B57" s="181"/>
+      <c r="C57" s="99" t="s">
+        <v>289</v>
+      </c>
+      <c r="D57" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="171"/>
-      <c r="B58" s="174"/>
-      <c r="C58" s="58" t="s">
-        <v>318</v>
-      </c>
-      <c r="D58" s="58" t="s">
-        <v>102</v>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="195"/>
+      <c r="B58" s="181"/>
+      <c r="C58" s="106" t="s">
+        <v>244</v>
+      </c>
+      <c r="D58" s="103" t="s">
+        <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="171"/>
-      <c r="B59" s="174"/>
-      <c r="C59" s="100" t="s">
-        <v>283</v>
-      </c>
-      <c r="D59" s="100" t="s">
-        <v>320</v>
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="195"/>
+      <c r="B59" s="181"/>
+      <c r="C59" s="107" t="s">
+        <v>311</v>
+      </c>
+      <c r="D59" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="171"/>
-      <c r="B60" s="174"/>
-      <c r="C60" s="100" t="s">
-        <v>319</v>
-      </c>
-      <c r="D60" s="100" t="s">
-        <v>251</v>
+      <c r="A60" s="195"/>
+      <c r="B60" s="181"/>
+      <c r="C60" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D60" s="58" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="171"/>
-      <c r="B61" s="174"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="109" t="s">
-        <v>321</v>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="195"/>
+      <c r="B61" s="181"/>
+      <c r="C61" s="99" t="s">
+        <v>313</v>
+      </c>
+      <c r="D61" s="99" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="171"/>
-      <c r="B62" s="174"/>
-      <c r="C62" s="100" t="s">
-        <v>322</v>
-      </c>
-      <c r="D62" s="100" t="s">
-        <v>251</v>
+      <c r="A62" s="195"/>
+      <c r="B62" s="181"/>
+      <c r="C62" s="99" t="s">
+        <v>315</v>
+      </c>
+      <c r="D62" s="99" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="171"/>
-      <c r="B63" s="174"/>
-      <c r="C63" s="100" t="s">
+      <c r="A63" s="195"/>
+      <c r="B63" s="181"/>
+      <c r="C63" s="99" t="s">
         <v>268</v>
       </c>
-      <c r="D63" s="100" t="s">
-        <v>251</v>
+      <c r="D63" s="99" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="171"/>
-      <c r="B64" s="174"/>
-      <c r="C64" s="100" t="s">
-        <v>339</v>
-      </c>
-      <c r="D64" s="100" t="s">
-        <v>251</v>
+      <c r="A64" s="195"/>
+      <c r="B64" s="181"/>
+      <c r="C64" s="58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D64" s="58" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="171"/>
-      <c r="B65" s="174"/>
-      <c r="C65" s="100" t="s">
-        <v>340</v>
-      </c>
-      <c r="D65" s="100" t="s">
-        <v>251</v>
+      <c r="A65" s="195"/>
+      <c r="B65" s="181"/>
+      <c r="C65" s="99" t="s">
+        <v>283</v>
+      </c>
+      <c r="D65" s="99" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="171"/>
-      <c r="B66" s="174"/>
-      <c r="C66" s="100" t="s">
-        <v>324</v>
-      </c>
-      <c r="D66" s="100" t="s">
-        <v>323</v>
+      <c r="A66" s="195"/>
+      <c r="B66" s="181"/>
+      <c r="C66" s="99" t="s">
+        <v>319</v>
+      </c>
+      <c r="D66" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="171"/>
-      <c r="B67" s="174"/>
-      <c r="C67" s="116" t="s">
-        <v>345</v>
-      </c>
-      <c r="D67" s="116" t="s">
-        <v>251</v>
+    <row r="67" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="195"/>
+      <c r="B67" s="181"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="108" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="172"/>
-      <c r="B68" s="175"/>
-      <c r="C68" s="100" t="s">
-        <v>338</v>
-      </c>
-      <c r="D68" s="100" t="s">
-        <v>337</v>
+      <c r="A68" s="195"/>
+      <c r="B68" s="181"/>
+      <c r="C68" s="99" t="s">
+        <v>322</v>
+      </c>
+      <c r="D68" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="B69" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C69" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D69" s="100" t="s">
-        <v>274</v>
+      <c r="A69" s="195"/>
+      <c r="B69" s="181"/>
+      <c r="C69" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="D69" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="58" t="s">
-        <v>310</v>
-      </c>
-      <c r="B70" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C70" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D70" s="100" t="s">
-        <v>274</v>
+      <c r="A70" s="195"/>
+      <c r="B70" s="181"/>
+      <c r="C70" s="99" t="s">
+        <v>339</v>
+      </c>
+      <c r="D70" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="44"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="195"/>
+      <c r="B71" s="181"/>
+      <c r="C71" s="99" t="s">
+        <v>340</v>
+      </c>
+      <c r="D71" s="99" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="72" spans="1:4" ht="31.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="99"/>
-      <c r="B72" s="67"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="79" t="s">
-        <v>261</v>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="195"/>
+      <c r="B72" s="181"/>
+      <c r="C72" s="99" t="s">
+        <v>324</v>
+      </c>
+      <c r="D72" s="99" t="s">
+        <v>323</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="168" t="s">
-        <v>84</v>
-      </c>
-      <c r="B73" s="168" t="s">
-        <v>234</v>
-      </c>
-      <c r="C73" s="106" t="s">
-        <v>246</v>
-      </c>
-      <c r="D73" s="58" t="s">
-        <v>253</v>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="195"/>
+      <c r="B73" s="181"/>
+      <c r="C73" s="115" t="s">
+        <v>345</v>
+      </c>
+      <c r="D73" s="115" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="168"/>
-      <c r="B74" s="168"/>
-      <c r="C74" s="106">
-        <v>10.1</v>
-      </c>
-      <c r="D74" s="58" t="s">
-        <v>272</v>
+      <c r="A74" s="195"/>
+      <c r="B74" s="181"/>
+      <c r="C74" s="99" t="s">
+        <v>338</v>
+      </c>
+      <c r="D74" s="99" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="168"/>
-      <c r="B75" s="168"/>
-      <c r="C75" s="106">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D75" s="58" t="s">
-        <v>272</v>
+      <c r="A75" s="195"/>
+      <c r="B75" s="181"/>
+      <c r="C75" s="99" t="s">
+        <v>353</v>
+      </c>
+      <c r="D75" s="99" t="s">
+        <v>354</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="168"/>
-      <c r="B76" s="168"/>
-      <c r="C76" s="111" t="s">
-        <v>293</v>
-      </c>
-      <c r="D76" s="101" t="s">
-        <v>294</v>
+    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="195"/>
+      <c r="B76" s="181"/>
+      <c r="C76" s="119" t="s">
+        <v>356</v>
+      </c>
+      <c r="D76" s="118" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="134" t="s">
-        <v>247</v>
-      </c>
-      <c r="B77" s="168" t="s">
-        <v>234</v>
-      </c>
-      <c r="C77" s="168"/>
-      <c r="D77" s="178" t="s">
-        <v>261</v>
+      <c r="A77" s="195"/>
+      <c r="B77" s="181"/>
+      <c r="C77" s="99" t="s">
+        <v>357</v>
+      </c>
+      <c r="D77" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="134"/>
-      <c r="B78" s="168"/>
-      <c r="C78" s="168"/>
-      <c r="D78" s="178"/>
+      <c r="A78" s="195"/>
+      <c r="B78" s="181"/>
+      <c r="C78" s="99" t="s">
+        <v>358</v>
+      </c>
+      <c r="D78" s="99" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="B79" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C79" s="106" t="s">
-        <v>250</v>
-      </c>
-      <c r="D79" s="100" t="s">
+      <c r="A79" s="195"/>
+      <c r="B79" s="181"/>
+      <c r="C79" s="99" t="s">
+        <v>364</v>
+      </c>
+      <c r="D79" s="99" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="196"/>
+      <c r="B80" s="182"/>
+      <c r="C80" s="99" t="s">
+        <v>366</v>
+      </c>
+      <c r="D80" s="99" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B80" s="39"/>
-      <c r="C80" s="98"/>
-      <c r="D80" s="98"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="58" t="s">
-        <v>249</v>
-      </c>
-      <c r="B81" s="106" t="s">
+      <c r="A81" s="96" t="s">
+        <v>309</v>
+      </c>
+      <c r="B81" s="125" t="s">
         <v>234</v>
       </c>
-      <c r="C81" s="112" t="s">
-        <v>265</v>
-      </c>
-      <c r="D81" s="58" t="s">
-        <v>267</v>
+      <c r="C81" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D81" s="99" t="s">
+        <v>274</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="134" t="s">
-        <v>285</v>
-      </c>
-      <c r="B82" s="168" t="s">
+    <row r="82" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="96" t="s">
+        <v>310</v>
+      </c>
+      <c r="B82" s="125" t="s">
         <v>234</v>
       </c>
-      <c r="C82" s="101" t="s">
-        <v>295</v>
-      </c>
-      <c r="D82" s="58" t="s">
-        <v>251</v>
+      <c r="C82" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D82" s="99" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="134"/>
-      <c r="B83" s="168"/>
-      <c r="C83" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="D83" s="100" t="s">
-        <v>306</v>
-      </c>
+      <c r="A83" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="44"/>
     </row>
-    <row r="84" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="134"/>
-      <c r="B84" s="168"/>
-      <c r="C84" s="112" t="s">
-        <v>286</v>
-      </c>
-      <c r="D84" s="58" t="s">
-        <v>287</v>
+    <row r="84" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="157" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="180" t="s">
+        <v>234</v>
+      </c>
+      <c r="C84" s="58"/>
+      <c r="D84" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B85" s="98"/>
-      <c r="C85" s="98"/>
-      <c r="D85" s="98"/>
+      <c r="A85" s="193"/>
+      <c r="B85" s="181"/>
+      <c r="C85" s="105" t="s">
+        <v>246</v>
+      </c>
+      <c r="D85" s="58" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="151" t="s">
-        <v>58</v>
-      </c>
-      <c r="B86" s="168" t="s">
-        <v>271</v>
-      </c>
-      <c r="C86" s="112" t="s">
-        <v>265</v>
+      <c r="A86" s="193"/>
+      <c r="B86" s="181"/>
+      <c r="C86" s="105">
+        <v>10.1</v>
       </c>
       <c r="D86" s="58" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="151"/>
-      <c r="B87" s="168"/>
-      <c r="C87" s="112" t="s">
-        <v>265</v>
+      <c r="A87" s="193"/>
+      <c r="B87" s="181"/>
+      <c r="C87" s="105">
+        <v>10.199999999999999</v>
       </c>
       <c r="D87" s="58" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="97" t="s">
-        <v>59</v>
-      </c>
-      <c r="B88" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C88" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D88" s="58" t="s">
-        <v>100</v>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="158"/>
+      <c r="B88" s="182"/>
+      <c r="C88" s="110" t="s">
+        <v>293</v>
+      </c>
+      <c r="D88" s="100" t="s">
+        <v>294</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="B89" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C89" s="58"/>
-      <c r="D89" s="61" t="s">
-        <v>292</v>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="157" t="s">
+        <v>247</v>
+      </c>
+      <c r="B89" s="180" t="s">
+        <v>234</v>
+      </c>
+      <c r="C89" s="166"/>
+      <c r="D89" s="178" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="97" t="s">
-        <v>60</v>
-      </c>
-      <c r="B90" s="106" t="s">
-        <v>271</v>
-      </c>
-      <c r="C90" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D90" s="58" t="s">
-        <v>263</v>
-      </c>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="158"/>
+      <c r="B90" s="182"/>
+      <c r="C90" s="166"/>
+      <c r="D90" s="178"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B91" s="98"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="98"/>
+    <row r="91" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="123" t="s">
+        <v>262</v>
+      </c>
+      <c r="B91" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="C91" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="D91" s="99" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="58"/>
-      <c r="B92" s="106" t="s">
-        <v>234</v>
-      </c>
-      <c r="C92" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D92" s="100" t="s">
-        <v>274</v>
-      </c>
+      <c r="A92" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B92" s="39"/>
+      <c r="C92" s="98"/>
+      <c r="D92" s="98"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="98" t="s">
-        <v>279</v>
-      </c>
-      <c r="B93" s="98"/>
-      <c r="C93" s="98"/>
-      <c r="D93" s="98"/>
+      <c r="A93" s="96" t="s">
+        <v>249</v>
+      </c>
+      <c r="B93" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="C93" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="D93" s="58" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="58"/>
-      <c r="B94" s="106" t="s">
+      <c r="A94" s="157" t="s">
+        <v>285</v>
+      </c>
+      <c r="B94" s="180" t="s">
         <v>234</v>
       </c>
-      <c r="C94" s="58" t="s">
+      <c r="C94" s="100" t="s">
+        <v>295</v>
+      </c>
+      <c r="D94" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="193"/>
+      <c r="B95" s="181"/>
+      <c r="C95" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D95" s="99" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="158"/>
+      <c r="B96" s="182"/>
+      <c r="C96" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="D96" s="58" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B97" s="98"/>
+      <c r="C97" s="98"/>
+      <c r="D97" s="98"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="197" t="s">
+        <v>58</v>
+      </c>
+      <c r="B98" s="180" t="s">
+        <v>271</v>
+      </c>
+      <c r="C98" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="D98" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="198"/>
+      <c r="B99" s="182"/>
+      <c r="C99" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="D99" s="58" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="199" t="s">
+        <v>59</v>
+      </c>
+      <c r="B100" s="125" t="s">
+        <v>271</v>
+      </c>
+      <c r="C100" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D100" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="96" t="s">
+        <v>291</v>
+      </c>
+      <c r="B101" s="125" t="s">
+        <v>271</v>
+      </c>
+      <c r="C101" s="58"/>
+      <c r="D101" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B102" s="125" t="s">
+        <v>271</v>
+      </c>
+      <c r="C102" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D102" s="58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B103" s="98"/>
+      <c r="C103" s="98"/>
+      <c r="D103" s="98"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="58"/>
+      <c r="B104" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="C104" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D94" s="100" t="s">
+      <c r="D104" s="99" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B105" s="98"/>
+      <c r="C105" s="98"/>
+      <c r="D105" s="98"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="58"/>
+      <c r="B106" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="C106" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D106" s="99" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="A26:A34"/>
+  <mergeCells count="32">
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="B84:B88"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A49:A80"/>
+    <mergeCell ref="B49:B80"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="A32:A40"/>
+    <mergeCell ref="B32:B40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A43:A68"/>
-    <mergeCell ref="B43:B68"/>
-    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D89:D90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
host url change in api.json
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="375">
   <si>
     <t>Document</t>
   </si>
@@ -2971,6 +2971,15 @@
   </si>
   <si>
     <t>Handshake API</t>
+  </si>
+  <si>
+    <t>code 2024</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corrected URL </t>
   </si>
 </sst>
 </file>
@@ -3959,8 +3968,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3983,66 +4022,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4064,22 +4043,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4090,6 +4111,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4106,25 +4130,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5139,7 +5148,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5149,7 +5158,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5259,10 +5268,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="161" t="s">
+      <c r="A7" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5273,8 +5282,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="161"/>
-      <c r="B8" s="160"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="147"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5283,8 +5292,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="161"/>
-      <c r="B9" s="160"/>
+      <c r="A9" s="146"/>
+      <c r="B9" s="147"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5293,8 +5302,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="161"/>
-      <c r="B10" s="160"/>
+      <c r="A10" s="146"/>
+      <c r="B10" s="147"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5303,8 +5312,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="161"/>
-      <c r="B11" s="160"/>
+      <c r="A11" s="146"/>
+      <c r="B11" s="147"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5313,8 +5322,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="161"/>
-      <c r="B12" s="160"/>
+      <c r="A12" s="146"/>
+      <c r="B12" s="147"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5323,10 +5332,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="163" t="s">
+      <c r="A13" s="149" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5337,8 +5346,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="163"/>
-      <c r="B14" s="160"/>
+      <c r="A14" s="149"/>
+      <c r="B14" s="147"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5347,8 +5356,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
-      <c r="B15" s="160"/>
+      <c r="A15" s="149"/>
+      <c r="B15" s="147"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5357,10 +5366,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="146" t="s">
+      <c r="A16" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="151" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5371,8 +5380,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="146"/>
-      <c r="B17" s="155"/>
+      <c r="A17" s="150"/>
+      <c r="B17" s="151"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5381,8 +5390,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="146"/>
-      <c r="B18" s="155"/>
+      <c r="A18" s="150"/>
+      <c r="B18" s="151"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5391,8 +5400,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="146"/>
-      <c r="B19" s="155"/>
+      <c r="A19" s="150"/>
+      <c r="B19" s="151"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5401,8 +5410,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="146"/>
-      <c r="B20" s="155"/>
+      <c r="A20" s="150"/>
+      <c r="B20" s="151"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5411,8 +5420,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="146"/>
-      <c r="B21" s="155"/>
+      <c r="A21" s="150"/>
+      <c r="B21" s="151"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5421,8 +5430,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="146"/>
-      <c r="B22" s="155"/>
+      <c r="A22" s="150"/>
+      <c r="B22" s="151"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5431,8 +5440,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="146"/>
-      <c r="B23" s="155"/>
+      <c r="A23" s="150"/>
+      <c r="B23" s="151"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5441,26 +5450,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="146"/>
-      <c r="B24" s="155"/>
-      <c r="C24" s="146" t="s">
+      <c r="A24" s="150"/>
+      <c r="B24" s="151"/>
+      <c r="C24" s="150" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="147" t="s">
+      <c r="D24" s="157" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="146"/>
-      <c r="B25" s="155"/>
-      <c r="C25" s="146"/>
-      <c r="D25" s="147"/>
+      <c r="A25" s="150"/>
+      <c r="B25" s="151"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="157"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="161" t="s">
+      <c r="A26" s="146" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="160" t="s">
+      <c r="B26" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5471,8 +5480,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="161"/>
-      <c r="B27" s="160"/>
+      <c r="A27" s="146"/>
+      <c r="B27" s="147"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5499,28 +5508,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="162" t="s">
+      <c r="A30" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="160" t="s">
+      <c r="B30" s="147" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="146" t="s">
+      <c r="C30" s="150" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="150" t="s">
+      <c r="D30" s="160" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="162"/>
-      <c r="B31" s="160"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="150"/>
+      <c r="A31" s="148"/>
+      <c r="B31" s="147"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="160"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="162"/>
-      <c r="B32" s="160"/>
+      <c r="A32" s="148"/>
+      <c r="B32" s="147"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5529,8 +5538,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="162"/>
-      <c r="B33" s="160"/>
+      <c r="A33" s="148"/>
+      <c r="B33" s="147"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5539,8 +5548,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="162"/>
-      <c r="B34" s="160"/>
+      <c r="A34" s="148"/>
+      <c r="B34" s="147"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5549,8 +5558,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="162"/>
-      <c r="B35" s="160"/>
+      <c r="A35" s="148"/>
+      <c r="B35" s="147"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5559,8 +5568,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="162"/>
-      <c r="B36" s="160"/>
+      <c r="A36" s="148"/>
+      <c r="B36" s="147"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5569,26 +5578,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="162"/>
-      <c r="B37" s="160"/>
-      <c r="C37" s="151" t="s">
+      <c r="A37" s="148"/>
+      <c r="B37" s="147"/>
+      <c r="C37" s="161" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="153" t="s">
+      <c r="D37" s="163" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="162"/>
-      <c r="B38" s="160"/>
-      <c r="C38" s="152"/>
-      <c r="D38" s="153"/>
+      <c r="A38" s="148"/>
+      <c r="B38" s="147"/>
+      <c r="C38" s="162"/>
+      <c r="D38" s="163"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="161" t="s">
+      <c r="A39" s="146" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5599,8 +5608,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="161"/>
-      <c r="B40" s="160"/>
+      <c r="A40" s="146"/>
+      <c r="B40" s="147"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5627,10 +5636,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="162" t="s">
+      <c r="A43" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="160" t="s">
+      <c r="B43" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5639,8 +5648,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="162"/>
-      <c r="B44" s="160"/>
+      <c r="A44" s="148"/>
+      <c r="B44" s="147"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5649,10 +5658,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="157" t="s">
+      <c r="A45" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="160" t="s">
+      <c r="B45" s="147" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5661,8 +5670,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="158"/>
-      <c r="B46" s="160"/>
+      <c r="A46" s="155"/>
+      <c r="B46" s="147"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5671,8 +5680,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="158"/>
-      <c r="B47" s="160"/>
+      <c r="A47" s="155"/>
+      <c r="B47" s="147"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5681,8 +5690,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="159"/>
-      <c r="B48" s="160"/>
+      <c r="A48" s="156"/>
+      <c r="B48" s="147"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5691,10 +5700,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="155" t="s">
+      <c r="A49" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="155" t="s">
+      <c r="B49" s="151" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9798,8 +9807,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="155"/>
-      <c r="B50" s="155"/>
+      <c r="A50" s="151"/>
+      <c r="B50" s="151"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13903,8 +13912,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="155"/>
-      <c r="B51" s="155"/>
+      <c r="A51" s="151"/>
+      <c r="B51" s="151"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18008,8 +18017,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="155"/>
-      <c r="B52" s="155"/>
+      <c r="A52" s="151"/>
+      <c r="B52" s="151"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22113,12 +22122,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="155"/>
-      <c r="B53" s="155"/>
-      <c r="C53" s="149" t="s">
+      <c r="A53" s="151"/>
+      <c r="B53" s="151"/>
+      <c r="C53" s="159" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="150" t="s">
+      <c r="D53" s="160" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26218,10 +26227,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="155"/>
-      <c r="B54" s="155"/>
-      <c r="C54" s="149"/>
-      <c r="D54" s="150"/>
+      <c r="A54" s="151"/>
+      <c r="B54" s="151"/>
+      <c r="C54" s="159"/>
+      <c r="D54" s="160"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30339,10 +30348,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="154" t="s">
+      <c r="A57" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="155" t="s">
+      <c r="B57" s="151" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30353,8 +30362,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="154"/>
-      <c r="B58" s="155"/>
+      <c r="A58" s="152"/>
+      <c r="B58" s="151"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30363,8 +30372,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="154"/>
-      <c r="B59" s="155"/>
+      <c r="A59" s="152"/>
+      <c r="B59" s="151"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30373,8 +30382,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="154"/>
-      <c r="B60" s="155"/>
+      <c r="A60" s="152"/>
+      <c r="B60" s="151"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30383,8 +30392,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="154"/>
-      <c r="B61" s="155"/>
+      <c r="A61" s="152"/>
+      <c r="B61" s="151"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30393,8 +30402,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="154"/>
-      <c r="B62" s="155"/>
+      <c r="A62" s="152"/>
+      <c r="B62" s="151"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30403,8 +30412,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="154"/>
-      <c r="B63" s="155"/>
+      <c r="A63" s="152"/>
+      <c r="B63" s="151"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30413,16 +30422,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="154"/>
-      <c r="B64" s="155"/>
+      <c r="A64" s="152"/>
+      <c r="B64" s="151"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="154"/>
-      <c r="B65" s="155"/>
+      <c r="A65" s="152"/>
+      <c r="B65" s="151"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30431,16 +30440,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="154"/>
-      <c r="B66" s="155"/>
+      <c r="A66" s="152"/>
+      <c r="B66" s="151"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="154"/>
-      <c r="B67" s="155"/>
+      <c r="A67" s="152"/>
+      <c r="B67" s="151"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30449,8 +30458,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="154"/>
-      <c r="B68" s="155"/>
+      <c r="A68" s="152"/>
+      <c r="B68" s="151"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30459,8 +30468,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="154"/>
-      <c r="B69" s="155"/>
+      <c r="A69" s="152"/>
+      <c r="B69" s="151"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30469,8 +30478,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="154"/>
-      <c r="B70" s="155"/>
+      <c r="A70" s="152"/>
+      <c r="B70" s="151"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30479,8 +30488,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="154"/>
-      <c r="B71" s="155"/>
+      <c r="A71" s="152"/>
+      <c r="B71" s="151"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30489,8 +30498,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="154"/>
-      <c r="B72" s="155"/>
+      <c r="A72" s="152"/>
+      <c r="B72" s="151"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30499,16 +30508,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="154"/>
-      <c r="B73" s="155"/>
+      <c r="A73" s="152"/>
+      <c r="B73" s="151"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="154"/>
-      <c r="B74" s="155"/>
+      <c r="A74" s="152"/>
+      <c r="B74" s="151"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30517,18 +30526,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="154"/>
-      <c r="B75" s="155"/>
-      <c r="C75" s="148"/>
-      <c r="D75" s="156" t="s">
+      <c r="A75" s="152"/>
+      <c r="B75" s="151"/>
+      <c r="C75" s="158"/>
+      <c r="D75" s="153" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="154"/>
-      <c r="B76" s="155"/>
-      <c r="C76" s="148"/>
-      <c r="D76" s="156"/>
+      <c r="A76" s="152"/>
+      <c r="B76" s="151"/>
+      <c r="C76" s="158"/>
+      <c r="D76" s="153"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30552,8 +30561,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30562,13 +30571,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30583,22 +30608,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30652,10 +30661,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="147" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30666,133 +30675,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="161"/>
-      <c r="B5" s="160"/>
-      <c r="C5" s="171" t="s">
+      <c r="A5" s="146"/>
+      <c r="B5" s="147"/>
+      <c r="C5" s="173" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="170" t="s">
+      <c r="D5" s="172" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="161"/>
-      <c r="B6" s="160"/>
-      <c r="C6" s="171"/>
-      <c r="D6" s="170"/>
+      <c r="A6" s="146"/>
+      <c r="B6" s="147"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="172"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="161"/>
-      <c r="B7" s="160"/>
+      <c r="A7" s="146"/>
+      <c r="B7" s="147"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="161"/>
-      <c r="B8" s="160"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="147"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="161"/>
-      <c r="B9" s="160"/>
+      <c r="A9" s="146"/>
+      <c r="B9" s="147"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="163" t="s">
+      <c r="A10" s="149" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="160" t="s">
+      <c r="B10" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="173"/>
-      <c r="D10" s="170" t="s">
+      <c r="C10" s="171"/>
+      <c r="D10" s="172" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="163"/>
-      <c r="B11" s="160"/>
-      <c r="C11" s="173"/>
-      <c r="D11" s="170"/>
+      <c r="A11" s="149"/>
+      <c r="B11" s="147"/>
+      <c r="C11" s="171"/>
+      <c r="D11" s="172"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="163"/>
-      <c r="B12" s="160"/>
-      <c r="C12" s="173"/>
-      <c r="D12" s="170"/>
+      <c r="A12" s="149"/>
+      <c r="B12" s="147"/>
+      <c r="C12" s="171"/>
+      <c r="D12" s="172"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="146" t="s">
+      <c r="A13" s="150" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="151" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="172"/>
-      <c r="D13" s="170" t="s">
+      <c r="C13" s="174"/>
+      <c r="D13" s="172" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="146"/>
-      <c r="B14" s="155"/>
-      <c r="C14" s="172"/>
-      <c r="D14" s="170"/>
+      <c r="A14" s="150"/>
+      <c r="B14" s="151"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="172"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="146"/>
-      <c r="B15" s="155"/>
-      <c r="C15" s="172"/>
+      <c r="A15" s="150"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="174"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="146"/>
-      <c r="B16" s="155"/>
-      <c r="C16" s="172"/>
+      <c r="A16" s="150"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="174"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="146"/>
-      <c r="B17" s="155"/>
-      <c r="C17" s="172"/>
+      <c r="A17" s="150"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="174"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="146"/>
-      <c r="B18" s="155"/>
-      <c r="C18" s="172"/>
+      <c r="A18" s="150"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="174"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="146"/>
-      <c r="B19" s="155"/>
-      <c r="C19" s="172"/>
+      <c r="A19" s="150"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="174"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="146"/>
-      <c r="B20" s="155"/>
-      <c r="C20" s="172"/>
+      <c r="A20" s="150"/>
+      <c r="B20" s="151"/>
+      <c r="C20" s="174"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="146"/>
-      <c r="B21" s="155"/>
-      <c r="C21" s="172"/>
+      <c r="A21" s="150"/>
+      <c r="B21" s="151"/>
+      <c r="C21" s="174"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="146"/>
-      <c r="B22" s="155"/>
-      <c r="C22" s="172"/>
+      <c r="A22" s="150"/>
+      <c r="B22" s="151"/>
+      <c r="C22" s="174"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="146"/>
-      <c r="B23" s="155"/>
-      <c r="C23" s="172"/>
+      <c r="A23" s="150"/>
+      <c r="B23" s="151"/>
+      <c r="C23" s="174"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30890,10 +30899,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="164" t="s">
+      <c r="A32" s="175" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="167" t="s">
+      <c r="B32" s="178" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30904,26 +30913,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="165"/>
-      <c r="B33" s="168"/>
+      <c r="A33" s="176"/>
+      <c r="B33" s="179"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="165"/>
-      <c r="B34" s="168"/>
+      <c r="A34" s="176"/>
+      <c r="B34" s="179"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="165"/>
-      <c r="B35" s="168"/>
+      <c r="A35" s="176"/>
+      <c r="B35" s="179"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="166"/>
-      <c r="B36" s="169"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="180"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30952,10 +30961,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="162" t="s">
+      <c r="A39" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="147" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30966,8 +30975,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="162"/>
-      <c r="B40" s="160"/>
+      <c r="A40" s="148"/>
+      <c r="B40" s="147"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30976,84 +30985,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="161" t="s">
+      <c r="A41" s="146" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="160" t="s">
+      <c r="B41" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="173" t="s">
+      <c r="C41" s="171" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="146" t="s">
+      <c r="D41" s="150" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="161"/>
-      <c r="B42" s="160"/>
-      <c r="C42" s="173"/>
-      <c r="D42" s="146"/>
+      <c r="A42" s="146"/>
+      <c r="B42" s="147"/>
+      <c r="C42" s="171"/>
+      <c r="D42" s="150"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="161"/>
-      <c r="B43" s="160"/>
-      <c r="C43" s="173" t="s">
+      <c r="A43" s="146"/>
+      <c r="B43" s="147"/>
+      <c r="C43" s="171" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="156" t="s">
+      <c r="D43" s="153" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="161"/>
-      <c r="B44" s="160"/>
-      <c r="C44" s="173"/>
-      <c r="D44" s="156"/>
+      <c r="A44" s="146"/>
+      <c r="B44" s="147"/>
+      <c r="C44" s="171"/>
+      <c r="D44" s="153"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="154" t="s">
+      <c r="A45" s="152" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="155" t="s">
+      <c r="B45" s="151" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="177"/>
+      <c r="C45" s="167"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="154"/>
-      <c r="B46" s="155"/>
-      <c r="C46" s="178"/>
-      <c r="D46" s="174" t="s">
+      <c r="A46" s="152"/>
+      <c r="B46" s="151"/>
+      <c r="C46" s="168"/>
+      <c r="D46" s="164" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="154"/>
-      <c r="B47" s="155"/>
-      <c r="C47" s="178"/>
-      <c r="D47" s="175"/>
+      <c r="A47" s="152"/>
+      <c r="B47" s="151"/>
+      <c r="C47" s="168"/>
+      <c r="D47" s="165"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="154"/>
-      <c r="B48" s="155"/>
-      <c r="C48" s="179"/>
-      <c r="D48" s="175"/>
+      <c r="A48" s="152"/>
+      <c r="B48" s="151"/>
+      <c r="C48" s="169"/>
+      <c r="D48" s="165"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="154"/>
-      <c r="B49" s="155"/>
-      <c r="C49" s="149"/>
-      <c r="D49" s="175"/>
+      <c r="A49" s="152"/>
+      <c r="B49" s="151"/>
+      <c r="C49" s="159"/>
+      <c r="D49" s="165"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="154"/>
-      <c r="B50" s="155"/>
-      <c r="C50" s="149"/>
-      <c r="D50" s="176"/>
+      <c r="A50" s="152"/>
+      <c r="B50" s="151"/>
+      <c r="C50" s="159"/>
+      <c r="D50" s="166"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31076,10 +31085,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="155" t="s">
+      <c r="A53" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="155" t="s">
+      <c r="B53" s="151" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31090,8 +31099,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="155"/>
-      <c r="B54" s="155"/>
+      <c r="A54" s="151"/>
+      <c r="B54" s="151"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31100,8 +31109,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="155"/>
-      <c r="B55" s="155"/>
+      <c r="A55" s="151"/>
+      <c r="B55" s="151"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31110,9 +31119,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="155"/>
-      <c r="B56" s="155"/>
-      <c r="C56" s="180" t="s">
+      <c r="A56" s="151"/>
+      <c r="B56" s="151"/>
+      <c r="C56" s="170" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31120,16 +31129,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="155"/>
-      <c r="B57" s="155"/>
-      <c r="C57" s="180"/>
+      <c r="A57" s="151"/>
+      <c r="B57" s="151"/>
+      <c r="C57" s="170"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="155"/>
-      <c r="B58" s="155"/>
+      <c r="A58" s="151"/>
+      <c r="B58" s="151"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31138,8 +31147,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="155"/>
-      <c r="B59" s="155"/>
+      <c r="A59" s="151"/>
+      <c r="B59" s="151"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31148,9 +31157,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="155"/>
-      <c r="B60" s="155"/>
-      <c r="C60" s="180" t="s">
+      <c r="A60" s="151"/>
+      <c r="B60" s="151"/>
+      <c r="C60" s="170" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31158,25 +31167,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="155"/>
-      <c r="B61" s="155"/>
-      <c r="C61" s="180"/>
+      <c r="A61" s="151"/>
+      <c r="B61" s="151"/>
+      <c r="C61" s="170"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="155"/>
-      <c r="B62" s="155"/>
-      <c r="C62" s="180"/>
+      <c r="A62" s="151"/>
+      <c r="B62" s="151"/>
+      <c r="C62" s="170"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="155"/>
-      <c r="B63" s="155"/>
-      <c r="C63" s="173" t="s">
+      <c r="A63" s="151"/>
+      <c r="B63" s="151"/>
+      <c r="C63" s="171" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31184,30 +31193,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="155"/>
-      <c r="B64" s="155"/>
-      <c r="C64" s="173"/>
-      <c r="D64" s="156" t="s">
+      <c r="A64" s="151"/>
+      <c r="B64" s="151"/>
+      <c r="C64" s="171"/>
+      <c r="D64" s="153" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="155"/>
-      <c r="B65" s="155"/>
-      <c r="C65" s="173"/>
-      <c r="D65" s="156"/>
+      <c r="A65" s="151"/>
+      <c r="B65" s="151"/>
+      <c r="C65" s="171"/>
+      <c r="D65" s="153"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="155"/>
-      <c r="B66" s="155"/>
-      <c r="C66" s="173"/>
-      <c r="D66" s="156"/>
+      <c r="A66" s="151"/>
+      <c r="B66" s="151"/>
+      <c r="C66" s="171"/>
+      <c r="D66" s="153"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="155"/>
-      <c r="B67" s="155"/>
-      <c r="C67" s="173"/>
-      <c r="D67" s="156"/>
+      <c r="A67" s="151"/>
+      <c r="B67" s="151"/>
+      <c r="C67" s="171"/>
+      <c r="D67" s="153"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31263,6 +31272,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31279,23 +31305,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31304,10 +31313,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:B42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31341,10 +31350,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="195" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="191" t="s">
+      <c r="B3" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="113" t="s">
@@ -31355,8 +31364,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="190"/>
-      <c r="B4" s="191"/>
+      <c r="A4" s="195"/>
+      <c r="B4" s="196"/>
       <c r="C4" s="113" t="s">
         <v>347</v>
       </c>
@@ -31373,10 +31382,10 @@
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="146" t="s">
+      <c r="A6" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="180" t="s">
+      <c r="B6" s="170" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="58"/>
@@ -31385,8 +31394,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="146"/>
-      <c r="B7" s="180"/>
+      <c r="A7" s="150"/>
+      <c r="B7" s="170"/>
       <c r="C7" s="105" t="s">
         <v>235</v>
       </c>
@@ -31423,10 +31432,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="146" t="s">
+      <c r="A10" s="150" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="180" t="s">
+      <c r="B10" s="170" t="s">
         <v>234</v>
       </c>
       <c r="C10" s="58"/>
@@ -31435,16 +31444,16 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="146"/>
-      <c r="B11" s="180"/>
+      <c r="A11" s="150"/>
+      <c r="B11" s="170"/>
       <c r="C11" s="58"/>
       <c r="D11" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="146"/>
-      <c r="B12" s="180"/>
+      <c r="A12" s="150"/>
+      <c r="B12" s="170"/>
       <c r="C12" s="109" t="s">
         <v>325</v>
       </c>
@@ -31465,10 +31474,10 @@
       <c r="D13" s="58"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="192" t="s">
+      <c r="A14" s="197" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="183" t="s">
+      <c r="B14" s="185" t="s">
         <v>234</v>
       </c>
       <c r="C14" s="58"/>
@@ -31477,7 +31486,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="193"/>
+      <c r="A15" s="198"/>
       <c r="B15" s="186"/>
       <c r="C15" s="120" t="s">
         <v>361</v>
@@ -31487,7 +31496,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="193"/>
+      <c r="A16" s="198"/>
       <c r="B16" s="186"/>
       <c r="C16" s="120" t="s">
         <v>359</v>
@@ -31497,7 +31506,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="193"/>
+      <c r="A17" s="198"/>
       <c r="B17" s="186"/>
       <c r="C17" s="126" t="s">
         <v>367</v>
@@ -31507,8 +31516,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="194"/>
-      <c r="B18" s="184"/>
+      <c r="A18" s="199"/>
+      <c r="B18" s="187"/>
       <c r="C18" s="120" t="s">
         <v>359</v>
       </c>
@@ -31563,10 +31572,10 @@
       <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="195" t="s">
+      <c r="A23" s="182" t="s">
         <v>237</v>
       </c>
-      <c r="B23" s="183" t="s">
+      <c r="B23" s="185" t="s">
         <v>234</v>
       </c>
       <c r="C23" s="58"/>
@@ -31575,7 +31584,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="196"/>
+      <c r="A24" s="183"/>
       <c r="B24" s="186"/>
       <c r="C24" s="58"/>
       <c r="D24" s="58" t="s">
@@ -31583,7 +31592,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="196"/>
+      <c r="A25" s="183"/>
       <c r="B25" s="186"/>
       <c r="C25" s="58"/>
       <c r="D25" s="58" t="s">
@@ -31591,7 +31600,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="196"/>
+      <c r="A26" s="183"/>
       <c r="B26" s="186"/>
       <c r="C26" s="58" t="s">
         <v>300</v>
@@ -31601,8 +31610,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="197"/>
-      <c r="B27" s="184"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="186"/>
       <c r="C27" s="58" t="s">
         <v>328</v>
       </c>
@@ -31611,818 +31620,812 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="157" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="183" t="s">
-        <v>234</v>
-      </c>
+      <c r="A28" s="184"/>
+      <c r="B28" s="187"/>
       <c r="C28" s="58" t="s">
-        <v>303</v>
+        <v>373</v>
       </c>
       <c r="D28" s="99" t="s">
-        <v>304</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="158"/>
-      <c r="B29" s="186"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58" t="s">
+      <c r="A29" s="154" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="185" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D29" s="99" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="155"/>
+      <c r="B30" s="186"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="158"/>
-      <c r="B30" s="186"/>
-      <c r="C30" s="107" t="s">
-        <v>329</v>
-      </c>
-      <c r="D30" s="99" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="158"/>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="155"/>
       <c r="B31" s="186"/>
       <c r="C31" s="107" t="s">
-        <v>359</v>
+        <v>329</v>
       </c>
       <c r="D31" s="99" t="s">
-        <v>360</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="158"/>
+      <c r="A32" s="155"/>
       <c r="B32" s="186"/>
       <c r="C32" s="107" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="D32" s="99" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="159"/>
-      <c r="B33" s="184"/>
+      <c r="A33" s="155"/>
+      <c r="B33" s="186"/>
       <c r="C33" s="107" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D33" s="99" t="s">
-        <v>251</v>
+        <v>368</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="151" t="s">
-        <v>222</v>
-      </c>
-      <c r="B34" s="183" t="s">
-        <v>234</v>
-      </c>
-      <c r="C34" s="198" t="s">
-        <v>239</v>
-      </c>
-      <c r="D34" s="102" t="s">
-        <v>241</v>
+      <c r="A34" s="156"/>
+      <c r="B34" s="187"/>
+      <c r="C34" s="107" t="s">
+        <v>371</v>
+      </c>
+      <c r="D34" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="185"/>
-      <c r="B35" s="186"/>
-      <c r="C35" s="199"/>
-      <c r="D35" s="99" t="s">
-        <v>278</v>
+      <c r="A35" s="161" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35" s="185" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" s="188" t="s">
+        <v>239</v>
+      </c>
+      <c r="D35" s="102" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="185"/>
+      <c r="A36" s="194"/>
       <c r="B36" s="186"/>
-      <c r="C36" s="200" t="s">
+      <c r="C36" s="189"/>
+      <c r="D36" s="99" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="194"/>
+      <c r="B37" s="186"/>
+      <c r="C37" s="190" t="s">
         <v>240</v>
       </c>
-      <c r="D36" s="58" t="s">
+      <c r="D37" s="58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="185"/>
-      <c r="B37" s="186"/>
-      <c r="C37" s="200"/>
-      <c r="D37" s="61" t="s">
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="194"/>
+      <c r="B38" s="186"/>
+      <c r="C38" s="190"/>
+      <c r="D38" s="61" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="185"/>
-      <c r="B38" s="186"/>
-      <c r="C38" s="104" t="s">
-        <v>307</v>
-      </c>
-      <c r="D38" s="58" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="185"/>
+      <c r="A39" s="194"/>
       <c r="B39" s="186"/>
-      <c r="C39" s="104">
-        <v>2.1</v>
+      <c r="C39" s="104" t="s">
+        <v>307</v>
       </c>
       <c r="D39" s="58" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="185"/>
+      <c r="A40" s="194"/>
       <c r="B40" s="186"/>
-      <c r="C40" s="104" t="s">
-        <v>239</v>
+      <c r="C40" s="104">
+        <v>2.1</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="185"/>
+      <c r="A41" s="194"/>
       <c r="B41" s="186"/>
-      <c r="C41" s="116" t="s">
+      <c r="C41" s="104" t="s">
         <v>239</v>
       </c>
-      <c r="D41" s="115" t="s">
+      <c r="D41" s="58" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="194"/>
+      <c r="B42" s="186"/>
+      <c r="C42" s="116" t="s">
+        <v>239</v>
+      </c>
+      <c r="D42" s="115" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="152"/>
-      <c r="B42" s="184"/>
-      <c r="C42" s="114" t="s">
+    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="162"/>
+      <c r="B43" s="187"/>
+      <c r="C43" s="114" t="s">
         <v>239</v>
       </c>
-      <c r="D42" s="99" t="s">
+      <c r="D43" s="99" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="187" t="s">
+    <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="191" t="s">
         <v>296</v>
       </c>
-      <c r="B43" s="183" t="s">
+      <c r="B44" s="185" t="s">
         <v>234</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C44" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D44" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="188"/>
-      <c r="B44" s="186"/>
-      <c r="C44" s="61" t="s">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="192"/>
+      <c r="B45" s="186"/>
+      <c r="C45" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D45" s="58" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="189"/>
-      <c r="B45" s="184"/>
-      <c r="C45" s="58" t="s">
-        <v>350</v>
-      </c>
-      <c r="D45" s="58" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="129" t="s">
+      <c r="A46" s="193"/>
+      <c r="B46" s="187"/>
+      <c r="C46" s="58" t="s">
+        <v>350</v>
+      </c>
+      <c r="D46" s="58" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="129" t="s">
         <v>370</v>
       </c>
-      <c r="B46" s="128" t="s">
+      <c r="B47" s="128" t="s">
         <v>234</v>
       </c>
-      <c r="C46" s="127" t="s">
+      <c r="C47" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="D46" s="58"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="44"/>
+      <c r="D47" s="58"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="151" t="s">
-        <v>260</v>
-      </c>
-      <c r="B48" s="183" t="s">
-        <v>234</v>
-      </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="79" t="s">
-        <v>261</v>
-      </c>
+      <c r="A48" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="44"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="152"/>
-      <c r="B49" s="184"/>
+      <c r="A49" s="161" t="s">
+        <v>260</v>
+      </c>
+      <c r="B49" s="185" t="s">
+        <v>234</v>
+      </c>
       <c r="C49" s="58"/>
-      <c r="D49" s="58" t="s">
-        <v>257</v>
+      <c r="D49" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="96" t="s">
+      <c r="A50" s="162"/>
+      <c r="B50" s="187"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="96" t="s">
         <v>334</v>
-      </c>
-      <c r="B50" s="124" t="s">
-        <v>234</v>
-      </c>
-      <c r="C50" s="79" t="s">
-        <v>335</v>
-      </c>
-      <c r="D50" s="99" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="96" t="s">
-        <v>243</v>
       </c>
       <c r="B51" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C51" s="105" t="s">
+      <c r="C51" s="79" t="s">
+        <v>335</v>
+      </c>
+      <c r="D51" s="99" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="B52" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C52" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="D51" s="103" t="s">
+      <c r="D52" s="103" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="187" t="s">
+    <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="183" t="s">
+      <c r="B53" s="185" t="s">
         <v>234</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="C53" s="58" t="s">
         <v>268</v>
-      </c>
-      <c r="D52" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="188"/>
-      <c r="B53" s="186"/>
-      <c r="C53" s="58" t="s">
-        <v>270</v>
       </c>
       <c r="D53" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="188"/>
+      <c r="A54" s="192"/>
       <c r="B54" s="186"/>
       <c r="C54" s="58" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D54" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="188"/>
+      <c r="A55" s="192"/>
       <c r="B55" s="186"/>
-      <c r="C55" s="99" t="s">
-        <v>277</v>
-      </c>
-      <c r="D55" s="99" t="s">
-        <v>102</v>
+      <c r="C55" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="188"/>
+      <c r="A56" s="192"/>
       <c r="B56" s="186"/>
-      <c r="C56" s="58" t="s">
-        <v>282</v>
-      </c>
-      <c r="D56" s="58" t="s">
-        <v>251</v>
+      <c r="C56" s="99" t="s">
+        <v>277</v>
+      </c>
+      <c r="D56" s="99" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="188"/>
+      <c r="A57" s="192"/>
       <c r="B57" s="186"/>
       <c r="C57" s="58" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D57" s="58" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="188"/>
+      <c r="A58" s="192"/>
       <c r="B58" s="186"/>
-      <c r="C58" s="99" t="s">
-        <v>288</v>
-      </c>
-      <c r="D58" s="99" t="s">
-        <v>251</v>
+      <c r="C58" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="D58" s="58" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="188"/>
+      <c r="A59" s="192"/>
       <c r="B59" s="186"/>
       <c r="C59" s="99" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="D59" s="99" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="188"/>
+      <c r="A60" s="192"/>
       <c r="B60" s="186"/>
       <c r="C60" s="99" t="s">
+        <v>302</v>
+      </c>
+      <c r="D60" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="192"/>
+      <c r="B61" s="186"/>
+      <c r="C61" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="D60" s="99" t="s">
+      <c r="D61" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="188"/>
-      <c r="B61" s="186"/>
-      <c r="C61" s="106" t="s">
+    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="192"/>
+      <c r="B62" s="186"/>
+      <c r="C62" s="106" t="s">
         <v>244</v>
       </c>
-      <c r="D61" s="103" t="s">
+      <c r="D62" s="103" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="188"/>
-      <c r="B62" s="186"/>
-      <c r="C62" s="107" t="s">
+    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="192"/>
+      <c r="B63" s="186"/>
+      <c r="C63" s="107" t="s">
         <v>311</v>
       </c>
-      <c r="D62" s="99" t="s">
+      <c r="D63" s="99" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="188"/>
-      <c r="B63" s="186"/>
-      <c r="C63" s="58" t="s">
-        <v>312</v>
-      </c>
-      <c r="D63" s="58" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="188"/>
+      <c r="A64" s="192"/>
       <c r="B64" s="186"/>
-      <c r="C64" s="99" t="s">
-        <v>313</v>
-      </c>
-      <c r="D64" s="99" t="s">
-        <v>314</v>
+      <c r="C64" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D64" s="58" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="188"/>
+      <c r="A65" s="192"/>
       <c r="B65" s="186"/>
       <c r="C65" s="99" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D65" s="99" t="s">
-        <v>102</v>
+        <v>314</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="188"/>
+      <c r="A66" s="192"/>
       <c r="B66" s="186"/>
       <c r="C66" s="99" t="s">
-        <v>268</v>
+        <v>315</v>
       </c>
       <c r="D66" s="99" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="188"/>
+      <c r="A67" s="192"/>
       <c r="B67" s="186"/>
-      <c r="C67" s="58" t="s">
-        <v>318</v>
-      </c>
-      <c r="D67" s="58" t="s">
+      <c r="C67" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67" s="99" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="188"/>
+      <c r="A68" s="192"/>
       <c r="B68" s="186"/>
-      <c r="C68" s="99" t="s">
-        <v>283</v>
-      </c>
-      <c r="D68" s="99" t="s">
-        <v>320</v>
+      <c r="C68" s="58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D68" s="58" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="188"/>
+      <c r="A69" s="192"/>
       <c r="B69" s="186"/>
       <c r="C69" s="99" t="s">
+        <v>283</v>
+      </c>
+      <c r="D69" s="99" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="192"/>
+      <c r="B70" s="186"/>
+      <c r="C70" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="D69" s="99" t="s">
+      <c r="D70" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="188"/>
-      <c r="B70" s="186"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="108" t="s">
+    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="192"/>
+      <c r="B71" s="186"/>
+      <c r="C71" s="58"/>
+      <c r="D71" s="108" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="188"/>
-      <c r="B71" s="186"/>
-      <c r="C71" s="99" t="s">
-        <v>322</v>
-      </c>
-      <c r="D71" s="99" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="188"/>
+      <c r="A72" s="192"/>
       <c r="B72" s="186"/>
       <c r="C72" s="99" t="s">
-        <v>268</v>
+        <v>322</v>
       </c>
       <c r="D72" s="99" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="188"/>
+      <c r="A73" s="192"/>
       <c r="B73" s="186"/>
       <c r="C73" s="99" t="s">
-        <v>339</v>
+        <v>268</v>
       </c>
       <c r="D73" s="99" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="188"/>
+      <c r="A74" s="192"/>
       <c r="B74" s="186"/>
       <c r="C74" s="99" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D74" s="99" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="188"/>
+      <c r="A75" s="192"/>
       <c r="B75" s="186"/>
       <c r="C75" s="99" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="D75" s="99" t="s">
-        <v>323</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="188"/>
+      <c r="A76" s="192"/>
       <c r="B76" s="186"/>
-      <c r="C76" s="115" t="s">
-        <v>345</v>
-      </c>
-      <c r="D76" s="115" t="s">
-        <v>251</v>
+      <c r="C76" s="99" t="s">
+        <v>324</v>
+      </c>
+      <c r="D76" s="99" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="188"/>
+      <c r="A77" s="192"/>
       <c r="B77" s="186"/>
-      <c r="C77" s="99" t="s">
-        <v>338</v>
-      </c>
-      <c r="D77" s="99" t="s">
-        <v>337</v>
+      <c r="C77" s="115" t="s">
+        <v>345</v>
+      </c>
+      <c r="D77" s="115" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="188"/>
+      <c r="A78" s="192"/>
       <c r="B78" s="186"/>
       <c r="C78" s="99" t="s">
+        <v>338</v>
+      </c>
+      <c r="D78" s="99" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="192"/>
+      <c r="B79" s="186"/>
+      <c r="C79" s="99" t="s">
         <v>353</v>
       </c>
-      <c r="D78" s="99" t="s">
+      <c r="D79" s="99" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="188"/>
-      <c r="B79" s="186"/>
-      <c r="C79" s="119" t="s">
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="192"/>
+      <c r="B80" s="186"/>
+      <c r="C80" s="119" t="s">
         <v>356</v>
       </c>
-      <c r="D79" s="118" t="s">
+      <c r="D80" s="118" t="s">
         <v>355</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="188"/>
-      <c r="B80" s="186"/>
-      <c r="C80" s="99" t="s">
-        <v>357</v>
-      </c>
-      <c r="D80" s="99" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="188"/>
+      <c r="A81" s="192"/>
       <c r="B81" s="186"/>
       <c r="C81" s="99" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D81" s="99" t="s">
-        <v>102</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="188"/>
+      <c r="A82" s="192"/>
       <c r="B82" s="186"/>
       <c r="C82" s="99" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D82" s="99" t="s">
-        <v>365</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="189"/>
-      <c r="B83" s="184"/>
+      <c r="A83" s="192"/>
+      <c r="B83" s="186"/>
       <c r="C83" s="99" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D83" s="99" t="s">
-        <v>251</v>
+        <v>365</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="96" t="s">
-        <v>309</v>
-      </c>
-      <c r="B84" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="C84" s="58" t="s">
-        <v>30</v>
+      <c r="A84" s="192"/>
+      <c r="B84" s="186"/>
+      <c r="C84" s="99" t="s">
+        <v>366</v>
       </c>
       <c r="D84" s="99" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="96" t="s">
-        <v>310</v>
-      </c>
-      <c r="B85" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="C85" s="58" t="s">
-        <v>30</v>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="193"/>
+      <c r="B85" s="187"/>
+      <c r="C85" s="99" t="s">
+        <v>372</v>
       </c>
       <c r="D85" s="99" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B86" s="39"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="44"/>
+      <c r="A86" s="96" t="s">
+        <v>309</v>
+      </c>
+      <c r="B86" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="C86" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D86" s="99" t="s">
+        <v>274</v>
+      </c>
     </row>
-    <row r="87" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="151" t="s">
-        <v>84</v>
-      </c>
-      <c r="B87" s="183" t="s">
+    <row r="87" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="96" t="s">
+        <v>310</v>
+      </c>
+      <c r="B87" s="125" t="s">
         <v>234</v>
       </c>
-      <c r="C87" s="58"/>
-      <c r="D87" s="79" t="s">
-        <v>261</v>
+      <c r="C87" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D87" s="99" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="185"/>
-      <c r="B88" s="186"/>
-      <c r="C88" s="105" t="s">
-        <v>246</v>
-      </c>
-      <c r="D88" s="58" t="s">
-        <v>253</v>
-      </c>
+      <c r="A88" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" s="39"/>
+      <c r="C88" s="39"/>
+      <c r="D88" s="44"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="185"/>
-      <c r="B89" s="186"/>
-      <c r="C89" s="105">
-        <v>10.1</v>
-      </c>
-      <c r="D89" s="58" t="s">
-        <v>272</v>
+    <row r="89" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="161" t="s">
+        <v>84</v>
+      </c>
+      <c r="B89" s="185" t="s">
+        <v>234</v>
+      </c>
+      <c r="C89" s="58"/>
+      <c r="D89" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="185"/>
+      <c r="A90" s="194"/>
       <c r="B90" s="186"/>
-      <c r="C90" s="105">
-        <v>10.199999999999999</v>
+      <c r="C90" s="105" t="s">
+        <v>246</v>
       </c>
       <c r="D90" s="58" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="152"/>
-      <c r="B91" s="184"/>
-      <c r="C91" s="110" t="s">
-        <v>293</v>
-      </c>
-      <c r="D91" s="100" t="s">
-        <v>294</v>
+      <c r="A91" s="194"/>
+      <c r="B91" s="186"/>
+      <c r="C91" s="105">
+        <v>10.1</v>
+      </c>
+      <c r="D91" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="151" t="s">
-        <v>247</v>
-      </c>
-      <c r="B92" s="183" t="s">
-        <v>234</v>
-      </c>
-      <c r="C92" s="180"/>
-      <c r="D92" s="201" t="s">
-        <v>261</v>
+      <c r="A92" s="194"/>
+      <c r="B92" s="186"/>
+      <c r="C92" s="105">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D92" s="58" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="152"/>
-      <c r="B93" s="184"/>
-      <c r="C93" s="180"/>
-      <c r="D93" s="201"/>
+      <c r="A93" s="162"/>
+      <c r="B93" s="187"/>
+      <c r="C93" s="110" t="s">
+        <v>293</v>
+      </c>
+      <c r="D93" s="100" t="s">
+        <v>294</v>
+      </c>
     </row>
-    <row r="94" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="123" t="s">
-        <v>262</v>
-      </c>
-      <c r="B94" s="125" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="161" t="s">
+        <v>247</v>
+      </c>
+      <c r="B94" s="185" t="s">
         <v>234</v>
       </c>
-      <c r="C94" s="105" t="s">
-        <v>250</v>
-      </c>
-      <c r="D94" s="99" t="s">
-        <v>251</v>
+      <c r="C94" s="170"/>
+      <c r="D94" s="181" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B95" s="39"/>
-      <c r="C95" s="98"/>
-      <c r="D95" s="98"/>
+      <c r="A95" s="162"/>
+      <c r="B95" s="187"/>
+      <c r="C95" s="170"/>
+      <c r="D95" s="181"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="96" t="s">
-        <v>249</v>
+    <row r="96" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="123" t="s">
+        <v>262</v>
       </c>
       <c r="B96" s="125" t="s">
         <v>234</v>
       </c>
-      <c r="C96" s="111" t="s">
-        <v>265</v>
-      </c>
-      <c r="D96" s="58" t="s">
-        <v>267</v>
+      <c r="C96" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="D96" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="151" t="s">
-        <v>285</v>
-      </c>
-      <c r="B97" s="183" t="s">
-        <v>234</v>
-      </c>
-      <c r="C97" s="100" t="s">
-        <v>295</v>
-      </c>
-      <c r="D97" s="58" t="s">
-        <v>251</v>
-      </c>
+      <c r="A97" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B97" s="39"/>
+      <c r="C97" s="98"/>
+      <c r="D97" s="98"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="185"/>
-      <c r="B98" s="186"/>
-      <c r="C98" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="D98" s="99" t="s">
-        <v>306</v>
+      <c r="A98" s="96" t="s">
+        <v>249</v>
+      </c>
+      <c r="B98" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="C98" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="D98" s="58" t="s">
+        <v>267</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="152"/>
-      <c r="B99" s="184"/>
-      <c r="C99" s="111" t="s">
-        <v>286</v>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="161" t="s">
+        <v>285</v>
+      </c>
+      <c r="B99" s="185" t="s">
+        <v>234</v>
+      </c>
+      <c r="C99" s="100" t="s">
+        <v>295</v>
       </c>
       <c r="D99" s="58" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="98" t="s">
+      <c r="A100" s="194"/>
+      <c r="B100" s="186"/>
+      <c r="C100" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D100" s="99" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="162"/>
+      <c r="B101" s="187"/>
+      <c r="C101" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="D101" s="58" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="B100" s="98"/>
-      <c r="C100" s="98"/>
-      <c r="D100" s="98"/>
+      <c r="B102" s="98"/>
+      <c r="C102" s="98"/>
+      <c r="D102" s="98"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="181" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="200" t="s">
         <v>58</v>
       </c>
-      <c r="B101" s="183" t="s">
+      <c r="B103" s="185" t="s">
         <v>271</v>
       </c>
-      <c r="C101" s="111" t="s">
+      <c r="C103" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D101" s="58" t="s">
+      <c r="D103" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="182"/>
-      <c r="B102" s="184"/>
-      <c r="C102" s="111" t="s">
+    <row r="104" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="201"/>
+      <c r="B104" s="187"/>
+      <c r="C104" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D102" s="58" t="s">
+      <c r="D104" s="58" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="130" t="s">
-        <v>59</v>
-      </c>
-      <c r="B103" s="125" t="s">
-        <v>271</v>
-      </c>
-      <c r="C103" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D103" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="96" t="s">
-        <v>291</v>
-      </c>
-      <c r="B104" s="125" t="s">
-        <v>271</v>
-      </c>
-      <c r="C104" s="58"/>
-      <c r="D104" s="61" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="97" t="s">
-        <v>60</v>
+      <c r="A105" s="130" t="s">
+        <v>59</v>
       </c>
       <c r="B105" s="125" t="s">
         <v>271</v>
@@ -32431,32 +32434,38 @@
         <v>264</v>
       </c>
       <c r="D105" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="96" t="s">
+        <v>291</v>
+      </c>
+      <c r="B106" s="125" t="s">
+        <v>271</v>
+      </c>
+      <c r="C106" s="58"/>
+      <c r="D106" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B107" s="125" t="s">
+        <v>271</v>
+      </c>
+      <c r="C107" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D107" s="58" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B106" s="98"/>
-      <c r="C106" s="98"/>
-      <c r="D106" s="98"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="58"/>
-      <c r="B107" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="C107" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D107" s="99" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="98" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B108" s="98"/>
       <c r="C108" s="98"/>
@@ -32474,14 +32483,36 @@
         <v>274</v>
       </c>
     </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="98" t="s">
+        <v>279</v>
+      </c>
+      <c r="B110" s="98"/>
+      <c r="C110" s="98"/>
+      <c r="D110" s="98"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="58"/>
+      <c r="B111" s="125" t="s">
+        <v>234</v>
+      </c>
+      <c r="C111" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D111" s="99" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B6:B7"/>
@@ -32490,24 +32521,22 @@
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A52:A83"/>
-    <mergeCell ref="B52:B83"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="A34:A42"/>
-    <mergeCell ref="B34:B42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="A53:A85"/>
+    <mergeCell ref="B53:B85"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="A35:A43"/>
+    <mergeCell ref="B35:B43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated to be inline with doucmentation
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="383">
   <si>
     <t>Document</t>
   </si>
@@ -2980,6 +2980,30 @@
   </si>
   <si>
     <t xml:space="preserve">corrected URL </t>
+  </si>
+  <si>
+    <t>Example 8</t>
+  </si>
+  <si>
+    <t>Specified batch timeout</t>
+  </si>
+  <si>
+    <t>Handshake Schema</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>Specified digest field required for POST requests</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>Payroll Submission Response</t>
+  </si>
+  <si>
+    <t>Removed reference to batch</t>
   </si>
 </sst>
 </file>
@@ -3581,7 +3605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3876,9 +3900,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3922,6 +3943,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4073,9 +4112,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4093,6 +4129,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4539,12 +4578,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="132"/>
-      <c r="D2" s="133"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="138"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4567,12 +4606,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="133"/>
+      <c r="B4" s="137"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="138"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4612,10 +4651,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="134" t="s">
+      <c r="A7" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="137">
+      <c r="B7" s="142">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4629,8 +4668,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="135"/>
-      <c r="B8" s="138"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="143"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4642,8 +4681,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="138"/>
+      <c r="A9" s="140"/>
+      <c r="B9" s="143"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4655,8 +4694,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="135"/>
-      <c r="B10" s="138"/>
+      <c r="A10" s="140"/>
+      <c r="B10" s="143"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4668,8 +4707,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="135"/>
-      <c r="B11" s="138"/>
+      <c r="A11" s="140"/>
+      <c r="B11" s="143"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4681,8 +4720,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="136"/>
-      <c r="B12" s="139"/>
+      <c r="A12" s="141"/>
+      <c r="B12" s="144"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4694,10 +4733,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="142" t="s">
+      <c r="A13" s="147" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="137">
+      <c r="B13" s="142">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4711,8 +4750,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
-      <c r="B14" s="139"/>
+      <c r="A14" s="148"/>
+      <c r="B14" s="144"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4758,12 +4797,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="131" t="s">
+      <c r="A17" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="132"/>
-      <c r="C17" s="132"/>
-      <c r="D17" s="133"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="138"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4803,21 +4842,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="131" t="s">
+      <c r="A20" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="132"/>
-      <c r="C20" s="132"/>
-      <c r="D20" s="133"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="138"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="144" t="s">
+      <c r="A21" s="149" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="141">
+      <c r="B21" s="146">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4831,8 +4870,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="145"/>
-      <c r="B22" s="139"/>
+      <c r="A22" s="150"/>
+      <c r="B22" s="144"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4855,18 +4894,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="131" t="s">
+      <c r="A24" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="132"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="133"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="138"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="140" t="s">
+      <c r="A25" s="145" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="141">
+      <c r="B25" s="146">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4880,8 +4919,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="135"/>
-      <c r="B26" s="138"/>
+      <c r="A26" s="140"/>
+      <c r="B26" s="143"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4893,8 +4932,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="135"/>
-      <c r="B27" s="138"/>
+      <c r="A27" s="140"/>
+      <c r="B27" s="143"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4906,8 +4945,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="135"/>
-      <c r="B28" s="138"/>
+      <c r="A28" s="140"/>
+      <c r="B28" s="143"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4919,8 +4958,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="135"/>
-      <c r="B29" s="138"/>
+      <c r="A29" s="140"/>
+      <c r="B29" s="143"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4932,8 +4971,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="135"/>
-      <c r="B30" s="138"/>
+      <c r="A30" s="140"/>
+      <c r="B30" s="143"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4945,8 +4984,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="135"/>
-      <c r="B31" s="138"/>
+      <c r="A31" s="140"/>
+      <c r="B31" s="143"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4958,8 +4997,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="136"/>
-      <c r="B32" s="139"/>
+      <c r="A32" s="141"/>
+      <c r="B32" s="144"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5083,12 +5122,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="131" t="s">
+      <c r="A41" s="136" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="132"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="133"/>
+      <c r="B41" s="137"/>
+      <c r="C41" s="137"/>
+      <c r="D41" s="138"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5268,10 +5307,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="146" t="s">
+      <c r="A7" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5282,8 +5321,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="146"/>
-      <c r="B8" s="147"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="152"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5292,8 +5331,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="146"/>
-      <c r="B9" s="147"/>
+      <c r="A9" s="151"/>
+      <c r="B9" s="152"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5302,8 +5341,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="146"/>
-      <c r="B10" s="147"/>
+      <c r="A10" s="151"/>
+      <c r="B10" s="152"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5312,8 +5351,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="146"/>
-      <c r="B11" s="147"/>
+      <c r="A11" s="151"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5322,8 +5361,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="146"/>
-      <c r="B12" s="147"/>
+      <c r="A12" s="151"/>
+      <c r="B12" s="152"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5332,10 +5371,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="149" t="s">
+      <c r="A13" s="154" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="147" t="s">
+      <c r="B13" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5346,8 +5385,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="149"/>
-      <c r="B14" s="147"/>
+      <c r="A14" s="154"/>
+      <c r="B14" s="152"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5356,8 +5395,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="149"/>
-      <c r="B15" s="147"/>
+      <c r="A15" s="154"/>
+      <c r="B15" s="152"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5366,10 +5405,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="150" t="s">
+      <c r="A16" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5380,8 +5419,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="150"/>
-      <c r="B17" s="151"/>
+      <c r="A17" s="155"/>
+      <c r="B17" s="156"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5390,8 +5429,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="150"/>
-      <c r="B18" s="151"/>
+      <c r="A18" s="155"/>
+      <c r="B18" s="156"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5400,8 +5439,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="150"/>
-      <c r="B19" s="151"/>
+      <c r="A19" s="155"/>
+      <c r="B19" s="156"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5410,8 +5449,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="150"/>
-      <c r="B20" s="151"/>
+      <c r="A20" s="155"/>
+      <c r="B20" s="156"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5420,8 +5459,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
-      <c r="B21" s="151"/>
+      <c r="A21" s="155"/>
+      <c r="B21" s="156"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5430,8 +5469,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
-      <c r="B22" s="151"/>
+      <c r="A22" s="155"/>
+      <c r="B22" s="156"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5440,8 +5479,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="150"/>
-      <c r="B23" s="151"/>
+      <c r="A23" s="155"/>
+      <c r="B23" s="156"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5450,26 +5489,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="150"/>
-      <c r="B24" s="151"/>
-      <c r="C24" s="150" t="s">
+      <c r="A24" s="155"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="155" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="157" t="s">
+      <c r="D24" s="162" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="150"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="157"/>
+      <c r="A25" s="155"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="155"/>
+      <c r="D25" s="162"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="146" t="s">
+      <c r="A26" s="151" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="147" t="s">
+      <c r="B26" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5480,8 +5519,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="146"/>
-      <c r="B27" s="147"/>
+      <c r="A27" s="151"/>
+      <c r="B27" s="152"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5508,28 +5547,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="148" t="s">
+      <c r="A30" s="153" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="147" t="s">
+      <c r="B30" s="152" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="150" t="s">
+      <c r="C30" s="155" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="160" t="s">
+      <c r="D30" s="165" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="148"/>
-      <c r="B31" s="147"/>
-      <c r="C31" s="150"/>
-      <c r="D31" s="160"/>
+      <c r="A31" s="153"/>
+      <c r="B31" s="152"/>
+      <c r="C31" s="155"/>
+      <c r="D31" s="165"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="148"/>
-      <c r="B32" s="147"/>
+      <c r="A32" s="153"/>
+      <c r="B32" s="152"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5538,8 +5577,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="148"/>
-      <c r="B33" s="147"/>
+      <c r="A33" s="153"/>
+      <c r="B33" s="152"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5548,8 +5587,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="148"/>
-      <c r="B34" s="147"/>
+      <c r="A34" s="153"/>
+      <c r="B34" s="152"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5558,8 +5597,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="148"/>
-      <c r="B35" s="147"/>
+      <c r="A35" s="153"/>
+      <c r="B35" s="152"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5568,8 +5607,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="148"/>
-      <c r="B36" s="147"/>
+      <c r="A36" s="153"/>
+      <c r="B36" s="152"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5578,26 +5617,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="148"/>
-      <c r="B37" s="147"/>
-      <c r="C37" s="161" t="s">
+      <c r="A37" s="153"/>
+      <c r="B37" s="152"/>
+      <c r="C37" s="166" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="163" t="s">
+      <c r="D37" s="168" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="148"/>
-      <c r="B38" s="147"/>
-      <c r="C38" s="162"/>
-      <c r="D38" s="163"/>
+      <c r="A38" s="153"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="167"/>
+      <c r="D38" s="168"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="146" t="s">
+      <c r="A39" s="151" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="147" t="s">
+      <c r="B39" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5608,8 +5647,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="146"/>
-      <c r="B40" s="147"/>
+      <c r="A40" s="151"/>
+      <c r="B40" s="152"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5636,10 +5675,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="148" t="s">
+      <c r="A43" s="153" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="147" t="s">
+      <c r="B43" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5648,8 +5687,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="148"/>
-      <c r="B44" s="147"/>
+      <c r="A44" s="153"/>
+      <c r="B44" s="152"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5658,10 +5697,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="154" t="s">
+      <c r="A45" s="159" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="147" t="s">
+      <c r="B45" s="152" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5670,8 +5709,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="155"/>
-      <c r="B46" s="147"/>
+      <c r="A46" s="160"/>
+      <c r="B46" s="152"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5680,8 +5719,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="155"/>
-      <c r="B47" s="147"/>
+      <c r="A47" s="160"/>
+      <c r="B47" s="152"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5690,8 +5729,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="156"/>
-      <c r="B48" s="147"/>
+      <c r="A48" s="161"/>
+      <c r="B48" s="152"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5700,10 +5739,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="151" t="s">
+      <c r="A49" s="156" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="151" t="s">
+      <c r="B49" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9807,8 +9846,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="151"/>
-      <c r="B50" s="151"/>
+      <c r="A50" s="156"/>
+      <c r="B50" s="156"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13912,8 +13951,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="151"/>
-      <c r="B51" s="151"/>
+      <c r="A51" s="156"/>
+      <c r="B51" s="156"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18017,8 +18056,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="151"/>
-      <c r="B52" s="151"/>
+      <c r="A52" s="156"/>
+      <c r="B52" s="156"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22122,12 +22161,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="151"/>
-      <c r="B53" s="151"/>
-      <c r="C53" s="159" t="s">
+      <c r="A53" s="156"/>
+      <c r="B53" s="156"/>
+      <c r="C53" s="164" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="160" t="s">
+      <c r="D53" s="165" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26227,10 +26266,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="151"/>
-      <c r="B54" s="151"/>
-      <c r="C54" s="159"/>
-      <c r="D54" s="160"/>
+      <c r="A54" s="156"/>
+      <c r="B54" s="156"/>
+      <c r="C54" s="164"/>
+      <c r="D54" s="165"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30348,10 +30387,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="152" t="s">
+      <c r="A57" s="157" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="151" t="s">
+      <c r="B57" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30362,8 +30401,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="152"/>
-      <c r="B58" s="151"/>
+      <c r="A58" s="157"/>
+      <c r="B58" s="156"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30372,8 +30411,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="152"/>
-      <c r="B59" s="151"/>
+      <c r="A59" s="157"/>
+      <c r="B59" s="156"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30382,8 +30421,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="152"/>
-      <c r="B60" s="151"/>
+      <c r="A60" s="157"/>
+      <c r="B60" s="156"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30392,8 +30431,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="152"/>
-      <c r="B61" s="151"/>
+      <c r="A61" s="157"/>
+      <c r="B61" s="156"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30402,8 +30441,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="152"/>
-      <c r="B62" s="151"/>
+      <c r="A62" s="157"/>
+      <c r="B62" s="156"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30412,8 +30451,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="152"/>
-      <c r="B63" s="151"/>
+      <c r="A63" s="157"/>
+      <c r="B63" s="156"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30422,16 +30461,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="152"/>
-      <c r="B64" s="151"/>
+      <c r="A64" s="157"/>
+      <c r="B64" s="156"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="152"/>
-      <c r="B65" s="151"/>
+      <c r="A65" s="157"/>
+      <c r="B65" s="156"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30440,16 +30479,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="152"/>
-      <c r="B66" s="151"/>
+      <c r="A66" s="157"/>
+      <c r="B66" s="156"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="152"/>
-      <c r="B67" s="151"/>
+      <c r="A67" s="157"/>
+      <c r="B67" s="156"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30458,8 +30497,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="152"/>
-      <c r="B68" s="151"/>
+      <c r="A68" s="157"/>
+      <c r="B68" s="156"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30468,8 +30507,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="152"/>
-      <c r="B69" s="151"/>
+      <c r="A69" s="157"/>
+      <c r="B69" s="156"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30478,8 +30517,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="152"/>
-      <c r="B70" s="151"/>
+      <c r="A70" s="157"/>
+      <c r="B70" s="156"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30488,8 +30527,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="152"/>
-      <c r="B71" s="151"/>
+      <c r="A71" s="157"/>
+      <c r="B71" s="156"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30498,8 +30537,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="152"/>
-      <c r="B72" s="151"/>
+      <c r="A72" s="157"/>
+      <c r="B72" s="156"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30508,16 +30547,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="152"/>
-      <c r="B73" s="151"/>
+      <c r="A73" s="157"/>
+      <c r="B73" s="156"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="152"/>
-      <c r="B74" s="151"/>
+      <c r="A74" s="157"/>
+      <c r="B74" s="156"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30526,18 +30565,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="152"/>
-      <c r="B75" s="151"/>
-      <c r="C75" s="158"/>
-      <c r="D75" s="153" t="s">
+      <c r="A75" s="157"/>
+      <c r="B75" s="156"/>
+      <c r="C75" s="163"/>
+      <c r="D75" s="158" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="152"/>
-      <c r="B76" s="151"/>
-      <c r="C76" s="158"/>
-      <c r="D76" s="153"/>
+      <c r="A76" s="157"/>
+      <c r="B76" s="156"/>
+      <c r="C76" s="163"/>
+      <c r="D76" s="158"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30661,10 +30700,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="146" t="s">
+      <c r="A4" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="147" t="s">
+      <c r="B4" s="152" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30675,133 +30714,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="146"/>
-      <c r="B5" s="147"/>
-      <c r="C5" s="173" t="s">
+      <c r="A5" s="151"/>
+      <c r="B5" s="152"/>
+      <c r="C5" s="178" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="172" t="s">
+      <c r="D5" s="177" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="146"/>
-      <c r="B6" s="147"/>
-      <c r="C6" s="173"/>
-      <c r="D6" s="172"/>
+      <c r="A6" s="151"/>
+      <c r="B6" s="152"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="177"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="146"/>
-      <c r="B7" s="147"/>
+      <c r="A7" s="151"/>
+      <c r="B7" s="152"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="146"/>
-      <c r="B8" s="147"/>
+      <c r="A8" s="151"/>
+      <c r="B8" s="152"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="146"/>
-      <c r="B9" s="147"/>
+      <c r="A9" s="151"/>
+      <c r="B9" s="152"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="149" t="s">
+      <c r="A10" s="154" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="147" t="s">
+      <c r="B10" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="171"/>
-      <c r="D10" s="172" t="s">
+      <c r="C10" s="176"/>
+      <c r="D10" s="177" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="149"/>
-      <c r="B11" s="147"/>
-      <c r="C11" s="171"/>
-      <c r="D11" s="172"/>
+      <c r="A11" s="154"/>
+      <c r="B11" s="152"/>
+      <c r="C11" s="176"/>
+      <c r="D11" s="177"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
-      <c r="B12" s="147"/>
-      <c r="C12" s="171"/>
-      <c r="D12" s="172"/>
+      <c r="A12" s="154"/>
+      <c r="B12" s="152"/>
+      <c r="C12" s="176"/>
+      <c r="D12" s="177"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="150" t="s">
+      <c r="A13" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="151" t="s">
+      <c r="B13" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="174"/>
-      <c r="D13" s="172" t="s">
+      <c r="C13" s="179"/>
+      <c r="D13" s="177" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="150"/>
-      <c r="B14" s="151"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="172"/>
+      <c r="A14" s="155"/>
+      <c r="B14" s="156"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="177"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="150"/>
-      <c r="B15" s="151"/>
-      <c r="C15" s="174"/>
+      <c r="A15" s="155"/>
+      <c r="B15" s="156"/>
+      <c r="C15" s="179"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="150"/>
-      <c r="B16" s="151"/>
-      <c r="C16" s="174"/>
+      <c r="A16" s="155"/>
+      <c r="B16" s="156"/>
+      <c r="C16" s="179"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="150"/>
-      <c r="B17" s="151"/>
-      <c r="C17" s="174"/>
+      <c r="A17" s="155"/>
+      <c r="B17" s="156"/>
+      <c r="C17" s="179"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="150"/>
-      <c r="B18" s="151"/>
-      <c r="C18" s="174"/>
+      <c r="A18" s="155"/>
+      <c r="B18" s="156"/>
+      <c r="C18" s="179"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="150"/>
-      <c r="B19" s="151"/>
-      <c r="C19" s="174"/>
+      <c r="A19" s="155"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="179"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="150"/>
-      <c r="B20" s="151"/>
-      <c r="C20" s="174"/>
+      <c r="A20" s="155"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="179"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
-      <c r="B21" s="151"/>
-      <c r="C21" s="174"/>
+      <c r="A21" s="155"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="179"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="174"/>
+      <c r="A22" s="155"/>
+      <c r="B22" s="156"/>
+      <c r="C22" s="179"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="150"/>
-      <c r="B23" s="151"/>
-      <c r="C23" s="174"/>
+      <c r="A23" s="155"/>
+      <c r="B23" s="156"/>
+      <c r="C23" s="179"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30899,10 +30938,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="175" t="s">
+      <c r="A32" s="180" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="178" t="s">
+      <c r="B32" s="183" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30913,26 +30952,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="176"/>
-      <c r="B33" s="179"/>
+      <c r="A33" s="181"/>
+      <c r="B33" s="184"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="176"/>
-      <c r="B34" s="179"/>
+      <c r="A34" s="181"/>
+      <c r="B34" s="184"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="176"/>
-      <c r="B35" s="179"/>
+      <c r="A35" s="181"/>
+      <c r="B35" s="184"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="177"/>
-      <c r="B36" s="180"/>
+      <c r="A36" s="182"/>
+      <c r="B36" s="185"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -30961,10 +31000,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="148" t="s">
+      <c r="A39" s="153" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="147" t="s">
+      <c r="B39" s="152" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -30975,8 +31014,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="148"/>
-      <c r="B40" s="147"/>
+      <c r="A40" s="153"/>
+      <c r="B40" s="152"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -30985,84 +31024,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="146" t="s">
+      <c r="A41" s="151" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="147" t="s">
+      <c r="B41" s="152" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="171" t="s">
+      <c r="C41" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="150" t="s">
+      <c r="D41" s="155" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="146"/>
-      <c r="B42" s="147"/>
-      <c r="C42" s="171"/>
-      <c r="D42" s="150"/>
+      <c r="A42" s="151"/>
+      <c r="B42" s="152"/>
+      <c r="C42" s="176"/>
+      <c r="D42" s="155"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="146"/>
-      <c r="B43" s="147"/>
-      <c r="C43" s="171" t="s">
+      <c r="A43" s="151"/>
+      <c r="B43" s="152"/>
+      <c r="C43" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="153" t="s">
+      <c r="D43" s="158" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="146"/>
-      <c r="B44" s="147"/>
-      <c r="C44" s="171"/>
-      <c r="D44" s="153"/>
+      <c r="A44" s="151"/>
+      <c r="B44" s="152"/>
+      <c r="C44" s="176"/>
+      <c r="D44" s="158"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="152" t="s">
+      <c r="A45" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="151" t="s">
+      <c r="B45" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="167"/>
+      <c r="C45" s="172"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="152"/>
-      <c r="B46" s="151"/>
-      <c r="C46" s="168"/>
-      <c r="D46" s="164" t="s">
+      <c r="A46" s="157"/>
+      <c r="B46" s="156"/>
+      <c r="C46" s="173"/>
+      <c r="D46" s="169" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="152"/>
-      <c r="B47" s="151"/>
-      <c r="C47" s="168"/>
-      <c r="D47" s="165"/>
+      <c r="A47" s="157"/>
+      <c r="B47" s="156"/>
+      <c r="C47" s="173"/>
+      <c r="D47" s="170"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="152"/>
-      <c r="B48" s="151"/>
-      <c r="C48" s="169"/>
-      <c r="D48" s="165"/>
+      <c r="A48" s="157"/>
+      <c r="B48" s="156"/>
+      <c r="C48" s="174"/>
+      <c r="D48" s="170"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="152"/>
-      <c r="B49" s="151"/>
-      <c r="C49" s="159"/>
-      <c r="D49" s="165"/>
+      <c r="A49" s="157"/>
+      <c r="B49" s="156"/>
+      <c r="C49" s="164"/>
+      <c r="D49" s="170"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="152"/>
-      <c r="B50" s="151"/>
-      <c r="C50" s="159"/>
-      <c r="D50" s="166"/>
+      <c r="A50" s="157"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="164"/>
+      <c r="D50" s="171"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31085,10 +31124,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="151" t="s">
+      <c r="A53" s="156" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="151" t="s">
+      <c r="B53" s="156" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31099,8 +31138,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="151"/>
-      <c r="B54" s="151"/>
+      <c r="A54" s="156"/>
+      <c r="B54" s="156"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31109,8 +31148,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="151"/>
-      <c r="B55" s="151"/>
+      <c r="A55" s="156"/>
+      <c r="B55" s="156"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31119,9 +31158,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="151"/>
-      <c r="B56" s="151"/>
-      <c r="C56" s="170" t="s">
+      <c r="A56" s="156"/>
+      <c r="B56" s="156"/>
+      <c r="C56" s="175" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31129,16 +31168,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="151"/>
-      <c r="B57" s="151"/>
-      <c r="C57" s="170"/>
+      <c r="A57" s="156"/>
+      <c r="B57" s="156"/>
+      <c r="C57" s="175"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="151"/>
-      <c r="B58" s="151"/>
+      <c r="A58" s="156"/>
+      <c r="B58" s="156"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31147,8 +31186,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="151"/>
-      <c r="B59" s="151"/>
+      <c r="A59" s="156"/>
+      <c r="B59" s="156"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31157,9 +31196,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="151"/>
-      <c r="B60" s="151"/>
-      <c r="C60" s="170" t="s">
+      <c r="A60" s="156"/>
+      <c r="B60" s="156"/>
+      <c r="C60" s="175" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31167,25 +31206,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="151"/>
-      <c r="B61" s="151"/>
-      <c r="C61" s="170"/>
+      <c r="A61" s="156"/>
+      <c r="B61" s="156"/>
+      <c r="C61" s="175"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="151"/>
-      <c r="B62" s="151"/>
-      <c r="C62" s="170"/>
+      <c r="A62" s="156"/>
+      <c r="B62" s="156"/>
+      <c r="C62" s="175"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="151"/>
-      <c r="B63" s="151"/>
-      <c r="C63" s="171" t="s">
+      <c r="A63" s="156"/>
+      <c r="B63" s="156"/>
+      <c r="C63" s="176" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31193,30 +31232,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="151"/>
-      <c r="B64" s="151"/>
-      <c r="C64" s="171"/>
-      <c r="D64" s="153" t="s">
+      <c r="A64" s="156"/>
+      <c r="B64" s="156"/>
+      <c r="C64" s="176"/>
+      <c r="D64" s="158" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="151"/>
-      <c r="B65" s="151"/>
-      <c r="C65" s="171"/>
-      <c r="D65" s="153"/>
+      <c r="A65" s="156"/>
+      <c r="B65" s="156"/>
+      <c r="C65" s="176"/>
+      <c r="D65" s="158"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="151"/>
-      <c r="B66" s="151"/>
-      <c r="C66" s="171"/>
-      <c r="D66" s="153"/>
+      <c r="A66" s="156"/>
+      <c r="B66" s="156"/>
+      <c r="C66" s="176"/>
+      <c r="D66" s="158"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="151"/>
-      <c r="B67" s="151"/>
-      <c r="C67" s="171"/>
-      <c r="D67" s="153"/>
+      <c r="A67" s="156"/>
+      <c r="B67" s="156"/>
+      <c r="C67" s="176"/>
+      <c r="D67" s="158"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31313,10 +31352,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58:B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31350,10 +31389,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="195" t="s">
+      <c r="A3" s="200" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="201" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="113" t="s">
@@ -31364,8 +31403,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="195"/>
-      <c r="B4" s="196"/>
+      <c r="A4" s="200"/>
+      <c r="B4" s="201"/>
       <c r="C4" s="113" t="s">
         <v>347</v>
       </c>
@@ -31382,10 +31421,10 @@
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="150" t="s">
+      <c r="A6" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="170" t="s">
+      <c r="B6" s="175" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="58"/>
@@ -31394,8 +31433,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="150"/>
-      <c r="B7" s="170"/>
+      <c r="A7" s="155"/>
+      <c r="B7" s="175"/>
       <c r="C7" s="105" t="s">
         <v>235</v>
       </c>
@@ -31407,7 +31446,7 @@
       <c r="A8" s="96" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="121" t="s">
         <v>234</v>
       </c>
       <c r="C8" s="105" t="s">
@@ -31421,1122 +31460,1198 @@
       <c r="A9" s="96" t="s">
         <v>255</v>
       </c>
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="132" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="103" t="s">
+      <c r="D9" s="131" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="150" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" s="170" t="s">
+      <c r="A10" s="96" t="s">
+        <v>377</v>
+      </c>
+      <c r="B10" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="79" t="s">
-        <v>261</v>
+      <c r="C10" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="103" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="150"/>
-      <c r="B11" s="170"/>
+      <c r="A11" s="155" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" s="175" t="s">
+        <v>234</v>
+      </c>
       <c r="C11" s="58"/>
-      <c r="D11" s="58" t="s">
-        <v>276</v>
+      <c r="D11" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="150"/>
-      <c r="B12" s="170"/>
-      <c r="C12" s="109" t="s">
-        <v>325</v>
-      </c>
+      <c r="A12" s="155"/>
+      <c r="B12" s="175"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="58" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="155"/>
+      <c r="B13" s="175"/>
+      <c r="C13" s="109" t="s">
+        <v>325</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="96" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="122" t="s">
+      <c r="B14" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C13" s="117" t="s">
+      <c r="C14" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="58"/>
+      <c r="D14" s="58"/>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="197" t="s">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="202" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="185" t="s">
+      <c r="B15" s="189" t="s">
         <v>234</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="121" t="s">
+      <c r="C15" s="58"/>
+      <c r="D15" s="120" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="198"/>
-      <c r="B15" s="186"/>
-      <c r="C15" s="120" t="s">
-        <v>361</v>
-      </c>
-      <c r="D15" s="58" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="198"/>
-      <c r="B16" s="186"/>
-      <c r="C16" s="120" t="s">
-        <v>359</v>
+      <c r="A16" s="203"/>
+      <c r="B16" s="190"/>
+      <c r="C16" s="119" t="s">
+        <v>361</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="198"/>
-      <c r="B17" s="186"/>
-      <c r="C17" s="126" t="s">
-        <v>367</v>
-      </c>
-      <c r="D17" s="99" t="s">
-        <v>365</v>
+      <c r="A17" s="203"/>
+      <c r="B17" s="190"/>
+      <c r="C17" s="119" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="199"/>
-      <c r="B18" s="187"/>
-      <c r="C18" s="120" t="s">
-        <v>359</v>
+      <c r="A18" s="203"/>
+      <c r="B18" s="190"/>
+      <c r="C18" s="125" t="s">
+        <v>367</v>
       </c>
       <c r="D18" s="99" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="129" t="s">
-        <v>331</v>
-      </c>
-      <c r="B19" s="122" t="s">
-        <v>234</v>
-      </c>
-      <c r="C19" s="117" t="s">
-        <v>332</v>
+      <c r="A19" s="203"/>
+      <c r="B19" s="190"/>
+      <c r="C19" s="133" t="s">
+        <v>359</v>
       </c>
       <c r="D19" s="99" t="s">
-        <v>333</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="129" t="s">
-        <v>351</v>
-      </c>
-      <c r="B20" s="128" t="s">
+      <c r="A20" s="204"/>
+      <c r="B20" s="191"/>
+      <c r="C20" s="119" t="s">
+        <v>371</v>
+      </c>
+      <c r="D20" s="99" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="128" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C20" s="127" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="99"/>
-    </row>
-    <row r="21" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="129" t="s">
-        <v>369</v>
-      </c>
-      <c r="B21" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="C21" s="117" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="99"/>
+      <c r="C21" s="116" t="s">
+        <v>332</v>
+      </c>
+      <c r="D21" s="99" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="A22" s="128" t="s">
+        <v>351</v>
+      </c>
+      <c r="B22" s="127" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="126" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="99"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="182" t="s">
-        <v>237</v>
-      </c>
-      <c r="B23" s="185" t="s">
+      <c r="A23" s="135" t="s">
+        <v>369</v>
+      </c>
+      <c r="B23" s="134" t="s">
         <v>234</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58" t="s">
-        <v>258</v>
-      </c>
+      <c r="C23" s="130" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="99"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="183"/>
-      <c r="B24" s="186"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58" t="s">
-        <v>252</v>
-      </c>
+      <c r="A24" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="183"/>
-      <c r="B25" s="186"/>
+      <c r="A25" s="186" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25" s="189" t="s">
+        <v>234</v>
+      </c>
       <c r="C25" s="58"/>
       <c r="D25" s="58" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="183"/>
-      <c r="B26" s="186"/>
-      <c r="C26" s="58" t="s">
-        <v>300</v>
-      </c>
+      <c r="A26" s="187"/>
+      <c r="B26" s="190"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="58" t="s">
-        <v>301</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="183"/>
-      <c r="B27" s="186"/>
-      <c r="C27" s="58" t="s">
-        <v>328</v>
-      </c>
-      <c r="D27" s="99" t="s">
-        <v>327</v>
+      <c r="A27" s="187"/>
+      <c r="B27" s="190"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="184"/>
-      <c r="B28" s="187"/>
+      <c r="A28" s="187"/>
+      <c r="B28" s="190"/>
       <c r="C28" s="58" t="s">
-        <v>373</v>
-      </c>
-      <c r="D28" s="99" t="s">
-        <v>374</v>
+        <v>300</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="154" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="185" t="s">
-        <v>234</v>
-      </c>
+      <c r="A29" s="187"/>
+      <c r="B29" s="190"/>
       <c r="C29" s="58" t="s">
-        <v>303</v>
+        <v>328</v>
       </c>
       <c r="D29" s="99" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="155"/>
-      <c r="B30" s="186"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58" t="s">
-        <v>238</v>
+      <c r="A30" s="188"/>
+      <c r="B30" s="191"/>
+      <c r="C30" s="58" t="s">
+        <v>373</v>
+      </c>
+      <c r="D30" s="99" t="s">
+        <v>374</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="155"/>
-      <c r="B31" s="186"/>
-      <c r="C31" s="107" t="s">
-        <v>329</v>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="159" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="189" t="s">
+        <v>234</v>
+      </c>
+      <c r="C31" s="58" t="s">
+        <v>303</v>
       </c>
       <c r="D31" s="99" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="155"/>
-      <c r="B32" s="186"/>
-      <c r="C32" s="107" t="s">
-        <v>359</v>
-      </c>
-      <c r="D32" s="99" t="s">
-        <v>360</v>
+      <c r="A32" s="160"/>
+      <c r="B32" s="190"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58" t="s">
+        <v>238</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="155"/>
-      <c r="B33" s="186"/>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="160"/>
+      <c r="B33" s="190"/>
       <c r="C33" s="107" t="s">
-        <v>367</v>
+        <v>329</v>
       </c>
       <c r="D33" s="99" t="s">
-        <v>368</v>
+        <v>330</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="156"/>
-      <c r="B34" s="187"/>
+      <c r="A34" s="160"/>
+      <c r="B34" s="190"/>
       <c r="C34" s="107" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="D34" s="99" t="s">
-        <v>251</v>
+        <v>360</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="161" t="s">
-        <v>222</v>
-      </c>
-      <c r="B35" s="185" t="s">
-        <v>234</v>
-      </c>
-      <c r="C35" s="188" t="s">
-        <v>239</v>
-      </c>
-      <c r="D35" s="102" t="s">
-        <v>241</v>
+      <c r="A35" s="160"/>
+      <c r="B35" s="190"/>
+      <c r="C35" s="107" t="s">
+        <v>367</v>
+      </c>
+      <c r="D35" s="99" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="194"/>
-      <c r="B36" s="186"/>
-      <c r="C36" s="189"/>
+      <c r="A36" s="160"/>
+      <c r="B36" s="190"/>
+      <c r="C36" s="107" t="s">
+        <v>371</v>
+      </c>
       <c r="D36" s="99" t="s">
-        <v>278</v>
+        <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="194"/>
-      <c r="B37" s="186"/>
-      <c r="C37" s="190" t="s">
-        <v>240</v>
-      </c>
-      <c r="D37" s="58" t="s">
-        <v>299</v>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="161"/>
+      <c r="B37" s="191"/>
+      <c r="C37" s="107" t="s">
+        <v>381</v>
+      </c>
+      <c r="D37" s="114" t="s">
+        <v>382</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="194"/>
-      <c r="B38" s="186"/>
-      <c r="C38" s="190"/>
-      <c r="D38" s="61" t="s">
-        <v>242</v>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="166" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="189" t="s">
+        <v>234</v>
+      </c>
+      <c r="C38" s="193" t="s">
+        <v>239</v>
+      </c>
+      <c r="D38" s="102" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="194"/>
-      <c r="B39" s="186"/>
-      <c r="C39" s="104" t="s">
-        <v>307</v>
-      </c>
-      <c r="D39" s="58" t="s">
-        <v>308</v>
+      <c r="A39" s="199"/>
+      <c r="B39" s="190"/>
+      <c r="C39" s="194"/>
+      <c r="D39" s="99" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="194"/>
-      <c r="B40" s="186"/>
-      <c r="C40" s="104">
-        <v>2.1</v>
+      <c r="A40" s="199"/>
+      <c r="B40" s="190"/>
+      <c r="C40" s="195" t="s">
+        <v>240</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="194"/>
-      <c r="B41" s="186"/>
-      <c r="C41" s="104" t="s">
-        <v>239</v>
-      </c>
-      <c r="D41" s="58" t="s">
-        <v>317</v>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="199"/>
+      <c r="B41" s="190"/>
+      <c r="C41" s="195"/>
+      <c r="D41" s="61" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="194"/>
-      <c r="B42" s="186"/>
-      <c r="C42" s="116" t="s">
+      <c r="A42" s="199"/>
+      <c r="B42" s="190"/>
+      <c r="C42" s="104" t="s">
+        <v>307</v>
+      </c>
+      <c r="D42" s="58" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="199"/>
+      <c r="B43" s="190"/>
+      <c r="C43" s="104">
+        <v>2.1</v>
+      </c>
+      <c r="D43" s="58" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="199"/>
+      <c r="B44" s="190"/>
+      <c r="C44" s="104" t="s">
         <v>239</v>
       </c>
-      <c r="D42" s="115" t="s">
+      <c r="D44" s="58" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="199"/>
+      <c r="B45" s="190"/>
+      <c r="C45" s="115" t="s">
+        <v>239</v>
+      </c>
+      <c r="D45" s="114" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="162"/>
-      <c r="B43" s="187"/>
-      <c r="C43" s="114" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="199"/>
+      <c r="B46" s="190"/>
+      <c r="C46" s="130" t="s">
         <v>239</v>
       </c>
-      <c r="D43" s="99" t="s">
+      <c r="D46" s="99" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="191" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="199"/>
+      <c r="B47" s="190"/>
+      <c r="C47" s="133" t="s">
+        <v>378</v>
+      </c>
+      <c r="D47" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="196" t="s">
         <v>296</v>
       </c>
-      <c r="B44" s="185" t="s">
+      <c r="B48" s="189" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C48" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D48" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="192"/>
-      <c r="B45" s="186"/>
-      <c r="C45" s="61" t="s">
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="197"/>
+      <c r="B49" s="190"/>
+      <c r="C49" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D45" s="58" t="s">
+      <c r="D49" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="193"/>
-      <c r="B46" s="187"/>
-      <c r="C46" s="58" t="s">
+    <row r="50" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="198"/>
+      <c r="B50" s="191"/>
+      <c r="C50" s="58" t="s">
         <v>350</v>
       </c>
-      <c r="D46" s="58" t="s">
+      <c r="D50" s="58" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="129" t="s">
+    <row r="51" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="186" t="s">
         <v>370</v>
       </c>
-      <c r="B47" s="128" t="s">
+      <c r="B51" s="189" t="s">
         <v>234</v>
       </c>
-      <c r="C47" s="127" t="s">
+      <c r="C51" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="D47" s="58"/>
+      <c r="D51" s="58"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
+    <row r="52" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="187"/>
+      <c r="B52" s="190"/>
+      <c r="C52" s="133" t="s">
+        <v>378</v>
+      </c>
+      <c r="D52" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="44"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="161" t="s">
-        <v>260</v>
-      </c>
-      <c r="B49" s="185" t="s">
-        <v>234</v>
-      </c>
-      <c r="C49" s="58"/>
-      <c r="D49" s="79" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="162"/>
-      <c r="B50" s="187"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="96" t="s">
-        <v>334</v>
-      </c>
-      <c r="B51" s="124" t="s">
-        <v>234</v>
-      </c>
-      <c r="C51" s="79" t="s">
-        <v>335</v>
-      </c>
-      <c r="D51" s="99" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="B52" s="124" t="s">
-        <v>234</v>
-      </c>
-      <c r="C52" s="105" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="103" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="191" t="s">
-        <v>32</v>
-      </c>
-      <c r="B53" s="185" t="s">
-        <v>234</v>
-      </c>
-      <c r="C53" s="58" t="s">
-        <v>268</v>
-      </c>
-      <c r="D53" s="58" t="s">
-        <v>251</v>
-      </c>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="44"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="192"/>
-      <c r="B54" s="186"/>
-      <c r="C54" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="D54" s="58" t="s">
-        <v>251</v>
+      <c r="A54" s="166" t="s">
+        <v>260</v>
+      </c>
+      <c r="B54" s="189" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="58"/>
+      <c r="D54" s="79" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="192"/>
-      <c r="B55" s="186"/>
-      <c r="C55" s="58" t="s">
-        <v>269</v>
-      </c>
+      <c r="A55" s="167"/>
+      <c r="B55" s="191"/>
+      <c r="C55" s="58"/>
       <c r="D55" s="58" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="192"/>
-      <c r="B56" s="186"/>
-      <c r="C56" s="99" t="s">
-        <v>277</v>
+      <c r="A56" s="96" t="s">
+        <v>334</v>
+      </c>
+      <c r="B56" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C56" s="79" t="s">
+        <v>335</v>
       </c>
       <c r="D56" s="99" t="s">
-        <v>102</v>
+        <v>336</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="192"/>
-      <c r="B57" s="186"/>
-      <c r="C57" s="58" t="s">
-        <v>282</v>
-      </c>
-      <c r="D57" s="58" t="s">
+    <row r="57" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="B57" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="103" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="196" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="189" t="s">
+        <v>234</v>
+      </c>
+      <c r="C58" s="58" t="s">
+        <v>268</v>
+      </c>
+      <c r="D58" s="58" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="192"/>
-      <c r="B58" s="186"/>
-      <c r="C58" s="58" t="s">
-        <v>283</v>
-      </c>
-      <c r="D58" s="58" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="192"/>
-      <c r="B59" s="186"/>
-      <c r="C59" s="99" t="s">
-        <v>288</v>
-      </c>
-      <c r="D59" s="99" t="s">
+      <c r="A59" s="197"/>
+      <c r="B59" s="190"/>
+      <c r="C59" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="D59" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="192"/>
-      <c r="B60" s="186"/>
-      <c r="C60" s="99" t="s">
-        <v>302</v>
-      </c>
-      <c r="D60" s="99" t="s">
+      <c r="A60" s="197"/>
+      <c r="B60" s="190"/>
+      <c r="C60" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D60" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="192"/>
-      <c r="B61" s="186"/>
+      <c r="A61" s="197"/>
+      <c r="B61" s="190"/>
       <c r="C61" s="99" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="D61" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="192"/>
-      <c r="B62" s="186"/>
-      <c r="C62" s="106" t="s">
-        <v>244</v>
-      </c>
-      <c r="D62" s="103" t="s">
-        <v>245</v>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="197"/>
+      <c r="B62" s="190"/>
+      <c r="C62" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="D62" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="192"/>
-      <c r="B63" s="186"/>
-      <c r="C63" s="107" t="s">
-        <v>311</v>
-      </c>
-      <c r="D63" s="99" t="s">
-        <v>251</v>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="197"/>
+      <c r="B63" s="190"/>
+      <c r="C63" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="D63" s="58" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="192"/>
-      <c r="B64" s="186"/>
-      <c r="C64" s="58" t="s">
-        <v>312</v>
-      </c>
-      <c r="D64" s="58" t="s">
-        <v>100</v>
+      <c r="A64" s="197"/>
+      <c r="B64" s="190"/>
+      <c r="C64" s="99" t="s">
+        <v>288</v>
+      </c>
+      <c r="D64" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="192"/>
-      <c r="B65" s="186"/>
+      <c r="A65" s="197"/>
+      <c r="B65" s="190"/>
       <c r="C65" s="99" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D65" s="99" t="s">
-        <v>314</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="192"/>
-      <c r="B66" s="186"/>
+      <c r="A66" s="197"/>
+      <c r="B66" s="190"/>
       <c r="C66" s="99" t="s">
-        <v>315</v>
+        <v>289</v>
       </c>
       <c r="D66" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="192"/>
-      <c r="B67" s="186"/>
-      <c r="C67" s="99" t="s">
-        <v>268</v>
-      </c>
-      <c r="D67" s="99" t="s">
-        <v>102</v>
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="197"/>
+      <c r="B67" s="190"/>
+      <c r="C67" s="106" t="s">
+        <v>244</v>
+      </c>
+      <c r="D67" s="103" t="s">
+        <v>245</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="192"/>
-      <c r="B68" s="186"/>
-      <c r="C68" s="58" t="s">
-        <v>318</v>
-      </c>
-      <c r="D68" s="58" t="s">
-        <v>102</v>
+    <row r="68" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="197"/>
+      <c r="B68" s="190"/>
+      <c r="C68" s="107" t="s">
+        <v>311</v>
+      </c>
+      <c r="D68" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="192"/>
-      <c r="B69" s="186"/>
-      <c r="C69" s="99" t="s">
-        <v>283</v>
-      </c>
-      <c r="D69" s="99" t="s">
-        <v>320</v>
+      <c r="A69" s="197"/>
+      <c r="B69" s="190"/>
+      <c r="C69" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D69" s="58" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="192"/>
-      <c r="B70" s="186"/>
+      <c r="A70" s="197"/>
+      <c r="B70" s="190"/>
       <c r="C70" s="99" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D70" s="99" t="s">
-        <v>251</v>
+        <v>314</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="192"/>
-      <c r="B71" s="186"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="108" t="s">
-        <v>321</v>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="197"/>
+      <c r="B71" s="190"/>
+      <c r="C71" s="99" t="s">
+        <v>315</v>
+      </c>
+      <c r="D71" s="99" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="192"/>
-      <c r="B72" s="186"/>
+      <c r="A72" s="197"/>
+      <c r="B72" s="190"/>
       <c r="C72" s="99" t="s">
-        <v>322</v>
+        <v>268</v>
       </c>
       <c r="D72" s="99" t="s">
-        <v>251</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="192"/>
-      <c r="B73" s="186"/>
-      <c r="C73" s="99" t="s">
-        <v>268</v>
-      </c>
-      <c r="D73" s="99" t="s">
-        <v>251</v>
+      <c r="A73" s="197"/>
+      <c r="B73" s="190"/>
+      <c r="C73" s="58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D73" s="58" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="192"/>
-      <c r="B74" s="186"/>
+      <c r="A74" s="197"/>
+      <c r="B74" s="190"/>
       <c r="C74" s="99" t="s">
-        <v>339</v>
+        <v>283</v>
       </c>
       <c r="D74" s="99" t="s">
-        <v>251</v>
+        <v>320</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="192"/>
-      <c r="B75" s="186"/>
+      <c r="A75" s="197"/>
+      <c r="B75" s="190"/>
       <c r="C75" s="99" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="D75" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="192"/>
-      <c r="B76" s="186"/>
-      <c r="C76" s="99" t="s">
-        <v>324</v>
-      </c>
-      <c r="D76" s="99" t="s">
-        <v>323</v>
+    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="197"/>
+      <c r="B76" s="190"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="108" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="192"/>
-      <c r="B77" s="186"/>
-      <c r="C77" s="115" t="s">
-        <v>345</v>
-      </c>
-      <c r="D77" s="115" t="s">
+      <c r="A77" s="197"/>
+      <c r="B77" s="190"/>
+      <c r="C77" s="99" t="s">
+        <v>322</v>
+      </c>
+      <c r="D77" s="99" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="192"/>
-      <c r="B78" s="186"/>
+      <c r="A78" s="197"/>
+      <c r="B78" s="190"/>
       <c r="C78" s="99" t="s">
-        <v>338</v>
+        <v>268</v>
       </c>
       <c r="D78" s="99" t="s">
-        <v>337</v>
+        <v>251</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="192"/>
-      <c r="B79" s="186"/>
+      <c r="A79" s="197"/>
+      <c r="B79" s="190"/>
       <c r="C79" s="99" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="D79" s="99" t="s">
-        <v>354</v>
+        <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="192"/>
-      <c r="B80" s="186"/>
-      <c r="C80" s="119" t="s">
-        <v>356</v>
-      </c>
-      <c r="D80" s="118" t="s">
-        <v>355</v>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="197"/>
+      <c r="B80" s="190"/>
+      <c r="C80" s="99" t="s">
+        <v>340</v>
+      </c>
+      <c r="D80" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="192"/>
-      <c r="B81" s="186"/>
+      <c r="A81" s="197"/>
+      <c r="B81" s="190"/>
       <c r="C81" s="99" t="s">
-        <v>357</v>
+        <v>324</v>
       </c>
       <c r="D81" s="99" t="s">
-        <v>251</v>
+        <v>323</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="192"/>
-      <c r="B82" s="186"/>
-      <c r="C82" s="99" t="s">
-        <v>358</v>
-      </c>
-      <c r="D82" s="99" t="s">
-        <v>102</v>
+      <c r="A82" s="197"/>
+      <c r="B82" s="190"/>
+      <c r="C82" s="114" t="s">
+        <v>345</v>
+      </c>
+      <c r="D82" s="114" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="192"/>
-      <c r="B83" s="186"/>
+      <c r="A83" s="197"/>
+      <c r="B83" s="190"/>
       <c r="C83" s="99" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="D83" s="99" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="192"/>
-      <c r="B84" s="186"/>
+      <c r="A84" s="197"/>
+      <c r="B84" s="190"/>
       <c r="C84" s="99" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="D84" s="99" t="s">
-        <v>251</v>
+        <v>354</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="193"/>
-      <c r="B85" s="187"/>
-      <c r="C85" s="99" t="s">
-        <v>372</v>
-      </c>
-      <c r="D85" s="99" t="s">
-        <v>251</v>
+    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="197"/>
+      <c r="B85" s="190"/>
+      <c r="C85" s="118" t="s">
+        <v>356</v>
+      </c>
+      <c r="D85" s="117" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="96" t="s">
-        <v>309</v>
-      </c>
-      <c r="B86" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="C86" s="58" t="s">
-        <v>30</v>
+      <c r="A86" s="197"/>
+      <c r="B86" s="190"/>
+      <c r="C86" s="99" t="s">
+        <v>357</v>
       </c>
       <c r="D86" s="99" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="96" t="s">
-        <v>310</v>
-      </c>
-      <c r="B87" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="C87" s="58" t="s">
-        <v>30</v>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="197"/>
+      <c r="B87" s="190"/>
+      <c r="C87" s="99" t="s">
+        <v>358</v>
       </c>
       <c r="D87" s="99" t="s">
-        <v>274</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B88" s="39"/>
-      <c r="C88" s="39"/>
-      <c r="D88" s="44"/>
+      <c r="A88" s="197"/>
+      <c r="B88" s="190"/>
+      <c r="C88" s="99" t="s">
+        <v>364</v>
+      </c>
+      <c r="D88" s="99" t="s">
+        <v>365</v>
+      </c>
     </row>
-    <row r="89" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="161" t="s">
-        <v>84</v>
-      </c>
-      <c r="B89" s="185" t="s">
-        <v>234</v>
-      </c>
-      <c r="C89" s="58"/>
-      <c r="D89" s="79" t="s">
-        <v>261</v>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="197"/>
+      <c r="B89" s="190"/>
+      <c r="C89" s="99" t="s">
+        <v>366</v>
+      </c>
+      <c r="D89" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="194"/>
-      <c r="B90" s="186"/>
-      <c r="C90" s="105" t="s">
-        <v>246</v>
-      </c>
-      <c r="D90" s="58" t="s">
-        <v>253</v>
+      <c r="A90" s="197"/>
+      <c r="B90" s="190"/>
+      <c r="C90" s="99" t="s">
+        <v>372</v>
+      </c>
+      <c r="D90" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="194"/>
-      <c r="B91" s="186"/>
-      <c r="C91" s="105">
-        <v>10.1</v>
-      </c>
-      <c r="D91" s="58" t="s">
-        <v>272</v>
+      <c r="A91" s="198"/>
+      <c r="B91" s="191"/>
+      <c r="C91" s="99" t="s">
+        <v>364</v>
+      </c>
+      <c r="D91" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="194"/>
-      <c r="B92" s="186"/>
-      <c r="C92" s="105">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D92" s="58" t="s">
-        <v>272</v>
+      <c r="A92" s="96" t="s">
+        <v>309</v>
+      </c>
+      <c r="B92" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C92" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D92" s="99" t="s">
+        <v>274</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="162"/>
-      <c r="B93" s="187"/>
-      <c r="C93" s="110" t="s">
-        <v>293</v>
-      </c>
-      <c r="D93" s="100" t="s">
-        <v>294</v>
+    <row r="93" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="96" t="s">
+        <v>310</v>
+      </c>
+      <c r="B93" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C93" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D93" s="99" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="161" t="s">
-        <v>247</v>
-      </c>
-      <c r="B94" s="185" t="s">
+      <c r="A94" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B94" s="39"/>
+      <c r="C94" s="39"/>
+      <c r="D94" s="44"/>
+    </row>
+    <row r="95" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="166" t="s">
+        <v>84</v>
+      </c>
+      <c r="B95" s="189" t="s">
         <v>234</v>
       </c>
-      <c r="C94" s="170"/>
-      <c r="D94" s="181" t="s">
+      <c r="C95" s="58"/>
+      <c r="D95" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="162"/>
-      <c r="B95" s="187"/>
-      <c r="C95" s="170"/>
-      <c r="D95" s="181"/>
-    </row>
-    <row r="96" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="123" t="s">
-        <v>262</v>
-      </c>
-      <c r="B96" s="125" t="s">
-        <v>234</v>
-      </c>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="199"/>
+      <c r="B96" s="190"/>
       <c r="C96" s="105" t="s">
-        <v>250</v>
-      </c>
-      <c r="D96" s="99" t="s">
-        <v>251</v>
+        <v>246</v>
+      </c>
+      <c r="D96" s="58" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B97" s="39"/>
-      <c r="C97" s="98"/>
-      <c r="D97" s="98"/>
+      <c r="A97" s="199"/>
+      <c r="B97" s="190"/>
+      <c r="C97" s="105">
+        <v>10.1</v>
+      </c>
+      <c r="D97" s="58" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="96" t="s">
-        <v>249</v>
-      </c>
-      <c r="B98" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="C98" s="111" t="s">
-        <v>265</v>
+      <c r="A98" s="199"/>
+      <c r="B98" s="190"/>
+      <c r="C98" s="105">
+        <v>10.199999999999999</v>
       </c>
       <c r="D98" s="58" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="161" t="s">
-        <v>285</v>
-      </c>
-      <c r="B99" s="185" t="s">
-        <v>234</v>
-      </c>
-      <c r="C99" s="100" t="s">
-        <v>295</v>
-      </c>
-      <c r="D99" s="58" t="s">
-        <v>251</v>
+      <c r="A99" s="199"/>
+      <c r="B99" s="190"/>
+      <c r="C99" s="110" t="s">
+        <v>293</v>
+      </c>
+      <c r="D99" s="100" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="194"/>
-      <c r="B100" s="186"/>
-      <c r="C100" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="D100" s="99" t="s">
-        <v>306</v>
+      <c r="A100" s="167"/>
+      <c r="B100" s="191"/>
+      <c r="C100" s="110" t="s">
+        <v>375</v>
+      </c>
+      <c r="D100" s="100" t="s">
+        <v>376</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="162"/>
-      <c r="B101" s="187"/>
-      <c r="C101" s="111" t="s">
-        <v>286</v>
-      </c>
-      <c r="D101" s="58" t="s">
-        <v>287</v>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="166" t="s">
+        <v>247</v>
+      </c>
+      <c r="B101" s="189" t="s">
+        <v>234</v>
+      </c>
+      <c r="C101" s="175"/>
+      <c r="D101" s="192" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="B102" s="98"/>
-      <c r="C102" s="98"/>
-      <c r="D102" s="98"/>
+      <c r="A102" s="167"/>
+      <c r="B102" s="191"/>
+      <c r="C102" s="175"/>
+      <c r="D102" s="192"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="200" t="s">
-        <v>58</v>
-      </c>
-      <c r="B103" s="185" t="s">
-        <v>271</v>
-      </c>
-      <c r="C103" s="111" t="s">
+    <row r="103" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="122" t="s">
+        <v>262</v>
+      </c>
+      <c r="B103" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C103" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="D103" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B104" s="39"/>
+      <c r="C104" s="98"/>
+      <c r="D104" s="98"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="96" t="s">
+        <v>249</v>
+      </c>
+      <c r="B105" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C105" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D103" s="58" t="s">
+      <c r="D105" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="201"/>
-      <c r="B104" s="187"/>
-      <c r="C104" s="111" t="s">
-        <v>265</v>
-      </c>
-      <c r="D104" s="58" t="s">
-        <v>266</v>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="166" t="s">
+        <v>285</v>
+      </c>
+      <c r="B106" s="189" t="s">
+        <v>234</v>
+      </c>
+      <c r="C106" s="100" t="s">
+        <v>295</v>
+      </c>
+      <c r="D106" s="58" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="130" t="s">
-        <v>59</v>
-      </c>
-      <c r="B105" s="125" t="s">
-        <v>271</v>
-      </c>
-      <c r="C105" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D105" s="58" t="s">
-        <v>100</v>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="199"/>
+      <c r="B107" s="190"/>
+      <c r="C107" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D107" s="99" t="s">
+        <v>306</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="96" t="s">
-        <v>291</v>
-      </c>
-      <c r="B106" s="125" t="s">
-        <v>271</v>
-      </c>
-      <c r="C106" s="58"/>
-      <c r="D106" s="61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="97" t="s">
-        <v>60</v>
-      </c>
-      <c r="B107" s="125" t="s">
-        <v>271</v>
-      </c>
-      <c r="C107" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D107" s="58" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="98" t="s">
-        <v>273</v>
-      </c>
-      <c r="B108" s="98"/>
-      <c r="C108" s="98"/>
-      <c r="D108" s="98"/>
+    <row r="108" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A108" s="167"/>
+      <c r="B108" s="191"/>
+      <c r="C108" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="D108" s="58" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="58"/>
-      <c r="B109" s="125" t="s">
-        <v>234</v>
-      </c>
-      <c r="C109" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D109" s="99" t="s">
-        <v>274</v>
-      </c>
+      <c r="A109" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="B109" s="98"/>
+      <c r="C109" s="98"/>
+      <c r="D109" s="98"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="98" t="s">
+      <c r="A110" s="205" t="s">
+        <v>58</v>
+      </c>
+      <c r="B110" s="189" t="s">
+        <v>271</v>
+      </c>
+      <c r="C110" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="D110" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="206"/>
+      <c r="B111" s="191"/>
+      <c r="C111" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="D111" s="58" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="B112" s="124" t="s">
+        <v>271</v>
+      </c>
+      <c r="C112" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D112" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="96" t="s">
+        <v>291</v>
+      </c>
+      <c r="B113" s="124" t="s">
+        <v>271</v>
+      </c>
+      <c r="C113" s="58"/>
+      <c r="D113" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="B114" s="124" t="s">
+        <v>271</v>
+      </c>
+      <c r="C114" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D114" s="58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="98" t="s">
+        <v>273</v>
+      </c>
+      <c r="B115" s="98"/>
+      <c r="C115" s="98"/>
+      <c r="D115" s="98"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="58"/>
+      <c r="B116" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C116" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D116" s="99" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="98" t="s">
         <v>279</v>
       </c>
-      <c r="B110" s="98"/>
-      <c r="C110" s="98"/>
-      <c r="D110" s="98"/>
+      <c r="B117" s="98"/>
+      <c r="C117" s="98"/>
+      <c r="D117" s="98"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="58"/>
-      <c r="B111" s="125" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="58"/>
+      <c r="B118" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C111" s="58" t="s">
+      <c r="C118" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D111" s="99" t="s">
+      <c r="D118" s="99" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
+  <mergeCells count="34">
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="A95:A100"/>
+    <mergeCell ref="B95:B100"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="B106:B108"/>
+    <mergeCell ref="A38:A47"/>
+    <mergeCell ref="B38:B47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="A53:A85"/>
-    <mergeCell ref="B53:B85"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="A35:A43"/>
-    <mergeCell ref="B35:B43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A58:A91"/>
+    <mergeCell ref="B58:B91"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="B31:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates r.e. email to Conor 13th Dec
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -18,7 +18,7 @@
     <sheet name="1.0 Release Candidate 2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc520203303" localSheetId="3">'1.0 Release Candidate 2'!$C$4</definedName>
+    <definedName name="_Toc520203303" localSheetId="3">'1.0 Release Candidate 2'!$C$5</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="399">
   <si>
     <t>Document</t>
   </si>
@@ -3004,6 +3004,67 @@
   </si>
   <si>
     <t>Removed reference to batch</t>
+  </si>
+  <si>
+    <t>PAYE Modernisation Overview</t>
+  </si>
+  <si>
+    <t>New Link</t>
+  </si>
+  <si>
+    <t>Code 2007, 2049</t>
+  </si>
+  <si>
+    <t>Moved to Employee Level from Request Level</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">removed spaces from example in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Payroll Run Reference</t>
+    </r>
+  </si>
+  <si>
+    <t>Changed date to 2018</t>
+  </si>
+  <si>
+    <t>Code 2024</t>
+  </si>
+  <si>
+    <t>Included for REST</t>
+  </si>
+  <si>
+    <t>Removed for REST</t>
+  </si>
+  <si>
+    <t>Code 3013</t>
+  </si>
+  <si>
+    <t>Code 3001</t>
+  </si>
+  <si>
+    <t>Code 5002, 5003</t>
+  </si>
+  <si>
+    <t>Code 1003</t>
+  </si>
+  <si>
+    <t>Code 2004</t>
+  </si>
+  <si>
+    <t>Specified Agent Tain is required when using Agent Cert</t>
+  </si>
+  <si>
+    <t>Added details around the compression of files less than 2kB</t>
   </si>
 </sst>
 </file>
@@ -3171,7 +3232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -3601,11 +3662,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -3962,6 +4032,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4118,20 +4198,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4142,6 +4222,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4150,9 +4233,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4578,12 +4658,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="140" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="138"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="142"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4606,12 +4686,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="136" t="s">
+      <c r="A4" s="140" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="137"/>
-      <c r="C4" s="137"/>
-      <c r="D4" s="138"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="142"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4651,10 +4731,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="139" t="s">
+      <c r="A7" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="142">
+      <c r="B7" s="146">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4668,8 +4748,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="143"/>
+      <c r="A8" s="144"/>
+      <c r="B8" s="147"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4681,8 +4761,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="140"/>
-      <c r="B9" s="143"/>
+      <c r="A9" s="144"/>
+      <c r="B9" s="147"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4694,8 +4774,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="140"/>
-      <c r="B10" s="143"/>
+      <c r="A10" s="144"/>
+      <c r="B10" s="147"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4707,8 +4787,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="140"/>
-      <c r="B11" s="143"/>
+      <c r="A11" s="144"/>
+      <c r="B11" s="147"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4720,8 +4800,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="141"/>
-      <c r="B12" s="144"/>
+      <c r="A12" s="145"/>
+      <c r="B12" s="148"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4733,10 +4813,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="147" t="s">
+      <c r="A13" s="151" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="142">
+      <c r="B13" s="146">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4750,8 +4830,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="148"/>
-      <c r="B14" s="144"/>
+      <c r="A14" s="152"/>
+      <c r="B14" s="148"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4797,12 +4877,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="136" t="s">
+      <c r="A17" s="140" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="137"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="138"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="141"/>
+      <c r="D17" s="142"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4842,21 +4922,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="136" t="s">
+      <c r="A20" s="140" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="137"/>
-      <c r="C20" s="137"/>
-      <c r="D20" s="138"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="142"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="149" t="s">
+      <c r="A21" s="153" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="146">
+      <c r="B21" s="150">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4870,8 +4950,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
-      <c r="B22" s="144"/>
+      <c r="A22" s="154"/>
+      <c r="B22" s="148"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4894,18 +4974,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="136" t="s">
+      <c r="A24" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="137"/>
-      <c r="C24" s="137"/>
-      <c r="D24" s="138"/>
+      <c r="B24" s="141"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="142"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="145" t="s">
+      <c r="A25" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="146">
+      <c r="B25" s="150">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4919,8 +4999,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="140"/>
-      <c r="B26" s="143"/>
+      <c r="A26" s="144"/>
+      <c r="B26" s="147"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -4932,8 +5012,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="140"/>
-      <c r="B27" s="143"/>
+      <c r="A27" s="144"/>
+      <c r="B27" s="147"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -4945,8 +5025,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="140"/>
-      <c r="B28" s="143"/>
+      <c r="A28" s="144"/>
+      <c r="B28" s="147"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -4958,8 +5038,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="140"/>
-      <c r="B29" s="143"/>
+      <c r="A29" s="144"/>
+      <c r="B29" s="147"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -4971,8 +5051,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="140"/>
-      <c r="B30" s="143"/>
+      <c r="A30" s="144"/>
+      <c r="B30" s="147"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -4984,8 +5064,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="140"/>
-      <c r="B31" s="143"/>
+      <c r="A31" s="144"/>
+      <c r="B31" s="147"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -4997,8 +5077,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="141"/>
-      <c r="B32" s="144"/>
+      <c r="A32" s="145"/>
+      <c r="B32" s="148"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5122,12 +5202,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="136" t="s">
+      <c r="A41" s="140" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="137"/>
-      <c r="C41" s="137"/>
-      <c r="D41" s="138"/>
+      <c r="B41" s="141"/>
+      <c r="C41" s="141"/>
+      <c r="D41" s="142"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5307,10 +5387,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="151" t="s">
+      <c r="A7" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="152" t="s">
+      <c r="B7" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5321,8 +5401,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="151"/>
-      <c r="B8" s="152"/>
+      <c r="A8" s="155"/>
+      <c r="B8" s="156"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5331,8 +5411,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="151"/>
-      <c r="B9" s="152"/>
+      <c r="A9" s="155"/>
+      <c r="B9" s="156"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5341,8 +5421,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="151"/>
-      <c r="B10" s="152"/>
+      <c r="A10" s="155"/>
+      <c r="B10" s="156"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5351,8 +5431,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="151"/>
-      <c r="B11" s="152"/>
+      <c r="A11" s="155"/>
+      <c r="B11" s="156"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5361,8 +5441,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="151"/>
-      <c r="B12" s="152"/>
+      <c r="A12" s="155"/>
+      <c r="B12" s="156"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5371,10 +5451,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="158" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="152" t="s">
+      <c r="B13" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5385,8 +5465,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="154"/>
-      <c r="B14" s="152"/>
+      <c r="A14" s="158"/>
+      <c r="B14" s="156"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5395,8 +5475,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="154"/>
-      <c r="B15" s="152"/>
+      <c r="A15" s="158"/>
+      <c r="B15" s="156"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5405,10 +5485,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="155" t="s">
+      <c r="A16" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5419,8 +5499,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="155"/>
-      <c r="B17" s="156"/>
+      <c r="A17" s="159"/>
+      <c r="B17" s="160"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5429,8 +5509,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="155"/>
-      <c r="B18" s="156"/>
+      <c r="A18" s="159"/>
+      <c r="B18" s="160"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5439,8 +5519,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="155"/>
-      <c r="B19" s="156"/>
+      <c r="A19" s="159"/>
+      <c r="B19" s="160"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5449,8 +5529,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="155"/>
-      <c r="B20" s="156"/>
+      <c r="A20" s="159"/>
+      <c r="B20" s="160"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5459,8 +5539,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="155"/>
-      <c r="B21" s="156"/>
+      <c r="A21" s="159"/>
+      <c r="B21" s="160"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5469,8 +5549,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="155"/>
-      <c r="B22" s="156"/>
+      <c r="A22" s="159"/>
+      <c r="B22" s="160"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5479,8 +5559,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
-      <c r="B23" s="156"/>
+      <c r="A23" s="159"/>
+      <c r="B23" s="160"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5489,26 +5569,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="155"/>
-      <c r="B24" s="156"/>
-      <c r="C24" s="155" t="s">
+      <c r="A24" s="159"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="159" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="162" t="s">
+      <c r="D24" s="166" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="155"/>
-      <c r="B25" s="156"/>
-      <c r="C25" s="155"/>
-      <c r="D25" s="162"/>
+      <c r="A25" s="159"/>
+      <c r="B25" s="160"/>
+      <c r="C25" s="159"/>
+      <c r="D25" s="166"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="151" t="s">
+      <c r="A26" s="155" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="152" t="s">
+      <c r="B26" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5519,8 +5599,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="151"/>
-      <c r="B27" s="152"/>
+      <c r="A27" s="155"/>
+      <c r="B27" s="156"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5547,28 +5627,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="153" t="s">
+      <c r="A30" s="157" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="152" t="s">
+      <c r="B30" s="156" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="155" t="s">
+      <c r="C30" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="165" t="s">
+      <c r="D30" s="169" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="153"/>
-      <c r="B31" s="152"/>
-      <c r="C31" s="155"/>
-      <c r="D31" s="165"/>
+      <c r="A31" s="157"/>
+      <c r="B31" s="156"/>
+      <c r="C31" s="159"/>
+      <c r="D31" s="169"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="153"/>
-      <c r="B32" s="152"/>
+      <c r="A32" s="157"/>
+      <c r="B32" s="156"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5577,8 +5657,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="153"/>
-      <c r="B33" s="152"/>
+      <c r="A33" s="157"/>
+      <c r="B33" s="156"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5587,8 +5667,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="153"/>
-      <c r="B34" s="152"/>
+      <c r="A34" s="157"/>
+      <c r="B34" s="156"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5597,8 +5677,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="153"/>
-      <c r="B35" s="152"/>
+      <c r="A35" s="157"/>
+      <c r="B35" s="156"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5607,8 +5687,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="153"/>
-      <c r="B36" s="152"/>
+      <c r="A36" s="157"/>
+      <c r="B36" s="156"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5617,26 +5697,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="153"/>
-      <c r="B37" s="152"/>
-      <c r="C37" s="166" t="s">
+      <c r="A37" s="157"/>
+      <c r="B37" s="156"/>
+      <c r="C37" s="170" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="168" t="s">
+      <c r="D37" s="172" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="153"/>
-      <c r="B38" s="152"/>
-      <c r="C38" s="167"/>
-      <c r="D38" s="168"/>
+      <c r="A38" s="157"/>
+      <c r="B38" s="156"/>
+      <c r="C38" s="171"/>
+      <c r="D38" s="172"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="151" t="s">
+      <c r="A39" s="155" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="152" t="s">
+      <c r="B39" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5647,8 +5727,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="151"/>
-      <c r="B40" s="152"/>
+      <c r="A40" s="155"/>
+      <c r="B40" s="156"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5675,10 +5755,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="153" t="s">
+      <c r="A43" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="152" t="s">
+      <c r="B43" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5687,8 +5767,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="153"/>
-      <c r="B44" s="152"/>
+      <c r="A44" s="157"/>
+      <c r="B44" s="156"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5697,10 +5777,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="159" t="s">
+      <c r="A45" s="163" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="152" t="s">
+      <c r="B45" s="156" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5709,8 +5789,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="160"/>
-      <c r="B46" s="152"/>
+      <c r="A46" s="164"/>
+      <c r="B46" s="156"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5719,8 +5799,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="160"/>
-      <c r="B47" s="152"/>
+      <c r="A47" s="164"/>
+      <c r="B47" s="156"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5729,8 +5809,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="161"/>
-      <c r="B48" s="152"/>
+      <c r="A48" s="165"/>
+      <c r="B48" s="156"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5739,10 +5819,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="156" t="s">
+      <c r="A49" s="160" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="156" t="s">
+      <c r="B49" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9846,8 +9926,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="156"/>
-      <c r="B50" s="156"/>
+      <c r="A50" s="160"/>
+      <c r="B50" s="160"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -13951,8 +14031,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="156"/>
-      <c r="B51" s="156"/>
+      <c r="A51" s="160"/>
+      <c r="B51" s="160"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18056,8 +18136,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="156"/>
-      <c r="B52" s="156"/>
+      <c r="A52" s="160"/>
+      <c r="B52" s="160"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22161,12 +22241,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="156"/>
-      <c r="B53" s="156"/>
-      <c r="C53" s="164" t="s">
+      <c r="A53" s="160"/>
+      <c r="B53" s="160"/>
+      <c r="C53" s="168" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="165" t="s">
+      <c r="D53" s="169" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26266,10 +26346,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="156"/>
-      <c r="B54" s="156"/>
-      <c r="C54" s="164"/>
-      <c r="D54" s="165"/>
+      <c r="A54" s="160"/>
+      <c r="B54" s="160"/>
+      <c r="C54" s="168"/>
+      <c r="D54" s="169"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30387,10 +30467,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="157" t="s">
+      <c r="A57" s="161" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="156" t="s">
+      <c r="B57" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30401,8 +30481,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="157"/>
-      <c r="B58" s="156"/>
+      <c r="A58" s="161"/>
+      <c r="B58" s="160"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30411,8 +30491,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="157"/>
-      <c r="B59" s="156"/>
+      <c r="A59" s="161"/>
+      <c r="B59" s="160"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30421,8 +30501,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="157"/>
-      <c r="B60" s="156"/>
+      <c r="A60" s="161"/>
+      <c r="B60" s="160"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30431,8 +30511,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="157"/>
-      <c r="B61" s="156"/>
+      <c r="A61" s="161"/>
+      <c r="B61" s="160"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30441,8 +30521,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="157"/>
-      <c r="B62" s="156"/>
+      <c r="A62" s="161"/>
+      <c r="B62" s="160"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30451,8 +30531,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="157"/>
-      <c r="B63" s="156"/>
+      <c r="A63" s="161"/>
+      <c r="B63" s="160"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30461,16 +30541,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="157"/>
-      <c r="B64" s="156"/>
+      <c r="A64" s="161"/>
+      <c r="B64" s="160"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="157"/>
-      <c r="B65" s="156"/>
+      <c r="A65" s="161"/>
+      <c r="B65" s="160"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30479,16 +30559,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="157"/>
-      <c r="B66" s="156"/>
+      <c r="A66" s="161"/>
+      <c r="B66" s="160"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="157"/>
-      <c r="B67" s="156"/>
+      <c r="A67" s="161"/>
+      <c r="B67" s="160"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30497,8 +30577,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="157"/>
-      <c r="B68" s="156"/>
+      <c r="A68" s="161"/>
+      <c r="B68" s="160"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30507,8 +30587,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="157"/>
-      <c r="B69" s="156"/>
+      <c r="A69" s="161"/>
+      <c r="B69" s="160"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30517,8 +30597,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="157"/>
-      <c r="B70" s="156"/>
+      <c r="A70" s="161"/>
+      <c r="B70" s="160"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30527,8 +30607,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="157"/>
-      <c r="B71" s="156"/>
+      <c r="A71" s="161"/>
+      <c r="B71" s="160"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30537,8 +30617,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="157"/>
-      <c r="B72" s="156"/>
+      <c r="A72" s="161"/>
+      <c r="B72" s="160"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30547,16 +30627,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="157"/>
-      <c r="B73" s="156"/>
+      <c r="A73" s="161"/>
+      <c r="B73" s="160"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="157"/>
-      <c r="B74" s="156"/>
+      <c r="A74" s="161"/>
+      <c r="B74" s="160"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30565,18 +30645,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="157"/>
-      <c r="B75" s="156"/>
-      <c r="C75" s="163"/>
-      <c r="D75" s="158" t="s">
+      <c r="A75" s="161"/>
+      <c r="B75" s="160"/>
+      <c r="C75" s="167"/>
+      <c r="D75" s="162" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="157"/>
-      <c r="B76" s="156"/>
-      <c r="C76" s="163"/>
-      <c r="D76" s="158"/>
+      <c r="A76" s="161"/>
+      <c r="B76" s="160"/>
+      <c r="C76" s="167"/>
+      <c r="D76" s="162"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30700,10 +30780,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="152" t="s">
+      <c r="B4" s="156" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30714,133 +30794,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="151"/>
-      <c r="B5" s="152"/>
-      <c r="C5" s="178" t="s">
+      <c r="A5" s="155"/>
+      <c r="B5" s="156"/>
+      <c r="C5" s="182" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="177" t="s">
+      <c r="D5" s="181" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="151"/>
-      <c r="B6" s="152"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="177"/>
+      <c r="A6" s="155"/>
+      <c r="B6" s="156"/>
+      <c r="C6" s="182"/>
+      <c r="D6" s="181"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="151"/>
-      <c r="B7" s="152"/>
+      <c r="A7" s="155"/>
+      <c r="B7" s="156"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="151"/>
-      <c r="B8" s="152"/>
+      <c r="A8" s="155"/>
+      <c r="B8" s="156"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="151"/>
-      <c r="B9" s="152"/>
+      <c r="A9" s="155"/>
+      <c r="B9" s="156"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="154" t="s">
+      <c r="A10" s="158" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="152" t="s">
+      <c r="B10" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="176"/>
-      <c r="D10" s="177" t="s">
+      <c r="C10" s="180"/>
+      <c r="D10" s="181" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="154"/>
-      <c r="B11" s="152"/>
-      <c r="C11" s="176"/>
-      <c r="D11" s="177"/>
+      <c r="A11" s="158"/>
+      <c r="B11" s="156"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="181"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="154"/>
-      <c r="B12" s="152"/>
-      <c r="C12" s="176"/>
-      <c r="D12" s="177"/>
+      <c r="A12" s="158"/>
+      <c r="B12" s="156"/>
+      <c r="C12" s="180"/>
+      <c r="D12" s="181"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="155" t="s">
+      <c r="A13" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="179"/>
-      <c r="D13" s="177" t="s">
+      <c r="C13" s="183"/>
+      <c r="D13" s="181" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="155"/>
-      <c r="B14" s="156"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="177"/>
+      <c r="A14" s="159"/>
+      <c r="B14" s="160"/>
+      <c r="C14" s="183"/>
+      <c r="D14" s="181"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="155"/>
-      <c r="B15" s="156"/>
-      <c r="C15" s="179"/>
+      <c r="A15" s="159"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="183"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="155"/>
-      <c r="B16" s="156"/>
-      <c r="C16" s="179"/>
+      <c r="A16" s="159"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="183"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="155"/>
-      <c r="B17" s="156"/>
-      <c r="C17" s="179"/>
+      <c r="A17" s="159"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="183"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="155"/>
-      <c r="B18" s="156"/>
-      <c r="C18" s="179"/>
+      <c r="A18" s="159"/>
+      <c r="B18" s="160"/>
+      <c r="C18" s="183"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="155"/>
-      <c r="B19" s="156"/>
-      <c r="C19" s="179"/>
+      <c r="A19" s="159"/>
+      <c r="B19" s="160"/>
+      <c r="C19" s="183"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="155"/>
-      <c r="B20" s="156"/>
-      <c r="C20" s="179"/>
+      <c r="A20" s="159"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="183"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="155"/>
-      <c r="B21" s="156"/>
-      <c r="C21" s="179"/>
+      <c r="A21" s="159"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="183"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="155"/>
-      <c r="B22" s="156"/>
-      <c r="C22" s="179"/>
+      <c r="A22" s="159"/>
+      <c r="B22" s="160"/>
+      <c r="C22" s="183"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
-      <c r="B23" s="156"/>
-      <c r="C23" s="179"/>
+      <c r="A23" s="159"/>
+      <c r="B23" s="160"/>
+      <c r="C23" s="183"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -30938,10 +31018,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="180" t="s">
+      <c r="A32" s="184" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="183" t="s">
+      <c r="B32" s="187" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -30952,26 +31032,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="181"/>
-      <c r="B33" s="184"/>
+      <c r="A33" s="185"/>
+      <c r="B33" s="188"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="181"/>
-      <c r="B34" s="184"/>
+      <c r="A34" s="185"/>
+      <c r="B34" s="188"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="181"/>
-      <c r="B35" s="184"/>
+      <c r="A35" s="185"/>
+      <c r="B35" s="188"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="182"/>
-      <c r="B36" s="185"/>
+      <c r="A36" s="186"/>
+      <c r="B36" s="189"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31000,10 +31080,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="153" t="s">
+      <c r="A39" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="152" t="s">
+      <c r="B39" s="156" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31014,8 +31094,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="153"/>
-      <c r="B40" s="152"/>
+      <c r="A40" s="157"/>
+      <c r="B40" s="156"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31024,84 +31104,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="151" t="s">
+      <c r="A41" s="155" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="152" t="s">
+      <c r="B41" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="176" t="s">
+      <c r="C41" s="180" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="155" t="s">
+      <c r="D41" s="159" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="151"/>
-      <c r="B42" s="152"/>
-      <c r="C42" s="176"/>
-      <c r="D42" s="155"/>
+      <c r="A42" s="155"/>
+      <c r="B42" s="156"/>
+      <c r="C42" s="180"/>
+      <c r="D42" s="159"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="151"/>
-      <c r="B43" s="152"/>
-      <c r="C43" s="176" t="s">
+      <c r="A43" s="155"/>
+      <c r="B43" s="156"/>
+      <c r="C43" s="180" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="158" t="s">
+      <c r="D43" s="162" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="151"/>
-      <c r="B44" s="152"/>
-      <c r="C44" s="176"/>
-      <c r="D44" s="158"/>
+      <c r="A44" s="155"/>
+      <c r="B44" s="156"/>
+      <c r="C44" s="180"/>
+      <c r="D44" s="162"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="157" t="s">
+      <c r="A45" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="156" t="s">
+      <c r="B45" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="172"/>
+      <c r="C45" s="176"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="157"/>
-      <c r="B46" s="156"/>
-      <c r="C46" s="173"/>
-      <c r="D46" s="169" t="s">
+      <c r="A46" s="161"/>
+      <c r="B46" s="160"/>
+      <c r="C46" s="177"/>
+      <c r="D46" s="173" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="157"/>
-      <c r="B47" s="156"/>
-      <c r="C47" s="173"/>
-      <c r="D47" s="170"/>
+      <c r="A47" s="161"/>
+      <c r="B47" s="160"/>
+      <c r="C47" s="177"/>
+      <c r="D47" s="174"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="157"/>
-      <c r="B48" s="156"/>
-      <c r="C48" s="174"/>
-      <c r="D48" s="170"/>
+      <c r="A48" s="161"/>
+      <c r="B48" s="160"/>
+      <c r="C48" s="178"/>
+      <c r="D48" s="174"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="157"/>
-      <c r="B49" s="156"/>
-      <c r="C49" s="164"/>
-      <c r="D49" s="170"/>
+      <c r="A49" s="161"/>
+      <c r="B49" s="160"/>
+      <c r="C49" s="168"/>
+      <c r="D49" s="174"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="157"/>
-      <c r="B50" s="156"/>
-      <c r="C50" s="164"/>
-      <c r="D50" s="171"/>
+      <c r="A50" s="161"/>
+      <c r="B50" s="160"/>
+      <c r="C50" s="168"/>
+      <c r="D50" s="175"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31124,10 +31204,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="160" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="156" t="s">
+      <c r="B53" s="160" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31138,8 +31218,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="156"/>
-      <c r="B54" s="156"/>
+      <c r="A54" s="160"/>
+      <c r="B54" s="160"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31148,8 +31228,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="156"/>
-      <c r="B55" s="156"/>
+      <c r="A55" s="160"/>
+      <c r="B55" s="160"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31158,9 +31238,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="156"/>
-      <c r="B56" s="156"/>
-      <c r="C56" s="175" t="s">
+      <c r="A56" s="160"/>
+      <c r="B56" s="160"/>
+      <c r="C56" s="179" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31168,16 +31248,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="156"/>
-      <c r="B57" s="156"/>
-      <c r="C57" s="175"/>
+      <c r="A57" s="160"/>
+      <c r="B57" s="160"/>
+      <c r="C57" s="179"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="156"/>
-      <c r="B58" s="156"/>
+      <c r="A58" s="160"/>
+      <c r="B58" s="160"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31186,8 +31266,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="156"/>
-      <c r="B59" s="156"/>
+      <c r="A59" s="160"/>
+      <c r="B59" s="160"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31196,9 +31276,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="156"/>
-      <c r="B60" s="156"/>
-      <c r="C60" s="175" t="s">
+      <c r="A60" s="160"/>
+      <c r="B60" s="160"/>
+      <c r="C60" s="179" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31206,25 +31286,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="156"/>
-      <c r="B61" s="156"/>
-      <c r="C61" s="175"/>
+      <c r="A61" s="160"/>
+      <c r="B61" s="160"/>
+      <c r="C61" s="179"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="156"/>
-      <c r="B62" s="156"/>
-      <c r="C62" s="175"/>
+      <c r="A62" s="160"/>
+      <c r="B62" s="160"/>
+      <c r="C62" s="179"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="156"/>
-      <c r="B63" s="156"/>
-      <c r="C63" s="176" t="s">
+      <c r="A63" s="160"/>
+      <c r="B63" s="160"/>
+      <c r="C63" s="180" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31232,30 +31312,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="156"/>
-      <c r="B64" s="156"/>
-      <c r="C64" s="176"/>
-      <c r="D64" s="158" t="s">
+      <c r="A64" s="160"/>
+      <c r="B64" s="160"/>
+      <c r="C64" s="180"/>
+      <c r="D64" s="162" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="156"/>
-      <c r="B65" s="156"/>
-      <c r="C65" s="176"/>
-      <c r="D65" s="158"/>
+      <c r="A65" s="160"/>
+      <c r="B65" s="160"/>
+      <c r="C65" s="180"/>
+      <c r="D65" s="162"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="156"/>
-      <c r="B66" s="156"/>
-      <c r="C66" s="176"/>
-      <c r="D66" s="158"/>
+      <c r="A66" s="160"/>
+      <c r="B66" s="160"/>
+      <c r="C66" s="180"/>
+      <c r="D66" s="162"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="156"/>
-      <c r="B67" s="156"/>
-      <c r="C67" s="176"/>
-      <c r="D67" s="158"/>
+      <c r="A67" s="160"/>
+      <c r="B67" s="160"/>
+      <c r="C67" s="180"/>
+      <c r="D67" s="162"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31352,10 +31432,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:B91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31389,10 +31469,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="204" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="201" t="s">
+      <c r="B3" s="205" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="113" t="s">
@@ -31403,8 +31483,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="200"/>
-      <c r="B4" s="201"/>
+      <c r="A4" s="204"/>
+      <c r="B4" s="205"/>
       <c r="C4" s="113" t="s">
         <v>347</v>
       </c>
@@ -31412,1246 +31492,1366 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="204"/>
+      <c r="B5" s="205"/>
+      <c r="C5" s="113" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="44"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="155" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="44"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="175" t="s">
+      <c r="B7" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58" t="s">
+      <c r="C7" s="58"/>
+      <c r="D7" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="155"/>
-      <c r="B7" s="175"/>
-      <c r="C7" s="105" t="s">
-        <v>235</v>
-      </c>
-      <c r="D7" s="101" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="96" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="121" t="s">
-        <v>234</v>
-      </c>
+    <row r="8" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="159"/>
+      <c r="B8" s="179"/>
       <c r="C8" s="105" t="s">
         <v>235</v>
       </c>
-      <c r="D8" s="103" t="s">
-        <v>236</v>
+      <c r="D8" s="101" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="96" t="s">
-        <v>255</v>
-      </c>
-      <c r="B9" s="132" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C9" s="132" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="131" t="s">
-        <v>30</v>
+      <c r="C9" s="105" t="s">
+        <v>235</v>
+      </c>
+      <c r="D9" s="103" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="96" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="132" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="131" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="96" t="s">
         <v>377</v>
       </c>
-      <c r="B10" s="121" t="s">
+      <c r="B11" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C11" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="103" t="s">
+      <c r="D11" s="103" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="155" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="159" t="s">
         <v>275</v>
       </c>
-      <c r="B11" s="175" t="s">
+      <c r="B12" s="179" t="s">
         <v>234</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="79" t="s">
+      <c r="C12" s="58"/>
+      <c r="D12" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="155"/>
-      <c r="B12" s="175"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="159"/>
+      <c r="B13" s="179"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="155"/>
-      <c r="B13" s="175"/>
-      <c r="C13" s="109" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="159"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="109" t="s">
         <v>325</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D14" s="58" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="96" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="96" t="s">
         <v>290</v>
       </c>
-      <c r="B14" s="121" t="s">
+      <c r="B15" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C15" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="58"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="202" t="s">
+      <c r="D15" s="58"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="206" t="s">
         <v>165</v>
       </c>
-      <c r="B15" s="189" t="s">
+      <c r="B16" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="120" t="s">
+      <c r="C16" s="58"/>
+      <c r="D16" s="120" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="203"/>
-      <c r="B16" s="190"/>
-      <c r="C16" s="119" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="207"/>
+      <c r="B17" s="193"/>
+      <c r="C17" s="119" t="s">
         <v>361</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D17" s="58" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="203"/>
-      <c r="B17" s="190"/>
-      <c r="C17" s="119" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="207"/>
+      <c r="B18" s="193"/>
+      <c r="C18" s="119" t="s">
         <v>359</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D18" s="58" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="203"/>
-      <c r="B18" s="190"/>
-      <c r="C18" s="125" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="207"/>
+      <c r="B19" s="193"/>
+      <c r="C19" s="125" t="s">
         <v>367</v>
       </c>
-      <c r="D18" s="99" t="s">
+      <c r="D19" s="99" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="203"/>
-      <c r="B19" s="190"/>
-      <c r="C19" s="133" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="207"/>
+      <c r="B20" s="193"/>
+      <c r="C20" s="133" t="s">
         <v>359</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="D20" s="99" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="204"/>
-      <c r="B20" s="191"/>
-      <c r="C20" s="119" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="208"/>
+      <c r="B21" s="196"/>
+      <c r="C21" s="119" t="s">
         <v>371</v>
       </c>
-      <c r="D20" s="99" t="s">
+      <c r="D21" s="99" t="s">
         <v>380</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="128" t="s">
-        <v>331</v>
-      </c>
-      <c r="B21" s="121" t="s">
-        <v>234</v>
-      </c>
-      <c r="C21" s="116" t="s">
-        <v>332</v>
-      </c>
-      <c r="D21" s="99" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="128" t="s">
+        <v>331</v>
+      </c>
+      <c r="B22" s="121" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="116" t="s">
+        <v>332</v>
+      </c>
+      <c r="D22" s="99" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="128" t="s">
         <v>351</v>
       </c>
-      <c r="B22" s="127" t="s">
+      <c r="B23" s="127" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="126" t="s">
+      <c r="C23" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="99"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="135" t="s">
+      <c r="D23" s="99"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="135" t="s">
         <v>369</v>
       </c>
-      <c r="B23" s="134" t="s">
+      <c r="B24" s="134" t="s">
         <v>234</v>
       </c>
-      <c r="C23" s="130" t="s">
+      <c r="C24" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="99"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="D24" s="99"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="186" t="s">
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="190" t="s">
         <v>237</v>
       </c>
-      <c r="B25" s="189" t="s">
+      <c r="B26" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="187"/>
-      <c r="B26" s="190"/>
       <c r="C26" s="58"/>
       <c r="D26" s="58" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="187"/>
-      <c r="B27" s="190"/>
+      <c r="A27" s="191"/>
+      <c r="B27" s="193"/>
       <c r="C27" s="58"/>
       <c r="D27" s="58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="191"/>
+      <c r="B28" s="193"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="58" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="187"/>
-      <c r="B28" s="190"/>
-      <c r="C28" s="58" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="191"/>
+      <c r="B29" s="193"/>
+      <c r="C29" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D29" s="58" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="187"/>
-      <c r="B29" s="190"/>
-      <c r="C29" s="58" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="191"/>
+      <c r="B30" s="193"/>
+      <c r="C30" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="D29" s="99" t="s">
+      <c r="D30" s="99" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="188"/>
-      <c r="B30" s="191"/>
-      <c r="C30" s="58" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="195"/>
+      <c r="B31" s="196"/>
+      <c r="C31" s="58" t="s">
         <v>373</v>
       </c>
-      <c r="D30" s="99" t="s">
+      <c r="D31" s="99" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="159" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="163" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="189" t="s">
+      <c r="B32" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C32" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="D31" s="99" t="s">
+      <c r="D32" s="99" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="160"/>
-      <c r="B32" s="190"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="164"/>
+      <c r="B33" s="193"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="160"/>
-      <c r="B33" s="190"/>
-      <c r="C33" s="107" t="s">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="164"/>
+      <c r="B34" s="193"/>
+      <c r="C34" s="107" t="s">
         <v>329</v>
       </c>
-      <c r="D33" s="99" t="s">
+      <c r="D34" s="99" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="160"/>
-      <c r="B34" s="190"/>
-      <c r="C34" s="107" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="164"/>
+      <c r="B35" s="193"/>
+      <c r="C35" s="107" t="s">
         <v>359</v>
       </c>
-      <c r="D34" s="99" t="s">
+      <c r="D35" s="99" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="160"/>
-      <c r="B35" s="190"/>
-      <c r="C35" s="107" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="164"/>
+      <c r="B36" s="193"/>
+      <c r="C36" s="107" t="s">
         <v>367</v>
       </c>
-      <c r="D35" s="99" t="s">
+      <c r="D36" s="99" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="160"/>
-      <c r="B36" s="190"/>
-      <c r="C36" s="107" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="164"/>
+      <c r="B37" s="193"/>
+      <c r="C37" s="107" t="s">
         <v>371</v>
       </c>
-      <c r="D36" s="99" t="s">
+      <c r="D37" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="161"/>
-      <c r="B37" s="191"/>
-      <c r="C37" s="107" t="s">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="165"/>
+      <c r="B38" s="196"/>
+      <c r="C38" s="107" t="s">
         <v>381</v>
       </c>
-      <c r="D37" s="114" t="s">
+      <c r="D38" s="114" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="166" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="170" t="s">
         <v>222</v>
       </c>
-      <c r="B38" s="189" t="s">
+      <c r="B39" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C38" s="193" t="s">
+      <c r="C39" s="197" t="s">
         <v>239</v>
       </c>
-      <c r="D38" s="102" t="s">
+      <c r="D39" s="102" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="199"/>
-      <c r="B39" s="190"/>
-      <c r="C39" s="194"/>
-      <c r="D39" s="99" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="200"/>
+      <c r="B40" s="193"/>
+      <c r="C40" s="198"/>
+      <c r="D40" s="99" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="199"/>
-      <c r="B40" s="190"/>
-      <c r="C40" s="195" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="200"/>
+      <c r="B41" s="193"/>
+      <c r="C41" s="199" t="s">
         <v>240</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D41" s="58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="199"/>
-      <c r="B41" s="190"/>
-      <c r="C41" s="195"/>
-      <c r="D41" s="61" t="s">
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="200"/>
+      <c r="B42" s="193"/>
+      <c r="C42" s="199"/>
+      <c r="D42" s="61" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="199"/>
-      <c r="B42" s="190"/>
-      <c r="C42" s="104" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="200"/>
+      <c r="B43" s="193"/>
+      <c r="C43" s="104" t="s">
         <v>307</v>
       </c>
-      <c r="D42" s="58" t="s">
+      <c r="D43" s="58" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="199"/>
-      <c r="B43" s="190"/>
-      <c r="C43" s="104">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="200"/>
+      <c r="B44" s="193"/>
+      <c r="C44" s="104">
         <v>2.1</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D44" s="58" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="199"/>
-      <c r="B44" s="190"/>
-      <c r="C44" s="104" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="200"/>
+      <c r="B45" s="193"/>
+      <c r="C45" s="104" t="s">
         <v>239</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D45" s="58" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="199"/>
-      <c r="B45" s="190"/>
-      <c r="C45" s="115" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="200"/>
+      <c r="B46" s="193"/>
+      <c r="C46" s="115" t="s">
         <v>239</v>
       </c>
-      <c r="D45" s="114" t="s">
+      <c r="D46" s="114" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="199"/>
-      <c r="B46" s="190"/>
-      <c r="C46" s="130" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="200"/>
+      <c r="B47" s="193"/>
+      <c r="C47" s="130" t="s">
         <v>239</v>
       </c>
-      <c r="D46" s="99" t="s">
+      <c r="D47" s="99" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="199"/>
-      <c r="B47" s="190"/>
-      <c r="C47" s="133" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="200"/>
+      <c r="B48" s="193"/>
+      <c r="C48" s="139" t="s">
         <v>378</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="196" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="200"/>
+      <c r="B49" s="193"/>
+      <c r="C49" s="138">
+        <v>2.1</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="201" t="s">
         <v>296</v>
       </c>
-      <c r="B48" s="189" t="s">
+      <c r="B50" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C48" s="58" t="s">
+      <c r="C50" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D48" s="58" t="s">
+      <c r="D50" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="197"/>
-      <c r="B49" s="190"/>
-      <c r="C49" s="61" t="s">
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="202"/>
+      <c r="B51" s="193"/>
+      <c r="C51" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D49" s="58" t="s">
+      <c r="D51" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="198"/>
-      <c r="B50" s="191"/>
-      <c r="C50" s="58" t="s">
+    <row r="52" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="203"/>
+      <c r="B52" s="196"/>
+      <c r="C52" s="58" t="s">
         <v>350</v>
       </c>
-      <c r="D50" s="58" t="s">
+      <c r="D52" s="58" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="186" t="s">
+    <row r="53" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="190" t="s">
         <v>370</v>
       </c>
-      <c r="B51" s="189" t="s">
+      <c r="B53" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C51" s="130" t="s">
+      <c r="C53" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="58"/>
-    </row>
-    <row r="52" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="187"/>
-      <c r="B52" s="190"/>
-      <c r="C52" s="133" t="s">
+      <c r="D53" s="58"/>
+    </row>
+    <row r="54" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="191"/>
+      <c r="B54" s="193"/>
+      <c r="C54" s="133" t="s">
         <v>378</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="39" t="s">
+    <row r="55" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="191"/>
+      <c r="B55" s="193"/>
+      <c r="C55" s="138">
+        <v>2.1</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B53" s="39"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="44"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="166" t="s">
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="44"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="96" t="s">
+        <v>383</v>
+      </c>
+      <c r="B57" s="136" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="136" t="s">
+        <v>384</v>
+      </c>
+      <c r="D57" s="99"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="170" t="s">
         <v>260</v>
       </c>
-      <c r="B54" s="189" t="s">
+      <c r="B58" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C54" s="58"/>
-      <c r="D54" s="79" t="s">
+      <c r="C58" s="58"/>
+      <c r="D58" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="167"/>
-      <c r="B55" s="191"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="200"/>
+      <c r="B59" s="193"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="96" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="171"/>
+      <c r="B60" s="196"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="137" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="96" t="s">
         <v>334</v>
       </c>
-      <c r="B56" s="123" t="s">
+      <c r="B61" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C56" s="79" t="s">
+      <c r="C61" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D56" s="99" t="s">
+      <c r="D61" s="99" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="96" t="s">
+    <row r="62" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B57" s="123" t="s">
+      <c r="B62" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C57" s="105" t="s">
+      <c r="C62" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="D57" s="103" t="s">
+      <c r="D62" s="103" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="196" t="s">
+    <row r="63" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="201" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="189" t="s">
+      <c r="B63" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C58" s="58" t="s">
+      <c r="C63" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="D58" s="58" t="s">
+      <c r="D63" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="197"/>
-      <c r="B59" s="190"/>
-      <c r="C59" s="58" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="202"/>
+      <c r="B64" s="193"/>
+      <c r="C64" s="58" t="s">
         <v>270</v>
       </c>
-      <c r="D59" s="58" t="s">
+      <c r="D64" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="197"/>
-      <c r="B60" s="190"/>
-      <c r="C60" s="58" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="202"/>
+      <c r="B65" s="193"/>
+      <c r="C65" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="D60" s="58" t="s">
+      <c r="D65" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="197"/>
-      <c r="B61" s="190"/>
-      <c r="C61" s="99" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="202"/>
+      <c r="B66" s="193"/>
+      <c r="C66" s="99" t="s">
         <v>277</v>
-      </c>
-      <c r="D61" s="99" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="197"/>
-      <c r="B62" s="190"/>
-      <c r="C62" s="58" t="s">
-        <v>282</v>
-      </c>
-      <c r="D62" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="197"/>
-      <c r="B63" s="190"/>
-      <c r="C63" s="58" t="s">
-        <v>283</v>
-      </c>
-      <c r="D63" s="58" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="197"/>
-      <c r="B64" s="190"/>
-      <c r="C64" s="99" t="s">
-        <v>288</v>
-      </c>
-      <c r="D64" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="197"/>
-      <c r="B65" s="190"/>
-      <c r="C65" s="99" t="s">
-        <v>302</v>
-      </c>
-      <c r="D65" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="197"/>
-      <c r="B66" s="190"/>
-      <c r="C66" s="99" t="s">
-        <v>289</v>
       </c>
       <c r="D66" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="197"/>
-      <c r="B67" s="190"/>
-      <c r="C67" s="106" t="s">
-        <v>244</v>
-      </c>
-      <c r="D67" s="103" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="197"/>
-      <c r="B68" s="190"/>
-      <c r="C68" s="107" t="s">
-        <v>311</v>
-      </c>
-      <c r="D68" s="99" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="202"/>
+      <c r="B67" s="193"/>
+      <c r="C67" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="D67" s="58" t="s">
         <v>251</v>
       </c>
     </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="202"/>
+      <c r="B68" s="193"/>
+      <c r="C68" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="D68" s="58" t="s">
+        <v>284</v>
+      </c>
+    </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="197"/>
-      <c r="B69" s="190"/>
-      <c r="C69" s="58" t="s">
-        <v>312</v>
-      </c>
-      <c r="D69" s="58" t="s">
-        <v>100</v>
+      <c r="A69" s="202"/>
+      <c r="B69" s="193"/>
+      <c r="C69" s="99" t="s">
+        <v>288</v>
+      </c>
+      <c r="D69" s="99" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="197"/>
-      <c r="B70" s="190"/>
+      <c r="A70" s="202"/>
+      <c r="B70" s="193"/>
       <c r="C70" s="99" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D70" s="99" t="s">
-        <v>314</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="197"/>
-      <c r="B71" s="190"/>
+      <c r="A71" s="202"/>
+      <c r="B71" s="193"/>
       <c r="C71" s="99" t="s">
-        <v>315</v>
+        <v>289</v>
       </c>
       <c r="D71" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="197"/>
-      <c r="B72" s="190"/>
-      <c r="C72" s="99" t="s">
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="202"/>
+      <c r="B72" s="193"/>
+      <c r="C72" s="106" t="s">
+        <v>244</v>
+      </c>
+      <c r="D72" s="103" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="202"/>
+      <c r="B73" s="193"/>
+      <c r="C73" s="107" t="s">
+        <v>311</v>
+      </c>
+      <c r="D73" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="202"/>
+      <c r="B74" s="193"/>
+      <c r="C74" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D74" s="58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="202"/>
+      <c r="B75" s="193"/>
+      <c r="C75" s="99" t="s">
+        <v>313</v>
+      </c>
+      <c r="D75" s="99" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="202"/>
+      <c r="B76" s="193"/>
+      <c r="C76" s="99" t="s">
+        <v>315</v>
+      </c>
+      <c r="D76" s="99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="202"/>
+      <c r="B77" s="193"/>
+      <c r="C77" s="99" t="s">
         <v>268</v>
       </c>
-      <c r="D72" s="99" t="s">
+      <c r="D77" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="197"/>
-      <c r="B73" s="190"/>
-      <c r="C73" s="58" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="202"/>
+      <c r="B78" s="193"/>
+      <c r="C78" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="D73" s="58" t="s">
+      <c r="D78" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="197"/>
-      <c r="B74" s="190"/>
-      <c r="C74" s="99" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="202"/>
+      <c r="B79" s="193"/>
+      <c r="C79" s="99" t="s">
         <v>283</v>
       </c>
-      <c r="D74" s="99" t="s">
+      <c r="D79" s="99" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="197"/>
-      <c r="B75" s="190"/>
-      <c r="C75" s="99" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="202"/>
+      <c r="B80" s="193"/>
+      <c r="C80" s="99" t="s">
         <v>319</v>
-      </c>
-      <c r="D75" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="197"/>
-      <c r="B76" s="190"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="108" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="197"/>
-      <c r="B77" s="190"/>
-      <c r="C77" s="99" t="s">
-        <v>322</v>
-      </c>
-      <c r="D77" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="197"/>
-      <c r="B78" s="190"/>
-      <c r="C78" s="99" t="s">
-        <v>268</v>
-      </c>
-      <c r="D78" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="197"/>
-      <c r="B79" s="190"/>
-      <c r="C79" s="99" t="s">
-        <v>339</v>
-      </c>
-      <c r="D79" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="197"/>
-      <c r="B80" s="190"/>
-      <c r="C80" s="99" t="s">
-        <v>340</v>
       </c>
       <c r="D80" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="197"/>
-      <c r="B81" s="190"/>
-      <c r="C81" s="99" t="s">
+    <row r="81" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="202"/>
+      <c r="B81" s="193"/>
+      <c r="C81" s="58"/>
+      <c r="D81" s="108" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="202"/>
+      <c r="B82" s="193"/>
+      <c r="C82" s="99" t="s">
+        <v>322</v>
+      </c>
+      <c r="D82" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="202"/>
+      <c r="B83" s="193"/>
+      <c r="C83" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="D83" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="202"/>
+      <c r="B84" s="193"/>
+      <c r="C84" s="99" t="s">
+        <v>339</v>
+      </c>
+      <c r="D84" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="202"/>
+      <c r="B85" s="193"/>
+      <c r="C85" s="99" t="s">
+        <v>340</v>
+      </c>
+      <c r="D85" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="202"/>
+      <c r="B86" s="193"/>
+      <c r="C86" s="99" t="s">
         <v>324</v>
       </c>
-      <c r="D81" s="99" t="s">
+      <c r="D86" s="99" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="197"/>
-      <c r="B82" s="190"/>
-      <c r="C82" s="114" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="202"/>
+      <c r="B87" s="193"/>
+      <c r="C87" s="114" t="s">
         <v>345</v>
       </c>
-      <c r="D82" s="114" t="s">
+      <c r="D87" s="114" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="197"/>
-      <c r="B83" s="190"/>
-      <c r="C83" s="99" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="202"/>
+      <c r="B88" s="193"/>
+      <c r="C88" s="99" t="s">
         <v>338</v>
       </c>
-      <c r="D83" s="99" t="s">
+      <c r="D88" s="99" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="197"/>
-      <c r="B84" s="190"/>
-      <c r="C84" s="99" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="202"/>
+      <c r="B89" s="193"/>
+      <c r="C89" s="99" t="s">
         <v>353</v>
       </c>
-      <c r="D84" s="99" t="s">
+      <c r="D89" s="99" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="197"/>
-      <c r="B85" s="190"/>
-      <c r="C85" s="118" t="s">
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="202"/>
+      <c r="B90" s="193"/>
+      <c r="C90" s="118" t="s">
         <v>356</v>
       </c>
-      <c r="D85" s="117" t="s">
+      <c r="D90" s="117" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="197"/>
-      <c r="B86" s="190"/>
-      <c r="C86" s="99" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="202"/>
+      <c r="B91" s="193"/>
+      <c r="C91" s="99" t="s">
         <v>357</v>
-      </c>
-      <c r="D86" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="197"/>
-      <c r="B87" s="190"/>
-      <c r="C87" s="99" t="s">
-        <v>358</v>
-      </c>
-      <c r="D87" s="99" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="197"/>
-      <c r="B88" s="190"/>
-      <c r="C88" s="99" t="s">
-        <v>364</v>
-      </c>
-      <c r="D88" s="99" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="197"/>
-      <c r="B89" s="190"/>
-      <c r="C89" s="99" t="s">
-        <v>366</v>
-      </c>
-      <c r="D89" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="197"/>
-      <c r="B90" s="190"/>
-      <c r="C90" s="99" t="s">
-        <v>372</v>
-      </c>
-      <c r="D90" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="198"/>
-      <c r="B91" s="191"/>
-      <c r="C91" s="99" t="s">
-        <v>364</v>
       </c>
       <c r="D91" s="99" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="96" t="s">
+      <c r="A92" s="202"/>
+      <c r="B92" s="193"/>
+      <c r="C92" s="99" t="s">
+        <v>358</v>
+      </c>
+      <c r="D92" s="99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="202"/>
+      <c r="B93" s="193"/>
+      <c r="C93" s="99" t="s">
+        <v>364</v>
+      </c>
+      <c r="D93" s="99" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="202"/>
+      <c r="B94" s="193"/>
+      <c r="C94" s="99" t="s">
+        <v>366</v>
+      </c>
+      <c r="D94" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="202"/>
+      <c r="B95" s="193"/>
+      <c r="C95" s="99" t="s">
+        <v>372</v>
+      </c>
+      <c r="D95" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="202"/>
+      <c r="B96" s="193"/>
+      <c r="C96" s="99" t="s">
+        <v>364</v>
+      </c>
+      <c r="D96" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="202"/>
+      <c r="B97" s="193"/>
+      <c r="C97" s="114" t="s">
+        <v>385</v>
+      </c>
+      <c r="D97" s="114" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="202"/>
+      <c r="B98" s="193"/>
+      <c r="C98" s="58" t="s">
+        <v>389</v>
+      </c>
+      <c r="D98" s="58" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="202"/>
+      <c r="B99" s="193"/>
+      <c r="C99" s="58" t="s">
+        <v>392</v>
+      </c>
+      <c r="D99" s="58" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="202"/>
+      <c r="B100" s="193"/>
+      <c r="C100" s="58" t="s">
+        <v>393</v>
+      </c>
+      <c r="D100" s="58" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="202"/>
+      <c r="B101" s="193"/>
+      <c r="C101" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="D101" s="58" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="202"/>
+      <c r="B102" s="193"/>
+      <c r="C102" s="58" t="s">
+        <v>395</v>
+      </c>
+      <c r="D102" s="58" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="203"/>
+      <c r="B103" s="196"/>
+      <c r="C103" s="58" t="s">
+        <v>396</v>
+      </c>
+      <c r="D103" s="58" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="96" t="s">
         <v>309</v>
       </c>
-      <c r="B92" s="124" t="s">
+      <c r="B104" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C92" s="58" t="s">
+      <c r="C104" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D92" s="99" t="s">
+      <c r="D104" s="99" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="96" t="s">
+    <row r="105" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="96" t="s">
         <v>310</v>
-      </c>
-      <c r="B93" s="124" t="s">
-        <v>234</v>
-      </c>
-      <c r="C93" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D93" s="99" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="44"/>
-    </row>
-    <row r="95" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="166" t="s">
-        <v>84</v>
-      </c>
-      <c r="B95" s="189" t="s">
-        <v>234</v>
-      </c>
-      <c r="C95" s="58"/>
-      <c r="D95" s="79" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="199"/>
-      <c r="B96" s="190"/>
-      <c r="C96" s="105" t="s">
-        <v>246</v>
-      </c>
-      <c r="D96" s="58" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="199"/>
-      <c r="B97" s="190"/>
-      <c r="C97" s="105">
-        <v>10.1</v>
-      </c>
-      <c r="D97" s="58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="199"/>
-      <c r="B98" s="190"/>
-      <c r="C98" s="105">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D98" s="58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="199"/>
-      <c r="B99" s="190"/>
-      <c r="C99" s="110" t="s">
-        <v>293</v>
-      </c>
-      <c r="D99" s="100" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="167"/>
-      <c r="B100" s="191"/>
-      <c r="C100" s="110" t="s">
-        <v>375</v>
-      </c>
-      <c r="D100" s="100" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="166" t="s">
-        <v>247</v>
-      </c>
-      <c r="B101" s="189" t="s">
-        <v>234</v>
-      </c>
-      <c r="C101" s="175"/>
-      <c r="D101" s="192" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="167"/>
-      <c r="B102" s="191"/>
-      <c r="C102" s="175"/>
-      <c r="D102" s="192"/>
-    </row>
-    <row r="103" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="122" t="s">
-        <v>262</v>
-      </c>
-      <c r="B103" s="124" t="s">
-        <v>234</v>
-      </c>
-      <c r="C103" s="105" t="s">
-        <v>250</v>
-      </c>
-      <c r="D103" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B104" s="39"/>
-      <c r="C104" s="98"/>
-      <c r="D104" s="98"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="96" t="s">
-        <v>249</v>
       </c>
       <c r="B105" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C105" s="111" t="s">
+      <c r="C105" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D105" s="99" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B106" s="39"/>
+      <c r="C106" s="39"/>
+      <c r="D106" s="44"/>
+    </row>
+    <row r="107" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="170" t="s">
+        <v>84</v>
+      </c>
+      <c r="B107" s="192" t="s">
+        <v>234</v>
+      </c>
+      <c r="C107" s="58"/>
+      <c r="D107" s="79" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="200"/>
+      <c r="B108" s="193"/>
+      <c r="C108" s="105" t="s">
+        <v>246</v>
+      </c>
+      <c r="D108" s="58" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="200"/>
+      <c r="B109" s="193"/>
+      <c r="C109" s="105">
+        <v>10.1</v>
+      </c>
+      <c r="D109" s="58" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="200"/>
+      <c r="B110" s="193"/>
+      <c r="C110" s="105">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D110" s="58" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="200"/>
+      <c r="B111" s="193"/>
+      <c r="C111" s="110" t="s">
+        <v>293</v>
+      </c>
+      <c r="D111" s="100" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="171"/>
+      <c r="B112" s="196"/>
+      <c r="C112" s="110" t="s">
+        <v>375</v>
+      </c>
+      <c r="D112" s="100" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="170" t="s">
+        <v>247</v>
+      </c>
+      <c r="B113" s="192" t="s">
+        <v>234</v>
+      </c>
+      <c r="C113" s="179"/>
+      <c r="D113" s="194" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="171"/>
+      <c r="B114" s="196"/>
+      <c r="C114" s="179"/>
+      <c r="D114" s="194"/>
+    </row>
+    <row r="115" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="122" t="s">
+        <v>262</v>
+      </c>
+      <c r="B115" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C115" s="105" t="s">
+        <v>250</v>
+      </c>
+      <c r="D115" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="95" t="s">
+        <v>248</v>
+      </c>
+      <c r="B116" s="39"/>
+      <c r="C116" s="98"/>
+      <c r="D116" s="98"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="96" t="s">
+        <v>249</v>
+      </c>
+      <c r="B117" s="124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C117" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D105" s="58" t="s">
+      <c r="D117" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="166" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="170" t="s">
         <v>285</v>
       </c>
-      <c r="B106" s="189" t="s">
+      <c r="B118" s="192" t="s">
         <v>234</v>
       </c>
-      <c r="C106" s="100" t="s">
+      <c r="C118" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="D106" s="58" t="s">
+      <c r="D118" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="199"/>
-      <c r="B107" s="190"/>
-      <c r="C107" s="58" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="200"/>
+      <c r="B119" s="193"/>
+      <c r="C119" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D107" s="99" t="s">
+      <c r="D119" s="99" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="167"/>
-      <c r="B108" s="191"/>
-      <c r="C108" s="111" t="s">
+    <row r="120" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="171"/>
+      <c r="B120" s="196"/>
+      <c r="C120" s="111" t="s">
         <v>286</v>
       </c>
-      <c r="D108" s="58" t="s">
+      <c r="D120" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="98" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="B109" s="98"/>
-      <c r="C109" s="98"/>
-      <c r="D109" s="98"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="205" t="s">
+      <c r="B121" s="98"/>
+      <c r="C121" s="98"/>
+      <c r="D121" s="98"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="209" t="s">
         <v>58</v>
       </c>
-      <c r="B110" s="189" t="s">
+      <c r="B122" s="192" t="s">
         <v>271</v>
       </c>
-      <c r="C110" s="111" t="s">
+      <c r="C122" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D110" s="58" t="s">
+      <c r="D122" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="206"/>
-      <c r="B111" s="191"/>
-      <c r="C111" s="111" t="s">
+    <row r="123" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="210"/>
+      <c r="B123" s="196"/>
+      <c r="C123" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D111" s="58" t="s">
+      <c r="D123" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="129" t="s">
+    <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="B112" s="124" t="s">
+      <c r="B124" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="C112" s="61" t="s">
+      <c r="C124" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D112" s="58" t="s">
+      <c r="D124" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="96" t="s">
+    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="96" t="s">
         <v>291</v>
       </c>
-      <c r="B113" s="124" t="s">
+      <c r="B125" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="C113" s="58"/>
-      <c r="D113" s="61" t="s">
+      <c r="C125" s="58"/>
+      <c r="D125" s="61" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="97" t="s">
+    <row r="126" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="B114" s="124" t="s">
+      <c r="B126" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="C114" s="61" t="s">
+      <c r="C126" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D114" s="58" t="s">
+      <c r="D126" s="58" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="98" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="98" t="s">
         <v>273</v>
       </c>
-      <c r="B115" s="98"/>
-      <c r="C115" s="98"/>
-      <c r="D115" s="98"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="58"/>
-      <c r="B116" s="124" t="s">
+      <c r="B127" s="98"/>
+      <c r="C127" s="98"/>
+      <c r="D127" s="98"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="58"/>
+      <c r="B128" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C116" s="58" t="s">
+      <c r="C128" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D116" s="99" t="s">
+      <c r="D128" s="99" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="98" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="98" t="s">
         <v>279</v>
       </c>
-      <c r="B117" s="98"/>
-      <c r="C117" s="98"/>
-      <c r="D117" s="98"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="58"/>
-      <c r="B118" s="124" t="s">
+      <c r="B129" s="98"/>
+      <c r="C129" s="98"/>
+      <c r="D129" s="98"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="58"/>
+      <c r="B130" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C118" s="58" t="s">
+      <c r="C130" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D118" s="99" t="s">
+      <c r="D130" s="99" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="A95:A100"/>
-    <mergeCell ref="B95:B100"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="A106:A108"/>
-    <mergeCell ref="B106:B108"/>
-    <mergeCell ref="A38:A47"/>
-    <mergeCell ref="B38:B47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="A58:A91"/>
-    <mergeCell ref="B58:B91"/>
-    <mergeCell ref="A31:A37"/>
-    <mergeCell ref="B31:B37"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="A107:A112"/>
+    <mergeCell ref="B107:B112"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="B118:B120"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="A63:A103"/>
+    <mergeCell ref="B63:B103"/>
+    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="A39:A49"/>
+    <mergeCell ref="B39:B49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates to live from test
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="409">
   <si>
     <t>Document</t>
   </si>
@@ -3065,6 +3065,36 @@
   </si>
   <si>
     <t>Added details around the compression of files less than 2kB</t>
+  </si>
+  <si>
+    <t>Code 4005</t>
+  </si>
+  <si>
+    <t>removed spaces from example in Payroll Run Reference</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Corrected to www.ros.ie</t>
+  </si>
+  <si>
+    <t>Updated timeout to 90 minutes</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>removed spaces from example in Payroll Run Reference and added regex</t>
+  </si>
+  <si>
+    <t>Added link to schema and wsdl</t>
+  </si>
+  <si>
+    <t>Common PAYE Types Schema</t>
+  </si>
+  <si>
+    <t>submissionID &amp; PayrollRunReference min length added</t>
   </si>
 </sst>
 </file>
@@ -3232,7 +3262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -3662,20 +3692,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -4026,21 +4047,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4087,38 +4116,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4141,6 +4140,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4162,68 +4221,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4249,11 +4263,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4658,12 +4687,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="140" t="s">
+      <c r="A2" s="142" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="141"/>
-      <c r="C2" s="141"/>
-      <c r="D2" s="142"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="144"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4686,12 +4715,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="142" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="142"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="144"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4731,10 +4760,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="143" t="s">
+      <c r="A7" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="146">
+      <c r="B7" s="148">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4748,8 +4777,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="144"/>
-      <c r="B8" s="147"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="149"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4761,8 +4790,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="144"/>
-      <c r="B9" s="147"/>
+      <c r="A9" s="146"/>
+      <c r="B9" s="149"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4774,8 +4803,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="144"/>
-      <c r="B10" s="147"/>
+      <c r="A10" s="146"/>
+      <c r="B10" s="149"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4787,8 +4816,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="144"/>
-      <c r="B11" s="147"/>
+      <c r="A11" s="146"/>
+      <c r="B11" s="149"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4800,8 +4829,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="145"/>
-      <c r="B12" s="148"/>
+      <c r="A12" s="147"/>
+      <c r="B12" s="150"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4813,10 +4842,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="151" t="s">
+      <c r="A13" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="146">
+      <c r="B13" s="148">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4830,8 +4859,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="152"/>
-      <c r="B14" s="148"/>
+      <c r="A14" s="154"/>
+      <c r="B14" s="150"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4877,12 +4906,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="140" t="s">
+      <c r="A17" s="142" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="141"/>
-      <c r="C17" s="141"/>
-      <c r="D17" s="142"/>
+      <c r="B17" s="143"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="144"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -4922,21 +4951,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="140" t="s">
+      <c r="A20" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="141"/>
-      <c r="C20" s="141"/>
-      <c r="D20" s="142"/>
+      <c r="B20" s="143"/>
+      <c r="C20" s="143"/>
+      <c r="D20" s="144"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="153" t="s">
+      <c r="A21" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="150">
+      <c r="B21" s="152">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4950,8 +4979,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="154"/>
-      <c r="B22" s="148"/>
+      <c r="A22" s="156"/>
+      <c r="B22" s="150"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -4974,18 +5003,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="140" t="s">
+      <c r="A24" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="141"/>
-      <c r="C24" s="141"/>
-      <c r="D24" s="142"/>
+      <c r="B24" s="143"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="144"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="149" t="s">
+      <c r="A25" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="150">
+      <c r="B25" s="152">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -4999,8 +5028,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="144"/>
-      <c r="B26" s="147"/>
+      <c r="A26" s="146"/>
+      <c r="B26" s="149"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -5012,8 +5041,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
-      <c r="B27" s="147"/>
+      <c r="A27" s="146"/>
+      <c r="B27" s="149"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -5025,8 +5054,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="144"/>
-      <c r="B28" s="147"/>
+      <c r="A28" s="146"/>
+      <c r="B28" s="149"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -5038,8 +5067,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="144"/>
-      <c r="B29" s="147"/>
+      <c r="A29" s="146"/>
+      <c r="B29" s="149"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -5051,8 +5080,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="144"/>
-      <c r="B30" s="147"/>
+      <c r="A30" s="146"/>
+      <c r="B30" s="149"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -5064,8 +5093,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="144"/>
-      <c r="B31" s="147"/>
+      <c r="A31" s="146"/>
+      <c r="B31" s="149"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -5077,8 +5106,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="145"/>
-      <c r="B32" s="148"/>
+      <c r="A32" s="147"/>
+      <c r="B32" s="150"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5202,12 +5231,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="140" t="s">
+      <c r="A41" s="142" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="141"/>
-      <c r="C41" s="141"/>
-      <c r="D41" s="142"/>
+      <c r="B41" s="143"/>
+      <c r="C41" s="143"/>
+      <c r="D41" s="144"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5267,7 +5296,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5277,7 +5306,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5387,10 +5416,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="155" t="s">
+      <c r="A7" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="156" t="s">
+      <c r="B7" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5401,8 +5430,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="155"/>
-      <c r="B8" s="156"/>
+      <c r="A8" s="172"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5411,8 +5440,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
-      <c r="B9" s="156"/>
+      <c r="A9" s="172"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5421,8 +5450,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="155"/>
-      <c r="B10" s="156"/>
+      <c r="A10" s="172"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5431,8 +5460,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="155"/>
-      <c r="B11" s="156"/>
+      <c r="A11" s="172"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5441,8 +5470,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="155"/>
-      <c r="B12" s="156"/>
+      <c r="A12" s="172"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5451,10 +5480,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="158" t="s">
+      <c r="A13" s="174" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5465,8 +5494,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="158"/>
-      <c r="B14" s="156"/>
+      <c r="A14" s="174"/>
+      <c r="B14" s="171"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5475,8 +5504,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="158"/>
-      <c r="B15" s="156"/>
+      <c r="A15" s="174"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5485,10 +5514,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="160" t="s">
+      <c r="B16" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5499,8 +5528,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="159"/>
-      <c r="B17" s="160"/>
+      <c r="A17" s="157"/>
+      <c r="B17" s="166"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5509,8 +5538,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="159"/>
-      <c r="B18" s="160"/>
+      <c r="A18" s="157"/>
+      <c r="B18" s="166"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5519,8 +5548,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="159"/>
-      <c r="B19" s="160"/>
+      <c r="A19" s="157"/>
+      <c r="B19" s="166"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5529,8 +5558,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="159"/>
-      <c r="B20" s="160"/>
+      <c r="A20" s="157"/>
+      <c r="B20" s="166"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5539,8 +5568,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="159"/>
-      <c r="B21" s="160"/>
+      <c r="A21" s="157"/>
+      <c r="B21" s="166"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5549,8 +5578,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="159"/>
-      <c r="B22" s="160"/>
+      <c r="A22" s="157"/>
+      <c r="B22" s="166"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5559,8 +5588,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="159"/>
-      <c r="B23" s="160"/>
+      <c r="A23" s="157"/>
+      <c r="B23" s="166"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5569,26 +5598,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="159"/>
-      <c r="B24" s="160"/>
-      <c r="C24" s="159" t="s">
+      <c r="A24" s="157"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="157" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="166" t="s">
+      <c r="D24" s="158" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="159"/>
-      <c r="B25" s="160"/>
-      <c r="C25" s="159"/>
-      <c r="D25" s="166"/>
+      <c r="A25" s="157"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="157"/>
+      <c r="D25" s="158"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="155" t="s">
+      <c r="A26" s="172" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="156" t="s">
+      <c r="B26" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5599,8 +5628,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
-      <c r="B27" s="156"/>
+      <c r="A27" s="172"/>
+      <c r="B27" s="171"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5627,28 +5656,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="157" t="s">
+      <c r="A30" s="173" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="156" t="s">
+      <c r="B30" s="171" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="159" t="s">
+      <c r="C30" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="169" t="s">
+      <c r="D30" s="161" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="157"/>
-      <c r="B31" s="156"/>
-      <c r="C31" s="159"/>
-      <c r="D31" s="169"/>
+      <c r="A31" s="173"/>
+      <c r="B31" s="171"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="161"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="157"/>
-      <c r="B32" s="156"/>
+      <c r="A32" s="173"/>
+      <c r="B32" s="171"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5657,8 +5686,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="157"/>
-      <c r="B33" s="156"/>
+      <c r="A33" s="173"/>
+      <c r="B33" s="171"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5667,8 +5696,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="157"/>
-      <c r="B34" s="156"/>
+      <c r="A34" s="173"/>
+      <c r="B34" s="171"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5677,8 +5706,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="157"/>
-      <c r="B35" s="156"/>
+      <c r="A35" s="173"/>
+      <c r="B35" s="171"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5687,8 +5716,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="157"/>
-      <c r="B36" s="156"/>
+      <c r="A36" s="173"/>
+      <c r="B36" s="171"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5697,26 +5726,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="157"/>
-      <c r="B37" s="156"/>
-      <c r="C37" s="170" t="s">
+      <c r="A37" s="173"/>
+      <c r="B37" s="171"/>
+      <c r="C37" s="162" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="172" t="s">
+      <c r="D37" s="164" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="157"/>
-      <c r="B38" s="156"/>
-      <c r="C38" s="171"/>
-      <c r="D38" s="172"/>
+      <c r="A38" s="173"/>
+      <c r="B38" s="171"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="164"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="155" t="s">
+      <c r="A39" s="172" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="156" t="s">
+      <c r="B39" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5727,8 +5756,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="155"/>
-      <c r="B40" s="156"/>
+      <c r="A40" s="172"/>
+      <c r="B40" s="171"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5755,10 +5784,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="157" t="s">
+      <c r="A43" s="173" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="156" t="s">
+      <c r="B43" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5767,8 +5796,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="157"/>
-      <c r="B44" s="156"/>
+      <c r="A44" s="173"/>
+      <c r="B44" s="171"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5777,10 +5806,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="163" t="s">
+      <c r="A45" s="168" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="156" t="s">
+      <c r="B45" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5789,8 +5818,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="164"/>
-      <c r="B46" s="156"/>
+      <c r="A46" s="169"/>
+      <c r="B46" s="171"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5799,8 +5828,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="164"/>
-      <c r="B47" s="156"/>
+      <c r="A47" s="169"/>
+      <c r="B47" s="171"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5809,8 +5838,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="165"/>
-      <c r="B48" s="156"/>
+      <c r="A48" s="170"/>
+      <c r="B48" s="171"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5819,10 +5848,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="160" t="s">
+      <c r="A49" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="160" t="s">
+      <c r="B49" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -9926,8 +9955,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="160"/>
-      <c r="B50" s="160"/>
+      <c r="A50" s="166"/>
+      <c r="B50" s="166"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14031,8 +14060,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="160"/>
-      <c r="B51" s="160"/>
+      <c r="A51" s="166"/>
+      <c r="B51" s="166"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18136,8 +18165,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="160"/>
-      <c r="B52" s="160"/>
+      <c r="A52" s="166"/>
+      <c r="B52" s="166"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22241,12 +22270,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="160"/>
-      <c r="B53" s="160"/>
-      <c r="C53" s="168" t="s">
+      <c r="A53" s="166"/>
+      <c r="B53" s="166"/>
+      <c r="C53" s="160" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="169" t="s">
+      <c r="D53" s="161" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26346,10 +26375,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="160"/>
-      <c r="B54" s="160"/>
-      <c r="C54" s="168"/>
-      <c r="D54" s="169"/>
+      <c r="A54" s="166"/>
+      <c r="B54" s="166"/>
+      <c r="C54" s="160"/>
+      <c r="D54" s="161"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30467,10 +30496,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="161" t="s">
+      <c r="A57" s="165" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="160" t="s">
+      <c r="B57" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30481,8 +30510,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="161"/>
-      <c r="B58" s="160"/>
+      <c r="A58" s="165"/>
+      <c r="B58" s="166"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30491,8 +30520,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="161"/>
-      <c r="B59" s="160"/>
+      <c r="A59" s="165"/>
+      <c r="B59" s="166"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30501,8 +30530,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="161"/>
-      <c r="B60" s="160"/>
+      <c r="A60" s="165"/>
+      <c r="B60" s="166"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30511,8 +30540,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="161"/>
-      <c r="B61" s="160"/>
+      <c r="A61" s="165"/>
+      <c r="B61" s="166"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30521,8 +30550,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="161"/>
-      <c r="B62" s="160"/>
+      <c r="A62" s="165"/>
+      <c r="B62" s="166"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30531,8 +30560,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="161"/>
-      <c r="B63" s="160"/>
+      <c r="A63" s="165"/>
+      <c r="B63" s="166"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30541,16 +30570,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="161"/>
-      <c r="B64" s="160"/>
+      <c r="A64" s="165"/>
+      <c r="B64" s="166"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="161"/>
-      <c r="B65" s="160"/>
+      <c r="A65" s="165"/>
+      <c r="B65" s="166"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30559,16 +30588,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="161"/>
-      <c r="B66" s="160"/>
+      <c r="A66" s="165"/>
+      <c r="B66" s="166"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="161"/>
-      <c r="B67" s="160"/>
+      <c r="A67" s="165"/>
+      <c r="B67" s="166"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30577,8 +30606,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="161"/>
-      <c r="B68" s="160"/>
+      <c r="A68" s="165"/>
+      <c r="B68" s="166"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30587,8 +30616,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="161"/>
-      <c r="B69" s="160"/>
+      <c r="A69" s="165"/>
+      <c r="B69" s="166"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30597,8 +30626,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="161"/>
-      <c r="B70" s="160"/>
+      <c r="A70" s="165"/>
+      <c r="B70" s="166"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30607,8 +30636,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="161"/>
-      <c r="B71" s="160"/>
+      <c r="A71" s="165"/>
+      <c r="B71" s="166"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30617,8 +30646,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="161"/>
-      <c r="B72" s="160"/>
+      <c r="A72" s="165"/>
+      <c r="B72" s="166"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30627,16 +30656,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="161"/>
-      <c r="B73" s="160"/>
+      <c r="A73" s="165"/>
+      <c r="B73" s="166"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="161"/>
-      <c r="B74" s="160"/>
+      <c r="A74" s="165"/>
+      <c r="B74" s="166"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30645,18 +30674,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="161"/>
-      <c r="B75" s="160"/>
-      <c r="C75" s="167"/>
-      <c r="D75" s="162" t="s">
+      <c r="A75" s="165"/>
+      <c r="B75" s="166"/>
+      <c r="C75" s="159"/>
+      <c r="D75" s="167" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="161"/>
-      <c r="B76" s="160"/>
-      <c r="C76" s="167"/>
-      <c r="D76" s="162"/>
+      <c r="A76" s="165"/>
+      <c r="B76" s="166"/>
+      <c r="C76" s="159"/>
+      <c r="D76" s="167"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30680,8 +30709,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30690,29 +30719,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30727,6 +30740,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30780,10 +30809,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="156" t="s">
+      <c r="B4" s="171" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30794,8 +30823,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="155"/>
-      <c r="B5" s="156"/>
+      <c r="A5" s="172"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="182" t="s">
         <v>190</v>
       </c>
@@ -30804,58 +30833,58 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="155"/>
-      <c r="B6" s="156"/>
+      <c r="A6" s="172"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="182"/>
       <c r="D6" s="181"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="155"/>
-      <c r="B7" s="156"/>
+      <c r="A7" s="172"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="155"/>
-      <c r="B8" s="156"/>
+      <c r="A8" s="172"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="155"/>
-      <c r="B9" s="156"/>
+      <c r="A9" s="172"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="158" t="s">
+      <c r="A10" s="174" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="156" t="s">
+      <c r="B10" s="171" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="180"/>
+      <c r="C10" s="184"/>
       <c r="D10" s="181" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="158"/>
-      <c r="B11" s="156"/>
-      <c r="C11" s="180"/>
+      <c r="A11" s="174"/>
+      <c r="B11" s="171"/>
+      <c r="C11" s="184"/>
       <c r="D11" s="181"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="158"/>
-      <c r="B12" s="156"/>
-      <c r="C12" s="180"/>
+      <c r="A12" s="174"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="184"/>
       <c r="D12" s="181"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="159" t="s">
+      <c r="A13" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="166" t="s">
         <v>185</v>
       </c>
       <c r="C13" s="183"/>
@@ -30864,62 +30893,62 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="159"/>
-      <c r="B14" s="160"/>
+      <c r="A14" s="157"/>
+      <c r="B14" s="166"/>
       <c r="C14" s="183"/>
       <c r="D14" s="181"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="159"/>
-      <c r="B15" s="160"/>
+      <c r="A15" s="157"/>
+      <c r="B15" s="166"/>
       <c r="C15" s="183"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="159"/>
-      <c r="B16" s="160"/>
+      <c r="A16" s="157"/>
+      <c r="B16" s="166"/>
       <c r="C16" s="183"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="159"/>
-      <c r="B17" s="160"/>
+      <c r="A17" s="157"/>
+      <c r="B17" s="166"/>
       <c r="C17" s="183"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="159"/>
-      <c r="B18" s="160"/>
+      <c r="A18" s="157"/>
+      <c r="B18" s="166"/>
       <c r="C18" s="183"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="159"/>
-      <c r="B19" s="160"/>
+      <c r="A19" s="157"/>
+      <c r="B19" s="166"/>
       <c r="C19" s="183"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="159"/>
-      <c r="B20" s="160"/>
+      <c r="A20" s="157"/>
+      <c r="B20" s="166"/>
       <c r="C20" s="183"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="159"/>
-      <c r="B21" s="160"/>
+      <c r="A21" s="157"/>
+      <c r="B21" s="166"/>
       <c r="C21" s="183"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="159"/>
-      <c r="B22" s="160"/>
+      <c r="A22" s="157"/>
+      <c r="B22" s="166"/>
       <c r="C22" s="183"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="159"/>
-      <c r="B23" s="160"/>
+      <c r="A23" s="157"/>
+      <c r="B23" s="166"/>
       <c r="C23" s="183"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
@@ -31018,10 +31047,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="184" t="s">
+      <c r="A32" s="175" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="187" t="s">
+      <c r="B32" s="178" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31032,26 +31061,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="185"/>
-      <c r="B33" s="188"/>
+      <c r="A33" s="176"/>
+      <c r="B33" s="179"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="185"/>
-      <c r="B34" s="188"/>
+      <c r="A34" s="176"/>
+      <c r="B34" s="179"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="185"/>
-      <c r="B35" s="188"/>
+      <c r="A35" s="176"/>
+      <c r="B35" s="179"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="186"/>
-      <c r="B36" s="189"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="180"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31080,10 +31109,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="157" t="s">
+      <c r="A39" s="173" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="156" t="s">
+      <c r="B39" s="171" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31094,8 +31123,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="157"/>
-      <c r="B40" s="156"/>
+      <c r="A40" s="173"/>
+      <c r="B40" s="171"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31104,84 +31133,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="155" t="s">
+      <c r="A41" s="172" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="156" t="s">
+      <c r="B41" s="171" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="180" t="s">
+      <c r="C41" s="184" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="159" t="s">
+      <c r="D41" s="157" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="155"/>
-      <c r="B42" s="156"/>
-      <c r="C42" s="180"/>
-      <c r="D42" s="159"/>
+      <c r="A42" s="172"/>
+      <c r="B42" s="171"/>
+      <c r="C42" s="184"/>
+      <c r="D42" s="157"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="155"/>
-      <c r="B43" s="156"/>
-      <c r="C43" s="180" t="s">
+      <c r="A43" s="172"/>
+      <c r="B43" s="171"/>
+      <c r="C43" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="162" t="s">
+      <c r="D43" s="167" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="155"/>
-      <c r="B44" s="156"/>
-      <c r="C44" s="180"/>
-      <c r="D44" s="162"/>
+      <c r="A44" s="172"/>
+      <c r="B44" s="171"/>
+      <c r="C44" s="184"/>
+      <c r="D44" s="167"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="161" t="s">
+      <c r="A45" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="160" t="s">
+      <c r="B45" s="166" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="176"/>
+      <c r="C45" s="188"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="161"/>
-      <c r="B46" s="160"/>
-      <c r="C46" s="177"/>
-      <c r="D46" s="173" t="s">
+      <c r="A46" s="165"/>
+      <c r="B46" s="166"/>
+      <c r="C46" s="189"/>
+      <c r="D46" s="185" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="161"/>
-      <c r="B47" s="160"/>
-      <c r="C47" s="177"/>
-      <c r="D47" s="174"/>
+      <c r="A47" s="165"/>
+      <c r="B47" s="166"/>
+      <c r="C47" s="189"/>
+      <c r="D47" s="186"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="161"/>
-      <c r="B48" s="160"/>
-      <c r="C48" s="178"/>
-      <c r="D48" s="174"/>
+      <c r="A48" s="165"/>
+      <c r="B48" s="166"/>
+      <c r="C48" s="190"/>
+      <c r="D48" s="186"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="161"/>
-      <c r="B49" s="160"/>
-      <c r="C49" s="168"/>
-      <c r="D49" s="174"/>
+      <c r="A49" s="165"/>
+      <c r="B49" s="166"/>
+      <c r="C49" s="160"/>
+      <c r="D49" s="186"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="161"/>
-      <c r="B50" s="160"/>
-      <c r="C50" s="168"/>
-      <c r="D50" s="175"/>
+      <c r="A50" s="165"/>
+      <c r="B50" s="166"/>
+      <c r="C50" s="160"/>
+      <c r="D50" s="187"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31204,10 +31233,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="160" t="s">
+      <c r="A53" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="160" t="s">
+      <c r="B53" s="166" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31218,8 +31247,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="160"/>
-      <c r="B54" s="160"/>
+      <c r="A54" s="166"/>
+      <c r="B54" s="166"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31228,8 +31257,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="160"/>
-      <c r="B55" s="160"/>
+      <c r="A55" s="166"/>
+      <c r="B55" s="166"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31238,9 +31267,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="160"/>
-      <c r="B56" s="160"/>
-      <c r="C56" s="179" t="s">
+      <c r="A56" s="166"/>
+      <c r="B56" s="166"/>
+      <c r="C56" s="191" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31248,16 +31277,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="160"/>
-      <c r="B57" s="160"/>
-      <c r="C57" s="179"/>
+      <c r="A57" s="166"/>
+      <c r="B57" s="166"/>
+      <c r="C57" s="191"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="160"/>
-      <c r="B58" s="160"/>
+      <c r="A58" s="166"/>
+      <c r="B58" s="166"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31266,8 +31295,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="160"/>
-      <c r="B59" s="160"/>
+      <c r="A59" s="166"/>
+      <c r="B59" s="166"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31276,9 +31305,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="160"/>
-      <c r="B60" s="160"/>
-      <c r="C60" s="179" t="s">
+      <c r="A60" s="166"/>
+      <c r="B60" s="166"/>
+      <c r="C60" s="191" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31286,25 +31315,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="160"/>
-      <c r="B61" s="160"/>
-      <c r="C61" s="179"/>
+      <c r="A61" s="166"/>
+      <c r="B61" s="166"/>
+      <c r="C61" s="191"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="160"/>
-      <c r="B62" s="160"/>
-      <c r="C62" s="179"/>
+      <c r="A62" s="166"/>
+      <c r="B62" s="166"/>
+      <c r="C62" s="191"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="160"/>
-      <c r="B63" s="160"/>
-      <c r="C63" s="180" t="s">
+      <c r="A63" s="166"/>
+      <c r="B63" s="166"/>
+      <c r="C63" s="184" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31312,30 +31341,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="160"/>
-      <c r="B64" s="160"/>
-      <c r="C64" s="180"/>
-      <c r="D64" s="162" t="s">
+      <c r="A64" s="166"/>
+      <c r="B64" s="166"/>
+      <c r="C64" s="184"/>
+      <c r="D64" s="167" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="160"/>
-      <c r="B65" s="160"/>
-      <c r="C65" s="180"/>
-      <c r="D65" s="162"/>
+      <c r="A65" s="166"/>
+      <c r="B65" s="166"/>
+      <c r="C65" s="184"/>
+      <c r="D65" s="167"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="160"/>
-      <c r="B66" s="160"/>
-      <c r="C66" s="180"/>
-      <c r="D66" s="162"/>
+      <c r="A66" s="166"/>
+      <c r="B66" s="166"/>
+      <c r="C66" s="184"/>
+      <c r="D66" s="167"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="160"/>
-      <c r="B67" s="160"/>
-      <c r="C67" s="180"/>
-      <c r="D67" s="162"/>
+      <c r="A67" s="166"/>
+      <c r="B67" s="166"/>
+      <c r="C67" s="184"/>
+      <c r="D67" s="167"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31391,23 +31420,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31424,6 +31436,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31432,10 +31461,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D130"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31469,10 +31498,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="201" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="205" t="s">
+      <c r="B3" s="202" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="113" t="s">
@@ -31483,8 +31512,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="204"/>
-      <c r="B4" s="205"/>
+      <c r="A4" s="201"/>
+      <c r="B4" s="202"/>
       <c r="C4" s="113" t="s">
         <v>347</v>
       </c>
@@ -31492,9 +31521,9 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="204"/>
-      <c r="B5" s="205"/>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="201"/>
+      <c r="B5" s="202"/>
       <c r="C5" s="113" t="s">
         <v>343</v>
       </c>
@@ -31511,10 +31540,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="159" t="s">
+      <c r="A7" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="179" t="s">
+      <c r="B7" s="191" t="s">
         <v>234</v>
       </c>
       <c r="C7" s="58"/>
@@ -31523,8 +31552,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="159"/>
-      <c r="B8" s="179"/>
+      <c r="A8" s="157"/>
+      <c r="B8" s="191"/>
       <c r="C8" s="105" t="s">
         <v>235</v>
       </c>
@@ -31575,1283 +31604,1387 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="159" t="s">
+      <c r="A12" s="96" t="s">
+        <v>407</v>
+      </c>
+      <c r="B12" s="141" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="141"/>
+      <c r="D12" s="140" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="157" t="s">
         <v>275</v>
       </c>
-      <c r="B12" s="179" t="s">
+      <c r="B13" s="191" t="s">
         <v>234</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="79" t="s">
+      <c r="C13" s="58"/>
+      <c r="D13" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="159"/>
-      <c r="B13" s="179"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="157"/>
+      <c r="B14" s="191"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="159"/>
-      <c r="B14" s="179"/>
-      <c r="C14" s="109" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="157"/>
+      <c r="B15" s="191"/>
+      <c r="C15" s="109" t="s">
         <v>325</v>
       </c>
-      <c r="D14" s="58" t="s">
+      <c r="D15" s="58" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="96" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="157"/>
+      <c r="B16" s="191"/>
+      <c r="C16" s="138" t="s">
+        <v>404</v>
+      </c>
+      <c r="D16" s="99" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="96" t="s">
         <v>290</v>
       </c>
-      <c r="B15" s="121" t="s">
+      <c r="B17" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="116" t="s">
+      <c r="C17" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="58"/>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="206" t="s">
+      <c r="D17" s="58"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="203" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="192" t="s">
+      <c r="B18" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="120" t="s">
+      <c r="C18" s="58"/>
+      <c r="D18" s="120" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="207"/>
-      <c r="B17" s="193"/>
-      <c r="C17" s="119" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="204"/>
+      <c r="B19" s="197"/>
+      <c r="C19" s="119" t="s">
         <v>361</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D19" s="58" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="207"/>
-      <c r="B18" s="193"/>
-      <c r="C18" s="119" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="204"/>
+      <c r="B20" s="197"/>
+      <c r="C20" s="119" t="s">
         <v>359</v>
       </c>
-      <c r="D18" s="58" t="s">
+      <c r="D20" s="58" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="207"/>
-      <c r="B19" s="193"/>
-      <c r="C19" s="125" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="204"/>
+      <c r="B21" s="197"/>
+      <c r="C21" s="125" t="s">
         <v>367</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="D21" s="99" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="207"/>
-      <c r="B20" s="193"/>
-      <c r="C20" s="133" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="204"/>
+      <c r="B22" s="197"/>
+      <c r="C22" s="133" t="s">
         <v>359</v>
       </c>
-      <c r="D20" s="99" t="s">
+      <c r="D22" s="99" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="208"/>
-      <c r="B21" s="196"/>
-      <c r="C21" s="119" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="204"/>
+      <c r="B23" s="197"/>
+      <c r="C23" s="137" t="s">
         <v>371</v>
       </c>
-      <c r="D21" s="99" t="s">
+      <c r="D23" s="99" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="128" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="205"/>
+      <c r="B24" s="195"/>
+      <c r="C24" s="137" t="s">
+        <v>359</v>
+      </c>
+      <c r="D24" s="99" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="128" t="s">
         <v>331</v>
       </c>
-      <c r="B22" s="121" t="s">
+      <c r="B25" s="121" t="s">
         <v>234</v>
       </c>
-      <c r="C22" s="116" t="s">
+      <c r="C25" s="116" t="s">
         <v>332</v>
       </c>
-      <c r="D22" s="99" t="s">
+      <c r="D25" s="99" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="128" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="128" t="s">
         <v>351</v>
       </c>
-      <c r="B23" s="127" t="s">
+      <c r="B26" s="127" t="s">
         <v>234</v>
       </c>
-      <c r="C23" s="126" t="s">
+      <c r="C26" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="99"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="135" t="s">
+      <c r="D26" s="99"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="206" t="s">
         <v>369</v>
       </c>
-      <c r="B24" s="134" t="s">
+      <c r="B27" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C24" s="130" t="s">
+      <c r="C27" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="99"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="D27" s="99"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="207"/>
+      <c r="B28" s="195"/>
+      <c r="C28" s="138" t="s">
+        <v>404</v>
+      </c>
+      <c r="D28" s="99" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="190" t="s">
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="206" t="s">
         <v>237</v>
       </c>
-      <c r="B26" s="192" t="s">
+      <c r="B30" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58" t="s">
+      <c r="C30" s="58"/>
+      <c r="D30" s="58" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="191"/>
-      <c r="B27" s="193"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="208"/>
+      <c r="B31" s="197"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="191"/>
-      <c r="B28" s="193"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="208"/>
+      <c r="B32" s="197"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="191"/>
-      <c r="B29" s="193"/>
-      <c r="C29" s="58" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="208"/>
+      <c r="B33" s="197"/>
+      <c r="C33" s="58" t="s">
         <v>300</v>
       </c>
-      <c r="D29" s="58" t="s">
+      <c r="D33" s="58" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="191"/>
-      <c r="B30" s="193"/>
-      <c r="C30" s="58" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="208"/>
+      <c r="B34" s="197"/>
+      <c r="C34" s="58" t="s">
         <v>328</v>
       </c>
-      <c r="D30" s="99" t="s">
+      <c r="D34" s="99" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="195"/>
-      <c r="B31" s="196"/>
-      <c r="C31" s="58" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="207"/>
+      <c r="B35" s="195"/>
+      <c r="C35" s="58" t="s">
         <v>373</v>
       </c>
-      <c r="D31" s="99" t="s">
+      <c r="D35" s="99" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="163" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="168" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="192" t="s">
+      <c r="B36" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C32" s="58" t="s">
+      <c r="C36" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="D32" s="99" t="s">
+      <c r="D36" s="99" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="164"/>
-      <c r="B33" s="193"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="169"/>
+      <c r="B37" s="197"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="164"/>
-      <c r="B34" s="193"/>
-      <c r="C34" s="107" t="s">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="169"/>
+      <c r="B38" s="197"/>
+      <c r="C38" s="107" t="s">
         <v>329</v>
       </c>
-      <c r="D34" s="99" t="s">
+      <c r="D38" s="99" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="164"/>
-      <c r="B35" s="193"/>
-      <c r="C35" s="107" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="169"/>
+      <c r="B39" s="197"/>
+      <c r="C39" s="107" t="s">
         <v>359</v>
       </c>
-      <c r="D35" s="99" t="s">
+      <c r="D39" s="99" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="164"/>
-      <c r="B36" s="193"/>
-      <c r="C36" s="107" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="169"/>
+      <c r="B40" s="197"/>
+      <c r="C40" s="107" t="s">
         <v>367</v>
       </c>
-      <c r="D36" s="99" t="s">
+      <c r="D40" s="99" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="164"/>
-      <c r="B37" s="193"/>
-      <c r="C37" s="107" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="169"/>
+      <c r="B41" s="197"/>
+      <c r="C41" s="107" t="s">
         <v>371</v>
       </c>
-      <c r="D37" s="99" t="s">
+      <c r="D41" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="165"/>
-      <c r="B38" s="196"/>
-      <c r="C38" s="107" t="s">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="169"/>
+      <c r="B42" s="197"/>
+      <c r="C42" s="107" t="s">
         <v>381</v>
       </c>
-      <c r="D38" s="114" t="s">
+      <c r="D42" s="114" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="170" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="170"/>
+      <c r="B43" s="195"/>
+      <c r="C43" s="96" t="s">
+        <v>359</v>
+      </c>
+      <c r="D43" s="99" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="162" t="s">
         <v>222</v>
       </c>
-      <c r="B39" s="192" t="s">
+      <c r="B44" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="197" t="s">
+      <c r="C44" s="210" t="s">
         <v>239</v>
       </c>
-      <c r="D39" s="102" t="s">
+      <c r="D44" s="102" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="200"/>
-      <c r="B40" s="193"/>
-      <c r="C40" s="198"/>
-      <c r="D40" s="99" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="196"/>
+      <c r="B45" s="197"/>
+      <c r="C45" s="211"/>
+      <c r="D45" s="99" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="200"/>
-      <c r="B41" s="193"/>
-      <c r="C41" s="199" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="196"/>
+      <c r="B46" s="197"/>
+      <c r="C46" s="212" t="s">
         <v>240</v>
       </c>
-      <c r="D41" s="58" t="s">
+      <c r="D46" s="58" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="200"/>
-      <c r="B42" s="193"/>
-      <c r="C42" s="199"/>
-      <c r="D42" s="61" t="s">
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="196"/>
+      <c r="B47" s="197"/>
+      <c r="C47" s="212"/>
+      <c r="D47" s="61" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="200"/>
-      <c r="B43" s="193"/>
-      <c r="C43" s="104" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="196"/>
+      <c r="B48" s="197"/>
+      <c r="C48" s="104" t="s">
         <v>307</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D48" s="58" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="200"/>
-      <c r="B44" s="193"/>
-      <c r="C44" s="104">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="196"/>
+      <c r="B49" s="197"/>
+      <c r="C49" s="104">
         <v>2.1</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D49" s="58" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="200"/>
-      <c r="B45" s="193"/>
-      <c r="C45" s="104" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="196"/>
+      <c r="B50" s="197"/>
+      <c r="C50" s="104" t="s">
         <v>239</v>
       </c>
-      <c r="D45" s="58" t="s">
+      <c r="D50" s="58" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="200"/>
-      <c r="B46" s="193"/>
-      <c r="C46" s="115" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="196"/>
+      <c r="B51" s="197"/>
+      <c r="C51" s="115" t="s">
         <v>239</v>
       </c>
-      <c r="D46" s="114" t="s">
+      <c r="D51" s="114" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="200"/>
-      <c r="B47" s="193"/>
-      <c r="C47" s="130" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="196"/>
+      <c r="B52" s="197"/>
+      <c r="C52" s="130" t="s">
         <v>239</v>
       </c>
-      <c r="D47" s="99" t="s">
+      <c r="D52" s="99" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="200"/>
-      <c r="B48" s="193"/>
-      <c r="C48" s="139" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="196"/>
+      <c r="B53" s="197"/>
+      <c r="C53" s="136" t="s">
         <v>378</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D53" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="200"/>
-      <c r="B49" s="193"/>
-      <c r="C49" s="138">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="196"/>
+      <c r="B54" s="197"/>
+      <c r="C54" s="138">
         <v>2.1</v>
       </c>
-      <c r="D49" s="58" t="s">
+      <c r="D54" s="58" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="201" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="196"/>
+      <c r="B55" s="197"/>
+      <c r="C55" s="138" t="s">
+        <v>239</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="198" t="s">
         <v>296</v>
       </c>
-      <c r="B50" s="192" t="s">
+      <c r="B56" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C50" s="58" t="s">
+      <c r="C56" s="58" t="s">
         <v>297</v>
       </c>
-      <c r="D50" s="58" t="s">
+      <c r="D56" s="58" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="202"/>
-      <c r="B51" s="193"/>
-      <c r="C51" s="61" t="s">
+    <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="199"/>
+      <c r="B57" s="197"/>
+      <c r="C57" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D51" s="58" t="s">
+      <c r="D57" s="58" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="203"/>
-      <c r="B52" s="196"/>
-      <c r="C52" s="58" t="s">
+    <row r="58" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="200"/>
+      <c r="B58" s="195"/>
+      <c r="C58" s="58" t="s">
         <v>350</v>
       </c>
-      <c r="D52" s="58" t="s">
+      <c r="D58" s="58" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="190" t="s">
+    <row r="59" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="206" t="s">
         <v>370</v>
       </c>
-      <c r="B53" s="192" t="s">
+      <c r="B59" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C53" s="130" t="s">
+      <c r="C59" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="D53" s="58"/>
-    </row>
-    <row r="54" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="191"/>
-      <c r="B54" s="193"/>
-      <c r="C54" s="133" t="s">
+      <c r="D59" s="58"/>
+    </row>
+    <row r="60" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="208"/>
+      <c r="B60" s="197"/>
+      <c r="C60" s="133" t="s">
         <v>378</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D60" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="191"/>
-      <c r="B55" s="193"/>
-      <c r="C55" s="138">
+    <row r="61" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="208"/>
+      <c r="B61" s="197"/>
+      <c r="C61" s="138">
         <v>2.1</v>
       </c>
-      <c r="D55" s="58" t="s">
+      <c r="D61" s="58" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
+    <row r="62" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="208"/>
+      <c r="B62" s="197"/>
+      <c r="C62" s="138" t="s">
+        <v>240</v>
+      </c>
+      <c r="D62" s="58" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="208"/>
+      <c r="B63" s="197"/>
+      <c r="C63" s="135" t="s">
+        <v>239</v>
+      </c>
+      <c r="D63" s="58" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="44"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="96" t="s">
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="44"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="96" t="s">
         <v>383</v>
       </c>
-      <c r="B57" s="136" t="s">
+      <c r="B65" s="134" t="s">
         <v>234</v>
       </c>
-      <c r="C57" s="136" t="s">
+      <c r="C65" s="134" t="s">
         <v>384</v>
       </c>
-      <c r="D57" s="99"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="170" t="s">
+      <c r="D65" s="99"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="162" t="s">
         <v>260</v>
       </c>
-      <c r="B58" s="192" t="s">
+      <c r="B66" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C58" s="58"/>
-      <c r="D58" s="79" t="s">
+      <c r="C66" s="58"/>
+      <c r="D66" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="200"/>
-      <c r="B59" s="193"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="196"/>
+      <c r="B67" s="197"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="58" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="171"/>
-      <c r="B60" s="196"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="137" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="196"/>
+      <c r="B68" s="197"/>
+      <c r="C68" s="58"/>
+      <c r="D68" s="99" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="96" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="96" t="s">
         <v>334</v>
       </c>
-      <c r="B61" s="123" t="s">
+      <c r="B69" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C61" s="79" t="s">
+      <c r="C69" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D61" s="99" t="s">
+      <c r="D69" s="99" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="96" t="s">
+    <row r="70" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B62" s="123" t="s">
+      <c r="B70" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C62" s="105" t="s">
+      <c r="C70" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="103" t="s">
+      <c r="D70" s="103" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="201" t="s">
+    <row r="71" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="198" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="192" t="s">
+      <c r="B71" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C63" s="58" t="s">
+      <c r="C71" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="D63" s="58" t="s">
+      <c r="D71" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="202"/>
-      <c r="B64" s="193"/>
-      <c r="C64" s="58" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="199"/>
+      <c r="B72" s="197"/>
+      <c r="C72" s="58" t="s">
         <v>270</v>
       </c>
-      <c r="D64" s="58" t="s">
+      <c r="D72" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="202"/>
-      <c r="B65" s="193"/>
-      <c r="C65" s="58" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="199"/>
+      <c r="B73" s="197"/>
+      <c r="C73" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="D65" s="58" t="s">
+      <c r="D73" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="202"/>
-      <c r="B66" s="193"/>
-      <c r="C66" s="99" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="199"/>
+      <c r="B74" s="197"/>
+      <c r="C74" s="99" t="s">
         <v>277</v>
       </c>
-      <c r="D66" s="99" t="s">
+      <c r="D74" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="202"/>
-      <c r="B67" s="193"/>
-      <c r="C67" s="58" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="199"/>
+      <c r="B75" s="197"/>
+      <c r="C75" s="58" t="s">
         <v>282</v>
       </c>
-      <c r="D67" s="58" t="s">
+      <c r="D75" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="202"/>
-      <c r="B68" s="193"/>
-      <c r="C68" s="58" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="199"/>
+      <c r="B76" s="197"/>
+      <c r="C76" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="D68" s="58" t="s">
+      <c r="D76" s="58" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="202"/>
-      <c r="B69" s="193"/>
-      <c r="C69" s="99" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="199"/>
+      <c r="B77" s="197"/>
+      <c r="C77" s="99" t="s">
         <v>288</v>
       </c>
-      <c r="D69" s="99" t="s">
+      <c r="D77" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="202"/>
-      <c r="B70" s="193"/>
-      <c r="C70" s="99" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="199"/>
+      <c r="B78" s="197"/>
+      <c r="C78" s="99" t="s">
         <v>302</v>
       </c>
-      <c r="D70" s="99" t="s">
+      <c r="D78" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="202"/>
-      <c r="B71" s="193"/>
-      <c r="C71" s="99" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="199"/>
+      <c r="B79" s="197"/>
+      <c r="C79" s="99" t="s">
         <v>289</v>
       </c>
-      <c r="D71" s="99" t="s">
+      <c r="D79" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="202"/>
-      <c r="B72" s="193"/>
-      <c r="C72" s="106" t="s">
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="199"/>
+      <c r="B80" s="197"/>
+      <c r="C80" s="106" t="s">
         <v>244</v>
       </c>
-      <c r="D72" s="103" t="s">
+      <c r="D80" s="103" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="202"/>
-      <c r="B73" s="193"/>
-      <c r="C73" s="107" t="s">
+    <row r="81" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="199"/>
+      <c r="B81" s="197"/>
+      <c r="C81" s="107" t="s">
         <v>311</v>
       </c>
-      <c r="D73" s="99" t="s">
+      <c r="D81" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="202"/>
-      <c r="B74" s="193"/>
-      <c r="C74" s="58" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="199"/>
+      <c r="B82" s="197"/>
+      <c r="C82" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="D74" s="58" t="s">
+      <c r="D82" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="202"/>
-      <c r="B75" s="193"/>
-      <c r="C75" s="99" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="199"/>
+      <c r="B83" s="197"/>
+      <c r="C83" s="99" t="s">
         <v>313</v>
       </c>
-      <c r="D75" s="99" t="s">
+      <c r="D83" s="99" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="202"/>
-      <c r="B76" s="193"/>
-      <c r="C76" s="99" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="199"/>
+      <c r="B84" s="197"/>
+      <c r="C84" s="99" t="s">
         <v>315</v>
       </c>
-      <c r="D76" s="99" t="s">
+      <c r="D84" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="202"/>
-      <c r="B77" s="193"/>
-      <c r="C77" s="99" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="199"/>
+      <c r="B85" s="197"/>
+      <c r="C85" s="99" t="s">
         <v>268</v>
       </c>
-      <c r="D77" s="99" t="s">
+      <c r="D85" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="202"/>
-      <c r="B78" s="193"/>
-      <c r="C78" s="58" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="199"/>
+      <c r="B86" s="197"/>
+      <c r="C86" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="D78" s="58" t="s">
+      <c r="D86" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="202"/>
-      <c r="B79" s="193"/>
-      <c r="C79" s="99" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="199"/>
+      <c r="B87" s="197"/>
+      <c r="C87" s="99" t="s">
         <v>283</v>
       </c>
-      <c r="D79" s="99" t="s">
+      <c r="D87" s="99" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="202"/>
-      <c r="B80" s="193"/>
-      <c r="C80" s="99" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="199"/>
+      <c r="B88" s="197"/>
+      <c r="C88" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="D80" s="99" t="s">
+      <c r="D88" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="202"/>
-      <c r="B81" s="193"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="108" t="s">
+    <row r="89" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="199"/>
+      <c r="B89" s="197"/>
+      <c r="C89" s="58"/>
+      <c r="D89" s="108" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="202"/>
-      <c r="B82" s="193"/>
-      <c r="C82" s="99" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="199"/>
+      <c r="B90" s="197"/>
+      <c r="C90" s="99" t="s">
         <v>322</v>
       </c>
-      <c r="D82" s="99" t="s">
+      <c r="D90" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="202"/>
-      <c r="B83" s="193"/>
-      <c r="C83" s="99" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="199"/>
+      <c r="B91" s="197"/>
+      <c r="C91" s="99" t="s">
         <v>268</v>
-      </c>
-      <c r="D83" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="202"/>
-      <c r="B84" s="193"/>
-      <c r="C84" s="99" t="s">
-        <v>339</v>
-      </c>
-      <c r="D84" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="202"/>
-      <c r="B85" s="193"/>
-      <c r="C85" s="99" t="s">
-        <v>340</v>
-      </c>
-      <c r="D85" s="99" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="202"/>
-      <c r="B86" s="193"/>
-      <c r="C86" s="99" t="s">
-        <v>324</v>
-      </c>
-      <c r="D86" s="99" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="202"/>
-      <c r="B87" s="193"/>
-      <c r="C87" s="114" t="s">
-        <v>345</v>
-      </c>
-      <c r="D87" s="114" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="202"/>
-      <c r="B88" s="193"/>
-      <c r="C88" s="99" t="s">
-        <v>338</v>
-      </c>
-      <c r="D88" s="99" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="202"/>
-      <c r="B89" s="193"/>
-      <c r="C89" s="99" t="s">
-        <v>353</v>
-      </c>
-      <c r="D89" s="99" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="202"/>
-      <c r="B90" s="193"/>
-      <c r="C90" s="118" t="s">
-        <v>356</v>
-      </c>
-      <c r="D90" s="117" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="202"/>
-      <c r="B91" s="193"/>
-      <c r="C91" s="99" t="s">
-        <v>357</v>
       </c>
       <c r="D91" s="99" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="202"/>
-      <c r="B92" s="193"/>
+      <c r="A92" s="199"/>
+      <c r="B92" s="197"/>
       <c r="C92" s="99" t="s">
+        <v>339</v>
+      </c>
+      <c r="D92" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="199"/>
+      <c r="B93" s="197"/>
+      <c r="C93" s="99" t="s">
+        <v>340</v>
+      </c>
+      <c r="D93" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="199"/>
+      <c r="B94" s="197"/>
+      <c r="C94" s="99" t="s">
+        <v>324</v>
+      </c>
+      <c r="D94" s="99" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="199"/>
+      <c r="B95" s="197"/>
+      <c r="C95" s="114" t="s">
+        <v>345</v>
+      </c>
+      <c r="D95" s="114" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="199"/>
+      <c r="B96" s="197"/>
+      <c r="C96" s="99" t="s">
+        <v>338</v>
+      </c>
+      <c r="D96" s="99" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="199"/>
+      <c r="B97" s="197"/>
+      <c r="C97" s="99" t="s">
+        <v>353</v>
+      </c>
+      <c r="D97" s="99" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="199"/>
+      <c r="B98" s="197"/>
+      <c r="C98" s="118" t="s">
+        <v>356</v>
+      </c>
+      <c r="D98" s="117" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="199"/>
+      <c r="B99" s="197"/>
+      <c r="C99" s="99" t="s">
+        <v>357</v>
+      </c>
+      <c r="D99" s="99" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="199"/>
+      <c r="B100" s="197"/>
+      <c r="C100" s="99" t="s">
         <v>358</v>
       </c>
-      <c r="D92" s="99" t="s">
+      <c r="D100" s="99" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="202"/>
-      <c r="B93" s="193"/>
-      <c r="C93" s="99" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="199"/>
+      <c r="B101" s="197"/>
+      <c r="C101" s="99" t="s">
         <v>364</v>
       </c>
-      <c r="D93" s="99" t="s">
+      <c r="D101" s="99" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="202"/>
-      <c r="B94" s="193"/>
-      <c r="C94" s="99" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="199"/>
+      <c r="B102" s="197"/>
+      <c r="C102" s="99" t="s">
         <v>366</v>
       </c>
-      <c r="D94" s="99" t="s">
+      <c r="D102" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="202"/>
-      <c r="B95" s="193"/>
-      <c r="C95" s="99" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="199"/>
+      <c r="B103" s="197"/>
+      <c r="C103" s="99" t="s">
         <v>372</v>
       </c>
-      <c r="D95" s="99" t="s">
+      <c r="D103" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="202"/>
-      <c r="B96" s="193"/>
-      <c r="C96" s="99" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="199"/>
+      <c r="B104" s="197"/>
+      <c r="C104" s="99" t="s">
         <v>364</v>
       </c>
-      <c r="D96" s="99" t="s">
+      <c r="D104" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="202"/>
-      <c r="B97" s="193"/>
-      <c r="C97" s="114" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="199"/>
+      <c r="B105" s="197"/>
+      <c r="C105" s="114" t="s">
         <v>385</v>
       </c>
-      <c r="D97" s="114" t="s">
+      <c r="D105" s="114" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="202"/>
-      <c r="B98" s="193"/>
-      <c r="C98" s="58" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="199"/>
+      <c r="B106" s="197"/>
+      <c r="C106" s="58" t="s">
         <v>389</v>
       </c>
-      <c r="D98" s="58" t="s">
+      <c r="D106" s="58" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="202"/>
-      <c r="B99" s="193"/>
-      <c r="C99" s="58" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="199"/>
+      <c r="B107" s="197"/>
+      <c r="C107" s="58" t="s">
         <v>392</v>
       </c>
-      <c r="D99" s="58" t="s">
+      <c r="D107" s="58" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="202"/>
-      <c r="B100" s="193"/>
-      <c r="C100" s="58" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="199"/>
+      <c r="B108" s="197"/>
+      <c r="C108" s="58" t="s">
         <v>393</v>
       </c>
-      <c r="D100" s="58" t="s">
+      <c r="D108" s="58" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="202"/>
-      <c r="B101" s="193"/>
-      <c r="C101" s="58" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="199"/>
+      <c r="B109" s="197"/>
+      <c r="C109" s="58" t="s">
         <v>394</v>
       </c>
-      <c r="D101" s="58" t="s">
+      <c r="D109" s="58" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="202"/>
-      <c r="B102" s="193"/>
-      <c r="C102" s="58" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="199"/>
+      <c r="B110" s="197"/>
+      <c r="C110" s="58" t="s">
         <v>395</v>
       </c>
-      <c r="D102" s="58" t="s">
+      <c r="D110" s="58" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="203"/>
-      <c r="B103" s="196"/>
-      <c r="C103" s="58" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="199"/>
+      <c r="B111" s="197"/>
+      <c r="C111" s="58" t="s">
         <v>396</v>
       </c>
-      <c r="D103" s="58" t="s">
+      <c r="D111" s="58" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="96" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="200"/>
+      <c r="B112" s="195"/>
+      <c r="C112" s="58" t="s">
+        <v>399</v>
+      </c>
+      <c r="D112" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="96" t="s">
         <v>309</v>
       </c>
-      <c r="B104" s="124" t="s">
+      <c r="B113" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C104" s="58" t="s">
+      <c r="C113" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D104" s="99" t="s">
+      <c r="D113" s="99" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="96" t="s">
+    <row r="114" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="96" t="s">
         <v>310</v>
       </c>
-      <c r="B105" s="124" t="s">
+      <c r="B114" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C105" s="58" t="s">
+      <c r="C114" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D105" s="99" t="s">
+      <c r="D114" s="99" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="39" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B106" s="39"/>
-      <c r="C106" s="39"/>
-      <c r="D106" s="44"/>
-    </row>
-    <row r="107" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="170" t="s">
+      <c r="B115" s="39"/>
+      <c r="C115" s="39"/>
+      <c r="D115" s="44"/>
+    </row>
+    <row r="116" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="162" t="s">
         <v>84</v>
       </c>
-      <c r="B107" s="192" t="s">
+      <c r="B116" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C107" s="58"/>
-      <c r="D107" s="79" t="s">
+      <c r="C116" s="58"/>
+      <c r="D116" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="200"/>
-      <c r="B108" s="193"/>
-      <c r="C108" s="105" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="196"/>
+      <c r="B117" s="197"/>
+      <c r="C117" s="105" t="s">
         <v>246</v>
       </c>
-      <c r="D108" s="58" t="s">
+      <c r="D117" s="58" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="200"/>
-      <c r="B109" s="193"/>
-      <c r="C109" s="105">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="196"/>
+      <c r="B118" s="197"/>
+      <c r="C118" s="105">
         <v>10.1</v>
       </c>
-      <c r="D109" s="58" t="s">
+      <c r="D118" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="200"/>
-      <c r="B110" s="193"/>
-      <c r="C110" s="105">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="196"/>
+      <c r="B119" s="197"/>
+      <c r="C119" s="105">
         <v>10.199999999999999</v>
       </c>
-      <c r="D110" s="58" t="s">
+      <c r="D119" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="200"/>
-      <c r="B111" s="193"/>
-      <c r="C111" s="110" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="196"/>
+      <c r="B120" s="197"/>
+      <c r="C120" s="110" t="s">
         <v>293</v>
       </c>
-      <c r="D111" s="100" t="s">
+      <c r="D120" s="100" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="171"/>
-      <c r="B112" s="196"/>
-      <c r="C112" s="110" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="163"/>
+      <c r="B121" s="195"/>
+      <c r="C121" s="110" t="s">
         <v>375</v>
       </c>
-      <c r="D112" s="100" t="s">
+      <c r="D121" s="100" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="170" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="162" t="s">
         <v>247</v>
       </c>
-      <c r="B113" s="192" t="s">
+      <c r="B122" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C113" s="179"/>
-      <c r="D113" s="194" t="s">
+      <c r="C122" s="191"/>
+      <c r="D122" s="209" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="171"/>
-      <c r="B114" s="196"/>
-      <c r="C114" s="179"/>
-      <c r="D114" s="194"/>
-    </row>
-    <row r="115" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="122" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="163"/>
+      <c r="B123" s="195"/>
+      <c r="C123" s="191"/>
+      <c r="D123" s="209"/>
+    </row>
+    <row r="124" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="122" t="s">
         <v>262</v>
       </c>
-      <c r="B115" s="124" t="s">
+      <c r="B124" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C115" s="105" t="s">
+      <c r="C124" s="105" t="s">
         <v>250</v>
       </c>
-      <c r="D115" s="99" t="s">
+      <c r="D124" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="95" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B116" s="39"/>
-      <c r="C116" s="98"/>
-      <c r="D116" s="98"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="96" t="s">
+      <c r="B125" s="39"/>
+      <c r="C125" s="98"/>
+      <c r="D125" s="98"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="B117" s="124" t="s">
+      <c r="B126" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C117" s="111" t="s">
+      <c r="C126" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D117" s="58" t="s">
+      <c r="D126" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="170" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="162" t="s">
         <v>285</v>
       </c>
-      <c r="B118" s="192" t="s">
+      <c r="B127" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C118" s="100" t="s">
+      <c r="C127" s="100" t="s">
         <v>295</v>
       </c>
-      <c r="D118" s="58" t="s">
+      <c r="D127" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="200"/>
-      <c r="B119" s="193"/>
-      <c r="C119" s="58" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="196"/>
+      <c r="B128" s="197"/>
+      <c r="C128" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D119" s="99" t="s">
+      <c r="D128" s="99" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A120" s="171"/>
-      <c r="B120" s="196"/>
-      <c r="C120" s="111" t="s">
+    <row r="129" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="163"/>
+      <c r="B129" s="195"/>
+      <c r="C129" s="111" t="s">
         <v>286</v>
       </c>
-      <c r="D120" s="58" t="s">
+      <c r="D129" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="98" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="B121" s="98"/>
-      <c r="C121" s="98"/>
-      <c r="D121" s="98"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="209" t="s">
+      <c r="B130" s="98"/>
+      <c r="C130" s="98"/>
+      <c r="D130" s="98"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="192" t="s">
         <v>58</v>
       </c>
-      <c r="B122" s="192" t="s">
+      <c r="B131" s="194" t="s">
         <v>271</v>
       </c>
-      <c r="C122" s="111" t="s">
+      <c r="C131" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D122" s="58" t="s">
+      <c r="D131" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="210"/>
-      <c r="B123" s="196"/>
-      <c r="C123" s="111" t="s">
+    <row r="132" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="193"/>
+      <c r="B132" s="195"/>
+      <c r="C132" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="D123" s="58" t="s">
+      <c r="D132" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="129" t="s">
+    <row r="133" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="B124" s="124" t="s">
+      <c r="B133" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="C124" s="61" t="s">
+      <c r="C133" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D124" s="58" t="s">
+      <c r="D133" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="96" t="s">
+    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="96" t="s">
         <v>291</v>
       </c>
-      <c r="B125" s="124" t="s">
+      <c r="B134" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="C125" s="58"/>
-      <c r="D125" s="61" t="s">
+      <c r="C134" s="58"/>
+      <c r="D134" s="61" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="97" t="s">
+    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="B126" s="124" t="s">
+      <c r="B135" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="C126" s="61" t="s">
+      <c r="C135" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D126" s="58" t="s">
+      <c r="D135" s="58" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="98" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="98" t="s">
         <v>273</v>
       </c>
-      <c r="B127" s="98"/>
-      <c r="C127" s="98"/>
-      <c r="D127" s="98"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="58"/>
-      <c r="B128" s="124" t="s">
+      <c r="B136" s="98"/>
+      <c r="C136" s="98"/>
+      <c r="D136" s="98"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="58"/>
+      <c r="B137" s="124" t="s">
         <v>234</v>
       </c>
-      <c r="C128" s="58" t="s">
+      <c r="C137" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D128" s="99" t="s">
+      <c r="D137" s="99" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="98" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="98" t="s">
         <v>279</v>
       </c>
-      <c r="B129" s="98"/>
-      <c r="C129" s="98"/>
-      <c r="D129" s="98"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="58"/>
-      <c r="B130" s="124" t="s">
+      <c r="B138" s="98"/>
+      <c r="C138" s="98"/>
+      <c r="D138" s="98"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="58"/>
+      <c r="B139" s="139" t="s">
         <v>234</v>
       </c>
-      <c r="C130" s="58" t="s">
+      <c r="C139" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D130" s="99" t="s">
+      <c r="D139" s="99" t="s">
         <v>274</v>
       </c>
     </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="58"/>
+      <c r="B140" s="124"/>
+      <c r="C140" s="58" t="s">
+        <v>401</v>
+      </c>
+      <c r="D140" s="99" t="s">
+        <v>402</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="A107:A112"/>
-    <mergeCell ref="B107:B112"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="A118:A120"/>
-    <mergeCell ref="B118:B120"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
+  <mergeCells count="36">
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="A71:A112"/>
+    <mergeCell ref="B71:B112"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="B36:B43"/>
+    <mergeCell ref="A44:A55"/>
+    <mergeCell ref="B44:B55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="A63:A103"/>
-    <mergeCell ref="B63:B103"/>
-    <mergeCell ref="A32:A38"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="A39:A49"/>
-    <mergeCell ref="B39:B49"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="A116:A121"/>
+    <mergeCell ref="B116:B121"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="A127:A129"/>
+    <mergeCell ref="B127:B129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added amend description for previous line item
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="421">
   <si>
     <t>Document</t>
   </si>
@@ -3128,6 +3128,9 @@
   </si>
   <si>
     <t>Added example string to be signed</t>
+  </si>
+  <si>
+    <t>Added description on Previous Line Item ID</t>
   </si>
 </sst>
 </file>
@@ -4151,38 +4154,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4205,6 +4178,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4226,41 +4259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4268,38 +4274,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4316,23 +4310,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5346,7 +5349,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5356,7 +5359,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5466,10 +5469,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="157" t="s">
+      <c r="A7" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="158" t="s">
+      <c r="B7" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5480,8 +5483,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="157"/>
-      <c r="B8" s="158"/>
+      <c r="A8" s="172"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5490,8 +5493,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="157"/>
-      <c r="B9" s="158"/>
+      <c r="A9" s="172"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5500,8 +5503,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="157"/>
-      <c r="B10" s="158"/>
+      <c r="A10" s="172"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5510,8 +5513,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="157"/>
-      <c r="B11" s="158"/>
+      <c r="A11" s="172"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5520,8 +5523,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="157"/>
-      <c r="B12" s="158"/>
+      <c r="A12" s="172"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5530,10 +5533,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="160" t="s">
+      <c r="A13" s="174" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5544,8 +5547,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="160"/>
-      <c r="B14" s="158"/>
+      <c r="A14" s="174"/>
+      <c r="B14" s="171"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5554,8 +5557,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="160"/>
-      <c r="B15" s="158"/>
+      <c r="A15" s="174"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5564,10 +5567,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="161" t="s">
+      <c r="A16" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5578,8 +5581,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="161"/>
-      <c r="B17" s="162"/>
+      <c r="A17" s="157"/>
+      <c r="B17" s="166"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5588,8 +5591,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="161"/>
-      <c r="B18" s="162"/>
+      <c r="A18" s="157"/>
+      <c r="B18" s="166"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5598,8 +5601,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="161"/>
-      <c r="B19" s="162"/>
+      <c r="A19" s="157"/>
+      <c r="B19" s="166"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5608,8 +5611,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="161"/>
-      <c r="B20" s="162"/>
+      <c r="A20" s="157"/>
+      <c r="B20" s="166"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5618,8 +5621,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="161"/>
-      <c r="B21" s="162"/>
+      <c r="A21" s="157"/>
+      <c r="B21" s="166"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5628,8 +5631,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="161"/>
-      <c r="B22" s="162"/>
+      <c r="A22" s="157"/>
+      <c r="B22" s="166"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5638,8 +5641,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="161"/>
-      <c r="B23" s="162"/>
+      <c r="A23" s="157"/>
+      <c r="B23" s="166"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5648,26 +5651,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="161"/>
-      <c r="B24" s="162"/>
-      <c r="C24" s="161" t="s">
+      <c r="A24" s="157"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="157" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="168" t="s">
+      <c r="D24" s="158" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="161"/>
-      <c r="B25" s="162"/>
-      <c r="C25" s="161"/>
-      <c r="D25" s="168"/>
+      <c r="A25" s="157"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="157"/>
+      <c r="D25" s="158"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="157" t="s">
+      <c r="A26" s="172" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="158" t="s">
+      <c r="B26" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5678,8 +5681,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="157"/>
-      <c r="B27" s="158"/>
+      <c r="A27" s="172"/>
+      <c r="B27" s="171"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5706,28 +5709,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="159" t="s">
+      <c r="A30" s="173" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="158" t="s">
+      <c r="B30" s="171" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="161" t="s">
+      <c r="C30" s="157" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="171" t="s">
+      <c r="D30" s="161" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="159"/>
-      <c r="B31" s="158"/>
-      <c r="C31" s="161"/>
-      <c r="D31" s="171"/>
+      <c r="A31" s="173"/>
+      <c r="B31" s="171"/>
+      <c r="C31" s="157"/>
+      <c r="D31" s="161"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="159"/>
-      <c r="B32" s="158"/>
+      <c r="A32" s="173"/>
+      <c r="B32" s="171"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5736,8 +5739,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="159"/>
-      <c r="B33" s="158"/>
+      <c r="A33" s="173"/>
+      <c r="B33" s="171"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5746,8 +5749,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="159"/>
-      <c r="B34" s="158"/>
+      <c r="A34" s="173"/>
+      <c r="B34" s="171"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5756,8 +5759,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="159"/>
-      <c r="B35" s="158"/>
+      <c r="A35" s="173"/>
+      <c r="B35" s="171"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5766,8 +5769,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="159"/>
-      <c r="B36" s="158"/>
+      <c r="A36" s="173"/>
+      <c r="B36" s="171"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5776,26 +5779,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="159"/>
-      <c r="B37" s="158"/>
-      <c r="C37" s="172" t="s">
+      <c r="A37" s="173"/>
+      <c r="B37" s="171"/>
+      <c r="C37" s="162" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="174" t="s">
+      <c r="D37" s="164" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="159"/>
-      <c r="B38" s="158"/>
-      <c r="C38" s="173"/>
-      <c r="D38" s="174"/>
+      <c r="A38" s="173"/>
+      <c r="B38" s="171"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="164"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="157" t="s">
+      <c r="A39" s="172" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="158" t="s">
+      <c r="B39" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5806,8 +5809,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="157"/>
-      <c r="B40" s="158"/>
+      <c r="A40" s="172"/>
+      <c r="B40" s="171"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5834,10 +5837,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="159" t="s">
+      <c r="A43" s="173" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="158" t="s">
+      <c r="B43" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5846,8 +5849,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="159"/>
-      <c r="B44" s="158"/>
+      <c r="A44" s="173"/>
+      <c r="B44" s="171"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5856,10 +5859,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="165" t="s">
+      <c r="A45" s="168" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="158" t="s">
+      <c r="B45" s="171" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5868,8 +5871,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="166"/>
-      <c r="B46" s="158"/>
+      <c r="A46" s="169"/>
+      <c r="B46" s="171"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5878,8 +5881,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="166"/>
-      <c r="B47" s="158"/>
+      <c r="A47" s="169"/>
+      <c r="B47" s="171"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5888,8 +5891,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="167"/>
-      <c r="B48" s="158"/>
+      <c r="A48" s="170"/>
+      <c r="B48" s="171"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5898,10 +5901,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="162" t="s">
+      <c r="A49" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="162" t="s">
+      <c r="B49" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10005,8 +10008,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="162"/>
-      <c r="B50" s="162"/>
+      <c r="A50" s="166"/>
+      <c r="B50" s="166"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14110,8 +14113,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="162"/>
-      <c r="B51" s="162"/>
+      <c r="A51" s="166"/>
+      <c r="B51" s="166"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18215,8 +18218,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="162"/>
-      <c r="B52" s="162"/>
+      <c r="A52" s="166"/>
+      <c r="B52" s="166"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22320,12 +22323,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="162"/>
-      <c r="B53" s="162"/>
-      <c r="C53" s="170" t="s">
+      <c r="A53" s="166"/>
+      <c r="B53" s="166"/>
+      <c r="C53" s="160" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="171" t="s">
+      <c r="D53" s="161" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26425,10 +26428,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="162"/>
-      <c r="B54" s="162"/>
-      <c r="C54" s="170"/>
-      <c r="D54" s="171"/>
+      <c r="A54" s="166"/>
+      <c r="B54" s="166"/>
+      <c r="C54" s="160"/>
+      <c r="D54" s="161"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30546,10 +30549,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="163" t="s">
+      <c r="A57" s="165" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="162" t="s">
+      <c r="B57" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30560,8 +30563,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="163"/>
-      <c r="B58" s="162"/>
+      <c r="A58" s="165"/>
+      <c r="B58" s="166"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30570,8 +30573,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="163"/>
-      <c r="B59" s="162"/>
+      <c r="A59" s="165"/>
+      <c r="B59" s="166"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30580,8 +30583,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="163"/>
-      <c r="B60" s="162"/>
+      <c r="A60" s="165"/>
+      <c r="B60" s="166"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30590,8 +30593,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="163"/>
-      <c r="B61" s="162"/>
+      <c r="A61" s="165"/>
+      <c r="B61" s="166"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30600,8 +30603,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="163"/>
-      <c r="B62" s="162"/>
+      <c r="A62" s="165"/>
+      <c r="B62" s="166"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30610,8 +30613,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="163"/>
-      <c r="B63" s="162"/>
+      <c r="A63" s="165"/>
+      <c r="B63" s="166"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30620,16 +30623,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="163"/>
-      <c r="B64" s="162"/>
+      <c r="A64" s="165"/>
+      <c r="B64" s="166"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="163"/>
-      <c r="B65" s="162"/>
+      <c r="A65" s="165"/>
+      <c r="B65" s="166"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30638,16 +30641,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="163"/>
-      <c r="B66" s="162"/>
+      <c r="A66" s="165"/>
+      <c r="B66" s="166"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="163"/>
-      <c r="B67" s="162"/>
+      <c r="A67" s="165"/>
+      <c r="B67" s="166"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30656,8 +30659,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="163"/>
-      <c r="B68" s="162"/>
+      <c r="A68" s="165"/>
+      <c r="B68" s="166"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30666,8 +30669,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="163"/>
-      <c r="B69" s="162"/>
+      <c r="A69" s="165"/>
+      <c r="B69" s="166"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30676,8 +30679,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="163"/>
-      <c r="B70" s="162"/>
+      <c r="A70" s="165"/>
+      <c r="B70" s="166"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30686,8 +30689,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="163"/>
-      <c r="B71" s="162"/>
+      <c r="A71" s="165"/>
+      <c r="B71" s="166"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30696,8 +30699,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="163"/>
-      <c r="B72" s="162"/>
+      <c r="A72" s="165"/>
+      <c r="B72" s="166"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30706,16 +30709,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="163"/>
-      <c r="B73" s="162"/>
+      <c r="A73" s="165"/>
+      <c r="B73" s="166"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="163"/>
-      <c r="B74" s="162"/>
+      <c r="A74" s="165"/>
+      <c r="B74" s="166"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30724,18 +30727,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="163"/>
-      <c r="B75" s="162"/>
-      <c r="C75" s="169"/>
-      <c r="D75" s="164" t="s">
+      <c r="A75" s="165"/>
+      <c r="B75" s="166"/>
+      <c r="C75" s="159"/>
+      <c r="D75" s="167" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="163"/>
-      <c r="B76" s="162"/>
-      <c r="C76" s="169"/>
-      <c r="D76" s="164"/>
+      <c r="A76" s="165"/>
+      <c r="B76" s="166"/>
+      <c r="C76" s="159"/>
+      <c r="D76" s="167"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30759,8 +30762,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30769,29 +30772,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30806,6 +30793,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30859,10 +30862,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="157" t="s">
+      <c r="A4" s="172" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="158" t="s">
+      <c r="B4" s="171" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30873,133 +30876,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="157"/>
-      <c r="B5" s="158"/>
-      <c r="C5" s="184" t="s">
+      <c r="A5" s="172"/>
+      <c r="B5" s="171"/>
+      <c r="C5" s="182" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="183" t="s">
+      <c r="D5" s="181" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="157"/>
-      <c r="B6" s="158"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="183"/>
+      <c r="A6" s="172"/>
+      <c r="B6" s="171"/>
+      <c r="C6" s="182"/>
+      <c r="D6" s="181"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="157"/>
-      <c r="B7" s="158"/>
+      <c r="A7" s="172"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="157"/>
-      <c r="B8" s="158"/>
+      <c r="A8" s="172"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="157"/>
-      <c r="B9" s="158"/>
+      <c r="A9" s="172"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="160" t="s">
+      <c r="A10" s="174" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="158" t="s">
+      <c r="B10" s="171" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="182"/>
-      <c r="D10" s="183" t="s">
+      <c r="C10" s="184"/>
+      <c r="D10" s="181" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="160"/>
-      <c r="B11" s="158"/>
-      <c r="C11" s="182"/>
-      <c r="D11" s="183"/>
+      <c r="A11" s="174"/>
+      <c r="B11" s="171"/>
+      <c r="C11" s="184"/>
+      <c r="D11" s="181"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="160"/>
-      <c r="B12" s="158"/>
-      <c r="C12" s="182"/>
-      <c r="D12" s="183"/>
+      <c r="A12" s="174"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="184"/>
+      <c r="D12" s="181"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="161" t="s">
+      <c r="A13" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="166" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="185"/>
-      <c r="D13" s="183" t="s">
+      <c r="C13" s="183"/>
+      <c r="D13" s="181" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="161"/>
-      <c r="B14" s="162"/>
-      <c r="C14" s="185"/>
-      <c r="D14" s="183"/>
+      <c r="A14" s="157"/>
+      <c r="B14" s="166"/>
+      <c r="C14" s="183"/>
+      <c r="D14" s="181"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="161"/>
-      <c r="B15" s="162"/>
-      <c r="C15" s="185"/>
+      <c r="A15" s="157"/>
+      <c r="B15" s="166"/>
+      <c r="C15" s="183"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="161"/>
-      <c r="B16" s="162"/>
-      <c r="C16" s="185"/>
+      <c r="A16" s="157"/>
+      <c r="B16" s="166"/>
+      <c r="C16" s="183"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="161"/>
-      <c r="B17" s="162"/>
-      <c r="C17" s="185"/>
+      <c r="A17" s="157"/>
+      <c r="B17" s="166"/>
+      <c r="C17" s="183"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="161"/>
-      <c r="B18" s="162"/>
-      <c r="C18" s="185"/>
+      <c r="A18" s="157"/>
+      <c r="B18" s="166"/>
+      <c r="C18" s="183"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="161"/>
-      <c r="B19" s="162"/>
-      <c r="C19" s="185"/>
+      <c r="A19" s="157"/>
+      <c r="B19" s="166"/>
+      <c r="C19" s="183"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="161"/>
-      <c r="B20" s="162"/>
-      <c r="C20" s="185"/>
+      <c r="A20" s="157"/>
+      <c r="B20" s="166"/>
+      <c r="C20" s="183"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="161"/>
-      <c r="B21" s="162"/>
-      <c r="C21" s="185"/>
+      <c r="A21" s="157"/>
+      <c r="B21" s="166"/>
+      <c r="C21" s="183"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="161"/>
-      <c r="B22" s="162"/>
-      <c r="C22" s="185"/>
+      <c r="A22" s="157"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="183"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="161"/>
-      <c r="B23" s="162"/>
-      <c r="C23" s="185"/>
+      <c r="A23" s="157"/>
+      <c r="B23" s="166"/>
+      <c r="C23" s="183"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31097,10 +31100,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="186" t="s">
+      <c r="A32" s="175" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="189" t="s">
+      <c r="B32" s="178" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31111,26 +31114,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="187"/>
-      <c r="B33" s="190"/>
+      <c r="A33" s="176"/>
+      <c r="B33" s="179"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="187"/>
-      <c r="B34" s="190"/>
+      <c r="A34" s="176"/>
+      <c r="B34" s="179"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="187"/>
-      <c r="B35" s="190"/>
+      <c r="A35" s="176"/>
+      <c r="B35" s="179"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="188"/>
-      <c r="B36" s="191"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="180"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31159,10 +31162,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="159" t="s">
+      <c r="A39" s="173" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="158" t="s">
+      <c r="B39" s="171" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31173,8 +31176,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="159"/>
-      <c r="B40" s="158"/>
+      <c r="A40" s="173"/>
+      <c r="B40" s="171"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31183,84 +31186,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="157" t="s">
+      <c r="A41" s="172" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="158" t="s">
+      <c r="B41" s="171" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="182" t="s">
+      <c r="C41" s="184" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="161" t="s">
+      <c r="D41" s="157" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="157"/>
-      <c r="B42" s="158"/>
-      <c r="C42" s="182"/>
-      <c r="D42" s="161"/>
+      <c r="A42" s="172"/>
+      <c r="B42" s="171"/>
+      <c r="C42" s="184"/>
+      <c r="D42" s="157"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="157"/>
-      <c r="B43" s="158"/>
-      <c r="C43" s="182" t="s">
+      <c r="A43" s="172"/>
+      <c r="B43" s="171"/>
+      <c r="C43" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="164" t="s">
+      <c r="D43" s="167" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="157"/>
-      <c r="B44" s="158"/>
-      <c r="C44" s="182"/>
-      <c r="D44" s="164"/>
+      <c r="A44" s="172"/>
+      <c r="B44" s="171"/>
+      <c r="C44" s="184"/>
+      <c r="D44" s="167"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="163" t="s">
+      <c r="A45" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="162" t="s">
+      <c r="B45" s="166" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="178"/>
+      <c r="C45" s="188"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="163"/>
-      <c r="B46" s="162"/>
-      <c r="C46" s="179"/>
-      <c r="D46" s="175" t="s">
+      <c r="A46" s="165"/>
+      <c r="B46" s="166"/>
+      <c r="C46" s="189"/>
+      <c r="D46" s="185" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="163"/>
-      <c r="B47" s="162"/>
-      <c r="C47" s="179"/>
-      <c r="D47" s="176"/>
+      <c r="A47" s="165"/>
+      <c r="B47" s="166"/>
+      <c r="C47" s="189"/>
+      <c r="D47" s="186"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="163"/>
-      <c r="B48" s="162"/>
-      <c r="C48" s="180"/>
-      <c r="D48" s="176"/>
+      <c r="A48" s="165"/>
+      <c r="B48" s="166"/>
+      <c r="C48" s="190"/>
+      <c r="D48" s="186"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="163"/>
-      <c r="B49" s="162"/>
-      <c r="C49" s="170"/>
-      <c r="D49" s="176"/>
+      <c r="A49" s="165"/>
+      <c r="B49" s="166"/>
+      <c r="C49" s="160"/>
+      <c r="D49" s="186"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="163"/>
-      <c r="B50" s="162"/>
-      <c r="C50" s="170"/>
-      <c r="D50" s="177"/>
+      <c r="A50" s="165"/>
+      <c r="B50" s="166"/>
+      <c r="C50" s="160"/>
+      <c r="D50" s="187"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31283,10 +31286,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="162" t="s">
+      <c r="A53" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="162" t="s">
+      <c r="B53" s="166" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31297,8 +31300,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="162"/>
-      <c r="B54" s="162"/>
+      <c r="A54" s="166"/>
+      <c r="B54" s="166"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31307,8 +31310,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="162"/>
-      <c r="B55" s="162"/>
+      <c r="A55" s="166"/>
+      <c r="B55" s="166"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31317,9 +31320,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="162"/>
-      <c r="B56" s="162"/>
-      <c r="C56" s="181" t="s">
+      <c r="A56" s="166"/>
+      <c r="B56" s="166"/>
+      <c r="C56" s="191" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31327,16 +31330,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="162"/>
-      <c r="B57" s="162"/>
-      <c r="C57" s="181"/>
+      <c r="A57" s="166"/>
+      <c r="B57" s="166"/>
+      <c r="C57" s="191"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="162"/>
-      <c r="B58" s="162"/>
+      <c r="A58" s="166"/>
+      <c r="B58" s="166"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31345,8 +31348,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="162"/>
-      <c r="B59" s="162"/>
+      <c r="A59" s="166"/>
+      <c r="B59" s="166"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31355,9 +31358,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="162"/>
-      <c r="B60" s="162"/>
-      <c r="C60" s="181" t="s">
+      <c r="A60" s="166"/>
+      <c r="B60" s="166"/>
+      <c r="C60" s="191" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31365,25 +31368,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="162"/>
-      <c r="B61" s="162"/>
-      <c r="C61" s="181"/>
+      <c r="A61" s="166"/>
+      <c r="B61" s="166"/>
+      <c r="C61" s="191"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="162"/>
-      <c r="B62" s="162"/>
-      <c r="C62" s="181"/>
+      <c r="A62" s="166"/>
+      <c r="B62" s="166"/>
+      <c r="C62" s="191"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="162"/>
-      <c r="B63" s="162"/>
-      <c r="C63" s="182" t="s">
+      <c r="A63" s="166"/>
+      <c r="B63" s="166"/>
+      <c r="C63" s="184" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31391,30 +31394,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="162"/>
-      <c r="B64" s="162"/>
-      <c r="C64" s="182"/>
-      <c r="D64" s="164" t="s">
+      <c r="A64" s="166"/>
+      <c r="B64" s="166"/>
+      <c r="C64" s="184"/>
+      <c r="D64" s="167" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="162"/>
-      <c r="B65" s="162"/>
-      <c r="C65" s="182"/>
-      <c r="D65" s="164"/>
+      <c r="A65" s="166"/>
+      <c r="B65" s="166"/>
+      <c r="C65" s="184"/>
+      <c r="D65" s="167"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="162"/>
-      <c r="B66" s="162"/>
-      <c r="C66" s="182"/>
-      <c r="D66" s="164"/>
+      <c r="A66" s="166"/>
+      <c r="B66" s="166"/>
+      <c r="C66" s="184"/>
+      <c r="D66" s="167"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="162"/>
-      <c r="B67" s="162"/>
-      <c r="C67" s="182"/>
-      <c r="D67" s="164"/>
+      <c r="A67" s="166"/>
+      <c r="B67" s="166"/>
+      <c r="C67" s="184"/>
+      <c r="D67" s="167"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31470,23 +31473,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31503,6 +31489,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31511,10 +31514,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D152"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31548,10 +31551,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="207" t="s">
+      <c r="A3" s="204" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="208" t="s">
+      <c r="B3" s="205" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="112" t="s">
@@ -31562,8 +31565,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="207"/>
-      <c r="B4" s="208"/>
+      <c r="A4" s="204"/>
+      <c r="B4" s="205"/>
       <c r="C4" s="112" t="s">
         <v>347</v>
       </c>
@@ -31572,8 +31575,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="207"/>
-      <c r="B5" s="208"/>
+      <c r="A5" s="204"/>
+      <c r="B5" s="205"/>
       <c r="C5" s="112" t="s">
         <v>343</v>
       </c>
@@ -31590,10 +31593,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="161" t="s">
+      <c r="A7" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="181" t="s">
+      <c r="B7" s="191" t="s">
         <v>234</v>
       </c>
       <c r="C7" s="58"/>
@@ -31602,8 +31605,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="161"/>
-      <c r="B8" s="181"/>
+      <c r="A8" s="157"/>
+      <c r="B8" s="191"/>
       <c r="C8" s="104" t="s">
         <v>235</v>
       </c>
@@ -31666,10 +31669,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="161" t="s">
+      <c r="A13" s="157" t="s">
         <v>275</v>
       </c>
-      <c r="B13" s="181" t="s">
+      <c r="B13" s="191" t="s">
         <v>234</v>
       </c>
       <c r="C13" s="58"/>
@@ -31678,16 +31681,16 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="161"/>
-      <c r="B14" s="181"/>
+      <c r="A14" s="157"/>
+      <c r="B14" s="191"/>
       <c r="C14" s="58"/>
       <c r="D14" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="161"/>
-      <c r="B15" s="181"/>
+      <c r="A15" s="157"/>
+      <c r="B15" s="191"/>
       <c r="C15" s="108" t="s">
         <v>325</v>
       </c>
@@ -31696,8 +31699,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="161"/>
-      <c r="B16" s="181"/>
+      <c r="A16" s="157"/>
+      <c r="B16" s="191"/>
       <c r="C16" s="136" t="s">
         <v>404</v>
       </c>
@@ -31718,10 +31721,10 @@
       <c r="D17" s="58"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="209" t="s">
+      <c r="A18" s="206" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="194" t="s">
+      <c r="B18" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C18" s="58"/>
@@ -31730,8 +31733,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="210"/>
-      <c r="B19" s="201"/>
+      <c r="A19" s="207"/>
+      <c r="B19" s="200"/>
       <c r="C19" s="118" t="s">
         <v>361</v>
       </c>
@@ -31740,8 +31743,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="210"/>
-      <c r="B20" s="201"/>
+      <c r="A20" s="207"/>
+      <c r="B20" s="200"/>
       <c r="C20" s="118" t="s">
         <v>359</v>
       </c>
@@ -31750,8 +31753,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="210"/>
-      <c r="B21" s="201"/>
+      <c r="A21" s="207"/>
+      <c r="B21" s="200"/>
       <c r="C21" s="124" t="s">
         <v>367</v>
       </c>
@@ -31760,8 +31763,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="210"/>
-      <c r="B22" s="201"/>
+      <c r="A22" s="207"/>
+      <c r="B22" s="200"/>
       <c r="C22" s="131" t="s">
         <v>359</v>
       </c>
@@ -31770,8 +31773,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="210"/>
-      <c r="B23" s="201"/>
+      <c r="A23" s="207"/>
+      <c r="B23" s="200"/>
       <c r="C23" s="135" t="s">
         <v>371</v>
       </c>
@@ -31780,8 +31783,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="211"/>
-      <c r="B24" s="195"/>
+      <c r="A24" s="208"/>
+      <c r="B24" s="196"/>
       <c r="C24" s="135" t="s">
         <v>359</v>
       </c>
@@ -31816,10 +31819,10 @@
       <c r="D26" s="98"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="205" t="s">
+      <c r="A27" s="192" t="s">
         <v>369</v>
       </c>
-      <c r="B27" s="194" t="s">
+      <c r="B27" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C27" s="136" t="s">
@@ -31828,8 +31831,8 @@
       <c r="D27" s="98"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="212"/>
-      <c r="B28" s="195"/>
+      <c r="A28" s="194"/>
+      <c r="B28" s="196"/>
       <c r="C28" s="136" t="s">
         <v>404</v>
       </c>
@@ -31846,10 +31849,10 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="205" t="s">
+      <c r="A30" s="192" t="s">
         <v>237</v>
       </c>
-      <c r="B30" s="194" t="s">
+      <c r="B30" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C30" s="58"/>
@@ -31858,24 +31861,24 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="206"/>
-      <c r="B31" s="201"/>
+      <c r="A31" s="193"/>
+      <c r="B31" s="200"/>
       <c r="C31" s="58"/>
       <c r="D31" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="206"/>
-      <c r="B32" s="201"/>
+      <c r="A32" s="193"/>
+      <c r="B32" s="200"/>
       <c r="C32" s="58"/>
       <c r="D32" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="206"/>
-      <c r="B33" s="201"/>
+      <c r="A33" s="193"/>
+      <c r="B33" s="200"/>
       <c r="C33" s="58" t="s">
         <v>300</v>
       </c>
@@ -31884,8 +31887,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="206"/>
-      <c r="B34" s="201"/>
+      <c r="A34" s="193"/>
+      <c r="B34" s="200"/>
       <c r="C34" s="58" t="s">
         <v>328</v>
       </c>
@@ -31894,8 +31897,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="212"/>
-      <c r="B35" s="195"/>
+      <c r="A35" s="194"/>
+      <c r="B35" s="196"/>
       <c r="C35" s="58" t="s">
         <v>373</v>
       </c>
@@ -31904,10 +31907,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="165" t="s">
+      <c r="A36" s="168" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="194" t="s">
+      <c r="B36" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C36" s="58" t="s">
@@ -31918,16 +31921,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="166"/>
-      <c r="B37" s="201"/>
+      <c r="A37" s="169"/>
+      <c r="B37" s="200"/>
       <c r="C37" s="58"/>
       <c r="D37" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="166"/>
-      <c r="B38" s="201"/>
+      <c r="A38" s="169"/>
+      <c r="B38" s="200"/>
       <c r="C38" s="106" t="s">
         <v>329</v>
       </c>
@@ -31936,8 +31939,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="166"/>
-      <c r="B39" s="201"/>
+      <c r="A39" s="169"/>
+      <c r="B39" s="200"/>
       <c r="C39" s="106" t="s">
         <v>359</v>
       </c>
@@ -31946,8 +31949,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="166"/>
-      <c r="B40" s="201"/>
+      <c r="A40" s="169"/>
+      <c r="B40" s="200"/>
       <c r="C40" s="106" t="s">
         <v>367</v>
       </c>
@@ -31956,8 +31959,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="166"/>
-      <c r="B41" s="201"/>
+      <c r="A41" s="169"/>
+      <c r="B41" s="200"/>
       <c r="C41" s="106" t="s">
         <v>371</v>
       </c>
@@ -31966,8 +31969,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="166"/>
-      <c r="B42" s="201"/>
+      <c r="A42" s="169"/>
+      <c r="B42" s="200"/>
       <c r="C42" s="106" t="s">
         <v>381</v>
       </c>
@@ -31976,8 +31979,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="167"/>
-      <c r="B43" s="195"/>
+      <c r="A43" s="170"/>
+      <c r="B43" s="196"/>
       <c r="C43" s="96" t="s">
         <v>359</v>
       </c>
@@ -31986,13 +31989,13 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="172" t="s">
+      <c r="A44" s="162" t="s">
         <v>222</v>
       </c>
-      <c r="B44" s="194" t="s">
+      <c r="B44" s="195" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="216" t="s">
+      <c r="C44" s="202" t="s">
         <v>239</v>
       </c>
       <c r="D44" s="101" t="s">
@@ -32000,17 +32003,17 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="200"/>
-      <c r="B45" s="201"/>
-      <c r="C45" s="217"/>
+      <c r="A45" s="201"/>
+      <c r="B45" s="200"/>
+      <c r="C45" s="203"/>
       <c r="D45" s="98" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="200"/>
-      <c r="B46" s="201"/>
-      <c r="C46" s="199" t="s">
+      <c r="A46" s="201"/>
+      <c r="B46" s="200"/>
+      <c r="C46" s="209" t="s">
         <v>240</v>
       </c>
       <c r="D46" s="58" t="s">
@@ -32018,16 +32021,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="200"/>
-      <c r="B47" s="201"/>
-      <c r="C47" s="199"/>
+      <c r="A47" s="201"/>
+      <c r="B47" s="200"/>
+      <c r="C47" s="209"/>
       <c r="D47" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="200"/>
-      <c r="B48" s="201"/>
+      <c r="A48" s="201"/>
+      <c r="B48" s="200"/>
       <c r="C48" s="103" t="s">
         <v>307</v>
       </c>
@@ -32036,8 +32039,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="200"/>
-      <c r="B49" s="201"/>
+      <c r="A49" s="201"/>
+      <c r="B49" s="200"/>
       <c r="C49" s="103">
         <v>2.1</v>
       </c>
@@ -32046,8 +32049,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="200"/>
-      <c r="B50" s="201"/>
+      <c r="A50" s="201"/>
+      <c r="B50" s="200"/>
       <c r="C50" s="103" t="s">
         <v>239</v>
       </c>
@@ -32056,8 +32059,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="200"/>
-      <c r="B51" s="201"/>
+      <c r="A51" s="201"/>
+      <c r="B51" s="200"/>
       <c r="C51" s="114" t="s">
         <v>239</v>
       </c>
@@ -32066,8 +32069,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="200"/>
-      <c r="B52" s="201"/>
+      <c r="A52" s="201"/>
+      <c r="B52" s="200"/>
       <c r="C52" s="128" t="s">
         <v>239</v>
       </c>
@@ -32076,8 +32079,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="200"/>
-      <c r="B53" s="201"/>
+      <c r="A53" s="201"/>
+      <c r="B53" s="200"/>
       <c r="C53" s="134" t="s">
         <v>378</v>
       </c>
@@ -32086,8 +32089,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="200"/>
-      <c r="B54" s="201"/>
+      <c r="A54" s="201"/>
+      <c r="B54" s="200"/>
       <c r="C54" s="136">
         <v>2.1</v>
       </c>
@@ -32096,8 +32099,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="200"/>
-      <c r="B55" s="201"/>
+      <c r="A55" s="201"/>
+      <c r="B55" s="200"/>
       <c r="C55" s="136" t="s">
         <v>239</v>
       </c>
@@ -32106,8 +32109,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="200"/>
-      <c r="B56" s="201"/>
+      <c r="A56" s="201"/>
+      <c r="B56" s="200"/>
       <c r="C56" s="141" t="s">
         <v>239</v>
       </c>
@@ -32116,10 +32119,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="202" t="s">
+      <c r="A57" s="210" t="s">
         <v>296</v>
       </c>
-      <c r="B57" s="194" t="s">
+      <c r="B57" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -32130,8 +32133,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="203"/>
-      <c r="B58" s="201"/>
+      <c r="A58" s="211"/>
+      <c r="B58" s="200"/>
       <c r="C58" s="61" t="s">
         <v>281</v>
       </c>
@@ -32140,8 +32143,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="204"/>
-      <c r="B59" s="195"/>
+      <c r="A59" s="212"/>
+      <c r="B59" s="196"/>
       <c r="C59" s="58" t="s">
         <v>350</v>
       </c>
@@ -32150,10 +32153,10 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="205" t="s">
+      <c r="A60" s="192" t="s">
         <v>370</v>
       </c>
-      <c r="B60" s="194" t="s">
+      <c r="B60" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C60" s="128" t="s">
@@ -32162,8 +32165,8 @@
       <c r="D60" s="58"/>
     </row>
     <row r="61" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="206"/>
-      <c r="B61" s="201"/>
+      <c r="A61" s="193"/>
+      <c r="B61" s="200"/>
       <c r="C61" s="131" t="s">
         <v>378</v>
       </c>
@@ -32172,8 +32175,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="206"/>
-      <c r="B62" s="201"/>
+      <c r="A62" s="193"/>
+      <c r="B62" s="200"/>
       <c r="C62" s="136">
         <v>2.1</v>
       </c>
@@ -32182,8 +32185,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="206"/>
-      <c r="B63" s="201"/>
+      <c r="A63" s="193"/>
+      <c r="B63" s="200"/>
       <c r="C63" s="136" t="s">
         <v>240</v>
       </c>
@@ -32192,8 +32195,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="206"/>
-      <c r="B64" s="201"/>
+      <c r="A64" s="193"/>
+      <c r="B64" s="200"/>
       <c r="C64" s="133" t="s">
         <v>239</v>
       </c>
@@ -32222,10 +32225,10 @@
       <c r="D66" s="98"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="172" t="s">
+      <c r="A67" s="162" t="s">
         <v>260</v>
       </c>
-      <c r="B67" s="194" t="s">
+      <c r="B67" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C67" s="58"/>
@@ -32234,26 +32237,26 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="200"/>
-      <c r="B68" s="201"/>
+      <c r="A68" s="201"/>
+      <c r="B68" s="200"/>
       <c r="C68" s="58"/>
       <c r="D68" s="58" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="200"/>
-      <c r="B69" s="201"/>
+      <c r="A69" s="201"/>
+      <c r="B69" s="200"/>
       <c r="C69" s="58"/>
       <c r="D69" s="98" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="161" t="s">
+      <c r="A70" s="157" t="s">
         <v>334</v>
       </c>
-      <c r="B70" s="181" t="s">
+      <c r="B70" s="191" t="s">
         <v>234</v>
       </c>
       <c r="C70" s="79" t="s">
@@ -32264,8 +32267,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="161"/>
-      <c r="B71" s="181"/>
+      <c r="A71" s="157"/>
+      <c r="B71" s="191"/>
       <c r="C71" s="58" t="s">
         <v>411</v>
       </c>
@@ -32274,38 +32277,38 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="161"/>
-      <c r="B72" s="181"/>
+      <c r="A72" s="157"/>
+      <c r="B72" s="191"/>
       <c r="C72" s="140" t="s">
         <v>414</v>
       </c>
-      <c r="D72" s="205" t="s">
+      <c r="D72" s="192" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="161"/>
-      <c r="B73" s="181"/>
+      <c r="A73" s="157"/>
+      <c r="B73" s="191"/>
       <c r="C73" s="140" t="s">
         <v>415</v>
       </c>
-      <c r="D73" s="206"/>
+      <c r="D73" s="193"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="161"/>
-      <c r="B74" s="181"/>
+      <c r="A74" s="157"/>
+      <c r="B74" s="191"/>
       <c r="C74" s="140" t="s">
         <v>416</v>
       </c>
-      <c r="D74" s="206"/>
+      <c r="D74" s="193"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="161"/>
-      <c r="B75" s="181"/>
+      <c r="A75" s="157"/>
+      <c r="B75" s="191"/>
       <c r="C75" s="140" t="s">
         <v>417</v>
       </c>
-      <c r="D75" s="212"/>
+      <c r="D75" s="194"/>
     </row>
     <row r="76" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="96" t="s">
@@ -32322,10 +32325,10 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="202" t="s">
+      <c r="A77" s="210" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="194" t="s">
+      <c r="B77" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C77" s="58" t="s">
@@ -32336,8 +32339,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="203"/>
-      <c r="B78" s="201"/>
+      <c r="A78" s="211"/>
+      <c r="B78" s="200"/>
       <c r="C78" s="58" t="s">
         <v>270</v>
       </c>
@@ -32346,8 +32349,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="203"/>
-      <c r="B79" s="201"/>
+      <c r="A79" s="211"/>
+      <c r="B79" s="200"/>
       <c r="C79" s="58" t="s">
         <v>269</v>
       </c>
@@ -32356,8 +32359,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="203"/>
-      <c r="B80" s="201"/>
+      <c r="A80" s="211"/>
+      <c r="B80" s="200"/>
       <c r="C80" s="98" t="s">
         <v>277</v>
       </c>
@@ -32366,8 +32369,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="203"/>
-      <c r="B81" s="201"/>
+      <c r="A81" s="211"/>
+      <c r="B81" s="200"/>
       <c r="C81" s="58" t="s">
         <v>282</v>
       </c>
@@ -32376,8 +32379,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="203"/>
-      <c r="B82" s="201"/>
+      <c r="A82" s="211"/>
+      <c r="B82" s="200"/>
       <c r="C82" s="58" t="s">
         <v>283</v>
       </c>
@@ -32386,8 +32389,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="203"/>
-      <c r="B83" s="201"/>
+      <c r="A83" s="211"/>
+      <c r="B83" s="200"/>
       <c r="C83" s="98" t="s">
         <v>288</v>
       </c>
@@ -32396,8 +32399,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="203"/>
-      <c r="B84" s="201"/>
+      <c r="A84" s="211"/>
+      <c r="B84" s="200"/>
       <c r="C84" s="98" t="s">
         <v>302</v>
       </c>
@@ -32406,8 +32409,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="203"/>
-      <c r="B85" s="201"/>
+      <c r="A85" s="211"/>
+      <c r="B85" s="200"/>
       <c r="C85" s="98" t="s">
         <v>289</v>
       </c>
@@ -32416,8 +32419,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="203"/>
-      <c r="B86" s="201"/>
+      <c r="A86" s="211"/>
+      <c r="B86" s="200"/>
       <c r="C86" s="105" t="s">
         <v>244</v>
       </c>
@@ -32426,8 +32429,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="203"/>
-      <c r="B87" s="201"/>
+      <c r="A87" s="211"/>
+      <c r="B87" s="200"/>
       <c r="C87" s="106" t="s">
         <v>311</v>
       </c>
@@ -32436,8 +32439,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="203"/>
-      <c r="B88" s="201"/>
+      <c r="A88" s="211"/>
+      <c r="B88" s="200"/>
       <c r="C88" s="58" t="s">
         <v>312</v>
       </c>
@@ -32446,8 +32449,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="203"/>
-      <c r="B89" s="201"/>
+      <c r="A89" s="211"/>
+      <c r="B89" s="200"/>
       <c r="C89" s="98" t="s">
         <v>313</v>
       </c>
@@ -32456,8 +32459,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="203"/>
-      <c r="B90" s="201"/>
+      <c r="A90" s="211"/>
+      <c r="B90" s="200"/>
       <c r="C90" s="98" t="s">
         <v>315</v>
       </c>
@@ -32466,8 +32469,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="203"/>
-      <c r="B91" s="201"/>
+      <c r="A91" s="211"/>
+      <c r="B91" s="200"/>
       <c r="C91" s="98" t="s">
         <v>268</v>
       </c>
@@ -32476,8 +32479,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="203"/>
-      <c r="B92" s="201"/>
+      <c r="A92" s="211"/>
+      <c r="B92" s="200"/>
       <c r="C92" s="58" t="s">
         <v>318</v>
       </c>
@@ -32486,8 +32489,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="203"/>
-      <c r="B93" s="201"/>
+      <c r="A93" s="211"/>
+      <c r="B93" s="200"/>
       <c r="C93" s="98" t="s">
         <v>283</v>
       </c>
@@ -32496,8 +32499,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="203"/>
-      <c r="B94" s="201"/>
+      <c r="A94" s="211"/>
+      <c r="B94" s="200"/>
       <c r="C94" s="98" t="s">
         <v>319</v>
       </c>
@@ -32506,16 +32509,16 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="203"/>
-      <c r="B95" s="201"/>
+      <c r="A95" s="211"/>
+      <c r="B95" s="200"/>
       <c r="C95" s="58"/>
       <c r="D95" s="107" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="203"/>
-      <c r="B96" s="201"/>
+      <c r="A96" s="211"/>
+      <c r="B96" s="200"/>
       <c r="C96" s="98" t="s">
         <v>322</v>
       </c>
@@ -32524,8 +32527,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="203"/>
-      <c r="B97" s="201"/>
+      <c r="A97" s="211"/>
+      <c r="B97" s="200"/>
       <c r="C97" s="98" t="s">
         <v>268</v>
       </c>
@@ -32534,8 +32537,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="203"/>
-      <c r="B98" s="201"/>
+      <c r="A98" s="211"/>
+      <c r="B98" s="200"/>
       <c r="C98" s="98" t="s">
         <v>339</v>
       </c>
@@ -32544,8 +32547,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="203"/>
-      <c r="B99" s="201"/>
+      <c r="A99" s="211"/>
+      <c r="B99" s="200"/>
       <c r="C99" s="98" t="s">
         <v>340</v>
       </c>
@@ -32554,8 +32557,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="203"/>
-      <c r="B100" s="201"/>
+      <c r="A100" s="211"/>
+      <c r="B100" s="200"/>
       <c r="C100" s="98" t="s">
         <v>324</v>
       </c>
@@ -32564,8 +32567,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="203"/>
-      <c r="B101" s="201"/>
+      <c r="A101" s="211"/>
+      <c r="B101" s="200"/>
       <c r="C101" s="113" t="s">
         <v>345</v>
       </c>
@@ -32574,8 +32577,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="203"/>
-      <c r="B102" s="201"/>
+      <c r="A102" s="211"/>
+      <c r="B102" s="200"/>
       <c r="C102" s="98" t="s">
         <v>338</v>
       </c>
@@ -32584,8 +32587,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="203"/>
-      <c r="B103" s="201"/>
+      <c r="A103" s="211"/>
+      <c r="B103" s="200"/>
       <c r="C103" s="98" t="s">
         <v>353</v>
       </c>
@@ -32594,8 +32597,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="203"/>
-      <c r="B104" s="201"/>
+      <c r="A104" s="211"/>
+      <c r="B104" s="200"/>
       <c r="C104" s="117" t="s">
         <v>356</v>
       </c>
@@ -32604,8 +32607,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="203"/>
-      <c r="B105" s="201"/>
+      <c r="A105" s="211"/>
+      <c r="B105" s="200"/>
       <c r="C105" s="98" t="s">
         <v>357</v>
       </c>
@@ -32614,8 +32617,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="203"/>
-      <c r="B106" s="201"/>
+      <c r="A106" s="211"/>
+      <c r="B106" s="200"/>
       <c r="C106" s="98" t="s">
         <v>358</v>
       </c>
@@ -32624,8 +32627,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="203"/>
-      <c r="B107" s="201"/>
+      <c r="A107" s="211"/>
+      <c r="B107" s="200"/>
       <c r="C107" s="98" t="s">
         <v>364</v>
       </c>
@@ -32634,8 +32637,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="203"/>
-      <c r="B108" s="201"/>
+      <c r="A108" s="211"/>
+      <c r="B108" s="200"/>
       <c r="C108" s="98" t="s">
         <v>366</v>
       </c>
@@ -32644,8 +32647,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="203"/>
-      <c r="B109" s="201"/>
+      <c r="A109" s="211"/>
+      <c r="B109" s="200"/>
       <c r="C109" s="98" t="s">
         <v>372</v>
       </c>
@@ -32654,8 +32657,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="203"/>
-      <c r="B110" s="201"/>
+      <c r="A110" s="211"/>
+      <c r="B110" s="200"/>
       <c r="C110" s="98" t="s">
         <v>364</v>
       </c>
@@ -32664,8 +32667,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="203"/>
-      <c r="B111" s="201"/>
+      <c r="A111" s="211"/>
+      <c r="B111" s="200"/>
       <c r="C111" s="113" t="s">
         <v>385</v>
       </c>
@@ -32674,8 +32677,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="203"/>
-      <c r="B112" s="201"/>
+      <c r="A112" s="211"/>
+      <c r="B112" s="200"/>
       <c r="C112" s="58" t="s">
         <v>389</v>
       </c>
@@ -32684,8 +32687,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="203"/>
-      <c r="B113" s="201"/>
+      <c r="A113" s="211"/>
+      <c r="B113" s="200"/>
       <c r="C113" s="58" t="s">
         <v>392</v>
       </c>
@@ -32694,8 +32697,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="203"/>
-      <c r="B114" s="201"/>
+      <c r="A114" s="211"/>
+      <c r="B114" s="200"/>
       <c r="C114" s="58" t="s">
         <v>393</v>
       </c>
@@ -32704,8 +32707,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="203"/>
-      <c r="B115" s="201"/>
+      <c r="A115" s="211"/>
+      <c r="B115" s="200"/>
       <c r="C115" s="58" t="s">
         <v>394</v>
       </c>
@@ -32714,8 +32717,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="203"/>
-      <c r="B116" s="201"/>
+      <c r="A116" s="211"/>
+      <c r="B116" s="200"/>
       <c r="C116" s="58" t="s">
         <v>395</v>
       </c>
@@ -32724,8 +32727,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="203"/>
-      <c r="B117" s="201"/>
+      <c r="A117" s="211"/>
+      <c r="B117" s="200"/>
       <c r="C117" s="58" t="s">
         <v>396</v>
       </c>
@@ -32734,8 +32737,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="203"/>
-      <c r="B118" s="201"/>
+      <c r="A118" s="211"/>
+      <c r="B118" s="200"/>
       <c r="C118" s="58" t="s">
         <v>399</v>
       </c>
@@ -32744,8 +32747,8 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="203"/>
-      <c r="B119" s="201"/>
+      <c r="A119" s="211"/>
+      <c r="B119" s="200"/>
       <c r="C119" s="58" t="s">
         <v>409</v>
       </c>
@@ -32754,8 +32757,8 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="204"/>
-      <c r="B120" s="195"/>
+      <c r="A120" s="212"/>
+      <c r="B120" s="196"/>
       <c r="C120" s="58" t="s">
         <v>410</v>
       </c>
@@ -32800,10 +32803,10 @@
       <c r="D123" s="44"/>
     </row>
     <row r="124" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="172" t="s">
+      <c r="A124" s="162" t="s">
         <v>84</v>
       </c>
-      <c r="B124" s="194" t="s">
+      <c r="B124" s="195" t="s">
         <v>234</v>
       </c>
       <c r="C124" s="58"/>
@@ -32812,8 +32815,8 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="200"/>
-      <c r="B125" s="201"/>
+      <c r="A125" s="201"/>
+      <c r="B125" s="200"/>
       <c r="C125" s="104" t="s">
         <v>246</v>
       </c>
@@ -32822,8 +32825,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="200"/>
-      <c r="B126" s="201"/>
+      <c r="A126" s="201"/>
+      <c r="B126" s="200"/>
       <c r="C126" s="104">
         <v>10.1</v>
       </c>
@@ -32832,8 +32835,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="200"/>
-      <c r="B127" s="201"/>
+      <c r="A127" s="201"/>
+      <c r="B127" s="200"/>
       <c r="C127" s="104">
         <v>10.199999999999999</v>
       </c>
@@ -32842,8 +32845,8 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="200"/>
-      <c r="B128" s="201"/>
+      <c r="A128" s="201"/>
+      <c r="B128" s="200"/>
       <c r="C128" s="109" t="s">
         <v>293</v>
       </c>
@@ -32852,8 +32855,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="173"/>
-      <c r="B129" s="195"/>
+      <c r="A129" s="201"/>
+      <c r="B129" s="200"/>
       <c r="C129" s="109" t="s">
         <v>375</v>
       </c>
@@ -32862,273 +32865,267 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="172" t="s">
+      <c r="A130" s="163"/>
+      <c r="B130" s="196"/>
+      <c r="C130" s="109" t="s">
+        <v>117</v>
+      </c>
+      <c r="D130" s="99" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="162" t="s">
         <v>247</v>
       </c>
-      <c r="B130" s="194" t="s">
+      <c r="B131" s="195" t="s">
         <v>234</v>
       </c>
-      <c r="C130" s="181"/>
-      <c r="D130" s="196" t="s">
+      <c r="C131" s="191"/>
+      <c r="D131" s="215" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="173"/>
-      <c r="B131" s="195"/>
-      <c r="C131" s="181"/>
-      <c r="D131" s="196"/>
-    </row>
-    <row r="132" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="121" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="163"/>
+      <c r="B132" s="196"/>
+      <c r="C132" s="191"/>
+      <c r="D132" s="215"/>
+    </row>
+    <row r="133" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="121" t="s">
         <v>262</v>
       </c>
-      <c r="B132" s="123" t="s">
+      <c r="B133" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C132" s="104" t="s">
+      <c r="C133" s="104" t="s">
         <v>250</v>
       </c>
-      <c r="D132" s="98" t="s">
+      <c r="D133" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="95" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B133" s="39"/>
-      <c r="C133" s="97"/>
-      <c r="D133" s="97"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="96" t="s">
+      <c r="B134" s="39"/>
+      <c r="C134" s="97"/>
+      <c r="D134" s="97"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="B134" s="123" t="s">
+      <c r="B135" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C134" s="110" t="s">
+      <c r="C135" s="110" t="s">
         <v>265</v>
       </c>
-      <c r="D134" s="58" t="s">
+      <c r="D135" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="172" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="162" t="s">
         <v>285</v>
       </c>
-      <c r="B135" s="194" t="s">
+      <c r="B136" s="195" t="s">
         <v>234</v>
       </c>
-      <c r="C135" s="99" t="s">
+      <c r="C136" s="99" t="s">
         <v>295</v>
       </c>
-      <c r="D135" s="58" t="s">
+      <c r="D136" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="200"/>
-      <c r="B136" s="201"/>
-      <c r="C136" s="58" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="201"/>
+      <c r="B137" s="200"/>
+      <c r="C137" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D136" s="98" t="s">
+      <c r="D137" s="98" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="173"/>
-      <c r="B137" s="195"/>
-      <c r="C137" s="110" t="s">
+    <row r="138" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="163"/>
+      <c r="B138" s="196"/>
+      <c r="C138" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="D137" s="58" t="s">
+      <c r="D138" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="97" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="B138" s="97"/>
-      <c r="C138" s="97"/>
-      <c r="D138" s="97"/>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="213" t="s">
+      <c r="B139" s="97"/>
+      <c r="C139" s="97"/>
+      <c r="D139" s="97"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="197" t="s">
         <v>58</v>
       </c>
-      <c r="B139" s="194" t="s">
+      <c r="B140" s="195" t="s">
         <v>271</v>
       </c>
-      <c r="C139" s="110" t="s">
-        <v>265</v>
-      </c>
-      <c r="D139" s="58" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="214"/>
-      <c r="B140" s="201"/>
       <c r="C140" s="110" t="s">
         <v>265</v>
       </c>
       <c r="D140" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="198"/>
+      <c r="B141" s="200"/>
+      <c r="C141" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="D141" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="215"/>
-      <c r="B141" s="195"/>
-      <c r="C141" s="58"/>
-      <c r="D141" s="58" t="s">
+    <row r="142" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="199"/>
+      <c r="B142" s="196"/>
+      <c r="C142" s="58"/>
+      <c r="D142" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A142" s="192" t="s">
+    <row r="143" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A143" s="213" t="s">
         <v>59</v>
       </c>
-      <c r="B142" s="194" t="s">
+      <c r="B143" s="195" t="s">
         <v>271</v>
       </c>
-      <c r="C142" s="61" t="s">
+      <c r="C143" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D142" s="58" t="s">
+      <c r="D143" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="193"/>
-      <c r="B143" s="195"/>
-      <c r="C143" s="61"/>
-      <c r="D143" s="58" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="214"/>
+      <c r="B144" s="196"/>
+      <c r="C144" s="61"/>
+      <c r="D144" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A144" s="197" t="s">
+    <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="216" t="s">
         <v>291</v>
       </c>
-      <c r="B144" s="194" t="s">
+      <c r="B145" s="195" t="s">
         <v>271</v>
       </c>
-      <c r="C144" s="61"/>
-      <c r="D144" s="61" t="s">
+      <c r="C145" s="61"/>
+      <c r="D145" s="61" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="198"/>
-      <c r="B145" s="195"/>
-      <c r="C145" s="58"/>
-      <c r="D145" s="58" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="217"/>
+      <c r="B146" s="196"/>
+      <c r="C146" s="58"/>
+      <c r="D146" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A146" s="192" t="s">
+    <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A147" s="213" t="s">
         <v>60</v>
       </c>
-      <c r="B146" s="194" t="s">
+      <c r="B147" s="195" t="s">
         <v>271</v>
       </c>
-      <c r="C146" s="61" t="s">
+      <c r="C147" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D146" s="58" t="s">
+      <c r="D147" s="58" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="193"/>
-      <c r="B147" s="195"/>
-      <c r="C147" s="58"/>
-      <c r="D147" s="58" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="214"/>
+      <c r="B148" s="196"/>
+      <c r="C148" s="58"/>
+      <c r="D148" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="97" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="97" t="s">
         <v>273</v>
       </c>
-      <c r="B148" s="97"/>
-      <c r="C148" s="97"/>
-      <c r="D148" s="97"/>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="58"/>
-      <c r="B149" s="123" t="s">
+      <c r="B149" s="97"/>
+      <c r="C149" s="97"/>
+      <c r="D149" s="97"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="58"/>
+      <c r="B150" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C149" s="58" t="s">
+      <c r="C150" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D149" s="98" t="s">
+      <c r="D150" s="98" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="97" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="B150" s="97"/>
-      <c r="C150" s="97"/>
-      <c r="D150" s="97"/>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="58"/>
-      <c r="B151" s="137" t="s">
-        <v>234</v>
-      </c>
-      <c r="C151" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D151" s="98" t="s">
-        <v>274</v>
-      </c>
+      <c r="B151" s="97"/>
+      <c r="C151" s="97"/>
+      <c r="D151" s="97"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="58"/>
-      <c r="B152" s="123"/>
+      <c r="B152" s="137" t="s">
+        <v>234</v>
+      </c>
       <c r="C152" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D152" s="98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="58"/>
+      <c r="B153" s="123"/>
+      <c r="C153" s="58" t="s">
         <v>401</v>
       </c>
-      <c r="D152" s="98" t="s">
+      <c r="D153" s="98" t="s">
         <v>402</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A139:A141"/>
-    <mergeCell ref="B139:B141"/>
-    <mergeCell ref="A124:A129"/>
-    <mergeCell ref="B124:B129"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A135:A137"/>
-    <mergeCell ref="B135:B137"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="B36:B43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="A145:A146"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="C131:C132"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="A67:A69"/>
     <mergeCell ref="B67:B69"/>
@@ -33142,14 +33139,30 @@
     <mergeCell ref="B70:B75"/>
     <mergeCell ref="A60:A64"/>
     <mergeCell ref="B60:B64"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A140:A142"/>
+    <mergeCell ref="B140:B142"/>
+    <mergeCell ref="A124:A130"/>
+    <mergeCell ref="B124:B130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="A136:A138"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="B36:B43"/>
+    <mergeCell ref="C44:C45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added line item correction doc
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="427">
   <si>
     <t>Document</t>
   </si>
@@ -3131,6 +3131,24 @@
   </si>
   <si>
     <t>Added description on Previous Line Item ID</t>
+  </si>
+  <si>
+    <t>Line Item Correction Rules</t>
+  </si>
+  <si>
+    <t>Section 4.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment ID </t>
+  </si>
+  <si>
+    <t>updated description</t>
+  </si>
+  <si>
+    <t>Added link to published document</t>
   </si>
 </sst>
 </file>
@@ -3732,7 +3750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -4108,6 +4126,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4740,12 +4764,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="144" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="144"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="146"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4768,12 +4792,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="142" t="s">
+      <c r="A4" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="143"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="144"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="146"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4813,10 +4837,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="145" t="s">
+      <c r="A7" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="148">
+      <c r="B7" s="150">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4830,8 +4854,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="146"/>
-      <c r="B8" s="149"/>
+      <c r="A8" s="148"/>
+      <c r="B8" s="151"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4843,8 +4867,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="146"/>
-      <c r="B9" s="149"/>
+      <c r="A9" s="148"/>
+      <c r="B9" s="151"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4856,8 +4880,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="146"/>
-      <c r="B10" s="149"/>
+      <c r="A10" s="148"/>
+      <c r="B10" s="151"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4869,8 +4893,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="146"/>
-      <c r="B11" s="149"/>
+      <c r="A11" s="148"/>
+      <c r="B11" s="151"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4882,8 +4906,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="147"/>
-      <c r="B12" s="150"/>
+      <c r="A12" s="149"/>
+      <c r="B12" s="152"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4895,10 +4919,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="153" t="s">
+      <c r="A13" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="148">
+      <c r="B13" s="150">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4912,8 +4936,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="154"/>
-      <c r="B14" s="150"/>
+      <c r="A14" s="156"/>
+      <c r="B14" s="152"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -4959,12 +4983,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="142" t="s">
+      <c r="A17" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="143"/>
-      <c r="C17" s="143"/>
-      <c r="D17" s="144"/>
+      <c r="B17" s="145"/>
+      <c r="C17" s="145"/>
+      <c r="D17" s="146"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5004,21 +5028,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="142" t="s">
+      <c r="A20" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="143"/>
-      <c r="C20" s="143"/>
-      <c r="D20" s="144"/>
+      <c r="B20" s="145"/>
+      <c r="C20" s="145"/>
+      <c r="D20" s="146"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="155" t="s">
+      <c r="A21" s="157" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="152">
+      <c r="B21" s="154">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -5032,8 +5056,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="156"/>
-      <c r="B22" s="150"/>
+      <c r="A22" s="158"/>
+      <c r="B22" s="152"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -5056,18 +5080,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="142" t="s">
+      <c r="A24" s="144" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="143"/>
-      <c r="C24" s="143"/>
-      <c r="D24" s="144"/>
+      <c r="B24" s="145"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="146"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="151" t="s">
+      <c r="A25" s="153" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="152">
+      <c r="B25" s="154">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5081,8 +5105,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="146"/>
-      <c r="B26" s="149"/>
+      <c r="A26" s="148"/>
+      <c r="B26" s="151"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -5094,8 +5118,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="146"/>
-      <c r="B27" s="149"/>
+      <c r="A27" s="148"/>
+      <c r="B27" s="151"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -5107,8 +5131,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="146"/>
-      <c r="B28" s="149"/>
+      <c r="A28" s="148"/>
+      <c r="B28" s="151"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -5120,8 +5144,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="146"/>
-      <c r="B29" s="149"/>
+      <c r="A29" s="148"/>
+      <c r="B29" s="151"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -5133,8 +5157,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="146"/>
-      <c r="B30" s="149"/>
+      <c r="A30" s="148"/>
+      <c r="B30" s="151"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -5146,8 +5170,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="146"/>
-      <c r="B31" s="149"/>
+      <c r="A31" s="148"/>
+      <c r="B31" s="151"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -5159,8 +5183,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="147"/>
-      <c r="B32" s="150"/>
+      <c r="A32" s="149"/>
+      <c r="B32" s="152"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5284,12 +5308,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="142" t="s">
+      <c r="A41" s="144" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="143"/>
-      <c r="C41" s="143"/>
-      <c r="D41" s="144"/>
+      <c r="B41" s="145"/>
+      <c r="C41" s="145"/>
+      <c r="D41" s="146"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5469,10 +5493,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="172" t="s">
+      <c r="A7" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="171" t="s">
+      <c r="B7" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5483,8 +5507,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="172"/>
-      <c r="B8" s="171"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="173"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5493,8 +5517,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="172"/>
-      <c r="B9" s="171"/>
+      <c r="A9" s="174"/>
+      <c r="B9" s="173"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5503,8 +5527,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="172"/>
-      <c r="B10" s="171"/>
+      <c r="A10" s="174"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5513,8 +5537,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="172"/>
-      <c r="B11" s="171"/>
+      <c r="A11" s="174"/>
+      <c r="B11" s="173"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5523,8 +5547,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="172"/>
-      <c r="B12" s="171"/>
+      <c r="A12" s="174"/>
+      <c r="B12" s="173"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5533,10 +5557,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="174" t="s">
+      <c r="A13" s="176" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="171" t="s">
+      <c r="B13" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5547,8 +5571,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="174"/>
-      <c r="B14" s="171"/>
+      <c r="A14" s="176"/>
+      <c r="B14" s="173"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5557,8 +5581,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="174"/>
-      <c r="B15" s="171"/>
+      <c r="A15" s="176"/>
+      <c r="B15" s="173"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5567,10 +5591,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="166" t="s">
+      <c r="B16" s="168" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5581,8 +5605,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="157"/>
-      <c r="B17" s="166"/>
+      <c r="A17" s="159"/>
+      <c r="B17" s="168"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5591,8 +5615,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="157"/>
-      <c r="B18" s="166"/>
+      <c r="A18" s="159"/>
+      <c r="B18" s="168"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5601,8 +5625,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="157"/>
-      <c r="B19" s="166"/>
+      <c r="A19" s="159"/>
+      <c r="B19" s="168"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5611,8 +5635,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="157"/>
-      <c r="B20" s="166"/>
+      <c r="A20" s="159"/>
+      <c r="B20" s="168"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5621,8 +5645,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="157"/>
-      <c r="B21" s="166"/>
+      <c r="A21" s="159"/>
+      <c r="B21" s="168"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5631,8 +5655,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="157"/>
-      <c r="B22" s="166"/>
+      <c r="A22" s="159"/>
+      <c r="B22" s="168"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5641,8 +5665,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="157"/>
-      <c r="B23" s="166"/>
+      <c r="A23" s="159"/>
+      <c r="B23" s="168"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5651,26 +5675,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="157"/>
-      <c r="B24" s="166"/>
-      <c r="C24" s="157" t="s">
+      <c r="A24" s="159"/>
+      <c r="B24" s="168"/>
+      <c r="C24" s="159" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="158" t="s">
+      <c r="D24" s="160" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="157"/>
-      <c r="B25" s="166"/>
-      <c r="C25" s="157"/>
-      <c r="D25" s="158"/>
+      <c r="A25" s="159"/>
+      <c r="B25" s="168"/>
+      <c r="C25" s="159"/>
+      <c r="D25" s="160"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="172" t="s">
+      <c r="A26" s="174" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="171" t="s">
+      <c r="B26" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5681,8 +5705,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="172"/>
-      <c r="B27" s="171"/>
+      <c r="A27" s="174"/>
+      <c r="B27" s="173"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5709,28 +5733,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="173" t="s">
+      <c r="A30" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="171" t="s">
+      <c r="B30" s="173" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="157" t="s">
+      <c r="C30" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="161" t="s">
+      <c r="D30" s="163" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="173"/>
-      <c r="B31" s="171"/>
-      <c r="C31" s="157"/>
-      <c r="D31" s="161"/>
+      <c r="A31" s="175"/>
+      <c r="B31" s="173"/>
+      <c r="C31" s="159"/>
+      <c r="D31" s="163"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="173"/>
-      <c r="B32" s="171"/>
+      <c r="A32" s="175"/>
+      <c r="B32" s="173"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5739,8 +5763,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="173"/>
-      <c r="B33" s="171"/>
+      <c r="A33" s="175"/>
+      <c r="B33" s="173"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5749,8 +5773,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="173"/>
-      <c r="B34" s="171"/>
+      <c r="A34" s="175"/>
+      <c r="B34" s="173"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5759,8 +5783,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="173"/>
-      <c r="B35" s="171"/>
+      <c r="A35" s="175"/>
+      <c r="B35" s="173"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5769,8 +5793,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="173"/>
-      <c r="B36" s="171"/>
+      <c r="A36" s="175"/>
+      <c r="B36" s="173"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5779,26 +5803,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="173"/>
-      <c r="B37" s="171"/>
-      <c r="C37" s="162" t="s">
+      <c r="A37" s="175"/>
+      <c r="B37" s="173"/>
+      <c r="C37" s="164" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="164" t="s">
+      <c r="D37" s="166" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="173"/>
-      <c r="B38" s="171"/>
-      <c r="C38" s="163"/>
-      <c r="D38" s="164"/>
+      <c r="A38" s="175"/>
+      <c r="B38" s="173"/>
+      <c r="C38" s="165"/>
+      <c r="D38" s="166"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="172" t="s">
+      <c r="A39" s="174" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="171" t="s">
+      <c r="B39" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5809,8 +5833,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="172"/>
-      <c r="B40" s="171"/>
+      <c r="A40" s="174"/>
+      <c r="B40" s="173"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5837,10 +5861,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="173" t="s">
+      <c r="A43" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="171" t="s">
+      <c r="B43" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5849,8 +5873,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="173"/>
-      <c r="B44" s="171"/>
+      <c r="A44" s="175"/>
+      <c r="B44" s="173"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5859,10 +5883,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="168" t="s">
+      <c r="A45" s="170" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="171" t="s">
+      <c r="B45" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5871,8 +5895,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="169"/>
-      <c r="B46" s="171"/>
+      <c r="A46" s="171"/>
+      <c r="B46" s="173"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5881,8 +5905,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="169"/>
-      <c r="B47" s="171"/>
+      <c r="A47" s="171"/>
+      <c r="B47" s="173"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5891,8 +5915,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="170"/>
-      <c r="B48" s="171"/>
+      <c r="A48" s="172"/>
+      <c r="B48" s="173"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5901,10 +5925,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="166" t="s">
+      <c r="A49" s="168" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="166" t="s">
+      <c r="B49" s="168" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10008,8 +10032,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="166"/>
-      <c r="B50" s="166"/>
+      <c r="A50" s="168"/>
+      <c r="B50" s="168"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14113,8 +14137,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="166"/>
-      <c r="B51" s="166"/>
+      <c r="A51" s="168"/>
+      <c r="B51" s="168"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18218,8 +18242,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="166"/>
-      <c r="B52" s="166"/>
+      <c r="A52" s="168"/>
+      <c r="B52" s="168"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22323,12 +22347,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="166"/>
-      <c r="B53" s="166"/>
-      <c r="C53" s="160" t="s">
+      <c r="A53" s="168"/>
+      <c r="B53" s="168"/>
+      <c r="C53" s="162" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="161" t="s">
+      <c r="D53" s="163" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26428,10 +26452,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="166"/>
-      <c r="B54" s="166"/>
-      <c r="C54" s="160"/>
-      <c r="D54" s="161"/>
+      <c r="A54" s="168"/>
+      <c r="B54" s="168"/>
+      <c r="C54" s="162"/>
+      <c r="D54" s="163"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30549,10 +30573,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="165" t="s">
+      <c r="A57" s="167" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="166" t="s">
+      <c r="B57" s="168" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30563,8 +30587,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="165"/>
-      <c r="B58" s="166"/>
+      <c r="A58" s="167"/>
+      <c r="B58" s="168"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30573,8 +30597,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="165"/>
-      <c r="B59" s="166"/>
+      <c r="A59" s="167"/>
+      <c r="B59" s="168"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30583,8 +30607,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="165"/>
-      <c r="B60" s="166"/>
+      <c r="A60" s="167"/>
+      <c r="B60" s="168"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30593,8 +30617,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="165"/>
-      <c r="B61" s="166"/>
+      <c r="A61" s="167"/>
+      <c r="B61" s="168"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30603,8 +30627,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="165"/>
-      <c r="B62" s="166"/>
+      <c r="A62" s="167"/>
+      <c r="B62" s="168"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30613,8 +30637,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="165"/>
-      <c r="B63" s="166"/>
+      <c r="A63" s="167"/>
+      <c r="B63" s="168"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30623,16 +30647,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="165"/>
-      <c r="B64" s="166"/>
+      <c r="A64" s="167"/>
+      <c r="B64" s="168"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="165"/>
-      <c r="B65" s="166"/>
+      <c r="A65" s="167"/>
+      <c r="B65" s="168"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30641,16 +30665,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="165"/>
-      <c r="B66" s="166"/>
+      <c r="A66" s="167"/>
+      <c r="B66" s="168"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="165"/>
-      <c r="B67" s="166"/>
+      <c r="A67" s="167"/>
+      <c r="B67" s="168"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30659,8 +30683,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="165"/>
-      <c r="B68" s="166"/>
+      <c r="A68" s="167"/>
+      <c r="B68" s="168"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30669,8 +30693,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="165"/>
-      <c r="B69" s="166"/>
+      <c r="A69" s="167"/>
+      <c r="B69" s="168"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30679,8 +30703,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="165"/>
-      <c r="B70" s="166"/>
+      <c r="A70" s="167"/>
+      <c r="B70" s="168"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30689,8 +30713,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="165"/>
-      <c r="B71" s="166"/>
+      <c r="A71" s="167"/>
+      <c r="B71" s="168"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30699,8 +30723,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="165"/>
-      <c r="B72" s="166"/>
+      <c r="A72" s="167"/>
+      <c r="B72" s="168"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30709,16 +30733,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="165"/>
-      <c r="B73" s="166"/>
+      <c r="A73" s="167"/>
+      <c r="B73" s="168"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="165"/>
-      <c r="B74" s="166"/>
+      <c r="A74" s="167"/>
+      <c r="B74" s="168"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30727,18 +30751,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="165"/>
-      <c r="B75" s="166"/>
-      <c r="C75" s="159"/>
-      <c r="D75" s="167" t="s">
+      <c r="A75" s="167"/>
+      <c r="B75" s="168"/>
+      <c r="C75" s="161"/>
+      <c r="D75" s="169" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="165"/>
-      <c r="B76" s="166"/>
-      <c r="C76" s="159"/>
-      <c r="D76" s="167"/>
+      <c r="A76" s="167"/>
+      <c r="B76" s="168"/>
+      <c r="C76" s="161"/>
+      <c r="D76" s="169"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30862,10 +30886,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="172" t="s">
+      <c r="A4" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="173" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30876,133 +30900,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="172"/>
-      <c r="B5" s="171"/>
-      <c r="C5" s="182" t="s">
+      <c r="A5" s="174"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="181" t="s">
+      <c r="D5" s="183" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="172"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="182"/>
-      <c r="D6" s="181"/>
+      <c r="A6" s="174"/>
+      <c r="B6" s="173"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="183"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="172"/>
-      <c r="B7" s="171"/>
+      <c r="A7" s="174"/>
+      <c r="B7" s="173"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="172"/>
-      <c r="B8" s="171"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="173"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="172"/>
-      <c r="B9" s="171"/>
+      <c r="A9" s="174"/>
+      <c r="B9" s="173"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="174" t="s">
+      <c r="A10" s="176" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="171" t="s">
+      <c r="B10" s="173" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="181" t="s">
+      <c r="C10" s="186"/>
+      <c r="D10" s="183" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="174"/>
-      <c r="B11" s="171"/>
-      <c r="C11" s="184"/>
-      <c r="D11" s="181"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="173"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="183"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="174"/>
-      <c r="B12" s="171"/>
-      <c r="C12" s="184"/>
-      <c r="D12" s="181"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="173"/>
+      <c r="C12" s="186"/>
+      <c r="D12" s="183"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="157" t="s">
+      <c r="A13" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="166" t="s">
+      <c r="B13" s="168" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="183"/>
-      <c r="D13" s="181" t="s">
+      <c r="C13" s="185"/>
+      <c r="D13" s="183" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="157"/>
-      <c r="B14" s="166"/>
-      <c r="C14" s="183"/>
-      <c r="D14" s="181"/>
+      <c r="A14" s="159"/>
+      <c r="B14" s="168"/>
+      <c r="C14" s="185"/>
+      <c r="D14" s="183"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="157"/>
-      <c r="B15" s="166"/>
-      <c r="C15" s="183"/>
+      <c r="A15" s="159"/>
+      <c r="B15" s="168"/>
+      <c r="C15" s="185"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="157"/>
-      <c r="B16" s="166"/>
-      <c r="C16" s="183"/>
+      <c r="A16" s="159"/>
+      <c r="B16" s="168"/>
+      <c r="C16" s="185"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="157"/>
-      <c r="B17" s="166"/>
-      <c r="C17" s="183"/>
+      <c r="A17" s="159"/>
+      <c r="B17" s="168"/>
+      <c r="C17" s="185"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="157"/>
-      <c r="B18" s="166"/>
-      <c r="C18" s="183"/>
+      <c r="A18" s="159"/>
+      <c r="B18" s="168"/>
+      <c r="C18" s="185"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="157"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="183"/>
+      <c r="A19" s="159"/>
+      <c r="B19" s="168"/>
+      <c r="C19" s="185"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="157"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="183"/>
+      <c r="A20" s="159"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="185"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="157"/>
-      <c r="B21" s="166"/>
-      <c r="C21" s="183"/>
+      <c r="A21" s="159"/>
+      <c r="B21" s="168"/>
+      <c r="C21" s="185"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="157"/>
-      <c r="B22" s="166"/>
-      <c r="C22" s="183"/>
+      <c r="A22" s="159"/>
+      <c r="B22" s="168"/>
+      <c r="C22" s="185"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="157"/>
-      <c r="B23" s="166"/>
-      <c r="C23" s="183"/>
+      <c r="A23" s="159"/>
+      <c r="B23" s="168"/>
+      <c r="C23" s="185"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31100,10 +31124,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="175" t="s">
+      <c r="A32" s="177" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="178" t="s">
+      <c r="B32" s="180" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31114,26 +31138,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="176"/>
-      <c r="B33" s="179"/>
+      <c r="A33" s="178"/>
+      <c r="B33" s="181"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="176"/>
-      <c r="B34" s="179"/>
+      <c r="A34" s="178"/>
+      <c r="B34" s="181"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="176"/>
-      <c r="B35" s="179"/>
+      <c r="A35" s="178"/>
+      <c r="B35" s="181"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="177"/>
-      <c r="B36" s="180"/>
+      <c r="A36" s="179"/>
+      <c r="B36" s="182"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31162,10 +31186,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="173" t="s">
+      <c r="A39" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="171" t="s">
+      <c r="B39" s="173" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31176,8 +31200,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="173"/>
-      <c r="B40" s="171"/>
+      <c r="A40" s="175"/>
+      <c r="B40" s="173"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31186,84 +31210,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="172" t="s">
+      <c r="A41" s="174" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="171" t="s">
+      <c r="B41" s="173" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="184" t="s">
+      <c r="C41" s="186" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="157" t="s">
+      <c r="D41" s="159" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="172"/>
-      <c r="B42" s="171"/>
-      <c r="C42" s="184"/>
-      <c r="D42" s="157"/>
+      <c r="A42" s="174"/>
+      <c r="B42" s="173"/>
+      <c r="C42" s="186"/>
+      <c r="D42" s="159"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="172"/>
-      <c r="B43" s="171"/>
-      <c r="C43" s="184" t="s">
+      <c r="A43" s="174"/>
+      <c r="B43" s="173"/>
+      <c r="C43" s="186" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="167" t="s">
+      <c r="D43" s="169" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="172"/>
-      <c r="B44" s="171"/>
-      <c r="C44" s="184"/>
-      <c r="D44" s="167"/>
+      <c r="A44" s="174"/>
+      <c r="B44" s="173"/>
+      <c r="C44" s="186"/>
+      <c r="D44" s="169"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="165" t="s">
+      <c r="A45" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="166" t="s">
+      <c r="B45" s="168" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="188"/>
+      <c r="C45" s="190"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="165"/>
-      <c r="B46" s="166"/>
-      <c r="C46" s="189"/>
-      <c r="D46" s="185" t="s">
+      <c r="A46" s="167"/>
+      <c r="B46" s="168"/>
+      <c r="C46" s="191"/>
+      <c r="D46" s="187" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="165"/>
-      <c r="B47" s="166"/>
-      <c r="C47" s="189"/>
-      <c r="D47" s="186"/>
+      <c r="A47" s="167"/>
+      <c r="B47" s="168"/>
+      <c r="C47" s="191"/>
+      <c r="D47" s="188"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="165"/>
-      <c r="B48" s="166"/>
-      <c r="C48" s="190"/>
-      <c r="D48" s="186"/>
+      <c r="A48" s="167"/>
+      <c r="B48" s="168"/>
+      <c r="C48" s="192"/>
+      <c r="D48" s="188"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="165"/>
-      <c r="B49" s="166"/>
-      <c r="C49" s="160"/>
-      <c r="D49" s="186"/>
+      <c r="A49" s="167"/>
+      <c r="B49" s="168"/>
+      <c r="C49" s="162"/>
+      <c r="D49" s="188"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="165"/>
-      <c r="B50" s="166"/>
-      <c r="C50" s="160"/>
-      <c r="D50" s="187"/>
+      <c r="A50" s="167"/>
+      <c r="B50" s="168"/>
+      <c r="C50" s="162"/>
+      <c r="D50" s="189"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31286,10 +31310,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="166" t="s">
+      <c r="A53" s="168" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="166" t="s">
+      <c r="B53" s="168" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31300,8 +31324,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="166"/>
-      <c r="B54" s="166"/>
+      <c r="A54" s="168"/>
+      <c r="B54" s="168"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31310,8 +31334,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="166"/>
-      <c r="B55" s="166"/>
+      <c r="A55" s="168"/>
+      <c r="B55" s="168"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31320,9 +31344,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="166"/>
-      <c r="B56" s="166"/>
-      <c r="C56" s="191" t="s">
+      <c r="A56" s="168"/>
+      <c r="B56" s="168"/>
+      <c r="C56" s="193" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31330,16 +31354,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="166"/>
-      <c r="B57" s="166"/>
-      <c r="C57" s="191"/>
+      <c r="A57" s="168"/>
+      <c r="B57" s="168"/>
+      <c r="C57" s="193"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="166"/>
-      <c r="B58" s="166"/>
+      <c r="A58" s="168"/>
+      <c r="B58" s="168"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31348,8 +31372,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="166"/>
-      <c r="B59" s="166"/>
+      <c r="A59" s="168"/>
+      <c r="B59" s="168"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31358,9 +31382,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="166"/>
-      <c r="B60" s="166"/>
-      <c r="C60" s="191" t="s">
+      <c r="A60" s="168"/>
+      <c r="B60" s="168"/>
+      <c r="C60" s="193" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31368,25 +31392,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="166"/>
-      <c r="B61" s="166"/>
-      <c r="C61" s="191"/>
+      <c r="A61" s="168"/>
+      <c r="B61" s="168"/>
+      <c r="C61" s="193"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="166"/>
-      <c r="B62" s="166"/>
-      <c r="C62" s="191"/>
+      <c r="A62" s="168"/>
+      <c r="B62" s="168"/>
+      <c r="C62" s="193"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="166"/>
-      <c r="B63" s="166"/>
-      <c r="C63" s="184" t="s">
+      <c r="A63" s="168"/>
+      <c r="B63" s="168"/>
+      <c r="C63" s="186" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31394,30 +31418,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="166"/>
-      <c r="B64" s="166"/>
-      <c r="C64" s="184"/>
-      <c r="D64" s="167" t="s">
+      <c r="A64" s="168"/>
+      <c r="B64" s="168"/>
+      <c r="C64" s="186"/>
+      <c r="D64" s="169" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="166"/>
-      <c r="B65" s="166"/>
-      <c r="C65" s="184"/>
-      <c r="D65" s="167"/>
+      <c r="A65" s="168"/>
+      <c r="B65" s="168"/>
+      <c r="C65" s="186"/>
+      <c r="D65" s="169"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="166"/>
-      <c r="B66" s="166"/>
-      <c r="C66" s="184"/>
-      <c r="D66" s="167"/>
+      <c r="A66" s="168"/>
+      <c r="B66" s="168"/>
+      <c r="C66" s="186"/>
+      <c r="D66" s="169"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="166"/>
-      <c r="B67" s="166"/>
-      <c r="C67" s="184"/>
-      <c r="D67" s="167"/>
+      <c r="A67" s="168"/>
+      <c r="B67" s="168"/>
+      <c r="C67" s="186"/>
+      <c r="D67" s="169"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31514,10 +31538,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31551,10 +31575,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="206" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="205" t="s">
+      <c r="B3" s="207" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="112" t="s">
@@ -31565,8 +31589,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="204"/>
-      <c r="B4" s="205"/>
+      <c r="A4" s="206"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="112" t="s">
         <v>347</v>
       </c>
@@ -31575,8 +31599,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="204"/>
-      <c r="B5" s="205"/>
+      <c r="A5" s="206"/>
+      <c r="B5" s="207"/>
       <c r="C5" s="112" t="s">
         <v>343</v>
       </c>
@@ -31593,10 +31617,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="157" t="s">
+      <c r="A7" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="191" t="s">
+      <c r="B7" s="193" t="s">
         <v>234</v>
       </c>
       <c r="C7" s="58"/>
@@ -31605,8 +31629,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="157"/>
-      <c r="B8" s="191"/>
+      <c r="A8" s="159"/>
+      <c r="B8" s="193"/>
       <c r="C8" s="104" t="s">
         <v>235</v>
       </c>
@@ -31669,10 +31693,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="157" t="s">
+      <c r="A13" s="159" t="s">
         <v>275</v>
       </c>
-      <c r="B13" s="191" t="s">
+      <c r="B13" s="193" t="s">
         <v>234</v>
       </c>
       <c r="C13" s="58"/>
@@ -31681,16 +31705,16 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="157"/>
-      <c r="B14" s="191"/>
+      <c r="A14" s="159"/>
+      <c r="B14" s="193"/>
       <c r="C14" s="58"/>
       <c r="D14" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="157"/>
-      <c r="B15" s="191"/>
+      <c r="A15" s="159"/>
+      <c r="B15" s="193"/>
       <c r="C15" s="108" t="s">
         <v>325</v>
       </c>
@@ -31699,8 +31723,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="157"/>
-      <c r="B16" s="191"/>
+      <c r="A16" s="159"/>
+      <c r="B16" s="193"/>
       <c r="C16" s="136" t="s">
         <v>404</v>
       </c>
@@ -31721,10 +31745,10 @@
       <c r="D17" s="58"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="206" t="s">
+      <c r="A18" s="208" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="195" t="s">
+      <c r="B18" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C18" s="58"/>
@@ -31733,8 +31757,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="207"/>
-      <c r="B19" s="200"/>
+      <c r="A19" s="209"/>
+      <c r="B19" s="202"/>
       <c r="C19" s="118" t="s">
         <v>361</v>
       </c>
@@ -31743,8 +31767,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="207"/>
-      <c r="B20" s="200"/>
+      <c r="A20" s="209"/>
+      <c r="B20" s="202"/>
       <c r="C20" s="118" t="s">
         <v>359</v>
       </c>
@@ -31753,8 +31777,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="207"/>
-      <c r="B21" s="200"/>
+      <c r="A21" s="209"/>
+      <c r="B21" s="202"/>
       <c r="C21" s="124" t="s">
         <v>367</v>
       </c>
@@ -31763,8 +31787,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="207"/>
-      <c r="B22" s="200"/>
+      <c r="A22" s="209"/>
+      <c r="B22" s="202"/>
       <c r="C22" s="131" t="s">
         <v>359</v>
       </c>
@@ -31773,8 +31797,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="207"/>
-      <c r="B23" s="200"/>
+      <c r="A23" s="209"/>
+      <c r="B23" s="202"/>
       <c r="C23" s="135" t="s">
         <v>371</v>
       </c>
@@ -31783,8 +31807,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="208"/>
-      <c r="B24" s="196"/>
+      <c r="A24" s="210"/>
+      <c r="B24" s="198"/>
       <c r="C24" s="135" t="s">
         <v>359</v>
       </c>
@@ -31819,10 +31843,10 @@
       <c r="D26" s="98"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="192" t="s">
+      <c r="A27" s="194" t="s">
         <v>369</v>
       </c>
-      <c r="B27" s="195" t="s">
+      <c r="B27" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C27" s="136" t="s">
@@ -31831,8 +31855,8 @@
       <c r="D27" s="98"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="194"/>
-      <c r="B28" s="196"/>
+      <c r="A28" s="196"/>
+      <c r="B28" s="198"/>
       <c r="C28" s="136" t="s">
         <v>404</v>
       </c>
@@ -31849,10 +31873,10 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="192" t="s">
+      <c r="A30" s="194" t="s">
         <v>237</v>
       </c>
-      <c r="B30" s="195" t="s">
+      <c r="B30" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C30" s="58"/>
@@ -31861,24 +31885,24 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="193"/>
-      <c r="B31" s="200"/>
+      <c r="A31" s="195"/>
+      <c r="B31" s="202"/>
       <c r="C31" s="58"/>
       <c r="D31" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="193"/>
-      <c r="B32" s="200"/>
+      <c r="A32" s="195"/>
+      <c r="B32" s="202"/>
       <c r="C32" s="58"/>
       <c r="D32" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="193"/>
-      <c r="B33" s="200"/>
+      <c r="A33" s="195"/>
+      <c r="B33" s="202"/>
       <c r="C33" s="58" t="s">
         <v>300</v>
       </c>
@@ -31887,8 +31911,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="193"/>
-      <c r="B34" s="200"/>
+      <c r="A34" s="195"/>
+      <c r="B34" s="202"/>
       <c r="C34" s="58" t="s">
         <v>328</v>
       </c>
@@ -31897,8 +31921,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="194"/>
-      <c r="B35" s="196"/>
+      <c r="A35" s="196"/>
+      <c r="B35" s="198"/>
       <c r="C35" s="58" t="s">
         <v>373</v>
       </c>
@@ -31907,10 +31931,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="168" t="s">
+      <c r="A36" s="170" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="195" t="s">
+      <c r="B36" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C36" s="58" t="s">
@@ -31921,16 +31945,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="169"/>
-      <c r="B37" s="200"/>
+      <c r="A37" s="171"/>
+      <c r="B37" s="202"/>
       <c r="C37" s="58"/>
       <c r="D37" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="169"/>
-      <c r="B38" s="200"/>
+      <c r="A38" s="171"/>
+      <c r="B38" s="202"/>
       <c r="C38" s="106" t="s">
         <v>329</v>
       </c>
@@ -31939,8 +31963,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="169"/>
-      <c r="B39" s="200"/>
+      <c r="A39" s="171"/>
+      <c r="B39" s="202"/>
       <c r="C39" s="106" t="s">
         <v>359</v>
       </c>
@@ -31949,8 +31973,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="169"/>
-      <c r="B40" s="200"/>
+      <c r="A40" s="171"/>
+      <c r="B40" s="202"/>
       <c r="C40" s="106" t="s">
         <v>367</v>
       </c>
@@ -31959,8 +31983,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="169"/>
-      <c r="B41" s="200"/>
+      <c r="A41" s="171"/>
+      <c r="B41" s="202"/>
       <c r="C41" s="106" t="s">
         <v>371</v>
       </c>
@@ -31969,8 +31993,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="169"/>
-      <c r="B42" s="200"/>
+      <c r="A42" s="171"/>
+      <c r="B42" s="202"/>
       <c r="C42" s="106" t="s">
         <v>381</v>
       </c>
@@ -31979,8 +32003,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="170"/>
-      <c r="B43" s="196"/>
+      <c r="A43" s="172"/>
+      <c r="B43" s="198"/>
       <c r="C43" s="96" t="s">
         <v>359</v>
       </c>
@@ -31989,13 +32013,13 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="162" t="s">
+      <c r="A44" s="164" t="s">
         <v>222</v>
       </c>
-      <c r="B44" s="195" t="s">
+      <c r="B44" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="202" t="s">
+      <c r="C44" s="204" t="s">
         <v>239</v>
       </c>
       <c r="D44" s="101" t="s">
@@ -32003,17 +32027,17 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="201"/>
-      <c r="B45" s="200"/>
-      <c r="C45" s="203"/>
+      <c r="A45" s="203"/>
+      <c r="B45" s="202"/>
+      <c r="C45" s="205"/>
       <c r="D45" s="98" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="201"/>
-      <c r="B46" s="200"/>
-      <c r="C46" s="209" t="s">
+      <c r="A46" s="203"/>
+      <c r="B46" s="202"/>
+      <c r="C46" s="211" t="s">
         <v>240</v>
       </c>
       <c r="D46" s="58" t="s">
@@ -32021,16 +32045,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="201"/>
-      <c r="B47" s="200"/>
-      <c r="C47" s="209"/>
+      <c r="A47" s="203"/>
+      <c r="B47" s="202"/>
+      <c r="C47" s="211"/>
       <c r="D47" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="201"/>
-      <c r="B48" s="200"/>
+      <c r="A48" s="203"/>
+      <c r="B48" s="202"/>
       <c r="C48" s="103" t="s">
         <v>307</v>
       </c>
@@ -32039,8 +32063,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="201"/>
-      <c r="B49" s="200"/>
+      <c r="A49" s="203"/>
+      <c r="B49" s="202"/>
       <c r="C49" s="103">
         <v>2.1</v>
       </c>
@@ -32049,8 +32073,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="201"/>
-      <c r="B50" s="200"/>
+      <c r="A50" s="203"/>
+      <c r="B50" s="202"/>
       <c r="C50" s="103" t="s">
         <v>239</v>
       </c>
@@ -32059,8 +32083,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="201"/>
-      <c r="B51" s="200"/>
+      <c r="A51" s="203"/>
+      <c r="B51" s="202"/>
       <c r="C51" s="114" t="s">
         <v>239</v>
       </c>
@@ -32069,8 +32093,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="201"/>
-      <c r="B52" s="200"/>
+      <c r="A52" s="203"/>
+      <c r="B52" s="202"/>
       <c r="C52" s="128" t="s">
         <v>239</v>
       </c>
@@ -32079,8 +32103,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="201"/>
-      <c r="B53" s="200"/>
+      <c r="A53" s="203"/>
+      <c r="B53" s="202"/>
       <c r="C53" s="134" t="s">
         <v>378</v>
       </c>
@@ -32089,8 +32113,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="201"/>
-      <c r="B54" s="200"/>
+      <c r="A54" s="203"/>
+      <c r="B54" s="202"/>
       <c r="C54" s="136">
         <v>2.1</v>
       </c>
@@ -32099,8 +32123,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="201"/>
-      <c r="B55" s="200"/>
+      <c r="A55" s="203"/>
+      <c r="B55" s="202"/>
       <c r="C55" s="136" t="s">
         <v>239</v>
       </c>
@@ -32109,8 +32133,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="201"/>
-      <c r="B56" s="200"/>
+      <c r="A56" s="203"/>
+      <c r="B56" s="202"/>
       <c r="C56" s="141" t="s">
         <v>239</v>
       </c>
@@ -32119,10 +32143,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="210" t="s">
+      <c r="A57" s="212" t="s">
         <v>296</v>
       </c>
-      <c r="B57" s="195" t="s">
+      <c r="B57" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -32133,8 +32157,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="211"/>
-      <c r="B58" s="200"/>
+      <c r="A58" s="213"/>
+      <c r="B58" s="202"/>
       <c r="C58" s="61" t="s">
         <v>281</v>
       </c>
@@ -32143,8 +32167,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="212"/>
-      <c r="B59" s="196"/>
+      <c r="A59" s="214"/>
+      <c r="B59" s="198"/>
       <c r="C59" s="58" t="s">
         <v>350</v>
       </c>
@@ -32153,10 +32177,10 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="192" t="s">
+      <c r="A60" s="194" t="s">
         <v>370</v>
       </c>
-      <c r="B60" s="195" t="s">
+      <c r="B60" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C60" s="128" t="s">
@@ -32165,8 +32189,8 @@
       <c r="D60" s="58"/>
     </row>
     <row r="61" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="193"/>
-      <c r="B61" s="200"/>
+      <c r="A61" s="195"/>
+      <c r="B61" s="202"/>
       <c r="C61" s="131" t="s">
         <v>378</v>
       </c>
@@ -32175,8 +32199,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="193"/>
-      <c r="B62" s="200"/>
+      <c r="A62" s="195"/>
+      <c r="B62" s="202"/>
       <c r="C62" s="136">
         <v>2.1</v>
       </c>
@@ -32185,8 +32209,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="193"/>
-      <c r="B63" s="200"/>
+      <c r="A63" s="195"/>
+      <c r="B63" s="202"/>
       <c r="C63" s="136" t="s">
         <v>240</v>
       </c>
@@ -32195,8 +32219,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="193"/>
-      <c r="B64" s="200"/>
+      <c r="A64" s="195"/>
+      <c r="B64" s="202"/>
       <c r="C64" s="133" t="s">
         <v>239</v>
       </c>
@@ -32225,10 +32249,10 @@
       <c r="D66" s="98"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="162" t="s">
+      <c r="A67" s="164" t="s">
         <v>260</v>
       </c>
-      <c r="B67" s="195" t="s">
+      <c r="B67" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C67" s="58"/>
@@ -32237,554 +32261,550 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="201"/>
-      <c r="B68" s="200"/>
+      <c r="A68" s="203"/>
+      <c r="B68" s="202"/>
       <c r="C68" s="58"/>
       <c r="D68" s="58" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="201"/>
-      <c r="B69" s="200"/>
+      <c r="A69" s="203"/>
+      <c r="B69" s="202"/>
       <c r="C69" s="58"/>
       <c r="D69" s="98" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="157" t="s">
+      <c r="A70" s="203"/>
+      <c r="B70" s="202"/>
+      <c r="C70" s="58" t="s">
+        <v>424</v>
+      </c>
+      <c r="D70" s="98" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="159" t="s">
         <v>334</v>
       </c>
-      <c r="B70" s="191" t="s">
+      <c r="B71" s="193" t="s">
         <v>234</v>
       </c>
-      <c r="C70" s="79" t="s">
+      <c r="C71" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D70" s="98" t="s">
+      <c r="D71" s="98" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="157"/>
-      <c r="B71" s="191"/>
-      <c r="C71" s="58" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="159"/>
+      <c r="B72" s="193"/>
+      <c r="C72" s="58" t="s">
         <v>411</v>
       </c>
-      <c r="D71" s="58" t="s">
+      <c r="D72" s="58" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="157"/>
-      <c r="B72" s="191"/>
-      <c r="C72" s="140" t="s">
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="159"/>
+      <c r="B73" s="193"/>
+      <c r="C73" s="140" t="s">
         <v>414</v>
       </c>
-      <c r="D72" s="192" t="s">
+      <c r="D73" s="194" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="157"/>
-      <c r="B73" s="191"/>
-      <c r="C73" s="140" t="s">
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="159"/>
+      <c r="B74" s="193"/>
+      <c r="C74" s="140" t="s">
         <v>415</v>
       </c>
-      <c r="D73" s="193"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="157"/>
-      <c r="B74" s="191"/>
-      <c r="C74" s="140" t="s">
+      <c r="D74" s="195"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="159"/>
+      <c r="B75" s="193"/>
+      <c r="C75" s="140" t="s">
         <v>416</v>
       </c>
-      <c r="D74" s="193"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="157"/>
-      <c r="B75" s="191"/>
-      <c r="C75" s="140" t="s">
+      <c r="D75" s="195"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="159"/>
+      <c r="B76" s="193"/>
+      <c r="C76" s="140" t="s">
         <v>417</v>
       </c>
-      <c r="D75" s="194"/>
-    </row>
-    <row r="76" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="96" t="s">
+      <c r="D76" s="196"/>
+    </row>
+    <row r="77" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B76" s="122" t="s">
+      <c r="B77" s="122" t="s">
         <v>234</v>
       </c>
-      <c r="C76" s="104" t="s">
+      <c r="C77" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="D76" s="102" t="s">
+      <c r="D77" s="102" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="210" t="s">
+    <row r="78" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="212" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="195" t="s">
+      <c r="B78" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C77" s="58" t="s">
+      <c r="C78" s="58" t="s">
         <v>268</v>
-      </c>
-      <c r="D77" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="211"/>
-      <c r="B78" s="200"/>
-      <c r="C78" s="58" t="s">
-        <v>270</v>
       </c>
       <c r="D78" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="211"/>
-      <c r="B79" s="200"/>
+      <c r="A79" s="213"/>
+      <c r="B79" s="202"/>
       <c r="C79" s="58" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D79" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="211"/>
-      <c r="B80" s="200"/>
-      <c r="C80" s="98" t="s">
+      <c r="A80" s="213"/>
+      <c r="B80" s="202"/>
+      <c r="C80" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D80" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="213"/>
+      <c r="B81" s="202"/>
+      <c r="C81" s="98" t="s">
         <v>277</v>
       </c>
-      <c r="D80" s="98" t="s">
+      <c r="D81" s="98" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="211"/>
-      <c r="B81" s="200"/>
-      <c r="C81" s="58" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="213"/>
+      <c r="B82" s="202"/>
+      <c r="C82" s="58" t="s">
         <v>282</v>
       </c>
-      <c r="D81" s="58" t="s">
+      <c r="D82" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="211"/>
-      <c r="B82" s="200"/>
-      <c r="C82" s="58" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="213"/>
+      <c r="B83" s="202"/>
+      <c r="C83" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="D82" s="58" t="s">
+      <c r="D83" s="58" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="211"/>
-      <c r="B83" s="200"/>
-      <c r="C83" s="98" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="213"/>
+      <c r="B84" s="202"/>
+      <c r="C84" s="98" t="s">
         <v>288</v>
-      </c>
-      <c r="D83" s="98" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="211"/>
-      <c r="B84" s="200"/>
-      <c r="C84" s="98" t="s">
-        <v>302</v>
       </c>
       <c r="D84" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="211"/>
-      <c r="B85" s="200"/>
+      <c r="A85" s="213"/>
+      <c r="B85" s="202"/>
       <c r="C85" s="98" t="s">
+        <v>302</v>
+      </c>
+      <c r="D85" s="98" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="213"/>
+      <c r="B86" s="202"/>
+      <c r="C86" s="98" t="s">
         <v>289</v>
       </c>
-      <c r="D85" s="98" t="s">
+      <c r="D86" s="98" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="211"/>
-      <c r="B86" s="200"/>
-      <c r="C86" s="105" t="s">
+    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="213"/>
+      <c r="B87" s="202"/>
+      <c r="C87" s="105" t="s">
         <v>244</v>
       </c>
-      <c r="D86" s="102" t="s">
+      <c r="D87" s="102" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="211"/>
-      <c r="B87" s="200"/>
-      <c r="C87" s="106" t="s">
+    <row r="88" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="213"/>
+      <c r="B88" s="202"/>
+      <c r="C88" s="106" t="s">
         <v>311</v>
       </c>
-      <c r="D87" s="98" t="s">
+      <c r="D88" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="211"/>
-      <c r="B88" s="200"/>
-      <c r="C88" s="58" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="213"/>
+      <c r="B89" s="202"/>
+      <c r="C89" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="D88" s="58" t="s">
+      <c r="D89" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="211"/>
-      <c r="B89" s="200"/>
-      <c r="C89" s="98" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="213"/>
+      <c r="B90" s="202"/>
+      <c r="C90" s="98" t="s">
         <v>313</v>
       </c>
-      <c r="D89" s="98" t="s">
+      <c r="D90" s="98" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="211"/>
-      <c r="B90" s="200"/>
-      <c r="C90" s="98" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="213"/>
+      <c r="B91" s="202"/>
+      <c r="C91" s="98" t="s">
         <v>315</v>
-      </c>
-      <c r="D90" s="98" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="211"/>
-      <c r="B91" s="200"/>
-      <c r="C91" s="98" t="s">
-        <v>268</v>
       </c>
       <c r="D91" s="98" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="211"/>
-      <c r="B92" s="200"/>
-      <c r="C92" s="58" t="s">
+      <c r="A92" s="213"/>
+      <c r="B92" s="202"/>
+      <c r="C92" s="98" t="s">
+        <v>268</v>
+      </c>
+      <c r="D92" s="98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="213"/>
+      <c r="B93" s="202"/>
+      <c r="C93" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="D92" s="58" t="s">
+      <c r="D93" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="211"/>
-      <c r="B93" s="200"/>
-      <c r="C93" s="98" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="213"/>
+      <c r="B94" s="202"/>
+      <c r="C94" s="98" t="s">
         <v>283</v>
       </c>
-      <c r="D93" s="98" t="s">
+      <c r="D94" s="98" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="211"/>
-      <c r="B94" s="200"/>
-      <c r="C94" s="98" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="213"/>
+      <c r="B95" s="202"/>
+      <c r="C95" s="98" t="s">
         <v>319</v>
       </c>
-      <c r="D94" s="98" t="s">
+      <c r="D95" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="211"/>
-      <c r="B95" s="200"/>
-      <c r="C95" s="58"/>
-      <c r="D95" s="107" t="s">
+    <row r="96" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="213"/>
+      <c r="B96" s="202"/>
+      <c r="C96" s="58"/>
+      <c r="D96" s="107" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="211"/>
-      <c r="B96" s="200"/>
-      <c r="C96" s="98" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="213"/>
+      <c r="B97" s="202"/>
+      <c r="C97" s="98" t="s">
         <v>322</v>
-      </c>
-      <c r="D96" s="98" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="211"/>
-      <c r="B97" s="200"/>
-      <c r="C97" s="98" t="s">
-        <v>268</v>
       </c>
       <c r="D97" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="211"/>
-      <c r="B98" s="200"/>
+      <c r="A98" s="213"/>
+      <c r="B98" s="202"/>
       <c r="C98" s="98" t="s">
-        <v>339</v>
+        <v>268</v>
       </c>
       <c r="D98" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="211"/>
-      <c r="B99" s="200"/>
+      <c r="A99" s="213"/>
+      <c r="B99" s="202"/>
       <c r="C99" s="98" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D99" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="211"/>
-      <c r="B100" s="200"/>
+      <c r="A100" s="213"/>
+      <c r="B100" s="202"/>
       <c r="C100" s="98" t="s">
+        <v>340</v>
+      </c>
+      <c r="D100" s="98" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="213"/>
+      <c r="B101" s="202"/>
+      <c r="C101" s="98" t="s">
         <v>324</v>
       </c>
-      <c r="D100" s="98" t="s">
+      <c r="D101" s="98" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="211"/>
-      <c r="B101" s="200"/>
-      <c r="C101" s="113" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="213"/>
+      <c r="B102" s="202"/>
+      <c r="C102" s="113" t="s">
         <v>345</v>
       </c>
-      <c r="D101" s="113" t="s">
+      <c r="D102" s="113" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="211"/>
-      <c r="B102" s="200"/>
-      <c r="C102" s="98" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="213"/>
+      <c r="B103" s="202"/>
+      <c r="C103" s="98" t="s">
         <v>338</v>
       </c>
-      <c r="D102" s="98" t="s">
+      <c r="D103" s="98" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="211"/>
-      <c r="B103" s="200"/>
-      <c r="C103" s="98" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="213"/>
+      <c r="B104" s="202"/>
+      <c r="C104" s="98" t="s">
         <v>353</v>
       </c>
-      <c r="D103" s="98" t="s">
+      <c r="D104" s="98" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="211"/>
-      <c r="B104" s="200"/>
-      <c r="C104" s="117" t="s">
+    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="213"/>
+      <c r="B105" s="202"/>
+      <c r="C105" s="117" t="s">
         <v>356</v>
       </c>
-      <c r="D104" s="116" t="s">
+      <c r="D105" s="116" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="211"/>
-      <c r="B105" s="200"/>
-      <c r="C105" s="98" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="213"/>
+      <c r="B106" s="202"/>
+      <c r="C106" s="98" t="s">
         <v>357</v>
       </c>
-      <c r="D105" s="98" t="s">
+      <c r="D106" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="211"/>
-      <c r="B106" s="200"/>
-      <c r="C106" s="98" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="213"/>
+      <c r="B107" s="202"/>
+      <c r="C107" s="98" t="s">
         <v>358</v>
       </c>
-      <c r="D106" s="98" t="s">
+      <c r="D107" s="98" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="211"/>
-      <c r="B107" s="200"/>
-      <c r="C107" s="98" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="213"/>
+      <c r="B108" s="202"/>
+      <c r="C108" s="98" t="s">
         <v>364</v>
       </c>
-      <c r="D107" s="98" t="s">
+      <c r="D108" s="98" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="211"/>
-      <c r="B108" s="200"/>
-      <c r="C108" s="98" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="213"/>
+      <c r="B109" s="202"/>
+      <c r="C109" s="98" t="s">
         <v>366</v>
-      </c>
-      <c r="D108" s="98" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="211"/>
-      <c r="B109" s="200"/>
-      <c r="C109" s="98" t="s">
-        <v>372</v>
       </c>
       <c r="D109" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="211"/>
-      <c r="B110" s="200"/>
+      <c r="A110" s="213"/>
+      <c r="B110" s="202"/>
       <c r="C110" s="98" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="D110" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="211"/>
-      <c r="B111" s="200"/>
-      <c r="C111" s="113" t="s">
+      <c r="A111" s="213"/>
+      <c r="B111" s="202"/>
+      <c r="C111" s="98" t="s">
+        <v>364</v>
+      </c>
+      <c r="D111" s="98" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="213"/>
+      <c r="B112" s="202"/>
+      <c r="C112" s="113" t="s">
         <v>385</v>
       </c>
-      <c r="D111" s="113" t="s">
+      <c r="D112" s="113" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="211"/>
-      <c r="B112" s="200"/>
-      <c r="C112" s="58" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="213"/>
+      <c r="B113" s="202"/>
+      <c r="C113" s="58" t="s">
         <v>389</v>
       </c>
-      <c r="D112" s="58" t="s">
+      <c r="D113" s="58" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="211"/>
-      <c r="B113" s="200"/>
-      <c r="C113" s="58" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="213"/>
+      <c r="B114" s="202"/>
+      <c r="C114" s="58" t="s">
         <v>392</v>
       </c>
-      <c r="D113" s="58" t="s">
+      <c r="D114" s="58" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="211"/>
-      <c r="B114" s="200"/>
-      <c r="C114" s="58" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="213"/>
+      <c r="B115" s="202"/>
+      <c r="C115" s="58" t="s">
         <v>393</v>
-      </c>
-      <c r="D114" s="58" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="211"/>
-      <c r="B115" s="200"/>
-      <c r="C115" s="58" t="s">
-        <v>394</v>
       </c>
       <c r="D115" s="58" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="211"/>
-      <c r="B116" s="200"/>
+      <c r="A116" s="213"/>
+      <c r="B116" s="202"/>
       <c r="C116" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="D116" s="58" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="213"/>
+      <c r="B117" s="202"/>
+      <c r="C117" s="58" t="s">
         <v>395</v>
-      </c>
-      <c r="D116" s="58" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="211"/>
-      <c r="B117" s="200"/>
-      <c r="C117" s="58" t="s">
-        <v>396</v>
       </c>
       <c r="D117" s="58" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="211"/>
-      <c r="B118" s="200"/>
+      <c r="A118" s="213"/>
+      <c r="B118" s="202"/>
       <c r="C118" s="58" t="s">
+        <v>396</v>
+      </c>
+      <c r="D118" s="58" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="213"/>
+      <c r="B119" s="202"/>
+      <c r="C119" s="58" t="s">
         <v>399</v>
-      </c>
-      <c r="D118" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="211"/>
-      <c r="B119" s="200"/>
-      <c r="C119" s="58" t="s">
-        <v>409</v>
       </c>
       <c r="D119" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="212"/>
-      <c r="B120" s="196"/>
+      <c r="A120" s="213"/>
+      <c r="B120" s="202"/>
       <c r="C120" s="58" t="s">
+        <v>409</v>
+      </c>
+      <c r="D120" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="214"/>
+      <c r="B121" s="198"/>
+      <c r="C121" s="58" t="s">
         <v>410</v>
       </c>
-      <c r="D120" s="58" t="s">
+      <c r="D121" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="96" t="s">
-        <v>309</v>
-      </c>
-      <c r="B121" s="123" t="s">
-        <v>234</v>
-      </c>
-      <c r="C121" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D121" s="98" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="96" t="s">
-        <v>310</v>
-      </c>
-      <c r="B122" s="123" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="143" t="s">
+        <v>421</v>
+      </c>
+      <c r="B122" s="142" t="s">
         <v>234</v>
       </c>
       <c r="C122" s="58" t="s">
@@ -32795,348 +32815,396 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="39" t="s">
+      <c r="A123" s="96" t="s">
+        <v>309</v>
+      </c>
+      <c r="B123" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C123" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D123" s="98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="96" t="s">
+        <v>310</v>
+      </c>
+      <c r="B124" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C124" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D124" s="98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="44"/>
-    </row>
-    <row r="124" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="162" t="s">
+      <c r="B125" s="39"/>
+      <c r="C125" s="39"/>
+      <c r="D125" s="44"/>
+    </row>
+    <row r="126" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="B124" s="195" t="s">
+      <c r="B126" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C124" s="58"/>
-      <c r="D124" s="79" t="s">
+      <c r="C126" s="58"/>
+      <c r="D126" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="201"/>
-      <c r="B125" s="200"/>
-      <c r="C125" s="104" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="203"/>
+      <c r="B127" s="202"/>
+      <c r="C127" s="104" t="s">
         <v>246</v>
       </c>
-      <c r="D125" s="58" t="s">
+      <c r="D127" s="58" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="201"/>
-      <c r="B126" s="200"/>
-      <c r="C126" s="104">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="203"/>
+      <c r="B128" s="202"/>
+      <c r="C128" s="104">
         <v>10.1</v>
       </c>
-      <c r="D126" s="58" t="s">
+      <c r="D128" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="201"/>
-      <c r="B127" s="200"/>
-      <c r="C127" s="104">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="203"/>
+      <c r="B129" s="202"/>
+      <c r="C129" s="104">
         <v>10.199999999999999</v>
       </c>
-      <c r="D127" s="58" t="s">
+      <c r="D129" s="58" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="201"/>
-      <c r="B128" s="200"/>
-      <c r="C128" s="109" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="203"/>
+      <c r="B130" s="202"/>
+      <c r="C130" s="109" t="s">
         <v>293</v>
       </c>
-      <c r="D128" s="99" t="s">
+      <c r="D130" s="99" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="201"/>
-      <c r="B129" s="200"/>
-      <c r="C129" s="109" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="203"/>
+      <c r="B131" s="202"/>
+      <c r="C131" s="109" t="s">
         <v>375</v>
       </c>
-      <c r="D129" s="99" t="s">
+      <c r="D131" s="99" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="163"/>
-      <c r="B130" s="196"/>
-      <c r="C130" s="109" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="203"/>
+      <c r="B132" s="202"/>
+      <c r="C132" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="D130" s="99" t="s">
+      <c r="D132" s="99" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="162" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="203"/>
+      <c r="B133" s="202"/>
+      <c r="C133" s="109" t="s">
+        <v>422</v>
+      </c>
+      <c r="D133" s="99" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="165"/>
+      <c r="B134" s="198"/>
+      <c r="C134" s="109" t="s">
+        <v>17</v>
+      </c>
+      <c r="D134" s="99" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="164" t="s">
         <v>247</v>
       </c>
-      <c r="B131" s="195" t="s">
+      <c r="B135" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C131" s="191"/>
-      <c r="D131" s="215" t="s">
+      <c r="C135" s="193"/>
+      <c r="D135" s="217" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="163"/>
-      <c r="B132" s="196"/>
-      <c r="C132" s="191"/>
-      <c r="D132" s="215"/>
-    </row>
-    <row r="133" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="121" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="165"/>
+      <c r="B136" s="198"/>
+      <c r="C136" s="193"/>
+      <c r="D136" s="217"/>
+    </row>
+    <row r="137" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="121" t="s">
         <v>262</v>
       </c>
-      <c r="B133" s="123" t="s">
+      <c r="B137" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C133" s="104" t="s">
+      <c r="C137" s="104" t="s">
         <v>250</v>
       </c>
-      <c r="D133" s="98" t="s">
+      <c r="D137" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="95" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B134" s="39"/>
-      <c r="C134" s="97"/>
-      <c r="D134" s="97"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="96" t="s">
+      <c r="B138" s="39"/>
+      <c r="C138" s="97"/>
+      <c r="D138" s="97"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="B135" s="123" t="s">
+      <c r="B139" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C135" s="110" t="s">
+      <c r="C139" s="110" t="s">
         <v>265</v>
       </c>
-      <c r="D135" s="58" t="s">
+      <c r="D139" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="162" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="164" t="s">
         <v>285</v>
       </c>
-      <c r="B136" s="195" t="s">
+      <c r="B140" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C136" s="99" t="s">
+      <c r="C140" s="99" t="s">
         <v>295</v>
       </c>
-      <c r="D136" s="58" t="s">
+      <c r="D140" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="201"/>
-      <c r="B137" s="200"/>
-      <c r="C137" s="58" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="203"/>
+      <c r="B141" s="202"/>
+      <c r="C141" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D137" s="98" t="s">
+      <c r="D141" s="98" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="163"/>
-      <c r="B138" s="196"/>
-      <c r="C138" s="110" t="s">
+    <row r="142" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="165"/>
+      <c r="B142" s="198"/>
+      <c r="C142" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="D138" s="58" t="s">
+      <c r="D142" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="97" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="B139" s="97"/>
-      <c r="C139" s="97"/>
-      <c r="D139" s="97"/>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="197" t="s">
+      <c r="B143" s="97"/>
+      <c r="C143" s="97"/>
+      <c r="D143" s="97"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="199" t="s">
         <v>58</v>
       </c>
-      <c r="B140" s="195" t="s">
+      <c r="B144" s="197" t="s">
         <v>271</v>
       </c>
-      <c r="C140" s="110" t="s">
+      <c r="C144" s="110" t="s">
         <v>265</v>
       </c>
-      <c r="D140" s="58" t="s">
+      <c r="D144" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="198"/>
-      <c r="B141" s="200"/>
-      <c r="C141" s="110" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="200"/>
+      <c r="B145" s="202"/>
+      <c r="C145" s="110" t="s">
         <v>265</v>
       </c>
-      <c r="D141" s="58" t="s">
+      <c r="D145" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="199"/>
-      <c r="B142" s="196"/>
-      <c r="C142" s="58"/>
-      <c r="D142" s="58" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A143" s="213" t="s">
-        <v>59</v>
-      </c>
-      <c r="B143" s="195" t="s">
-        <v>271</v>
-      </c>
-      <c r="C143" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="D143" s="58" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="214"/>
-      <c r="B144" s="196"/>
-      <c r="C144" s="61"/>
-      <c r="D144" s="58" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A145" s="216" t="s">
-        <v>291</v>
-      </c>
-      <c r="B145" s="195" t="s">
-        <v>271</v>
-      </c>
-      <c r="C145" s="61"/>
-      <c r="D145" s="61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="217"/>
-      <c r="B146" s="196"/>
+    <row r="146" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="201"/>
+      <c r="B146" s="198"/>
       <c r="C146" s="58"/>
       <c r="D146" s="58" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A147" s="213" t="s">
-        <v>60</v>
-      </c>
-      <c r="B147" s="195" t="s">
+      <c r="A147" s="215" t="s">
+        <v>59</v>
+      </c>
+      <c r="B147" s="197" t="s">
         <v>271</v>
       </c>
       <c r="C147" s="61" t="s">
         <v>264</v>
       </c>
       <c r="D147" s="58" t="s">
-        <v>263</v>
+        <v>100</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="214"/>
-      <c r="B148" s="196"/>
-      <c r="C148" s="58"/>
+      <c r="A148" s="216"/>
+      <c r="B148" s="198"/>
+      <c r="C148" s="61"/>
       <c r="D148" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="97" t="s">
+    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="218" t="s">
+        <v>291</v>
+      </c>
+      <c r="B149" s="197" t="s">
+        <v>271</v>
+      </c>
+      <c r="C149" s="61"/>
+      <c r="D149" s="61" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="219"/>
+      <c r="B150" s="198"/>
+      <c r="C150" s="58"/>
+      <c r="D150" s="58" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="215" t="s">
+        <v>60</v>
+      </c>
+      <c r="B151" s="197" t="s">
+        <v>271</v>
+      </c>
+      <c r="C151" s="61" t="s">
+        <v>264</v>
+      </c>
+      <c r="D151" s="58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="216"/>
+      <c r="B152" s="198"/>
+      <c r="C152" s="58"/>
+      <c r="D152" s="58" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="97" t="s">
         <v>273</v>
       </c>
-      <c r="B149" s="97"/>
-      <c r="C149" s="97"/>
-      <c r="D149" s="97"/>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="58"/>
-      <c r="B150" s="123" t="s">
+      <c r="B153" s="97"/>
+      <c r="C153" s="97"/>
+      <c r="D153" s="97"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="58"/>
+      <c r="B154" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C150" s="58" t="s">
+      <c r="C154" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D150" s="98" t="s">
+      <c r="D154" s="98" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="97" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="B151" s="97"/>
-      <c r="C151" s="97"/>
-      <c r="D151" s="97"/>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="58"/>
-      <c r="B152" s="137" t="s">
+      <c r="B155" s="97"/>
+      <c r="C155" s="97"/>
+      <c r="D155" s="97"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="58"/>
+      <c r="B156" s="137" t="s">
         <v>234</v>
       </c>
-      <c r="C152" s="58" t="s">
+      <c r="C156" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D152" s="98" t="s">
+      <c r="D156" s="98" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="58"/>
-      <c r="B153" s="123"/>
-      <c r="C153" s="58" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="58"/>
+      <c r="B157" s="123"/>
+      <c r="C157" s="58" t="s">
         <v>401</v>
       </c>
-      <c r="D153" s="98" t="s">
+      <c r="D157" s="98" t="s">
         <v>402</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="D135:D136"/>
     <mergeCell ref="A147:A148"/>
     <mergeCell ref="B147:B148"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="B143:B144"/>
-    <mergeCell ref="A145:A146"/>
-    <mergeCell ref="B145:B146"/>
-    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="C135:C136"/>
     <mergeCell ref="C46:C47"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="A77:A120"/>
-    <mergeCell ref="B77:B120"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="A78:A121"/>
+    <mergeCell ref="B78:B121"/>
     <mergeCell ref="A44:A56"/>
     <mergeCell ref="B44:B56"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A70:A75"/>
-    <mergeCell ref="B70:B75"/>
+    <mergeCell ref="A71:A76"/>
+    <mergeCell ref="B71:B76"/>
     <mergeCell ref="A60:A64"/>
     <mergeCell ref="B60:B64"/>
     <mergeCell ref="A3:A5"/>
@@ -33147,17 +33215,17 @@
     <mergeCell ref="B18:B24"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A13:A16"/>
-    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="D73:D76"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="B144:B146"/>
+    <mergeCell ref="A126:A134"/>
+    <mergeCell ref="B126:B134"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="B135:B136"/>
     <mergeCell ref="A140:A142"/>
     <mergeCell ref="B140:B142"/>
-    <mergeCell ref="A124:A130"/>
-    <mergeCell ref="B124:B130"/>
-    <mergeCell ref="A131:A132"/>
-    <mergeCell ref="B131:B132"/>
-    <mergeCell ref="A136:A138"/>
-    <mergeCell ref="B136:B138"/>
     <mergeCell ref="A30:A35"/>
     <mergeCell ref="B30:B35"/>
     <mergeCell ref="A36:A43"/>

</xml_diff>

<commit_message>
updated employers guide to paye link
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="431">
   <si>
     <t>Document</t>
   </si>
@@ -3155,6 +3155,12 @@
   </si>
   <si>
     <t>Code 4006</t>
+  </si>
+  <si>
+    <t>Gross Pay</t>
+  </si>
+  <si>
+    <t>Updated link to the new Employer's Guide to PAYE</t>
   </si>
 </sst>
 </file>
@@ -4184,38 +4190,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4238,6 +4214,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4259,41 +4295,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4301,38 +4310,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4349,23 +4346,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5379,7 +5385,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5389,7 +5395,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5499,10 +5505,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="159" t="s">
+      <c r="A7" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5513,8 +5519,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="159"/>
-      <c r="B8" s="160"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="173"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5523,8 +5529,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="159"/>
-      <c r="B9" s="160"/>
+      <c r="A9" s="174"/>
+      <c r="B9" s="173"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5533,8 +5539,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="159"/>
-      <c r="B10" s="160"/>
+      <c r="A10" s="174"/>
+      <c r="B10" s="173"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5543,8 +5549,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="159"/>
-      <c r="B11" s="160"/>
+      <c r="A11" s="174"/>
+      <c r="B11" s="173"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5553,8 +5559,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="159"/>
-      <c r="B12" s="160"/>
+      <c r="A12" s="174"/>
+      <c r="B12" s="173"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5563,10 +5569,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="162" t="s">
+      <c r="A13" s="176" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5577,8 +5583,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="162"/>
-      <c r="B14" s="160"/>
+      <c r="A14" s="176"/>
+      <c r="B14" s="173"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5587,8 +5593,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="162"/>
-      <c r="B15" s="160"/>
+      <c r="A15" s="176"/>
+      <c r="B15" s="173"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5597,10 +5603,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="163" t="s">
+      <c r="A16" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="164" t="s">
+      <c r="B16" s="168" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5611,8 +5617,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="163"/>
-      <c r="B17" s="164"/>
+      <c r="A17" s="159"/>
+      <c r="B17" s="168"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5621,8 +5627,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="163"/>
-      <c r="B18" s="164"/>
+      <c r="A18" s="159"/>
+      <c r="B18" s="168"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5631,8 +5637,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="163"/>
-      <c r="B19" s="164"/>
+      <c r="A19" s="159"/>
+      <c r="B19" s="168"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5641,8 +5647,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="163"/>
-      <c r="B20" s="164"/>
+      <c r="A20" s="159"/>
+      <c r="B20" s="168"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5651,8 +5657,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="163"/>
-      <c r="B21" s="164"/>
+      <c r="A21" s="159"/>
+      <c r="B21" s="168"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5661,8 +5667,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="163"/>
-      <c r="B22" s="164"/>
+      <c r="A22" s="159"/>
+      <c r="B22" s="168"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5671,8 +5677,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="163"/>
-      <c r="B23" s="164"/>
+      <c r="A23" s="159"/>
+      <c r="B23" s="168"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5681,26 +5687,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="163"/>
-      <c r="B24" s="164"/>
-      <c r="C24" s="163" t="s">
+      <c r="A24" s="159"/>
+      <c r="B24" s="168"/>
+      <c r="C24" s="159" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="170" t="s">
+      <c r="D24" s="160" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="163"/>
-      <c r="B25" s="164"/>
-      <c r="C25" s="163"/>
-      <c r="D25" s="170"/>
+      <c r="A25" s="159"/>
+      <c r="B25" s="168"/>
+      <c r="C25" s="159"/>
+      <c r="D25" s="160"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="159" t="s">
+      <c r="A26" s="174" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="160" t="s">
+      <c r="B26" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5711,8 +5717,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="159"/>
-      <c r="B27" s="160"/>
+      <c r="A27" s="174"/>
+      <c r="B27" s="173"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5739,28 +5745,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="161" t="s">
+      <c r="A30" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="160" t="s">
+      <c r="B30" s="173" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="163" t="s">
+      <c r="C30" s="159" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="173" t="s">
+      <c r="D30" s="163" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="161"/>
-      <c r="B31" s="160"/>
-      <c r="C31" s="163"/>
-      <c r="D31" s="173"/>
+      <c r="A31" s="175"/>
+      <c r="B31" s="173"/>
+      <c r="C31" s="159"/>
+      <c r="D31" s="163"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="161"/>
-      <c r="B32" s="160"/>
+      <c r="A32" s="175"/>
+      <c r="B32" s="173"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5769,8 +5775,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="161"/>
-      <c r="B33" s="160"/>
+      <c r="A33" s="175"/>
+      <c r="B33" s="173"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5779,8 +5785,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="161"/>
-      <c r="B34" s="160"/>
+      <c r="A34" s="175"/>
+      <c r="B34" s="173"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5789,8 +5795,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="161"/>
-      <c r="B35" s="160"/>
+      <c r="A35" s="175"/>
+      <c r="B35" s="173"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5799,8 +5805,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="161"/>
-      <c r="B36" s="160"/>
+      <c r="A36" s="175"/>
+      <c r="B36" s="173"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5809,26 +5815,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="161"/>
-      <c r="B37" s="160"/>
-      <c r="C37" s="174" t="s">
+      <c r="A37" s="175"/>
+      <c r="B37" s="173"/>
+      <c r="C37" s="164" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="176" t="s">
+      <c r="D37" s="166" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="161"/>
-      <c r="B38" s="160"/>
-      <c r="C38" s="175"/>
-      <c r="D38" s="176"/>
+      <c r="A38" s="175"/>
+      <c r="B38" s="173"/>
+      <c r="C38" s="165"/>
+      <c r="D38" s="166"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="159" t="s">
+      <c r="A39" s="174" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5839,8 +5845,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="159"/>
-      <c r="B40" s="160"/>
+      <c r="A40" s="174"/>
+      <c r="B40" s="173"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5867,10 +5873,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="161" t="s">
+      <c r="A43" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="160" t="s">
+      <c r="B43" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5879,8 +5885,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="161"/>
-      <c r="B44" s="160"/>
+      <c r="A44" s="175"/>
+      <c r="B44" s="173"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5889,10 +5895,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="167" t="s">
+      <c r="A45" s="170" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="160" t="s">
+      <c r="B45" s="173" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5901,8 +5907,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="168"/>
-      <c r="B46" s="160"/>
+      <c r="A46" s="171"/>
+      <c r="B46" s="173"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5911,8 +5917,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="168"/>
-      <c r="B47" s="160"/>
+      <c r="A47" s="171"/>
+      <c r="B47" s="173"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5921,8 +5927,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="169"/>
-      <c r="B48" s="160"/>
+      <c r="A48" s="172"/>
+      <c r="B48" s="173"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5931,10 +5937,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="164" t="s">
+      <c r="A49" s="168" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="164" t="s">
+      <c r="B49" s="168" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10038,8 +10044,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="164"/>
-      <c r="B50" s="164"/>
+      <c r="A50" s="168"/>
+      <c r="B50" s="168"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14143,8 +14149,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="164"/>
-      <c r="B51" s="164"/>
+      <c r="A51" s="168"/>
+      <c r="B51" s="168"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18248,8 +18254,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="164"/>
-      <c r="B52" s="164"/>
+      <c r="A52" s="168"/>
+      <c r="B52" s="168"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22353,12 +22359,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="164"/>
-      <c r="B53" s="164"/>
-      <c r="C53" s="172" t="s">
+      <c r="A53" s="168"/>
+      <c r="B53" s="168"/>
+      <c r="C53" s="162" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="173" t="s">
+      <c r="D53" s="163" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26458,10 +26464,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="164"/>
-      <c r="B54" s="164"/>
-      <c r="C54" s="172"/>
-      <c r="D54" s="173"/>
+      <c r="A54" s="168"/>
+      <c r="B54" s="168"/>
+      <c r="C54" s="162"/>
+      <c r="D54" s="163"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30579,10 +30585,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="165" t="s">
+      <c r="A57" s="167" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="164" t="s">
+      <c r="B57" s="168" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30593,8 +30599,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="165"/>
-      <c r="B58" s="164"/>
+      <c r="A58" s="167"/>
+      <c r="B58" s="168"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30603,8 +30609,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="165"/>
-      <c r="B59" s="164"/>
+      <c r="A59" s="167"/>
+      <c r="B59" s="168"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30613,8 +30619,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="165"/>
-      <c r="B60" s="164"/>
+      <c r="A60" s="167"/>
+      <c r="B60" s="168"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30623,8 +30629,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="165"/>
-      <c r="B61" s="164"/>
+      <c r="A61" s="167"/>
+      <c r="B61" s="168"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30633,8 +30639,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="165"/>
-      <c r="B62" s="164"/>
+      <c r="A62" s="167"/>
+      <c r="B62" s="168"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30643,8 +30649,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="165"/>
-      <c r="B63" s="164"/>
+      <c r="A63" s="167"/>
+      <c r="B63" s="168"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30653,16 +30659,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="165"/>
-      <c r="B64" s="164"/>
+      <c r="A64" s="167"/>
+      <c r="B64" s="168"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="165"/>
-      <c r="B65" s="164"/>
+      <c r="A65" s="167"/>
+      <c r="B65" s="168"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30671,16 +30677,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="165"/>
-      <c r="B66" s="164"/>
+      <c r="A66" s="167"/>
+      <c r="B66" s="168"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="165"/>
-      <c r="B67" s="164"/>
+      <c r="A67" s="167"/>
+      <c r="B67" s="168"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30689,8 +30695,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="165"/>
-      <c r="B68" s="164"/>
+      <c r="A68" s="167"/>
+      <c r="B68" s="168"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30699,8 +30705,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="165"/>
-      <c r="B69" s="164"/>
+      <c r="A69" s="167"/>
+      <c r="B69" s="168"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30709,8 +30715,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="165"/>
-      <c r="B70" s="164"/>
+      <c r="A70" s="167"/>
+      <c r="B70" s="168"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30719,8 +30725,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="165"/>
-      <c r="B71" s="164"/>
+      <c r="A71" s="167"/>
+      <c r="B71" s="168"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30729,8 +30735,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="165"/>
-      <c r="B72" s="164"/>
+      <c r="A72" s="167"/>
+      <c r="B72" s="168"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30739,16 +30745,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="165"/>
-      <c r="B73" s="164"/>
+      <c r="A73" s="167"/>
+      <c r="B73" s="168"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="165"/>
-      <c r="B74" s="164"/>
+      <c r="A74" s="167"/>
+      <c r="B74" s="168"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30757,18 +30763,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="165"/>
-      <c r="B75" s="164"/>
-      <c r="C75" s="171"/>
-      <c r="D75" s="166" t="s">
+      <c r="A75" s="167"/>
+      <c r="B75" s="168"/>
+      <c r="C75" s="161"/>
+      <c r="D75" s="169" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="165"/>
-      <c r="B76" s="164"/>
-      <c r="C76" s="171"/>
-      <c r="D76" s="166"/>
+      <c r="A76" s="167"/>
+      <c r="B76" s="168"/>
+      <c r="C76" s="161"/>
+      <c r="D76" s="169"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30792,8 +30798,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30802,29 +30808,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30839,6 +30829,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30892,10 +30898,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="159" t="s">
+      <c r="A4" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="173" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30906,133 +30912,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="159"/>
-      <c r="B5" s="160"/>
-      <c r="C5" s="186" t="s">
+      <c r="A5" s="174"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="185" t="s">
+      <c r="D5" s="183" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="159"/>
-      <c r="B6" s="160"/>
-      <c r="C6" s="186"/>
-      <c r="D6" s="185"/>
+      <c r="A6" s="174"/>
+      <c r="B6" s="173"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="183"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="159"/>
-      <c r="B7" s="160"/>
+      <c r="A7" s="174"/>
+      <c r="B7" s="173"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="159"/>
-      <c r="B8" s="160"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="173"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="159"/>
-      <c r="B9" s="160"/>
+      <c r="A9" s="174"/>
+      <c r="B9" s="173"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="162" t="s">
+      <c r="A10" s="176" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="160" t="s">
+      <c r="B10" s="173" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="184"/>
-      <c r="D10" s="185" t="s">
+      <c r="C10" s="186"/>
+      <c r="D10" s="183" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="162"/>
-      <c r="B11" s="160"/>
-      <c r="C11" s="184"/>
-      <c r="D11" s="185"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="173"/>
+      <c r="C11" s="186"/>
+      <c r="D11" s="183"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="162"/>
-      <c r="B12" s="160"/>
-      <c r="C12" s="184"/>
-      <c r="D12" s="185"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="173"/>
+      <c r="C12" s="186"/>
+      <c r="D12" s="183"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="163" t="s">
+      <c r="A13" s="159" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="168" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="187"/>
-      <c r="D13" s="185" t="s">
+      <c r="C13" s="185"/>
+      <c r="D13" s="183" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="163"/>
-      <c r="B14" s="164"/>
-      <c r="C14" s="187"/>
-      <c r="D14" s="185"/>
+      <c r="A14" s="159"/>
+      <c r="B14" s="168"/>
+      <c r="C14" s="185"/>
+      <c r="D14" s="183"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
-      <c r="B15" s="164"/>
-      <c r="C15" s="187"/>
+      <c r="A15" s="159"/>
+      <c r="B15" s="168"/>
+      <c r="C15" s="185"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="163"/>
-      <c r="B16" s="164"/>
-      <c r="C16" s="187"/>
+      <c r="A16" s="159"/>
+      <c r="B16" s="168"/>
+      <c r="C16" s="185"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="163"/>
-      <c r="B17" s="164"/>
-      <c r="C17" s="187"/>
+      <c r="A17" s="159"/>
+      <c r="B17" s="168"/>
+      <c r="C17" s="185"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="163"/>
-      <c r="B18" s="164"/>
-      <c r="C18" s="187"/>
+      <c r="A18" s="159"/>
+      <c r="B18" s="168"/>
+      <c r="C18" s="185"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="163"/>
-      <c r="B19" s="164"/>
-      <c r="C19" s="187"/>
+      <c r="A19" s="159"/>
+      <c r="B19" s="168"/>
+      <c r="C19" s="185"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="163"/>
-      <c r="B20" s="164"/>
-      <c r="C20" s="187"/>
+      <c r="A20" s="159"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="185"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="163"/>
-      <c r="B21" s="164"/>
-      <c r="C21" s="187"/>
+      <c r="A21" s="159"/>
+      <c r="B21" s="168"/>
+      <c r="C21" s="185"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="163"/>
-      <c r="B22" s="164"/>
-      <c r="C22" s="187"/>
+      <c r="A22" s="159"/>
+      <c r="B22" s="168"/>
+      <c r="C22" s="185"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="163"/>
-      <c r="B23" s="164"/>
-      <c r="C23" s="187"/>
+      <c r="A23" s="159"/>
+      <c r="B23" s="168"/>
+      <c r="C23" s="185"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31130,10 +31136,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="188" t="s">
+      <c r="A32" s="177" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="191" t="s">
+      <c r="B32" s="180" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31144,26 +31150,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="189"/>
-      <c r="B33" s="192"/>
+      <c r="A33" s="178"/>
+      <c r="B33" s="181"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="189"/>
-      <c r="B34" s="192"/>
+      <c r="A34" s="178"/>
+      <c r="B34" s="181"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="189"/>
-      <c r="B35" s="192"/>
+      <c r="A35" s="178"/>
+      <c r="B35" s="181"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="190"/>
-      <c r="B36" s="193"/>
+      <c r="A36" s="179"/>
+      <c r="B36" s="182"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31192,10 +31198,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="161" t="s">
+      <c r="A39" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="173" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31206,8 +31212,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="161"/>
-      <c r="B40" s="160"/>
+      <c r="A40" s="175"/>
+      <c r="B40" s="173"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31216,84 +31222,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="159" t="s">
+      <c r="A41" s="174" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="160" t="s">
+      <c r="B41" s="173" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="184" t="s">
+      <c r="C41" s="186" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="163" t="s">
+      <c r="D41" s="159" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="159"/>
-      <c r="B42" s="160"/>
-      <c r="C42" s="184"/>
-      <c r="D42" s="163"/>
+      <c r="A42" s="174"/>
+      <c r="B42" s="173"/>
+      <c r="C42" s="186"/>
+      <c r="D42" s="159"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="159"/>
-      <c r="B43" s="160"/>
-      <c r="C43" s="184" t="s">
+      <c r="A43" s="174"/>
+      <c r="B43" s="173"/>
+      <c r="C43" s="186" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="166" t="s">
+      <c r="D43" s="169" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="159"/>
-      <c r="B44" s="160"/>
-      <c r="C44" s="184"/>
-      <c r="D44" s="166"/>
+      <c r="A44" s="174"/>
+      <c r="B44" s="173"/>
+      <c r="C44" s="186"/>
+      <c r="D44" s="169"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="165" t="s">
+      <c r="A45" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="164" t="s">
+      <c r="B45" s="168" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="180"/>
+      <c r="C45" s="190"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="165"/>
-      <c r="B46" s="164"/>
-      <c r="C46" s="181"/>
-      <c r="D46" s="177" t="s">
+      <c r="A46" s="167"/>
+      <c r="B46" s="168"/>
+      <c r="C46" s="191"/>
+      <c r="D46" s="187" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="165"/>
-      <c r="B47" s="164"/>
-      <c r="C47" s="181"/>
-      <c r="D47" s="178"/>
+      <c r="A47" s="167"/>
+      <c r="B47" s="168"/>
+      <c r="C47" s="191"/>
+      <c r="D47" s="188"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="165"/>
-      <c r="B48" s="164"/>
-      <c r="C48" s="182"/>
-      <c r="D48" s="178"/>
+      <c r="A48" s="167"/>
+      <c r="B48" s="168"/>
+      <c r="C48" s="192"/>
+      <c r="D48" s="188"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="165"/>
-      <c r="B49" s="164"/>
-      <c r="C49" s="172"/>
-      <c r="D49" s="178"/>
+      <c r="A49" s="167"/>
+      <c r="B49" s="168"/>
+      <c r="C49" s="162"/>
+      <c r="D49" s="188"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="165"/>
-      <c r="B50" s="164"/>
-      <c r="C50" s="172"/>
-      <c r="D50" s="179"/>
+      <c r="A50" s="167"/>
+      <c r="B50" s="168"/>
+      <c r="C50" s="162"/>
+      <c r="D50" s="189"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31316,10 +31322,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="164" t="s">
+      <c r="A53" s="168" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="164" t="s">
+      <c r="B53" s="168" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31330,8 +31336,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="164"/>
-      <c r="B54" s="164"/>
+      <c r="A54" s="168"/>
+      <c r="B54" s="168"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31340,8 +31346,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="164"/>
-      <c r="B55" s="164"/>
+      <c r="A55" s="168"/>
+      <c r="B55" s="168"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31350,9 +31356,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="164"/>
-      <c r="B56" s="164"/>
-      <c r="C56" s="183" t="s">
+      <c r="A56" s="168"/>
+      <c r="B56" s="168"/>
+      <c r="C56" s="193" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31360,16 +31366,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="164"/>
-      <c r="B57" s="164"/>
-      <c r="C57" s="183"/>
+      <c r="A57" s="168"/>
+      <c r="B57" s="168"/>
+      <c r="C57" s="193"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="164"/>
-      <c r="B58" s="164"/>
+      <c r="A58" s="168"/>
+      <c r="B58" s="168"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31378,8 +31384,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="164"/>
-      <c r="B59" s="164"/>
+      <c r="A59" s="168"/>
+      <c r="B59" s="168"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31388,9 +31394,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="164"/>
-      <c r="B60" s="164"/>
-      <c r="C60" s="183" t="s">
+      <c r="A60" s="168"/>
+      <c r="B60" s="168"/>
+      <c r="C60" s="193" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31398,25 +31404,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="164"/>
-      <c r="B61" s="164"/>
-      <c r="C61" s="183"/>
+      <c r="A61" s="168"/>
+      <c r="B61" s="168"/>
+      <c r="C61" s="193"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="164"/>
-      <c r="B62" s="164"/>
-      <c r="C62" s="183"/>
+      <c r="A62" s="168"/>
+      <c r="B62" s="168"/>
+      <c r="C62" s="193"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="164"/>
-      <c r="B63" s="164"/>
-      <c r="C63" s="184" t="s">
+      <c r="A63" s="168"/>
+      <c r="B63" s="168"/>
+      <c r="C63" s="186" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31424,30 +31430,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="164"/>
-      <c r="B64" s="164"/>
-      <c r="C64" s="184"/>
-      <c r="D64" s="166" t="s">
+      <c r="A64" s="168"/>
+      <c r="B64" s="168"/>
+      <c r="C64" s="186"/>
+      <c r="D64" s="169" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="164"/>
-      <c r="B65" s="164"/>
-      <c r="C65" s="184"/>
-      <c r="D65" s="166"/>
+      <c r="A65" s="168"/>
+      <c r="B65" s="168"/>
+      <c r="C65" s="186"/>
+      <c r="D65" s="169"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="164"/>
-      <c r="B66" s="164"/>
-      <c r="C66" s="184"/>
-      <c r="D66" s="166"/>
+      <c r="A66" s="168"/>
+      <c r="B66" s="168"/>
+      <c r="C66" s="186"/>
+      <c r="D66" s="169"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="164"/>
-      <c r="B67" s="164"/>
-      <c r="C67" s="184"/>
-      <c r="D67" s="166"/>
+      <c r="A67" s="168"/>
+      <c r="B67" s="168"/>
+      <c r="C67" s="186"/>
+      <c r="D67" s="169"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31503,23 +31509,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31536,6 +31525,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31544,10 +31550,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D159"/>
+  <dimension ref="A1:D160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74:D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31581,10 +31587,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="209" t="s">
+      <c r="A3" s="206" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="210" t="s">
+      <c r="B3" s="207" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="112" t="s">
@@ -31595,8 +31601,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="209"/>
-      <c r="B4" s="210"/>
+      <c r="A4" s="206"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="112" t="s">
         <v>347</v>
       </c>
@@ -31605,8 +31611,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="209"/>
-      <c r="B5" s="210"/>
+      <c r="A5" s="206"/>
+      <c r="B5" s="207"/>
       <c r="C5" s="112" t="s">
         <v>343</v>
       </c>
@@ -31623,10 +31629,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="163" t="s">
+      <c r="A7" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="183" t="s">
+      <c r="B7" s="193" t="s">
         <v>234</v>
       </c>
       <c r="C7" s="58"/>
@@ -31635,8 +31641,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="163"/>
-      <c r="B8" s="183"/>
+      <c r="A8" s="159"/>
+      <c r="B8" s="193"/>
       <c r="C8" s="104" t="s">
         <v>235</v>
       </c>
@@ -31699,10 +31705,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="163" t="s">
+      <c r="A13" s="159" t="s">
         <v>275</v>
       </c>
-      <c r="B13" s="183" t="s">
+      <c r="B13" s="193" t="s">
         <v>234</v>
       </c>
       <c r="C13" s="58"/>
@@ -31711,16 +31717,16 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="163"/>
-      <c r="B14" s="183"/>
+      <c r="A14" s="159"/>
+      <c r="B14" s="193"/>
       <c r="C14" s="58"/>
       <c r="D14" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="163"/>
-      <c r="B15" s="183"/>
+      <c r="A15" s="159"/>
+      <c r="B15" s="193"/>
       <c r="C15" s="108" t="s">
         <v>325</v>
       </c>
@@ -31729,8 +31735,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="163"/>
-      <c r="B16" s="183"/>
+      <c r="A16" s="159"/>
+      <c r="B16" s="193"/>
       <c r="C16" s="136" t="s">
         <v>404</v>
       </c>
@@ -31751,10 +31757,10 @@
       <c r="D17" s="58"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="211" t="s">
+      <c r="A18" s="208" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="196" t="s">
+      <c r="B18" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C18" s="58"/>
@@ -31763,8 +31769,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="212"/>
-      <c r="B19" s="203"/>
+      <c r="A19" s="209"/>
+      <c r="B19" s="202"/>
       <c r="C19" s="118" t="s">
         <v>361</v>
       </c>
@@ -31773,8 +31779,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="212"/>
-      <c r="B20" s="203"/>
+      <c r="A20" s="209"/>
+      <c r="B20" s="202"/>
       <c r="C20" s="118" t="s">
         <v>359</v>
       </c>
@@ -31783,8 +31789,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="212"/>
-      <c r="B21" s="203"/>
+      <c r="A21" s="209"/>
+      <c r="B21" s="202"/>
       <c r="C21" s="124" t="s">
         <v>367</v>
       </c>
@@ -31793,8 +31799,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="212"/>
-      <c r="B22" s="203"/>
+      <c r="A22" s="209"/>
+      <c r="B22" s="202"/>
       <c r="C22" s="131" t="s">
         <v>359</v>
       </c>
@@ -31803,8 +31809,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="212"/>
-      <c r="B23" s="203"/>
+      <c r="A23" s="209"/>
+      <c r="B23" s="202"/>
       <c r="C23" s="135" t="s">
         <v>371</v>
       </c>
@@ -31813,8 +31819,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="213"/>
-      <c r="B24" s="197"/>
+      <c r="A24" s="210"/>
+      <c r="B24" s="198"/>
       <c r="C24" s="135" t="s">
         <v>359</v>
       </c>
@@ -31849,10 +31855,10 @@
       <c r="D26" s="98"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="207" t="s">
+      <c r="A27" s="194" t="s">
         <v>369</v>
       </c>
-      <c r="B27" s="196" t="s">
+      <c r="B27" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C27" s="136" t="s">
@@ -31861,8 +31867,8 @@
       <c r="D27" s="98"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="214"/>
-      <c r="B28" s="197"/>
+      <c r="A28" s="196"/>
+      <c r="B28" s="198"/>
       <c r="C28" s="136" t="s">
         <v>404</v>
       </c>
@@ -31879,10 +31885,10 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="207" t="s">
+      <c r="A30" s="194" t="s">
         <v>237</v>
       </c>
-      <c r="B30" s="196" t="s">
+      <c r="B30" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C30" s="58"/>
@@ -31891,24 +31897,24 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="208"/>
-      <c r="B31" s="203"/>
+      <c r="A31" s="195"/>
+      <c r="B31" s="202"/>
       <c r="C31" s="58"/>
       <c r="D31" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="208"/>
-      <c r="B32" s="203"/>
+      <c r="A32" s="195"/>
+      <c r="B32" s="202"/>
       <c r="C32" s="58"/>
       <c r="D32" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="208"/>
-      <c r="B33" s="203"/>
+      <c r="A33" s="195"/>
+      <c r="B33" s="202"/>
       <c r="C33" s="58" t="s">
         <v>300</v>
       </c>
@@ -31917,8 +31923,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="208"/>
-      <c r="B34" s="203"/>
+      <c r="A34" s="195"/>
+      <c r="B34" s="202"/>
       <c r="C34" s="58" t="s">
         <v>328</v>
       </c>
@@ -31927,8 +31933,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="214"/>
-      <c r="B35" s="197"/>
+      <c r="A35" s="196"/>
+      <c r="B35" s="198"/>
       <c r="C35" s="58" t="s">
         <v>373</v>
       </c>
@@ -31937,10 +31943,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="167" t="s">
+      <c r="A36" s="170" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="196" t="s">
+      <c r="B36" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C36" s="58" t="s">
@@ -31951,16 +31957,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="168"/>
-      <c r="B37" s="203"/>
+      <c r="A37" s="171"/>
+      <c r="B37" s="202"/>
       <c r="C37" s="58"/>
       <c r="D37" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="168"/>
-      <c r="B38" s="203"/>
+      <c r="A38" s="171"/>
+      <c r="B38" s="202"/>
       <c r="C38" s="106" t="s">
         <v>329</v>
       </c>
@@ -31969,8 +31975,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="168"/>
-      <c r="B39" s="203"/>
+      <c r="A39" s="171"/>
+      <c r="B39" s="202"/>
       <c r="C39" s="106" t="s">
         <v>359</v>
       </c>
@@ -31979,8 +31985,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="168"/>
-      <c r="B40" s="203"/>
+      <c r="A40" s="171"/>
+      <c r="B40" s="202"/>
       <c r="C40" s="106" t="s">
         <v>367</v>
       </c>
@@ -31989,8 +31995,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="168"/>
-      <c r="B41" s="203"/>
+      <c r="A41" s="171"/>
+      <c r="B41" s="202"/>
       <c r="C41" s="106" t="s">
         <v>371</v>
       </c>
@@ -31999,8 +32005,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="168"/>
-      <c r="B42" s="203"/>
+      <c r="A42" s="171"/>
+      <c r="B42" s="202"/>
       <c r="C42" s="106" t="s">
         <v>381</v>
       </c>
@@ -32009,8 +32015,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="169"/>
-      <c r="B43" s="197"/>
+      <c r="A43" s="172"/>
+      <c r="B43" s="198"/>
       <c r="C43" s="96" t="s">
         <v>359</v>
       </c>
@@ -32019,13 +32025,13 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="174" t="s">
+      <c r="A44" s="164" t="s">
         <v>222</v>
       </c>
-      <c r="B44" s="196" t="s">
+      <c r="B44" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="218" t="s">
+      <c r="C44" s="204" t="s">
         <v>239</v>
       </c>
       <c r="D44" s="101" t="s">
@@ -32033,17 +32039,17 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="202"/>
-      <c r="B45" s="203"/>
-      <c r="C45" s="219"/>
+      <c r="A45" s="203"/>
+      <c r="B45" s="202"/>
+      <c r="C45" s="205"/>
       <c r="D45" s="98" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="202"/>
-      <c r="B46" s="203"/>
-      <c r="C46" s="201" t="s">
+      <c r="A46" s="203"/>
+      <c r="B46" s="202"/>
+      <c r="C46" s="211" t="s">
         <v>240</v>
       </c>
       <c r="D46" s="58" t="s">
@@ -32051,16 +32057,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="202"/>
-      <c r="B47" s="203"/>
-      <c r="C47" s="201"/>
+      <c r="A47" s="203"/>
+      <c r="B47" s="202"/>
+      <c r="C47" s="211"/>
       <c r="D47" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="202"/>
-      <c r="B48" s="203"/>
+      <c r="A48" s="203"/>
+      <c r="B48" s="202"/>
       <c r="C48" s="103" t="s">
         <v>307</v>
       </c>
@@ -32069,8 +32075,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="202"/>
-      <c r="B49" s="203"/>
+      <c r="A49" s="203"/>
+      <c r="B49" s="202"/>
       <c r="C49" s="103">
         <v>2.1</v>
       </c>
@@ -32079,8 +32085,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="202"/>
-      <c r="B50" s="203"/>
+      <c r="A50" s="203"/>
+      <c r="B50" s="202"/>
       <c r="C50" s="103" t="s">
         <v>239</v>
       </c>
@@ -32089,8 +32095,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="202"/>
-      <c r="B51" s="203"/>
+      <c r="A51" s="203"/>
+      <c r="B51" s="202"/>
       <c r="C51" s="114" t="s">
         <v>239</v>
       </c>
@@ -32099,8 +32105,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="202"/>
-      <c r="B52" s="203"/>
+      <c r="A52" s="203"/>
+      <c r="B52" s="202"/>
       <c r="C52" s="128" t="s">
         <v>239</v>
       </c>
@@ -32109,8 +32115,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="202"/>
-      <c r="B53" s="203"/>
+      <c r="A53" s="203"/>
+      <c r="B53" s="202"/>
       <c r="C53" s="134" t="s">
         <v>378</v>
       </c>
@@ -32119,8 +32125,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="202"/>
-      <c r="B54" s="203"/>
+      <c r="A54" s="203"/>
+      <c r="B54" s="202"/>
       <c r="C54" s="136">
         <v>2.1</v>
       </c>
@@ -32129,8 +32135,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="202"/>
-      <c r="B55" s="203"/>
+      <c r="A55" s="203"/>
+      <c r="B55" s="202"/>
       <c r="C55" s="136" t="s">
         <v>239</v>
       </c>
@@ -32139,8 +32145,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="202"/>
-      <c r="B56" s="203"/>
+      <c r="A56" s="203"/>
+      <c r="B56" s="202"/>
       <c r="C56" s="141" t="s">
         <v>239</v>
       </c>
@@ -32149,10 +32155,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="204" t="s">
+      <c r="A57" s="212" t="s">
         <v>296</v>
       </c>
-      <c r="B57" s="196" t="s">
+      <c r="B57" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -32163,8 +32169,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="205"/>
-      <c r="B58" s="203"/>
+      <c r="A58" s="213"/>
+      <c r="B58" s="202"/>
       <c r="C58" s="61" t="s">
         <v>281</v>
       </c>
@@ -32173,8 +32179,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="206"/>
-      <c r="B59" s="197"/>
+      <c r="A59" s="214"/>
+      <c r="B59" s="198"/>
       <c r="C59" s="58" t="s">
         <v>350</v>
       </c>
@@ -32183,10 +32189,10 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="207" t="s">
+      <c r="A60" s="194" t="s">
         <v>370</v>
       </c>
-      <c r="B60" s="196" t="s">
+      <c r="B60" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C60" s="128" t="s">
@@ -32195,8 +32201,8 @@
       <c r="D60" s="58"/>
     </row>
     <row r="61" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="208"/>
-      <c r="B61" s="203"/>
+      <c r="A61" s="195"/>
+      <c r="B61" s="202"/>
       <c r="C61" s="131" t="s">
         <v>378</v>
       </c>
@@ -32205,8 +32211,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="208"/>
-      <c r="B62" s="203"/>
+      <c r="A62" s="195"/>
+      <c r="B62" s="202"/>
       <c r="C62" s="136">
         <v>2.1</v>
       </c>
@@ -32215,8 +32221,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="208"/>
-      <c r="B63" s="203"/>
+      <c r="A63" s="195"/>
+      <c r="B63" s="202"/>
       <c r="C63" s="136" t="s">
         <v>240</v>
       </c>
@@ -32225,8 +32231,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="208"/>
-      <c r="B64" s="203"/>
+      <c r="A64" s="195"/>
+      <c r="B64" s="202"/>
       <c r="C64" s="133" t="s">
         <v>239</v>
       </c>
@@ -32255,10 +32261,10 @@
       <c r="D66" s="98"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="174" t="s">
+      <c r="A67" s="164" t="s">
         <v>260</v>
       </c>
-      <c r="B67" s="196" t="s">
+      <c r="B67" s="197" t="s">
         <v>234</v>
       </c>
       <c r="C67" s="58"/>
@@ -32267,24 +32273,24 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="202"/>
-      <c r="B68" s="203"/>
+      <c r="A68" s="203"/>
+      <c r="B68" s="202"/>
       <c r="C68" s="58"/>
       <c r="D68" s="58" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="202"/>
-      <c r="B69" s="203"/>
+      <c r="A69" s="203"/>
+      <c r="B69" s="202"/>
       <c r="C69" s="58"/>
       <c r="D69" s="98" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="202"/>
-      <c r="B70" s="203"/>
+      <c r="A70" s="203"/>
+      <c r="B70" s="202"/>
       <c r="C70" s="58" t="s">
         <v>424</v>
       </c>
@@ -32293,558 +32299,554 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="163" t="s">
+      <c r="A71" s="203"/>
+      <c r="B71" s="202"/>
+      <c r="C71" s="58" t="s">
+        <v>429</v>
+      </c>
+      <c r="D71" s="98" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="159" t="s">
         <v>334</v>
       </c>
-      <c r="B71" s="183" t="s">
+      <c r="B72" s="193" t="s">
         <v>234</v>
       </c>
-      <c r="C71" s="79" t="s">
+      <c r="C72" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D71" s="98" t="s">
+      <c r="D72" s="98" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="163"/>
-      <c r="B72" s="183"/>
-      <c r="C72" s="58" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="159"/>
+      <c r="B73" s="193"/>
+      <c r="C73" s="58" t="s">
         <v>411</v>
       </c>
-      <c r="D72" s="58" t="s">
+      <c r="D73" s="58" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="163"/>
-      <c r="B73" s="183"/>
-      <c r="C73" s="140" t="s">
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="159"/>
+      <c r="B74" s="193"/>
+      <c r="C74" s="140" t="s">
         <v>414</v>
       </c>
-      <c r="D73" s="207" t="s">
+      <c r="D74" s="194" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="163"/>
-      <c r="B74" s="183"/>
-      <c r="C74" s="140" t="s">
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="159"/>
+      <c r="B75" s="193"/>
+      <c r="C75" s="140" t="s">
         <v>415</v>
       </c>
-      <c r="D74" s="208"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="163"/>
-      <c r="B75" s="183"/>
-      <c r="C75" s="140" t="s">
+      <c r="D75" s="195"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="159"/>
+      <c r="B76" s="193"/>
+      <c r="C76" s="140" t="s">
         <v>416</v>
       </c>
-      <c r="D75" s="208"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="163"/>
-      <c r="B76" s="183"/>
-      <c r="C76" s="140" t="s">
+      <c r="D76" s="195"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="159"/>
+      <c r="B77" s="193"/>
+      <c r="C77" s="140" t="s">
         <v>417</v>
       </c>
-      <c r="D76" s="214"/>
-    </row>
-    <row r="77" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="96" t="s">
+      <c r="D77" s="196"/>
+    </row>
+    <row r="78" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="B77" s="122" t="s">
+      <c r="B78" s="122" t="s">
         <v>234</v>
       </c>
-      <c r="C77" s="104" t="s">
+      <c r="C78" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="D77" s="102" t="s">
+      <c r="D78" s="102" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="204" t="s">
+    <row r="79" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="212" t="s">
         <v>32</v>
       </c>
-      <c r="B78" s="196" t="s">
+      <c r="B79" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C78" s="58" t="s">
+      <c r="C79" s="58" t="s">
         <v>268</v>
-      </c>
-      <c r="D78" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="205"/>
-      <c r="B79" s="203"/>
-      <c r="C79" s="58" t="s">
-        <v>270</v>
       </c>
       <c r="D79" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="205"/>
-      <c r="B80" s="203"/>
+      <c r="A80" s="213"/>
+      <c r="B80" s="202"/>
       <c r="C80" s="58" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D80" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="205"/>
-      <c r="B81" s="203"/>
-      <c r="C81" s="98" t="s">
+      <c r="A81" s="213"/>
+      <c r="B81" s="202"/>
+      <c r="C81" s="58" t="s">
+        <v>269</v>
+      </c>
+      <c r="D81" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="213"/>
+      <c r="B82" s="202"/>
+      <c r="C82" s="98" t="s">
         <v>277</v>
       </c>
-      <c r="D81" s="98" t="s">
+      <c r="D82" s="98" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="205"/>
-      <c r="B82" s="203"/>
-      <c r="C82" s="58" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="213"/>
+      <c r="B83" s="202"/>
+      <c r="C83" s="58" t="s">
         <v>282</v>
       </c>
-      <c r="D82" s="58" t="s">
+      <c r="D83" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="205"/>
-      <c r="B83" s="203"/>
-      <c r="C83" s="58" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="213"/>
+      <c r="B84" s="202"/>
+      <c r="C84" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="D83" s="58" t="s">
+      <c r="D84" s="58" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="205"/>
-      <c r="B84" s="203"/>
-      <c r="C84" s="98" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="213"/>
+      <c r="B85" s="202"/>
+      <c r="C85" s="98" t="s">
         <v>288</v>
-      </c>
-      <c r="D84" s="98" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="205"/>
-      <c r="B85" s="203"/>
-      <c r="C85" s="98" t="s">
-        <v>302</v>
       </c>
       <c r="D85" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="205"/>
-      <c r="B86" s="203"/>
+      <c r="A86" s="213"/>
+      <c r="B86" s="202"/>
       <c r="C86" s="98" t="s">
+        <v>302</v>
+      </c>
+      <c r="D86" s="98" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="213"/>
+      <c r="B87" s="202"/>
+      <c r="C87" s="98" t="s">
         <v>289</v>
       </c>
-      <c r="D86" s="98" t="s">
+      <c r="D87" s="98" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="205"/>
-      <c r="B87" s="203"/>
-      <c r="C87" s="105" t="s">
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="213"/>
+      <c r="B88" s="202"/>
+      <c r="C88" s="105" t="s">
         <v>244</v>
       </c>
-      <c r="D87" s="102" t="s">
+      <c r="D88" s="102" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="205"/>
-      <c r="B88" s="203"/>
-      <c r="C88" s="106" t="s">
+    <row r="89" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="213"/>
+      <c r="B89" s="202"/>
+      <c r="C89" s="106" t="s">
         <v>311</v>
       </c>
-      <c r="D88" s="98" t="s">
+      <c r="D89" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="205"/>
-      <c r="B89" s="203"/>
-      <c r="C89" s="58" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="213"/>
+      <c r="B90" s="202"/>
+      <c r="C90" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="D89" s="58" t="s">
+      <c r="D90" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="205"/>
-      <c r="B90" s="203"/>
-      <c r="C90" s="98" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="213"/>
+      <c r="B91" s="202"/>
+      <c r="C91" s="98" t="s">
         <v>313</v>
       </c>
-      <c r="D90" s="98" t="s">
+      <c r="D91" s="98" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="205"/>
-      <c r="B91" s="203"/>
-      <c r="C91" s="98" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="213"/>
+      <c r="B92" s="202"/>
+      <c r="C92" s="98" t="s">
         <v>315</v>
-      </c>
-      <c r="D91" s="98" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="205"/>
-      <c r="B92" s="203"/>
-      <c r="C92" s="98" t="s">
-        <v>268</v>
       </c>
       <c r="D92" s="98" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="205"/>
-      <c r="B93" s="203"/>
-      <c r="C93" s="58" t="s">
+      <c r="A93" s="213"/>
+      <c r="B93" s="202"/>
+      <c r="C93" s="98" t="s">
+        <v>268</v>
+      </c>
+      <c r="D93" s="98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="213"/>
+      <c r="B94" s="202"/>
+      <c r="C94" s="58" t="s">
         <v>318</v>
       </c>
-      <c r="D93" s="58" t="s">
+      <c r="D94" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="205"/>
-      <c r="B94" s="203"/>
-      <c r="C94" s="98" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="213"/>
+      <c r="B95" s="202"/>
+      <c r="C95" s="98" t="s">
         <v>283</v>
       </c>
-      <c r="D94" s="98" t="s">
+      <c r="D95" s="98" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="205"/>
-      <c r="B95" s="203"/>
-      <c r="C95" s="98" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="213"/>
+      <c r="B96" s="202"/>
+      <c r="C96" s="98" t="s">
         <v>319</v>
       </c>
-      <c r="D95" s="98" t="s">
+      <c r="D96" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="205"/>
-      <c r="B96" s="203"/>
-      <c r="C96" s="58"/>
-      <c r="D96" s="107" t="s">
+    <row r="97" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="213"/>
+      <c r="B97" s="202"/>
+      <c r="C97" s="58"/>
+      <c r="D97" s="107" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="205"/>
-      <c r="B97" s="203"/>
-      <c r="C97" s="98" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="213"/>
+      <c r="B98" s="202"/>
+      <c r="C98" s="98" t="s">
         <v>322</v>
-      </c>
-      <c r="D97" s="98" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="205"/>
-      <c r="B98" s="203"/>
-      <c r="C98" s="98" t="s">
-        <v>268</v>
       </c>
       <c r="D98" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="205"/>
-      <c r="B99" s="203"/>
+      <c r="A99" s="213"/>
+      <c r="B99" s="202"/>
       <c r="C99" s="98" t="s">
-        <v>339</v>
+        <v>268</v>
       </c>
       <c r="D99" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="205"/>
-      <c r="B100" s="203"/>
+      <c r="A100" s="213"/>
+      <c r="B100" s="202"/>
       <c r="C100" s="98" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D100" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="205"/>
-      <c r="B101" s="203"/>
+      <c r="A101" s="213"/>
+      <c r="B101" s="202"/>
       <c r="C101" s="98" t="s">
+        <v>340</v>
+      </c>
+      <c r="D101" s="98" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="213"/>
+      <c r="B102" s="202"/>
+      <c r="C102" s="98" t="s">
         <v>324</v>
       </c>
-      <c r="D101" s="98" t="s">
+      <c r="D102" s="98" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="205"/>
-      <c r="B102" s="203"/>
-      <c r="C102" s="113" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="213"/>
+      <c r="B103" s="202"/>
+      <c r="C103" s="113" t="s">
         <v>345</v>
       </c>
-      <c r="D102" s="113" t="s">
+      <c r="D103" s="113" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="205"/>
-      <c r="B103" s="203"/>
-      <c r="C103" s="98" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="213"/>
+      <c r="B104" s="202"/>
+      <c r="C104" s="98" t="s">
         <v>338</v>
       </c>
-      <c r="D103" s="98" t="s">
+      <c r="D104" s="98" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="205"/>
-      <c r="B104" s="203"/>
-      <c r="C104" s="98" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="213"/>
+      <c r="B105" s="202"/>
+      <c r="C105" s="98" t="s">
         <v>353</v>
       </c>
-      <c r="D104" s="98" t="s">
+      <c r="D105" s="98" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="205"/>
-      <c r="B105" s="203"/>
-      <c r="C105" s="117" t="s">
+    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="213"/>
+      <c r="B106" s="202"/>
+      <c r="C106" s="117" t="s">
         <v>356</v>
       </c>
-      <c r="D105" s="116" t="s">
+      <c r="D106" s="116" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="205"/>
-      <c r="B106" s="203"/>
-      <c r="C106" s="98" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="213"/>
+      <c r="B107" s="202"/>
+      <c r="C107" s="98" t="s">
         <v>357</v>
       </c>
-      <c r="D106" s="98" t="s">
+      <c r="D107" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="205"/>
-      <c r="B107" s="203"/>
-      <c r="C107" s="98" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="213"/>
+      <c r="B108" s="202"/>
+      <c r="C108" s="98" t="s">
         <v>358</v>
       </c>
-      <c r="D107" s="98" t="s">
+      <c r="D108" s="98" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="205"/>
-      <c r="B108" s="203"/>
-      <c r="C108" s="98" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="213"/>
+      <c r="B109" s="202"/>
+      <c r="C109" s="98" t="s">
         <v>364</v>
       </c>
-      <c r="D108" s="98" t="s">
+      <c r="D109" s="98" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="205"/>
-      <c r="B109" s="203"/>
-      <c r="C109" s="98" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="213"/>
+      <c r="B110" s="202"/>
+      <c r="C110" s="98" t="s">
         <v>366</v>
-      </c>
-      <c r="D109" s="98" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="205"/>
-      <c r="B110" s="203"/>
-      <c r="C110" s="98" t="s">
-        <v>372</v>
       </c>
       <c r="D110" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="205"/>
-      <c r="B111" s="203"/>
+      <c r="A111" s="213"/>
+      <c r="B111" s="202"/>
       <c r="C111" s="98" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="D111" s="98" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="205"/>
-      <c r="B112" s="203"/>
-      <c r="C112" s="113" t="s">
+      <c r="A112" s="213"/>
+      <c r="B112" s="202"/>
+      <c r="C112" s="98" t="s">
+        <v>364</v>
+      </c>
+      <c r="D112" s="98" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="213"/>
+      <c r="B113" s="202"/>
+      <c r="C113" s="113" t="s">
         <v>385</v>
       </c>
-      <c r="D112" s="113" t="s">
+      <c r="D113" s="113" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="205"/>
-      <c r="B113" s="203"/>
-      <c r="C113" s="58" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="213"/>
+      <c r="B114" s="202"/>
+      <c r="C114" s="58" t="s">
         <v>389</v>
       </c>
-      <c r="D113" s="58" t="s">
+      <c r="D114" s="58" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="205"/>
-      <c r="B114" s="203"/>
-      <c r="C114" s="58" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="213"/>
+      <c r="B115" s="202"/>
+      <c r="C115" s="58" t="s">
         <v>392</v>
       </c>
-      <c r="D114" s="58" t="s">
+      <c r="D115" s="58" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="205"/>
-      <c r="B115" s="203"/>
-      <c r="C115" s="58" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="213"/>
+      <c r="B116" s="202"/>
+      <c r="C116" s="58" t="s">
         <v>393</v>
-      </c>
-      <c r="D115" s="58" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="205"/>
-      <c r="B116" s="203"/>
-      <c r="C116" s="58" t="s">
-        <v>394</v>
       </c>
       <c r="D116" s="58" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="205"/>
-      <c r="B117" s="203"/>
+      <c r="A117" s="213"/>
+      <c r="B117" s="202"/>
       <c r="C117" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="D117" s="58" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="213"/>
+      <c r="B118" s="202"/>
+      <c r="C118" s="58" t="s">
         <v>395</v>
-      </c>
-      <c r="D117" s="58" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="205"/>
-      <c r="B118" s="203"/>
-      <c r="C118" s="58" t="s">
-        <v>396</v>
       </c>
       <c r="D118" s="58" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="205"/>
-      <c r="B119" s="203"/>
+      <c r="A119" s="213"/>
+      <c r="B119" s="202"/>
       <c r="C119" s="58" t="s">
+        <v>396</v>
+      </c>
+      <c r="D119" s="58" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="213"/>
+      <c r="B120" s="202"/>
+      <c r="C120" s="58" t="s">
         <v>399</v>
-      </c>
-      <c r="D119" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="205"/>
-      <c r="B120" s="203"/>
-      <c r="C120" s="58" t="s">
-        <v>409</v>
       </c>
       <c r="D120" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="205"/>
-      <c r="B121" s="203"/>
+      <c r="A121" s="213"/>
+      <c r="B121" s="202"/>
       <c r="C121" s="58" t="s">
+        <v>409</v>
+      </c>
+      <c r="D121" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="213"/>
+      <c r="B122" s="202"/>
+      <c r="C122" s="58" t="s">
         <v>410</v>
       </c>
-      <c r="D121" s="58" t="s">
+      <c r="D122" s="58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="205"/>
-      <c r="B122" s="203"/>
-      <c r="C122" s="58" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="213"/>
+      <c r="B123" s="202"/>
+      <c r="C123" s="58" t="s">
         <v>427</v>
-      </c>
-      <c r="D122" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="206"/>
-      <c r="B123" s="197"/>
-      <c r="C123" s="58" t="s">
-        <v>428</v>
       </c>
       <c r="D123" s="58" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="143" t="s">
+      <c r="A124" s="214"/>
+      <c r="B124" s="198"/>
+      <c r="C124" s="58" t="s">
+        <v>428</v>
+      </c>
+      <c r="D124" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="143" t="s">
         <v>421</v>
       </c>
-      <c r="B124" s="142" t="s">
-        <v>234</v>
-      </c>
-      <c r="C124" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D124" s="98" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="96" t="s">
-        <v>309</v>
-      </c>
-      <c r="B125" s="123" t="s">
+      <c r="B125" s="142" t="s">
         <v>234</v>
       </c>
       <c r="C125" s="58" t="s">
@@ -32854,9 +32856,9 @@
         <v>274</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="96" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B126" s="123" t="s">
         <v>234</v>
@@ -32868,366 +32870,385 @@
         <v>274</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="39" t="s">
+    <row r="127" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="96" t="s">
+        <v>310</v>
+      </c>
+      <c r="B127" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C127" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D127" s="98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B127" s="39"/>
-      <c r="C127" s="39"/>
-      <c r="D127" s="44"/>
-    </row>
-    <row r="128" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="174" t="s">
+      <c r="B128" s="39"/>
+      <c r="C128" s="39"/>
+      <c r="D128" s="44"/>
+    </row>
+    <row r="129" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="B128" s="196" t="s">
+      <c r="B129" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C128" s="58"/>
-      <c r="D128" s="79" t="s">
+      <c r="C129" s="58"/>
+      <c r="D129" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="202"/>
-      <c r="B129" s="203"/>
-      <c r="C129" s="104" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="203"/>
+      <c r="B130" s="202"/>
+      <c r="C130" s="104" t="s">
         <v>246</v>
       </c>
-      <c r="D129" s="58" t="s">
+      <c r="D130" s="58" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="202"/>
-      <c r="B130" s="203"/>
-      <c r="C130" s="104">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="203"/>
+      <c r="B131" s="202"/>
+      <c r="C131" s="104">
         <v>10.1</v>
-      </c>
-      <c r="D130" s="58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="202"/>
-      <c r="B131" s="203"/>
-      <c r="C131" s="104">
-        <v>10.199999999999999</v>
       </c>
       <c r="D131" s="58" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="202"/>
-      <c r="B132" s="203"/>
-      <c r="C132" s="109" t="s">
+      <c r="A132" s="203"/>
+      <c r="B132" s="202"/>
+      <c r="C132" s="104">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D132" s="58" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="203"/>
+      <c r="B133" s="202"/>
+      <c r="C133" s="109" t="s">
         <v>293</v>
       </c>
-      <c r="D132" s="99" t="s">
+      <c r="D133" s="99" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="202"/>
-      <c r="B133" s="203"/>
-      <c r="C133" s="109" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="203"/>
+      <c r="B134" s="202"/>
+      <c r="C134" s="109" t="s">
         <v>375</v>
       </c>
-      <c r="D133" s="99" t="s">
+      <c r="D134" s="99" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="202"/>
-      <c r="B134" s="203"/>
-      <c r="C134" s="109" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="203"/>
+      <c r="B135" s="202"/>
+      <c r="C135" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="D134" s="99" t="s">
+      <c r="D135" s="99" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="202"/>
-      <c r="B135" s="203"/>
-      <c r="C135" s="109" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="203"/>
+      <c r="B136" s="202"/>
+      <c r="C136" s="109" t="s">
         <v>422</v>
       </c>
-      <c r="D135" s="99" t="s">
+      <c r="D136" s="99" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="175"/>
-      <c r="B136" s="197"/>
-      <c r="C136" s="109" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="165"/>
+      <c r="B137" s="198"/>
+      <c r="C137" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="D136" s="99" t="s">
+      <c r="D137" s="99" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="174" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="164" t="s">
         <v>247</v>
       </c>
-      <c r="B137" s="196" t="s">
+      <c r="B138" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C137" s="183"/>
-      <c r="D137" s="198" t="s">
+      <c r="C138" s="193"/>
+      <c r="D138" s="217" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="175"/>
-      <c r="B138" s="197"/>
-      <c r="C138" s="183"/>
-      <c r="D138" s="198"/>
-    </row>
-    <row r="139" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="121" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="165"/>
+      <c r="B139" s="198"/>
+      <c r="C139" s="193"/>
+      <c r="D139" s="217"/>
+    </row>
+    <row r="140" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="121" t="s">
         <v>262</v>
       </c>
-      <c r="B139" s="123" t="s">
+      <c r="B140" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C139" s="104" t="s">
+      <c r="C140" s="104" t="s">
         <v>250</v>
       </c>
-      <c r="D139" s="98" t="s">
+      <c r="D140" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="95" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B140" s="39"/>
-      <c r="C140" s="97"/>
-      <c r="D140" s="97"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="96" t="s">
+      <c r="B141" s="39"/>
+      <c r="C141" s="97"/>
+      <c r="D141" s="97"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="B141" s="123" t="s">
+      <c r="B142" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C141" s="110" t="s">
+      <c r="C142" s="110" t="s">
         <v>265</v>
       </c>
-      <c r="D141" s="58" t="s">
+      <c r="D142" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="174" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="164" t="s">
         <v>285</v>
       </c>
-      <c r="B142" s="196" t="s">
+      <c r="B143" s="197" t="s">
         <v>234</v>
       </c>
-      <c r="C142" s="99" t="s">
+      <c r="C143" s="99" t="s">
         <v>295</v>
       </c>
-      <c r="D142" s="58" t="s">
+      <c r="D143" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="202"/>
-      <c r="B143" s="203"/>
-      <c r="C143" s="58" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="203"/>
+      <c r="B144" s="202"/>
+      <c r="C144" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D143" s="98" t="s">
+      <c r="D144" s="98" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A144" s="175"/>
-      <c r="B144" s="197"/>
-      <c r="C144" s="110" t="s">
+    <row r="145" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="165"/>
+      <c r="B145" s="198"/>
+      <c r="C145" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="D144" s="58" t="s">
+      <c r="D145" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="97" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="B145" s="97"/>
-      <c r="C145" s="97"/>
-      <c r="D145" s="97"/>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="215" t="s">
+      <c r="B146" s="97"/>
+      <c r="C146" s="97"/>
+      <c r="D146" s="97"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="199" t="s">
         <v>58</v>
       </c>
-      <c r="B146" s="196" t="s">
+      <c r="B147" s="197" t="s">
         <v>271</v>
       </c>
-      <c r="C146" s="110" t="s">
-        <v>265</v>
-      </c>
-      <c r="D146" s="58" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="216"/>
-      <c r="B147" s="203"/>
       <c r="C147" s="110" t="s">
         <v>265</v>
       </c>
       <c r="D147" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="200"/>
+      <c r="B148" s="202"/>
+      <c r="C148" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="D148" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="217"/>
-      <c r="B148" s="197"/>
-      <c r="C148" s="58"/>
-      <c r="D148" s="58" t="s">
+    <row r="149" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="201"/>
+      <c r="B149" s="198"/>
+      <c r="C149" s="58"/>
+      <c r="D149" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="194" t="s">
+    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="215" t="s">
         <v>59</v>
       </c>
-      <c r="B149" s="196" t="s">
+      <c r="B150" s="197" t="s">
         <v>271</v>
       </c>
-      <c r="C149" s="61" t="s">
+      <c r="C150" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D149" s="58" t="s">
+      <c r="D150" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="195"/>
-      <c r="B150" s="197"/>
-      <c r="C150" s="61"/>
-      <c r="D150" s="58" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="216"/>
+      <c r="B151" s="198"/>
+      <c r="C151" s="61"/>
+      <c r="D151" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A151" s="199" t="s">
+    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="218" t="s">
         <v>291</v>
       </c>
-      <c r="B151" s="196" t="s">
+      <c r="B152" s="197" t="s">
         <v>271</v>
       </c>
-      <c r="C151" s="61"/>
-      <c r="D151" s="61" t="s">
+      <c r="C152" s="61"/>
+      <c r="D152" s="61" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="200"/>
-      <c r="B152" s="197"/>
-      <c r="C152" s="58"/>
-      <c r="D152" s="58" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="219"/>
+      <c r="B153" s="198"/>
+      <c r="C153" s="58"/>
+      <c r="D153" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="194" t="s">
+    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="215" t="s">
         <v>60</v>
       </c>
-      <c r="B153" s="196" t="s">
+      <c r="B154" s="197" t="s">
         <v>271</v>
       </c>
-      <c r="C153" s="61" t="s">
+      <c r="C154" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D153" s="58" t="s">
+      <c r="D154" s="58" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="195"/>
-      <c r="B154" s="197"/>
-      <c r="C154" s="58"/>
-      <c r="D154" s="58" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="216"/>
+      <c r="B155" s="198"/>
+      <c r="C155" s="58"/>
+      <c r="D155" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="97" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="97" t="s">
         <v>273</v>
       </c>
-      <c r="B155" s="97"/>
-      <c r="C155" s="97"/>
-      <c r="D155" s="97"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="58"/>
-      <c r="B156" s="123" t="s">
+      <c r="B156" s="97"/>
+      <c r="C156" s="97"/>
+      <c r="D156" s="97"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="58"/>
+      <c r="B157" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C156" s="58" t="s">
+      <c r="C157" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D156" s="98" t="s">
+      <c r="D157" s="98" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="97" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="B157" s="97"/>
-      <c r="C157" s="97"/>
-      <c r="D157" s="97"/>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="58"/>
-      <c r="B158" s="137" t="s">
-        <v>234</v>
-      </c>
-      <c r="C158" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D158" s="98" t="s">
-        <v>274</v>
-      </c>
+      <c r="B158" s="97"/>
+      <c r="C158" s="97"/>
+      <c r="D158" s="97"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="58"/>
-      <c r="B159" s="123"/>
+      <c r="B159" s="137" t="s">
+        <v>234</v>
+      </c>
       <c r="C159" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D159" s="98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="58"/>
+      <c r="B160" s="123"/>
+      <c r="C160" s="58" t="s">
         <v>401</v>
       </c>
-      <c r="D159" s="98" t="s">
+      <c r="D160" s="98" t="s">
         <v>402</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D73:D76"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A146:A148"/>
-    <mergeCell ref="B146:B148"/>
-    <mergeCell ref="A128:A136"/>
-    <mergeCell ref="B128:B136"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="B137:B138"/>
-    <mergeCell ref="A142:A144"/>
-    <mergeCell ref="B142:B144"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="B36:B43"/>
-    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A154:A155"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="A152:A153"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="A79:A124"/>
+    <mergeCell ref="B79:B124"/>
+    <mergeCell ref="A44:A56"/>
+    <mergeCell ref="B44:B56"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A72:A77"/>
+    <mergeCell ref="B72:B77"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="B60:B64"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B7:B8"/>
@@ -33236,27 +33257,22 @@
     <mergeCell ref="B18:B24"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A13:A16"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="A78:A123"/>
-    <mergeCell ref="B78:B123"/>
-    <mergeCell ref="A44:A56"/>
-    <mergeCell ref="B44:B56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A71:A76"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="A153:A154"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="D137:D138"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="A151:A152"/>
-    <mergeCell ref="B151:B152"/>
-    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A147:A149"/>
+    <mergeCell ref="B147:B149"/>
+    <mergeCell ref="A129:A137"/>
+    <mergeCell ref="B129:B137"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="B143:B145"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="B36:B43"/>
+    <mergeCell ref="C44:C45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
corrected validation rule 5005
</commit_message>
<xml_diff>
--- a/Schema Publication Changelog.xlsx
+++ b/Schema Publication Changelog.xlsx
@@ -22,15 +22,15 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="433">
   <si>
     <t>Document</t>
   </si>
@@ -3161,6 +3161,12 @@
   </si>
   <si>
     <t>Updated link to the new Employer's Guide to PAYE</t>
+  </si>
+  <si>
+    <t>Code 5005</t>
+  </si>
+  <si>
+    <t>Corrected rule code</t>
   </si>
 </sst>
 </file>
@@ -4190,8 +4196,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4214,66 +4250,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4295,14 +4271,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4310,26 +4313,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4346,32 +4361,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5385,7 +5391,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5395,7 +5401,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5505,10 +5511,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="174" t="s">
+      <c r="A7" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="173" t="s">
+      <c r="B7" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5519,8 +5525,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="174"/>
-      <c r="B8" s="173"/>
+      <c r="A8" s="159"/>
+      <c r="B8" s="160"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5529,8 +5535,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="174"/>
-      <c r="B9" s="173"/>
+      <c r="A9" s="159"/>
+      <c r="B9" s="160"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5539,8 +5545,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="174"/>
-      <c r="B10" s="173"/>
+      <c r="A10" s="159"/>
+      <c r="B10" s="160"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5549,8 +5555,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="174"/>
-      <c r="B11" s="173"/>
+      <c r="A11" s="159"/>
+      <c r="B11" s="160"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5559,8 +5565,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="174"/>
-      <c r="B12" s="173"/>
+      <c r="A12" s="159"/>
+      <c r="B12" s="160"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5569,10 +5575,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="176" t="s">
+      <c r="A13" s="162" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="173" t="s">
+      <c r="B13" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5583,8 +5589,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="176"/>
-      <c r="B14" s="173"/>
+      <c r="A14" s="162"/>
+      <c r="B14" s="160"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5593,8 +5599,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="176"/>
-      <c r="B15" s="173"/>
+      <c r="A15" s="162"/>
+      <c r="B15" s="160"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5603,10 +5609,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="163" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="168" t="s">
+      <c r="B16" s="164" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5617,8 +5623,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="159"/>
-      <c r="B17" s="168"/>
+      <c r="A17" s="163"/>
+      <c r="B17" s="164"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5627,8 +5633,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="159"/>
-      <c r="B18" s="168"/>
+      <c r="A18" s="163"/>
+      <c r="B18" s="164"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5637,8 +5643,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="159"/>
-      <c r="B19" s="168"/>
+      <c r="A19" s="163"/>
+      <c r="B19" s="164"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5647,8 +5653,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="159"/>
-      <c r="B20" s="168"/>
+      <c r="A20" s="163"/>
+      <c r="B20" s="164"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5657,8 +5663,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="159"/>
-      <c r="B21" s="168"/>
+      <c r="A21" s="163"/>
+      <c r="B21" s="164"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5667,8 +5673,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="159"/>
-      <c r="B22" s="168"/>
+      <c r="A22" s="163"/>
+      <c r="B22" s="164"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5677,8 +5683,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="159"/>
-      <c r="B23" s="168"/>
+      <c r="A23" s="163"/>
+      <c r="B23" s="164"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5687,26 +5693,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="159"/>
-      <c r="B24" s="168"/>
-      <c r="C24" s="159" t="s">
+      <c r="A24" s="163"/>
+      <c r="B24" s="164"/>
+      <c r="C24" s="163" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="160" t="s">
+      <c r="D24" s="170" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="159"/>
-      <c r="B25" s="168"/>
-      <c r="C25" s="159"/>
-      <c r="D25" s="160"/>
+      <c r="A25" s="163"/>
+      <c r="B25" s="164"/>
+      <c r="C25" s="163"/>
+      <c r="D25" s="170"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="174" t="s">
+      <c r="A26" s="159" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="173" t="s">
+      <c r="B26" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5717,8 +5723,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="174"/>
-      <c r="B27" s="173"/>
+      <c r="A27" s="159"/>
+      <c r="B27" s="160"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5745,28 +5751,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="175" t="s">
+      <c r="A30" s="161" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="173" t="s">
+      <c r="B30" s="160" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="159" t="s">
+      <c r="C30" s="163" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="163" t="s">
+      <c r="D30" s="173" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="175"/>
-      <c r="B31" s="173"/>
-      <c r="C31" s="159"/>
-      <c r="D31" s="163"/>
+      <c r="A31" s="161"/>
+      <c r="B31" s="160"/>
+      <c r="C31" s="163"/>
+      <c r="D31" s="173"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="175"/>
-      <c r="B32" s="173"/>
+      <c r="A32" s="161"/>
+      <c r="B32" s="160"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5775,8 +5781,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="175"/>
-      <c r="B33" s="173"/>
+      <c r="A33" s="161"/>
+      <c r="B33" s="160"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5785,8 +5791,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="175"/>
-      <c r="B34" s="173"/>
+      <c r="A34" s="161"/>
+      <c r="B34" s="160"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5795,8 +5801,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="175"/>
-      <c r="B35" s="173"/>
+      <c r="A35" s="161"/>
+      <c r="B35" s="160"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5805,8 +5811,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="175"/>
-      <c r="B36" s="173"/>
+      <c r="A36" s="161"/>
+      <c r="B36" s="160"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5815,26 +5821,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="175"/>
-      <c r="B37" s="173"/>
-      <c r="C37" s="164" t="s">
+      <c r="A37" s="161"/>
+      <c r="B37" s="160"/>
+      <c r="C37" s="174" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="166" t="s">
+      <c r="D37" s="176" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="175"/>
-      <c r="B38" s="173"/>
-      <c r="C38" s="165"/>
-      <c r="D38" s="166"/>
+      <c r="A38" s="161"/>
+      <c r="B38" s="160"/>
+      <c r="C38" s="175"/>
+      <c r="D38" s="176"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="174" t="s">
+      <c r="A39" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="173" t="s">
+      <c r="B39" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5845,8 +5851,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="174"/>
-      <c r="B40" s="173"/>
+      <c r="A40" s="159"/>
+      <c r="B40" s="160"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5873,10 +5879,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="175" t="s">
+      <c r="A43" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="173" t="s">
+      <c r="B43" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5885,8 +5891,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="175"/>
-      <c r="B44" s="173"/>
+      <c r="A44" s="161"/>
+      <c r="B44" s="160"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5895,10 +5901,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="170" t="s">
+      <c r="A45" s="167" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="173" t="s">
+      <c r="B45" s="160" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5907,8 +5913,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="171"/>
-      <c r="B46" s="173"/>
+      <c r="A46" s="168"/>
+      <c r="B46" s="160"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5917,8 +5923,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="171"/>
-      <c r="B47" s="173"/>
+      <c r="A47" s="168"/>
+      <c r="B47" s="160"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5927,8 +5933,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="172"/>
-      <c r="B48" s="173"/>
+      <c r="A48" s="169"/>
+      <c r="B48" s="160"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5937,10 +5943,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="168" t="s">
+      <c r="A49" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="168" t="s">
+      <c r="B49" s="164" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10044,8 +10050,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="168"/>
-      <c r="B50" s="168"/>
+      <c r="A50" s="164"/>
+      <c r="B50" s="164"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14149,8 +14155,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="168"/>
-      <c r="B51" s="168"/>
+      <c r="A51" s="164"/>
+      <c r="B51" s="164"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18254,8 +18260,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="168"/>
-      <c r="B52" s="168"/>
+      <c r="A52" s="164"/>
+      <c r="B52" s="164"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22359,12 +22365,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="168"/>
-      <c r="B53" s="168"/>
-      <c r="C53" s="162" t="s">
+      <c r="A53" s="164"/>
+      <c r="B53" s="164"/>
+      <c r="C53" s="172" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="163" t="s">
+      <c r="D53" s="173" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26464,10 +26470,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="168"/>
-      <c r="B54" s="168"/>
-      <c r="C54" s="162"/>
-      <c r="D54" s="163"/>
+      <c r="A54" s="164"/>
+      <c r="B54" s="164"/>
+      <c r="C54" s="172"/>
+      <c r="D54" s="173"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30585,10 +30591,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="167" t="s">
+      <c r="A57" s="165" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="168" t="s">
+      <c r="B57" s="164" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30599,8 +30605,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="167"/>
-      <c r="B58" s="168"/>
+      <c r="A58" s="165"/>
+      <c r="B58" s="164"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30609,8 +30615,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="167"/>
-      <c r="B59" s="168"/>
+      <c r="A59" s="165"/>
+      <c r="B59" s="164"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30619,8 +30625,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="167"/>
-      <c r="B60" s="168"/>
+      <c r="A60" s="165"/>
+      <c r="B60" s="164"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30629,8 +30635,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="167"/>
-      <c r="B61" s="168"/>
+      <c r="A61" s="165"/>
+      <c r="B61" s="164"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30639,8 +30645,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="167"/>
-      <c r="B62" s="168"/>
+      <c r="A62" s="165"/>
+      <c r="B62" s="164"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30649,8 +30655,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="167"/>
-      <c r="B63" s="168"/>
+      <c r="A63" s="165"/>
+      <c r="B63" s="164"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30659,16 +30665,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="167"/>
-      <c r="B64" s="168"/>
+      <c r="A64" s="165"/>
+      <c r="B64" s="164"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="167"/>
-      <c r="B65" s="168"/>
+      <c r="A65" s="165"/>
+      <c r="B65" s="164"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30677,16 +30683,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="167"/>
-      <c r="B66" s="168"/>
+      <c r="A66" s="165"/>
+      <c r="B66" s="164"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="167"/>
-      <c r="B67" s="168"/>
+      <c r="A67" s="165"/>
+      <c r="B67" s="164"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30695,8 +30701,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="167"/>
-      <c r="B68" s="168"/>
+      <c r="A68" s="165"/>
+      <c r="B68" s="164"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30705,8 +30711,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="167"/>
-      <c r="B69" s="168"/>
+      <c r="A69" s="165"/>
+      <c r="B69" s="164"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30715,8 +30721,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="167"/>
-      <c r="B70" s="168"/>
+      <c r="A70" s="165"/>
+      <c r="B70" s="164"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30725,8 +30731,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="167"/>
-      <c r="B71" s="168"/>
+      <c r="A71" s="165"/>
+      <c r="B71" s="164"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30735,8 +30741,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="167"/>
-      <c r="B72" s="168"/>
+      <c r="A72" s="165"/>
+      <c r="B72" s="164"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30745,16 +30751,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="167"/>
-      <c r="B73" s="168"/>
+      <c r="A73" s="165"/>
+      <c r="B73" s="164"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="167"/>
-      <c r="B74" s="168"/>
+      <c r="A74" s="165"/>
+      <c r="B74" s="164"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30763,18 +30769,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="167"/>
-      <c r="B75" s="168"/>
-      <c r="C75" s="161"/>
-      <c r="D75" s="169" t="s">
+      <c r="A75" s="165"/>
+      <c r="B75" s="164"/>
+      <c r="C75" s="171"/>
+      <c r="D75" s="166" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="167"/>
-      <c r="B76" s="168"/>
-      <c r="C76" s="161"/>
-      <c r="D76" s="169"/>
+      <c r="A76" s="165"/>
+      <c r="B76" s="164"/>
+      <c r="C76" s="171"/>
+      <c r="D76" s="166"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30798,8 +30804,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30808,13 +30814,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30829,22 +30851,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30898,10 +30904,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="174" t="s">
+      <c r="A4" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="173" t="s">
+      <c r="B4" s="160" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30912,133 +30918,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="174"/>
-      <c r="B5" s="173"/>
-      <c r="C5" s="184" t="s">
+      <c r="A5" s="159"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="186" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="183" t="s">
+      <c r="D5" s="185" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="174"/>
-      <c r="B6" s="173"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="183"/>
+      <c r="A6" s="159"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="186"/>
+      <c r="D6" s="185"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="174"/>
-      <c r="B7" s="173"/>
+      <c r="A7" s="159"/>
+      <c r="B7" s="160"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="174"/>
-      <c r="B8" s="173"/>
+      <c r="A8" s="159"/>
+      <c r="B8" s="160"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="174"/>
-      <c r="B9" s="173"/>
+      <c r="A9" s="159"/>
+      <c r="B9" s="160"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="162" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="173" t="s">
+      <c r="B10" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="186"/>
-      <c r="D10" s="183" t="s">
+      <c r="C10" s="184"/>
+      <c r="D10" s="185" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="176"/>
-      <c r="B11" s="173"/>
-      <c r="C11" s="186"/>
-      <c r="D11" s="183"/>
+      <c r="A11" s="162"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="184"/>
+      <c r="D11" s="185"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="176"/>
-      <c r="B12" s="173"/>
-      <c r="C12" s="186"/>
-      <c r="D12" s="183"/>
+      <c r="A12" s="162"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="184"/>
+      <c r="D12" s="185"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="159" t="s">
+      <c r="A13" s="163" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="168" t="s">
+      <c r="B13" s="164" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="185"/>
-      <c r="D13" s="183" t="s">
+      <c r="C13" s="187"/>
+      <c r="D13" s="185" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="159"/>
-      <c r="B14" s="168"/>
-      <c r="C14" s="185"/>
-      <c r="D14" s="183"/>
+      <c r="A14" s="163"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="187"/>
+      <c r="D14" s="185"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="159"/>
-      <c r="B15" s="168"/>
-      <c r="C15" s="185"/>
+      <c r="A15" s="163"/>
+      <c r="B15" s="164"/>
+      <c r="C15" s="187"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="159"/>
-      <c r="B16" s="168"/>
-      <c r="C16" s="185"/>
+      <c r="A16" s="163"/>
+      <c r="B16" s="164"/>
+      <c r="C16" s="187"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="159"/>
-      <c r="B17" s="168"/>
-      <c r="C17" s="185"/>
+      <c r="A17" s="163"/>
+      <c r="B17" s="164"/>
+      <c r="C17" s="187"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="159"/>
-      <c r="B18" s="168"/>
-      <c r="C18" s="185"/>
+      <c r="A18" s="163"/>
+      <c r="B18" s="164"/>
+      <c r="C18" s="187"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="159"/>
-      <c r="B19" s="168"/>
-      <c r="C19" s="185"/>
+      <c r="A19" s="163"/>
+      <c r="B19" s="164"/>
+      <c r="C19" s="187"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="159"/>
-      <c r="B20" s="168"/>
-      <c r="C20" s="185"/>
+      <c r="A20" s="163"/>
+      <c r="B20" s="164"/>
+      <c r="C20" s="187"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="159"/>
-      <c r="B21" s="168"/>
-      <c r="C21" s="185"/>
+      <c r="A21" s="163"/>
+      <c r="B21" s="164"/>
+      <c r="C21" s="187"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="159"/>
-      <c r="B22" s="168"/>
-      <c r="C22" s="185"/>
+      <c r="A22" s="163"/>
+      <c r="B22" s="164"/>
+      <c r="C22" s="187"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="159"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="185"/>
+      <c r="A23" s="163"/>
+      <c r="B23" s="164"/>
+      <c r="C23" s="187"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31136,10 +31142,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="177" t="s">
+      <c r="A32" s="188" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="180" t="s">
+      <c r="B32" s="191" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31150,26 +31156,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="178"/>
-      <c r="B33" s="181"/>
+      <c r="A33" s="189"/>
+      <c r="B33" s="192"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="178"/>
-      <c r="B34" s="181"/>
+      <c r="A34" s="189"/>
+      <c r="B34" s="192"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="178"/>
-      <c r="B35" s="181"/>
+      <c r="A35" s="189"/>
+      <c r="B35" s="192"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="179"/>
-      <c r="B36" s="182"/>
+      <c r="A36" s="190"/>
+      <c r="B36" s="193"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31198,10 +31204,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="175" t="s">
+      <c r="A39" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="173" t="s">
+      <c r="B39" s="160" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31212,8 +31218,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="175"/>
-      <c r="B40" s="173"/>
+      <c r="A40" s="161"/>
+      <c r="B40" s="160"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31222,84 +31228,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="174" t="s">
+      <c r="A41" s="159" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="173" t="s">
+      <c r="B41" s="160" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="186" t="s">
+      <c r="C41" s="184" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="159" t="s">
+      <c r="D41" s="163" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="174"/>
-      <c r="B42" s="173"/>
-      <c r="C42" s="186"/>
-      <c r="D42" s="159"/>
+      <c r="A42" s="159"/>
+      <c r="B42" s="160"/>
+      <c r="C42" s="184"/>
+      <c r="D42" s="163"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="174"/>
-      <c r="B43" s="173"/>
-      <c r="C43" s="186" t="s">
+      <c r="A43" s="159"/>
+      <c r="B43" s="160"/>
+      <c r="C43" s="184" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="169" t="s">
+      <c r="D43" s="166" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="174"/>
-      <c r="B44" s="173"/>
-      <c r="C44" s="186"/>
-      <c r="D44" s="169"/>
+      <c r="A44" s="159"/>
+      <c r="B44" s="160"/>
+      <c r="C44" s="184"/>
+      <c r="D44" s="166"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="167" t="s">
+      <c r="A45" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="168" t="s">
+      <c r="B45" s="164" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="190"/>
+      <c r="C45" s="180"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="167"/>
-      <c r="B46" s="168"/>
-      <c r="C46" s="191"/>
-      <c r="D46" s="187" t="s">
+      <c r="A46" s="165"/>
+      <c r="B46" s="164"/>
+      <c r="C46" s="181"/>
+      <c r="D46" s="177" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="167"/>
-      <c r="B47" s="168"/>
-      <c r="C47" s="191"/>
-      <c r="D47" s="188"/>
+      <c r="A47" s="165"/>
+      <c r="B47" s="164"/>
+      <c r="C47" s="181"/>
+      <c r="D47" s="178"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="167"/>
-      <c r="B48" s="168"/>
-      <c r="C48" s="192"/>
-      <c r="D48" s="188"/>
+      <c r="A48" s="165"/>
+      <c r="B48" s="164"/>
+      <c r="C48" s="182"/>
+      <c r="D48" s="178"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="167"/>
-      <c r="B49" s="168"/>
-      <c r="C49" s="162"/>
-      <c r="D49" s="188"/>
+      <c r="A49" s="165"/>
+      <c r="B49" s="164"/>
+      <c r="C49" s="172"/>
+      <c r="D49" s="178"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="167"/>
-      <c r="B50" s="168"/>
-      <c r="C50" s="162"/>
-      <c r="D50" s="189"/>
+      <c r="A50" s="165"/>
+      <c r="B50" s="164"/>
+      <c r="C50" s="172"/>
+      <c r="D50" s="179"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31322,10 +31328,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="168" t="s">
+      <c r="A53" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="168" t="s">
+      <c r="B53" s="164" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31336,8 +31342,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="168"/>
-      <c r="B54" s="168"/>
+      <c r="A54" s="164"/>
+      <c r="B54" s="164"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31346,8 +31352,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="168"/>
-      <c r="B55" s="168"/>
+      <c r="A55" s="164"/>
+      <c r="B55" s="164"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31356,9 +31362,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="168"/>
-      <c r="B56" s="168"/>
-      <c r="C56" s="193" t="s">
+      <c r="A56" s="164"/>
+      <c r="B56" s="164"/>
+      <c r="C56" s="183" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31366,16 +31372,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="168"/>
-      <c r="B57" s="168"/>
-      <c r="C57" s="193"/>
+      <c r="A57" s="164"/>
+      <c r="B57" s="164"/>
+      <c r="C57" s="183"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="168"/>
-      <c r="B58" s="168"/>
+      <c r="A58" s="164"/>
+      <c r="B58" s="164"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31384,8 +31390,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="168"/>
-      <c r="B59" s="168"/>
+      <c r="A59" s="164"/>
+      <c r="B59" s="164"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31394,9 +31400,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="168"/>
-      <c r="B60" s="168"/>
-      <c r="C60" s="193" t="s">
+      <c r="A60" s="164"/>
+      <c r="B60" s="164"/>
+      <c r="C60" s="183" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31404,25 +31410,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="168"/>
-      <c r="B61" s="168"/>
-      <c r="C61" s="193"/>
+      <c r="A61" s="164"/>
+      <c r="B61" s="164"/>
+      <c r="C61" s="183"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="168"/>
-      <c r="B62" s="168"/>
-      <c r="C62" s="193"/>
+      <c r="A62" s="164"/>
+      <c r="B62" s="164"/>
+      <c r="C62" s="183"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="168"/>
-      <c r="B63" s="168"/>
-      <c r="C63" s="186" t="s">
+      <c r="A63" s="164"/>
+      <c r="B63" s="164"/>
+      <c r="C63" s="184" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31430,30 +31436,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="168"/>
-      <c r="B64" s="168"/>
-      <c r="C64" s="186"/>
-      <c r="D64" s="169" t="s">
+      <c r="A64" s="164"/>
+      <c r="B64" s="164"/>
+      <c r="C64" s="184"/>
+      <c r="D64" s="166" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="168"/>
-      <c r="B65" s="168"/>
-      <c r="C65" s="186"/>
-      <c r="D65" s="169"/>
+      <c r="A65" s="164"/>
+      <c r="B65" s="164"/>
+      <c r="C65" s="184"/>
+      <c r="D65" s="166"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="168"/>
-      <c r="B66" s="168"/>
-      <c r="C66" s="186"/>
-      <c r="D66" s="169"/>
+      <c r="A66" s="164"/>
+      <c r="B66" s="164"/>
+      <c r="C66" s="184"/>
+      <c r="D66" s="166"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="168"/>
-      <c r="B67" s="168"/>
-      <c r="C67" s="186"/>
-      <c r="D67" s="169"/>
+      <c r="A67" s="164"/>
+      <c r="B67" s="164"/>
+      <c r="C67" s="184"/>
+      <c r="D67" s="166"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31509,6 +31515,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31525,23 +31548,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31550,10 +31556,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74:D77"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31587,10 +31593,10 @@
       <c r="D2" s="44"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="206" t="s">
+      <c r="A3" s="209" t="s">
         <v>342</v>
       </c>
-      <c r="B3" s="207" t="s">
+      <c r="B3" s="210" t="s">
         <v>234</v>
       </c>
       <c r="C3" s="112" t="s">
@@ -31601,8 +31607,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="206"/>
-      <c r="B4" s="207"/>
+      <c r="A4" s="209"/>
+      <c r="B4" s="210"/>
       <c r="C4" s="112" t="s">
         <v>347</v>
       </c>
@@ -31611,8 +31617,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="206"/>
-      <c r="B5" s="207"/>
+      <c r="A5" s="209"/>
+      <c r="B5" s="210"/>
       <c r="C5" s="112" t="s">
         <v>343</v>
       </c>
@@ -31629,10 +31635,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="159" t="s">
+      <c r="A7" s="163" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="183" t="s">
         <v>234</v>
       </c>
       <c r="C7" s="58"/>
@@ -31641,8 +31647,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="159"/>
-      <c r="B8" s="193"/>
+      <c r="A8" s="163"/>
+      <c r="B8" s="183"/>
       <c r="C8" s="104" t="s">
         <v>235</v>
       </c>
@@ -31705,10 +31711,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="159" t="s">
+      <c r="A13" s="163" t="s">
         <v>275</v>
       </c>
-      <c r="B13" s="193" t="s">
+      <c r="B13" s="183" t="s">
         <v>234</v>
       </c>
       <c r="C13" s="58"/>
@@ -31717,16 +31723,16 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="159"/>
-      <c r="B14" s="193"/>
+      <c r="A14" s="163"/>
+      <c r="B14" s="183"/>
       <c r="C14" s="58"/>
       <c r="D14" s="58" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="159"/>
-      <c r="B15" s="193"/>
+      <c r="A15" s="163"/>
+      <c r="B15" s="183"/>
       <c r="C15" s="108" t="s">
         <v>325</v>
       </c>
@@ -31735,8 +31741,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="159"/>
-      <c r="B16" s="193"/>
+      <c r="A16" s="163"/>
+      <c r="B16" s="183"/>
       <c r="C16" s="136" t="s">
         <v>404</v>
       </c>
@@ -31757,10 +31763,10 @@
       <c r="D17" s="58"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="208" t="s">
+      <c r="A18" s="211" t="s">
         <v>165</v>
       </c>
-      <c r="B18" s="197" t="s">
+      <c r="B18" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C18" s="58"/>
@@ -31769,8 +31775,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="209"/>
-      <c r="B19" s="202"/>
+      <c r="A19" s="212"/>
+      <c r="B19" s="203"/>
       <c r="C19" s="118" t="s">
         <v>361</v>
       </c>
@@ -31779,8 +31785,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="209"/>
-      <c r="B20" s="202"/>
+      <c r="A20" s="212"/>
+      <c r="B20" s="203"/>
       <c r="C20" s="118" t="s">
         <v>359</v>
       </c>
@@ -31789,8 +31795,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="209"/>
-      <c r="B21" s="202"/>
+      <c r="A21" s="212"/>
+      <c r="B21" s="203"/>
       <c r="C21" s="124" t="s">
         <v>367</v>
       </c>
@@ -31799,8 +31805,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="209"/>
-      <c r="B22" s="202"/>
+      <c r="A22" s="212"/>
+      <c r="B22" s="203"/>
       <c r="C22" s="131" t="s">
         <v>359</v>
       </c>
@@ -31809,8 +31815,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="209"/>
-      <c r="B23" s="202"/>
+      <c r="A23" s="212"/>
+      <c r="B23" s="203"/>
       <c r="C23" s="135" t="s">
         <v>371</v>
       </c>
@@ -31819,8 +31825,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="210"/>
-      <c r="B24" s="198"/>
+      <c r="A24" s="213"/>
+      <c r="B24" s="197"/>
       <c r="C24" s="135" t="s">
         <v>359</v>
       </c>
@@ -31855,10 +31861,10 @@
       <c r="D26" s="98"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="194" t="s">
+      <c r="A27" s="207" t="s">
         <v>369</v>
       </c>
-      <c r="B27" s="197" t="s">
+      <c r="B27" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C27" s="136" t="s">
@@ -31867,8 +31873,8 @@
       <c r="D27" s="98"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="196"/>
-      <c r="B28" s="198"/>
+      <c r="A28" s="214"/>
+      <c r="B28" s="197"/>
       <c r="C28" s="136" t="s">
         <v>404</v>
       </c>
@@ -31885,10 +31891,10 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="194" t="s">
+      <c r="A30" s="207" t="s">
         <v>237</v>
       </c>
-      <c r="B30" s="197" t="s">
+      <c r="B30" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C30" s="58"/>
@@ -31897,24 +31903,24 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="195"/>
-      <c r="B31" s="202"/>
+      <c r="A31" s="208"/>
+      <c r="B31" s="203"/>
       <c r="C31" s="58"/>
       <c r="D31" s="58" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="195"/>
-      <c r="B32" s="202"/>
+      <c r="A32" s="208"/>
+      <c r="B32" s="203"/>
       <c r="C32" s="58"/>
       <c r="D32" s="58" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="195"/>
-      <c r="B33" s="202"/>
+      <c r="A33" s="208"/>
+      <c r="B33" s="203"/>
       <c r="C33" s="58" t="s">
         <v>300</v>
       </c>
@@ -31923,8 +31929,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="195"/>
-      <c r="B34" s="202"/>
+      <c r="A34" s="208"/>
+      <c r="B34" s="203"/>
       <c r="C34" s="58" t="s">
         <v>328</v>
       </c>
@@ -31933,8 +31939,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="196"/>
-      <c r="B35" s="198"/>
+      <c r="A35" s="214"/>
+      <c r="B35" s="197"/>
       <c r="C35" s="58" t="s">
         <v>373</v>
       </c>
@@ -31943,10 +31949,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="170" t="s">
+      <c r="A36" s="167" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="197" t="s">
+      <c r="B36" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C36" s="58" t="s">
@@ -31957,16 +31963,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="171"/>
-      <c r="B37" s="202"/>
+      <c r="A37" s="168"/>
+      <c r="B37" s="203"/>
       <c r="C37" s="58"/>
       <c r="D37" s="58" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="171"/>
-      <c r="B38" s="202"/>
+      <c r="A38" s="168"/>
+      <c r="B38" s="203"/>
       <c r="C38" s="106" t="s">
         <v>329</v>
       </c>
@@ -31975,8 +31981,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="171"/>
-      <c r="B39" s="202"/>
+      <c r="A39" s="168"/>
+      <c r="B39" s="203"/>
       <c r="C39" s="106" t="s">
         <v>359</v>
       </c>
@@ -31985,8 +31991,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="171"/>
-      <c r="B40" s="202"/>
+      <c r="A40" s="168"/>
+      <c r="B40" s="203"/>
       <c r="C40" s="106" t="s">
         <v>367</v>
       </c>
@@ -31995,8 +32001,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="171"/>
-      <c r="B41" s="202"/>
+      <c r="A41" s="168"/>
+      <c r="B41" s="203"/>
       <c r="C41" s="106" t="s">
         <v>371</v>
       </c>
@@ -32005,8 +32011,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="171"/>
-      <c r="B42" s="202"/>
+      <c r="A42" s="168"/>
+      <c r="B42" s="203"/>
       <c r="C42" s="106" t="s">
         <v>381</v>
       </c>
@@ -32015,8 +32021,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="172"/>
-      <c r="B43" s="198"/>
+      <c r="A43" s="169"/>
+      <c r="B43" s="197"/>
       <c r="C43" s="96" t="s">
         <v>359</v>
       </c>
@@ -32025,13 +32031,13 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="164" t="s">
+      <c r="A44" s="174" t="s">
         <v>222</v>
       </c>
-      <c r="B44" s="197" t="s">
+      <c r="B44" s="196" t="s">
         <v>234</v>
       </c>
-      <c r="C44" s="204" t="s">
+      <c r="C44" s="218" t="s">
         <v>239</v>
       </c>
       <c r="D44" s="101" t="s">
@@ -32039,17 +32045,17 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="203"/>
-      <c r="B45" s="202"/>
-      <c r="C45" s="205"/>
+      <c r="A45" s="202"/>
+      <c r="B45" s="203"/>
+      <c r="C45" s="219"/>
       <c r="D45" s="98" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="203"/>
-      <c r="B46" s="202"/>
-      <c r="C46" s="211" t="s">
+      <c r="A46" s="202"/>
+      <c r="B46" s="203"/>
+      <c r="C46" s="201" t="s">
         <v>240</v>
       </c>
       <c r="D46" s="58" t="s">
@@ -32057,16 +32063,16 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="203"/>
-      <c r="B47" s="202"/>
-      <c r="C47" s="211"/>
+      <c r="A47" s="202"/>
+      <c r="B47" s="203"/>
+      <c r="C47" s="201"/>
       <c r="D47" s="61" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="203"/>
-      <c r="B48" s="202"/>
+      <c r="A48" s="202"/>
+      <c r="B48" s="203"/>
       <c r="C48" s="103" t="s">
         <v>307</v>
       </c>
@@ -32075,8 +32081,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="203"/>
-      <c r="B49" s="202"/>
+      <c r="A49" s="202"/>
+      <c r="B49" s="203"/>
       <c r="C49" s="103">
         <v>2.1</v>
       </c>
@@ -32085,8 +32091,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="203"/>
-      <c r="B50" s="202"/>
+      <c r="A50" s="202"/>
+      <c r="B50" s="203"/>
       <c r="C50" s="103" t="s">
         <v>239</v>
       </c>
@@ -32095,8 +32101,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="203"/>
-      <c r="B51" s="202"/>
+      <c r="A51" s="202"/>
+      <c r="B51" s="203"/>
       <c r="C51" s="114" t="s">
         <v>239</v>
       </c>
@@ -32105,8 +32111,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="203"/>
-      <c r="B52" s="202"/>
+      <c r="A52" s="202"/>
+      <c r="B52" s="203"/>
       <c r="C52" s="128" t="s">
         <v>239</v>
       </c>
@@ -32115,8 +32121,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="203"/>
-      <c r="B53" s="202"/>
+      <c r="A53" s="202"/>
+      <c r="B53" s="203"/>
       <c r="C53" s="134" t="s">
         <v>378</v>
       </c>
@@ -32125,8 +32131,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="203"/>
-      <c r="B54" s="202"/>
+      <c r="A54" s="202"/>
+      <c r="B54" s="203"/>
       <c r="C54" s="136">
         <v>2.1</v>
       </c>
@@ -32135,8 +32141,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="203"/>
-      <c r="B55" s="202"/>
+      <c r="A55" s="202"/>
+      <c r="B55" s="203"/>
       <c r="C55" s="136" t="s">
         <v>239</v>
       </c>
@@ -32145,8 +32151,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="203"/>
-      <c r="B56" s="202"/>
+      <c r="A56" s="202"/>
+      <c r="B56" s="203"/>
       <c r="C56" s="141" t="s">
         <v>239</v>
       </c>
@@ -32155,10 +32161,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="212" t="s">
+      <c r="A57" s="204" t="s">
         <v>296</v>
       </c>
-      <c r="B57" s="197" t="s">
+      <c r="B57" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -32169,8 +32175,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="213"/>
-      <c r="B58" s="202"/>
+      <c r="A58" s="205"/>
+      <c r="B58" s="203"/>
       <c r="C58" s="61" t="s">
         <v>281</v>
       </c>
@@ -32179,8 +32185,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="214"/>
-      <c r="B59" s="198"/>
+      <c r="A59" s="206"/>
+      <c r="B59" s="197"/>
       <c r="C59" s="58" t="s">
         <v>350</v>
       </c>
@@ -32189,10 +32195,10 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="194" t="s">
+      <c r="A60" s="207" t="s">
         <v>370</v>
       </c>
-      <c r="B60" s="197" t="s">
+      <c r="B60" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C60" s="128" t="s">
@@ -32201,8 +32207,8 @@
       <c r="D60" s="58"/>
     </row>
     <row r="61" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="195"/>
-      <c r="B61" s="202"/>
+      <c r="A61" s="208"/>
+      <c r="B61" s="203"/>
       <c r="C61" s="131" t="s">
         <v>378</v>
       </c>
@@ -32211,8 +32217,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="195"/>
-      <c r="B62" s="202"/>
+      <c r="A62" s="208"/>
+      <c r="B62" s="203"/>
       <c r="C62" s="136">
         <v>2.1</v>
       </c>
@@ -32221,8 +32227,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="195"/>
-      <c r="B63" s="202"/>
+      <c r="A63" s="208"/>
+      <c r="B63" s="203"/>
       <c r="C63" s="136" t="s">
         <v>240</v>
       </c>
@@ -32231,8 +32237,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="195"/>
-      <c r="B64" s="202"/>
+      <c r="A64" s="208"/>
+      <c r="B64" s="203"/>
       <c r="C64" s="133" t="s">
         <v>239</v>
       </c>
@@ -32261,10 +32267,10 @@
       <c r="D66" s="98"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="164" t="s">
+      <c r="A67" s="174" t="s">
         <v>260</v>
       </c>
-      <c r="B67" s="197" t="s">
+      <c r="B67" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C67" s="58"/>
@@ -32273,24 +32279,24 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="203"/>
-      <c r="B68" s="202"/>
+      <c r="A68" s="202"/>
+      <c r="B68" s="203"/>
       <c r="C68" s="58"/>
       <c r="D68" s="58" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="203"/>
-      <c r="B69" s="202"/>
+      <c r="A69" s="202"/>
+      <c r="B69" s="203"/>
       <c r="C69" s="58"/>
       <c r="D69" s="98" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="203"/>
-      <c r="B70" s="202"/>
+      <c r="A70" s="202"/>
+      <c r="B70" s="203"/>
       <c r="C70" s="58" t="s">
         <v>424</v>
       </c>
@@ -32299,8 +32305,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="203"/>
-      <c r="B71" s="202"/>
+      <c r="A71" s="202"/>
+      <c r="B71" s="203"/>
       <c r="C71" s="58" t="s">
         <v>429</v>
       </c>
@@ -32309,10 +32315,10 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="159" t="s">
+      <c r="A72" s="163" t="s">
         <v>334</v>
       </c>
-      <c r="B72" s="193" t="s">
+      <c r="B72" s="183" t="s">
         <v>234</v>
       </c>
       <c r="C72" s="79" t="s">
@@ -32323,8 +32329,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="159"/>
-      <c r="B73" s="193"/>
+      <c r="A73" s="163"/>
+      <c r="B73" s="183"/>
       <c r="C73" s="58" t="s">
         <v>411</v>
       </c>
@@ -32333,38 +32339,38 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="159"/>
-      <c r="B74" s="193"/>
+      <c r="A74" s="163"/>
+      <c r="B74" s="183"/>
       <c r="C74" s="140" t="s">
         <v>414</v>
       </c>
-      <c r="D74" s="194" t="s">
+      <c r="D74" s="207" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="159"/>
-      <c r="B75" s="193"/>
+      <c r="A75" s="163"/>
+      <c r="B75" s="183"/>
       <c r="C75" s="140" t="s">
         <v>415</v>
       </c>
-      <c r="D75" s="195"/>
+      <c r="D75" s="208"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="159"/>
-      <c r="B76" s="193"/>
+      <c r="A76" s="163"/>
+      <c r="B76" s="183"/>
       <c r="C76" s="140" t="s">
         <v>416</v>
       </c>
-      <c r="D76" s="195"/>
+      <c r="D76" s="208"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="159"/>
-      <c r="B77" s="193"/>
+      <c r="A77" s="163"/>
+      <c r="B77" s="183"/>
       <c r="C77" s="140" t="s">
         <v>417</v>
       </c>
-      <c r="D77" s="196"/>
+      <c r="D77" s="214"/>
     </row>
     <row r="78" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="96" t="s">
@@ -32381,10 +32387,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="212" t="s">
+      <c r="A79" s="204" t="s">
         <v>32</v>
       </c>
-      <c r="B79" s="197" t="s">
+      <c r="B79" s="196" t="s">
         <v>234</v>
       </c>
       <c r="C79" s="58" t="s">
@@ -32395,8 +32401,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="213"/>
-      <c r="B80" s="202"/>
+      <c r="A80" s="205"/>
+      <c r="B80" s="203"/>
       <c r="C80" s="58" t="s">
         <v>270</v>
       </c>
@@ -32405,8 +32411,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="213"/>
-      <c r="B81" s="202"/>
+      <c r="A81" s="205"/>
+      <c r="B81" s="203"/>
       <c r="C81" s="58" t="s">
         <v>269</v>
       </c>
@@ -32415,8 +32421,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="213"/>
-      <c r="B82" s="202"/>
+      <c r="A82" s="205"/>
+      <c r="B82" s="203"/>
       <c r="C82" s="98" t="s">
         <v>277</v>
       </c>
@@ -32425,8 +32431,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="213"/>
-      <c r="B83" s="202"/>
+      <c r="A83" s="205"/>
+      <c r="B83" s="203"/>
       <c r="C83" s="58" t="s">
         <v>282</v>
       </c>
@@ -32435,8 +32441,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="213"/>
-      <c r="B84" s="202"/>
+      <c r="A84" s="205"/>
+      <c r="B84" s="203"/>
       <c r="C84" s="58" t="s">
         <v>283</v>
       </c>
@@ -32445,8 +32451,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="213"/>
-      <c r="B85" s="202"/>
+      <c r="A85" s="205"/>
+      <c r="B85" s="203"/>
       <c r="C85" s="98" t="s">
         <v>288</v>
       </c>
@@ -32455,8 +32461,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="213"/>
-      <c r="B86" s="202"/>
+      <c r="A86" s="205"/>
+      <c r="B86" s="203"/>
       <c r="C86" s="98" t="s">
         <v>302</v>
       </c>
@@ -32465,8 +32471,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="213"/>
-      <c r="B87" s="202"/>
+      <c r="A87" s="205"/>
+      <c r="B87" s="203"/>
       <c r="C87" s="98" t="s">
         <v>289</v>
       </c>
@@ -32475,8 +32481,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="213"/>
-      <c r="B88" s="202"/>
+      <c r="A88" s="205"/>
+      <c r="B88" s="203"/>
       <c r="C88" s="105" t="s">
         <v>244</v>
       </c>
@@ -32485,8 +32491,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="213"/>
-      <c r="B89" s="202"/>
+      <c r="A89" s="205"/>
+      <c r="B89" s="203"/>
       <c r="C89" s="106" t="s">
         <v>311</v>
       </c>
@@ -32495,8 +32501,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="213"/>
-      <c r="B90" s="202"/>
+      <c r="A90" s="205"/>
+      <c r="B90" s="203"/>
       <c r="C90" s="58" t="s">
         <v>312</v>
       </c>
@@ -32505,8 +32511,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="213"/>
-      <c r="B91" s="202"/>
+      <c r="A91" s="205"/>
+      <c r="B91" s="203"/>
       <c r="C91" s="98" t="s">
         <v>313</v>
       </c>
@@ -32515,8 +32521,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="213"/>
-      <c r="B92" s="202"/>
+      <c r="A92" s="205"/>
+      <c r="B92" s="203"/>
       <c r="C92" s="98" t="s">
         <v>315</v>
       </c>
@@ -32525,8 +32531,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="213"/>
-      <c r="B93" s="202"/>
+      <c r="A93" s="205"/>
+      <c r="B93" s="203"/>
       <c r="C93" s="98" t="s">
         <v>268</v>
       </c>
@@ -32535,8 +32541,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="213"/>
-      <c r="B94" s="202"/>
+      <c r="A94" s="205"/>
+      <c r="B94" s="203"/>
       <c r="C94" s="58" t="s">
         <v>318</v>
       </c>
@@ -32545,8 +32551,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="213"/>
-      <c r="B95" s="202"/>
+      <c r="A95" s="205"/>
+      <c r="B95" s="203"/>
       <c r="C95" s="98" t="s">
         <v>283</v>
       </c>
@@ -32555,8 +32561,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="213"/>
-      <c r="B96" s="202"/>
+      <c r="A96" s="205"/>
+      <c r="B96" s="203"/>
       <c r="C96" s="98" t="s">
         <v>319</v>
       </c>
@@ -32565,16 +32571,16 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="213"/>
-      <c r="B97" s="202"/>
+      <c r="A97" s="205"/>
+      <c r="B97" s="203"/>
       <c r="C97" s="58"/>
       <c r="D97" s="107" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="213"/>
-      <c r="B98" s="202"/>
+      <c r="A98" s="205"/>
+      <c r="B98" s="203"/>
       <c r="C98" s="98" t="s">
         <v>322</v>
       </c>
@@ -32583,8 +32589,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="213"/>
-      <c r="B99" s="202"/>
+      <c r="A99" s="205"/>
+      <c r="B99" s="203"/>
       <c r="C99" s="98" t="s">
         <v>268</v>
       </c>
@@ -32593,8 +32599,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="213"/>
-      <c r="B100" s="202"/>
+      <c r="A100" s="205"/>
+      <c r="B100" s="203"/>
       <c r="C100" s="98" t="s">
         <v>339</v>
       </c>
@@ -32603,8 +32609,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="213"/>
-      <c r="B101" s="202"/>
+      <c r="A101" s="205"/>
+      <c r="B101" s="203"/>
       <c r="C101" s="98" t="s">
         <v>340</v>
       </c>
@@ -32613,8 +32619,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="213"/>
-      <c r="B102" s="202"/>
+      <c r="A102" s="205"/>
+      <c r="B102" s="203"/>
       <c r="C102" s="98" t="s">
         <v>324</v>
       </c>
@@ -32623,8 +32629,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="213"/>
-      <c r="B103" s="202"/>
+      <c r="A103" s="205"/>
+      <c r="B103" s="203"/>
       <c r="C103" s="113" t="s">
         <v>345</v>
       </c>
@@ -32633,8 +32639,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="213"/>
-      <c r="B104" s="202"/>
+      <c r="A104" s="205"/>
+      <c r="B104" s="203"/>
       <c r="C104" s="98" t="s">
         <v>338</v>
       </c>
@@ -32643,8 +32649,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="213"/>
-      <c r="B105" s="202"/>
+      <c r="A105" s="205"/>
+      <c r="B105" s="203"/>
       <c r="C105" s="98" t="s">
         <v>353</v>
       </c>
@@ -32653,8 +32659,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="213"/>
-      <c r="B106" s="202"/>
+      <c r="A106" s="205"/>
+      <c r="B106" s="203"/>
       <c r="C106" s="117" t="s">
         <v>356</v>
       </c>
@@ -32663,8 +32669,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="213"/>
-      <c r="B107" s="202"/>
+      <c r="A107" s="205"/>
+      <c r="B107" s="203"/>
       <c r="C107" s="98" t="s">
         <v>357</v>
       </c>
@@ -32673,8 +32679,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="213"/>
-      <c r="B108" s="202"/>
+      <c r="A108" s="205"/>
+      <c r="B108" s="203"/>
       <c r="C108" s="98" t="s">
         <v>358</v>
       </c>
@@ -32683,8 +32689,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="213"/>
-      <c r="B109" s="202"/>
+      <c r="A109" s="205"/>
+      <c r="B109" s="203"/>
       <c r="C109" s="98" t="s">
         <v>364</v>
       </c>
@@ -32693,8 +32699,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="213"/>
-      <c r="B110" s="202"/>
+      <c r="A110" s="205"/>
+      <c r="B110" s="203"/>
       <c r="C110" s="98" t="s">
         <v>366</v>
       </c>
@@ -32703,8 +32709,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="213"/>
-      <c r="B111" s="202"/>
+      <c r="A111" s="205"/>
+      <c r="B111" s="203"/>
       <c r="C111" s="98" t="s">
         <v>372</v>
       </c>
@@ -32713,8 +32719,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="213"/>
-      <c r="B112" s="202"/>
+      <c r="A112" s="205"/>
+      <c r="B112" s="203"/>
       <c r="C112" s="98" t="s">
         <v>364</v>
       </c>
@@ -32723,8 +32729,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="213"/>
-      <c r="B113" s="202"/>
+      <c r="A113" s="205"/>
+      <c r="B113" s="203"/>
       <c r="C113" s="113" t="s">
         <v>385</v>
       </c>
@@ -32733,8 +32739,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="213"/>
-      <c r="B114" s="202"/>
+      <c r="A114" s="205"/>
+      <c r="B114" s="203"/>
       <c r="C114" s="58" t="s">
         <v>389</v>
       </c>
@@ -32743,8 +32749,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="213"/>
-      <c r="B115" s="202"/>
+      <c r="A115" s="205"/>
+      <c r="B115" s="203"/>
       <c r="C115" s="58" t="s">
         <v>392</v>
       </c>
@@ -32753,8 +32759,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="213"/>
-      <c r="B116" s="202"/>
+      <c r="A116" s="205"/>
+      <c r="B116" s="203"/>
       <c r="C116" s="58" t="s">
         <v>393</v>
       </c>
@@ -32763,8 +32769,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="213"/>
-      <c r="B117" s="202"/>
+      <c r="A117" s="205"/>
+      <c r="B117" s="203"/>
       <c r="C117" s="58" t="s">
         <v>394</v>
       </c>
@@ -32773,8 +32779,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="213"/>
-      <c r="B118" s="202"/>
+      <c r="A118" s="205"/>
+      <c r="B118" s="203"/>
       <c r="C118" s="58" t="s">
         <v>395</v>
       </c>
@@ -32783,8 +32789,8 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="213"/>
-      <c r="B119" s="202"/>
+      <c r="A119" s="205"/>
+      <c r="B119" s="203"/>
       <c r="C119" s="58" t="s">
         <v>396</v>
       </c>
@@ -32793,8 +32799,8 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="213"/>
-      <c r="B120" s="202"/>
+      <c r="A120" s="205"/>
+      <c r="B120" s="203"/>
       <c r="C120" s="58" t="s">
         <v>399</v>
       </c>
@@ -32803,8 +32809,8 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="213"/>
-      <c r="B121" s="202"/>
+      <c r="A121" s="205"/>
+      <c r="B121" s="203"/>
       <c r="C121" s="58" t="s">
         <v>409</v>
       </c>
@@ -32813,8 +32819,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="213"/>
-      <c r="B122" s="202"/>
+      <c r="A122" s="205"/>
+      <c r="B122" s="203"/>
       <c r="C122" s="58" t="s">
         <v>410</v>
       </c>
@@ -32823,8 +32829,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="213"/>
-      <c r="B123" s="202"/>
+      <c r="A123" s="205"/>
+      <c r="B123" s="203"/>
       <c r="C123" s="58" t="s">
         <v>427</v>
       </c>
@@ -32833,8 +32839,8 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="214"/>
-      <c r="B124" s="198"/>
+      <c r="A124" s="205"/>
+      <c r="B124" s="203"/>
       <c r="C124" s="58" t="s">
         <v>428</v>
       </c>
@@ -32843,24 +32849,20 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="143" t="s">
+      <c r="A125" s="206"/>
+      <c r="B125" s="197"/>
+      <c r="C125" s="58" t="s">
+        <v>431</v>
+      </c>
+      <c r="D125" s="58" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="143" t="s">
         <v>421</v>
       </c>
-      <c r="B125" s="142" t="s">
-        <v>234</v>
-      </c>
-      <c r="C125" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D125" s="98" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="96" t="s">
-        <v>309</v>
-      </c>
-      <c r="B126" s="123" t="s">
+      <c r="B126" s="142" t="s">
         <v>234</v>
       </c>
       <c r="C126" s="58" t="s">
@@ -32870,9 +32872,9 @@
         <v>274</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="96" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B127" s="123" t="s">
         <v>234</v>
@@ -32884,363 +32886,393 @@
         <v>274</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="39" t="s">
+    <row r="128" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="96" t="s">
+        <v>310</v>
+      </c>
+      <c r="B128" s="123" t="s">
+        <v>234</v>
+      </c>
+      <c r="C128" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D128" s="98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B128" s="39"/>
-      <c r="C128" s="39"/>
-      <c r="D128" s="44"/>
-    </row>
-    <row r="129" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="164" t="s">
+      <c r="B129" s="39"/>
+      <c r="C129" s="39"/>
+      <c r="D129" s="44"/>
+    </row>
+    <row r="130" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="174" t="s">
         <v>84</v>
       </c>
-      <c r="B129" s="197" t="s">
+      <c r="B130" s="196" t="s">
         <v>234</v>
       </c>
-      <c r="C129" s="58"/>
-      <c r="D129" s="79" t="s">
+      <c r="C130" s="58"/>
+      <c r="D130" s="79" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="203"/>
-      <c r="B130" s="202"/>
-      <c r="C130" s="104" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="202"/>
+      <c r="B131" s="203"/>
+      <c r="C131" s="104" t="s">
         <v>246</v>
       </c>
-      <c r="D130" s="58" t="s">
+      <c r="D131" s="58" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="203"/>
-      <c r="B131" s="202"/>
-      <c r="C131" s="104">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="202"/>
+      <c r="B132" s="203"/>
+      <c r="C132" s="104">
         <v>10.1</v>
-      </c>
-      <c r="D131" s="58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="203"/>
-      <c r="B132" s="202"/>
-      <c r="C132" s="104">
-        <v>10.199999999999999</v>
       </c>
       <c r="D132" s="58" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="203"/>
-      <c r="B133" s="202"/>
-      <c r="C133" s="109" t="s">
+      <c r="A133" s="202"/>
+      <c r="B133" s="203"/>
+      <c r="C133" s="104">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D133" s="58" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="202"/>
+      <c r="B134" s="203"/>
+      <c r="C134" s="109" t="s">
         <v>293</v>
       </c>
-      <c r="D133" s="99" t="s">
+      <c r="D134" s="99" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="203"/>
-      <c r="B134" s="202"/>
-      <c r="C134" s="109" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="202"/>
+      <c r="B135" s="203"/>
+      <c r="C135" s="109" t="s">
         <v>375</v>
       </c>
-      <c r="D134" s="99" t="s">
+      <c r="D135" s="99" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="203"/>
-      <c r="B135" s="202"/>
-      <c r="C135" s="109" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="202"/>
+      <c r="B136" s="203"/>
+      <c r="C136" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="D135" s="99" t="s">
+      <c r="D136" s="99" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="203"/>
-      <c r="B136" s="202"/>
-      <c r="C136" s="109" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="202"/>
+      <c r="B137" s="203"/>
+      <c r="C137" s="109" t="s">
         <v>422</v>
       </c>
-      <c r="D136" s="99" t="s">
+      <c r="D137" s="99" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="165"/>
-      <c r="B137" s="198"/>
-      <c r="C137" s="109" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="175"/>
+      <c r="B138" s="197"/>
+      <c r="C138" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="D137" s="99" t="s">
+      <c r="D138" s="99" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="164" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="174" t="s">
         <v>247</v>
       </c>
-      <c r="B138" s="197" t="s">
+      <c r="B139" s="196" t="s">
         <v>234</v>
       </c>
-      <c r="C138" s="193"/>
-      <c r="D138" s="217" t="s">
+      <c r="C139" s="183"/>
+      <c r="D139" s="198" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="165"/>
-      <c r="B139" s="198"/>
-      <c r="C139" s="193"/>
-      <c r="D139" s="217"/>
-    </row>
-    <row r="140" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="121" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="175"/>
+      <c r="B140" s="197"/>
+      <c r="C140" s="183"/>
+      <c r="D140" s="198"/>
+    </row>
+    <row r="141" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="121" t="s">
         <v>262</v>
       </c>
-      <c r="B140" s="123" t="s">
+      <c r="B141" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C140" s="104" t="s">
+      <c r="C141" s="104" t="s">
         <v>250</v>
       </c>
-      <c r="D140" s="98" t="s">
+      <c r="D141" s="98" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="95" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B141" s="39"/>
-      <c r="C141" s="97"/>
-      <c r="D141" s="97"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="96" t="s">
+      <c r="B142" s="39"/>
+      <c r="C142" s="97"/>
+      <c r="D142" s="97"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="B142" s="123" t="s">
+      <c r="B143" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C142" s="110" t="s">
+      <c r="C143" s="110" t="s">
         <v>265</v>
       </c>
-      <c r="D142" s="58" t="s">
+      <c r="D143" s="58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="164" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="174" t="s">
         <v>285</v>
       </c>
-      <c r="B143" s="197" t="s">
+      <c r="B144" s="196" t="s">
         <v>234</v>
       </c>
-      <c r="C143" s="99" t="s">
+      <c r="C144" s="99" t="s">
         <v>295</v>
       </c>
-      <c r="D143" s="58" t="s">
+      <c r="D144" s="58" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="203"/>
-      <c r="B144" s="202"/>
-      <c r="C144" s="58" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="202"/>
+      <c r="B145" s="203"/>
+      <c r="C145" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="D144" s="98" t="s">
+      <c r="D145" s="98" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A145" s="165"/>
-      <c r="B145" s="198"/>
-      <c r="C145" s="110" t="s">
+    <row r="146" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A146" s="175"/>
+      <c r="B146" s="197"/>
+      <c r="C146" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="D145" s="58" t="s">
+      <c r="D146" s="58" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="97" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="B146" s="97"/>
-      <c r="C146" s="97"/>
-      <c r="D146" s="97"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="199" t="s">
+      <c r="B147" s="97"/>
+      <c r="C147" s="97"/>
+      <c r="D147" s="97"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="215" t="s">
         <v>58</v>
       </c>
-      <c r="B147" s="197" t="s">
+      <c r="B148" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="C147" s="110" t="s">
-        <v>265</v>
-      </c>
-      <c r="D147" s="58" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="200"/>
-      <c r="B148" s="202"/>
       <c r="C148" s="110" t="s">
         <v>265</v>
       </c>
       <c r="D148" s="58" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="216"/>
+      <c r="B149" s="203"/>
+      <c r="C149" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="D149" s="58" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="201"/>
-      <c r="B149" s="198"/>
-      <c r="C149" s="58"/>
-      <c r="D149" s="58" t="s">
+    <row r="150" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="217"/>
+      <c r="B150" s="197"/>
+      <c r="C150" s="58"/>
+      <c r="D150" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="215" t="s">
+    <row r="151" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A151" s="194" t="s">
         <v>59</v>
       </c>
-      <c r="B150" s="197" t="s">
+      <c r="B151" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="C150" s="61" t="s">
+      <c r="C151" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D150" s="58" t="s">
+      <c r="D151" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="216"/>
-      <c r="B151" s="198"/>
-      <c r="C151" s="61"/>
-      <c r="D151" s="58" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="195"/>
+      <c r="B152" s="197"/>
+      <c r="C152" s="61"/>
+      <c r="D152" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A152" s="218" t="s">
+    <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A153" s="199" t="s">
         <v>291</v>
       </c>
-      <c r="B152" s="197" t="s">
+      <c r="B153" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="C152" s="61"/>
-      <c r="D152" s="61" t="s">
+      <c r="C153" s="61"/>
+      <c r="D153" s="61" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="219"/>
-      <c r="B153" s="198"/>
-      <c r="C153" s="58"/>
-      <c r="D153" s="58" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="200"/>
+      <c r="B154" s="197"/>
+      <c r="C154" s="58"/>
+      <c r="D154" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="215" t="s">
+    <row r="155" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="194" t="s">
         <v>60</v>
       </c>
-      <c r="B154" s="197" t="s">
+      <c r="B155" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="C154" s="61" t="s">
+      <c r="C155" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D154" s="58" t="s">
+      <c r="D155" s="58" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="216"/>
-      <c r="B155" s="198"/>
-      <c r="C155" s="58"/>
-      <c r="D155" s="58" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="195"/>
+      <c r="B156" s="197"/>
+      <c r="C156" s="58"/>
+      <c r="D156" s="58" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="97" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="97" t="s">
         <v>273</v>
       </c>
-      <c r="B156" s="97"/>
-      <c r="C156" s="97"/>
-      <c r="D156" s="97"/>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="58"/>
-      <c r="B157" s="123" t="s">
+      <c r="B157" s="97"/>
+      <c r="C157" s="97"/>
+      <c r="D157" s="97"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="58"/>
+      <c r="B158" s="123" t="s">
         <v>234</v>
       </c>
-      <c r="C157" s="58" t="s">
+      <c r="C158" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D157" s="98" t="s">
+      <c r="D158" s="98" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="97" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="97" t="s">
         <v>279</v>
       </c>
-      <c r="B158" s="97"/>
-      <c r="C158" s="97"/>
-      <c r="D158" s="97"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="58"/>
-      <c r="B159" s="137" t="s">
-        <v>234</v>
-      </c>
-      <c r="C159" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D159" s="98" t="s">
-        <v>274</v>
-      </c>
+      <c r="B159" s="97"/>
+      <c r="C159" s="97"/>
+      <c r="D159" s="97"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="58"/>
-      <c r="B160" s="123"/>
+      <c r="B160" s="137" t="s">
+        <v>234</v>
+      </c>
       <c r="C160" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D160" s="98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="58"/>
+      <c r="B161" s="123"/>
+      <c r="C161" s="58" t="s">
         <v>401</v>
       </c>
-      <c r="D160" s="98" t="s">
+      <c r="D161" s="98" t="s">
         <v>402</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A154:A155"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="A152:A153"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A148:A150"/>
+    <mergeCell ref="B148:B150"/>
+    <mergeCell ref="A130:A138"/>
+    <mergeCell ref="B130:B138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="B139:B140"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="B144:B146"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="B36:B43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A13:A16"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="A67:A71"/>
     <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A79:A124"/>
-    <mergeCell ref="B79:B124"/>
+    <mergeCell ref="A79:A125"/>
+    <mergeCell ref="B79:B125"/>
     <mergeCell ref="A44:A56"/>
     <mergeCell ref="B44:B56"/>
     <mergeCell ref="A57:A59"/>
@@ -33249,30 +33281,14 @@
     <mergeCell ref="B72:B77"/>
     <mergeCell ref="A60:A64"/>
     <mergeCell ref="B60:B64"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A18:A24"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A147:A149"/>
-    <mergeCell ref="B147:B149"/>
-    <mergeCell ref="A129:A137"/>
-    <mergeCell ref="B129:B137"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="B143:B145"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="B36:B43"/>
-    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A155:A156"/>
+    <mergeCell ref="B155:B156"/>
+    <mergeCell ref="D139:D140"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="A153:A154"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="C139:C140"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>